<commit_message>
Planung verlief gut habe die modelle erstellt und die doku ergänz
</commit_message>
<xml_diff>
--- a/Doku/Shannon_Neil_Schuerch_Zeitplan_IPA_2022.xlsx
+++ b/Doku/Shannon_Neil_Schuerch_Zeitplan_IPA_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Dashboard\Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62145DE4-8E4B-417C-B9B1-218E026F8D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20095296-03B1-4979-8F57-584E35EB148C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14625" xr2:uid="{B08A1154-B080-432D-B17F-9B53C1DBF0AA}"/>
+    <workbookView xWindow="-28260" yWindow="-120" windowWidth="28380" windowHeight="14220" xr2:uid="{B08A1154-B080-432D-B17F-9B53C1DBF0AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1043,7 +1043,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1114,7 +1114,6 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1274,6 +1273,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1594,7 +1597,7 @@
   <dimension ref="A1:BC66"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BB29" sqref="BB29"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1651,169 +1654,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="74" t="s">
+      <c r="C1" s="70"/>
+      <c r="D1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="74" t="s">
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="74" t="s">
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="74" t="s">
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="74" t="s">
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="76"/>
-      <c r="X1" s="74" t="s">
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="75"/>
+      <c r="X1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="75"/>
-      <c r="AA1" s="76"/>
-      <c r="AB1" s="74" t="s">
+      <c r="Y1" s="74"/>
+      <c r="Z1" s="74"/>
+      <c r="AA1" s="75"/>
+      <c r="AB1" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="AC1" s="75"/>
-      <c r="AD1" s="75"/>
-      <c r="AE1" s="76"/>
-      <c r="AF1" s="74" t="s">
+      <c r="AC1" s="74"/>
+      <c r="AD1" s="74"/>
+      <c r="AE1" s="75"/>
+      <c r="AF1" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="AG1" s="75"/>
-      <c r="AH1" s="75"/>
-      <c r="AI1" s="76"/>
-      <c r="AJ1" s="74" t="s">
+      <c r="AG1" s="74"/>
+      <c r="AH1" s="74"/>
+      <c r="AI1" s="75"/>
+      <c r="AJ1" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="AK1" s="75"/>
-      <c r="AL1" s="75"/>
-      <c r="AM1" s="76"/>
-      <c r="AN1" s="74" t="s">
+      <c r="AK1" s="74"/>
+      <c r="AL1" s="74"/>
+      <c r="AM1" s="75"/>
+      <c r="AN1" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="AO1" s="75"/>
-      <c r="AP1" s="75"/>
-      <c r="AQ1" s="76"/>
-      <c r="AR1" s="74" t="s">
+      <c r="AO1" s="74"/>
+      <c r="AP1" s="74"/>
+      <c r="AQ1" s="75"/>
+      <c r="AR1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="AS1" s="75"/>
-      <c r="AT1" s="75"/>
-      <c r="AU1" s="76"/>
-      <c r="AV1" s="74" t="s">
+      <c r="AS1" s="74"/>
+      <c r="AT1" s="74"/>
+      <c r="AU1" s="75"/>
+      <c r="AV1" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="AW1" s="75"/>
-      <c r="AX1" s="75"/>
-      <c r="AY1" s="76"/>
-      <c r="AZ1" s="105" t="s">
+      <c r="AW1" s="74"/>
+      <c r="AX1" s="74"/>
+      <c r="AY1" s="75"/>
+      <c r="AZ1" s="104" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A2" s="68"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="77">
+      <c r="A2" s="67"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="76">
         <v>44627</v>
       </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="77">
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="76">
         <v>44628</v>
       </c>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="77">
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="76">
         <v>44629</v>
       </c>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="77">
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="76">
         <v>44630</v>
       </c>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="77">
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="76">
         <v>44631</v>
       </c>
-      <c r="U2" s="78"/>
-      <c r="V2" s="78"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="77">
+      <c r="U2" s="77"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="78"/>
+      <c r="X2" s="76">
         <v>44634</v>
       </c>
-      <c r="Y2" s="78"/>
-      <c r="Z2" s="78"/>
-      <c r="AA2" s="79"/>
-      <c r="AB2" s="77">
+      <c r="Y2" s="77"/>
+      <c r="Z2" s="77"/>
+      <c r="AA2" s="78"/>
+      <c r="AB2" s="76">
         <v>44635</v>
       </c>
-      <c r="AC2" s="78"/>
-      <c r="AD2" s="78"/>
-      <c r="AE2" s="79"/>
-      <c r="AF2" s="77">
+      <c r="AC2" s="77"/>
+      <c r="AD2" s="77"/>
+      <c r="AE2" s="78"/>
+      <c r="AF2" s="76">
         <v>44636</v>
       </c>
-      <c r="AG2" s="78"/>
-      <c r="AH2" s="78"/>
-      <c r="AI2" s="79"/>
-      <c r="AJ2" s="77">
+      <c r="AG2" s="77"/>
+      <c r="AH2" s="77"/>
+      <c r="AI2" s="78"/>
+      <c r="AJ2" s="76">
         <v>44637</v>
       </c>
-      <c r="AK2" s="78"/>
-      <c r="AL2" s="78"/>
-      <c r="AM2" s="79"/>
-      <c r="AN2" s="77">
+      <c r="AK2" s="77"/>
+      <c r="AL2" s="77"/>
+      <c r="AM2" s="78"/>
+      <c r="AN2" s="76">
         <v>44638</v>
       </c>
-      <c r="AO2" s="78"/>
-      <c r="AP2" s="78"/>
-      <c r="AQ2" s="79"/>
-      <c r="AR2" s="77">
+      <c r="AO2" s="77"/>
+      <c r="AP2" s="77"/>
+      <c r="AQ2" s="78"/>
+      <c r="AR2" s="76">
         <v>44641</v>
       </c>
-      <c r="AS2" s="78"/>
-      <c r="AT2" s="78"/>
-      <c r="AU2" s="79"/>
-      <c r="AV2" s="77">
+      <c r="AS2" s="77"/>
+      <c r="AT2" s="77"/>
+      <c r="AU2" s="78"/>
+      <c r="AV2" s="76">
         <v>44642</v>
       </c>
-      <c r="AW2" s="78"/>
-      <c r="AX2" s="78"/>
-      <c r="AY2" s="79"/>
-      <c r="AZ2" s="106"/>
+      <c r="AW2" s="77"/>
+      <c r="AX2" s="77"/>
+      <c r="AY2" s="78"/>
+      <c r="AZ2" s="105"/>
     </row>
     <row r="3" spans="1:55" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69"/>
+      <c r="A3" s="68"/>
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
@@ -1964,16 +1967,16 @@
       <c r="AY3" s="12">
         <v>17</v>
       </c>
-      <c r="AZ3" s="107"/>
+      <c r="AZ3" s="106"/>
     </row>
     <row r="4" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="91">
+      <c r="B4" s="90">
         <v>4</v>
       </c>
-      <c r="C4" s="93">
+      <c r="C4" s="92">
         <v>2</v>
       </c>
       <c r="D4" s="15"/>
@@ -1992,12 +1995,12 @@
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
       <c r="S4" s="17"/>
-      <c r="T4" s="108" t="s">
+      <c r="T4" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="U4" s="109"/>
-      <c r="V4" s="109"/>
-      <c r="W4" s="99"/>
+      <c r="U4" s="108"/>
+      <c r="V4" s="108"/>
+      <c r="W4" s="98"/>
       <c r="X4" s="15"/>
       <c r="Y4" s="16"/>
       <c r="Z4" s="16"/>
@@ -2014,32 +2017,32 @@
       <c r="AK4" s="16"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="17"/>
-      <c r="AN4" s="108" t="s">
+      <c r="AN4" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="AO4" s="109"/>
-      <c r="AP4" s="109"/>
-      <c r="AQ4" s="99"/>
+      <c r="AO4" s="108"/>
+      <c r="AP4" s="108"/>
+      <c r="AQ4" s="98"/>
       <c r="AR4" s="15"/>
       <c r="AS4" s="16"/>
       <c r="AT4" s="16"/>
       <c r="AU4" s="17"/>
       <c r="AV4" s="15"/>
       <c r="AW4" s="16"/>
-      <c r="AX4" s="98" t="s">
+      <c r="AX4" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="AY4" s="99"/>
-      <c r="AZ4" s="105"/>
+      <c r="AY4" s="98"/>
+      <c r="AZ4" s="104"/>
       <c r="BB4" s="60" t="s">
         <v>50</v>
       </c>
       <c r="BC4" s="61"/>
     </row>
     <row r="5" spans="1:55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="113"/>
-      <c r="B5" s="114"/>
-      <c r="C5" s="115"/>
+      <c r="A5" s="112"/>
+      <c r="B5" s="113"/>
+      <c r="C5" s="114"/>
       <c r="D5" s="33"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -2056,10 +2059,10 @@
       <c r="Q5" s="32"/>
       <c r="R5" s="3"/>
       <c r="S5" s="12"/>
-      <c r="T5" s="110"/>
-      <c r="U5" s="102"/>
-      <c r="V5" s="102"/>
-      <c r="W5" s="101"/>
+      <c r="T5" s="109"/>
+      <c r="U5" s="101"/>
+      <c r="V5" s="101"/>
+      <c r="W5" s="100"/>
       <c r="X5" s="11"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="32"/>
@@ -2076,32 +2079,32 @@
       <c r="AK5" s="3"/>
       <c r="AL5" s="3"/>
       <c r="AM5" s="12"/>
-      <c r="AN5" s="110"/>
-      <c r="AO5" s="102"/>
-      <c r="AP5" s="102"/>
-      <c r="AQ5" s="101"/>
+      <c r="AN5" s="109"/>
+      <c r="AO5" s="101"/>
+      <c r="AP5" s="101"/>
+      <c r="AQ5" s="100"/>
       <c r="AR5" s="11"/>
       <c r="AS5" s="3"/>
       <c r="AT5" s="3"/>
       <c r="AU5" s="12"/>
       <c r="AV5" s="11"/>
       <c r="AW5" s="3"/>
-      <c r="AX5" s="100"/>
-      <c r="AY5" s="101"/>
-      <c r="AZ5" s="106"/>
+      <c r="AX5" s="99"/>
+      <c r="AY5" s="100"/>
+      <c r="AZ5" s="105"/>
       <c r="BB5" s="62" t="s">
         <v>51</v>
       </c>
       <c r="BC5" s="63"/>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="115" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="85">
+      <c r="B6" s="84">
         <v>32</v>
       </c>
-      <c r="C6" s="117"/>
+      <c r="C6" s="116"/>
       <c r="D6" s="13"/>
       <c r="E6" s="35"/>
       <c r="F6" s="30"/>
@@ -2118,10 +2121,10 @@
       <c r="Q6" s="24"/>
       <c r="R6" s="47"/>
       <c r="S6" s="48"/>
-      <c r="T6" s="110"/>
-      <c r="U6" s="102"/>
-      <c r="V6" s="102"/>
-      <c r="W6" s="101"/>
+      <c r="T6" s="109"/>
+      <c r="U6" s="101"/>
+      <c r="V6" s="101"/>
+      <c r="W6" s="100"/>
       <c r="X6" s="38"/>
       <c r="Y6" s="34"/>
       <c r="Z6" s="24"/>
@@ -2138,28 +2141,28 @@
       <c r="AK6" s="34"/>
       <c r="AL6" s="34"/>
       <c r="AM6" s="49"/>
-      <c r="AN6" s="110"/>
-      <c r="AO6" s="102"/>
-      <c r="AP6" s="102"/>
-      <c r="AQ6" s="101"/>
+      <c r="AN6" s="109"/>
+      <c r="AO6" s="101"/>
+      <c r="AP6" s="101"/>
+      <c r="AQ6" s="100"/>
       <c r="AR6" s="38"/>
       <c r="AS6" s="34"/>
       <c r="AT6" s="34"/>
       <c r="AU6" s="49"/>
       <c r="AV6" s="38"/>
       <c r="AW6" s="34"/>
-      <c r="AX6" s="100"/>
-      <c r="AY6" s="101"/>
-      <c r="AZ6" s="106"/>
+      <c r="AX6" s="99"/>
+      <c r="AY6" s="100"/>
+      <c r="AZ6" s="105"/>
       <c r="BB6" s="62" t="s">
         <v>52</v>
       </c>
       <c r="BC6" s="64"/>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A7" s="113"/>
-      <c r="B7" s="114"/>
-      <c r="C7" s="115"/>
+      <c r="A7" s="112"/>
+      <c r="B7" s="113"/>
+      <c r="C7" s="114"/>
       <c r="D7" s="33"/>
       <c r="E7" s="32"/>
       <c r="F7" s="3"/>
@@ -2168,18 +2171,18 @@
       <c r="I7" s="40"/>
       <c r="J7" s="40"/>
       <c r="K7" s="65"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="31"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="122"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="12"/>
-      <c r="T7" s="110"/>
-      <c r="U7" s="102"/>
-      <c r="V7" s="102"/>
-      <c r="W7" s="101"/>
+      <c r="T7" s="109"/>
+      <c r="U7" s="101"/>
+      <c r="V7" s="101"/>
+      <c r="W7" s="100"/>
       <c r="X7" s="33"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
@@ -2196,30 +2199,30 @@
       <c r="AK7" s="3"/>
       <c r="AL7" s="3"/>
       <c r="AM7" s="12"/>
-      <c r="AN7" s="110"/>
-      <c r="AO7" s="102"/>
-      <c r="AP7" s="102"/>
-      <c r="AQ7" s="101"/>
+      <c r="AN7" s="109"/>
+      <c r="AO7" s="101"/>
+      <c r="AP7" s="101"/>
+      <c r="AQ7" s="100"/>
       <c r="AR7" s="11"/>
       <c r="AS7" s="3"/>
       <c r="AT7" s="3"/>
       <c r="AU7" s="12"/>
       <c r="AV7" s="11"/>
       <c r="AW7" s="3"/>
-      <c r="AX7" s="100"/>
-      <c r="AY7" s="101"/>
-      <c r="AZ7" s="106"/>
+      <c r="AX7" s="99"/>
+      <c r="AY7" s="100"/>
+      <c r="AZ7" s="105"/>
       <c r="BB7" s="4"/>
       <c r="BC7" s="4"/>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A8" s="116" t="s">
+      <c r="A8" s="115" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="118">
+      <c r="B8" s="117">
         <v>4</v>
       </c>
-      <c r="C8" s="117">
+      <c r="C8" s="116">
         <v>5</v>
       </c>
       <c r="D8" s="26"/>
@@ -2238,10 +2241,10 @@
       <c r="Q8" s="30"/>
       <c r="R8" s="30"/>
       <c r="S8" s="29"/>
-      <c r="T8" s="110"/>
-      <c r="U8" s="102"/>
-      <c r="V8" s="102"/>
-      <c r="W8" s="101"/>
+      <c r="T8" s="109"/>
+      <c r="U8" s="101"/>
+      <c r="V8" s="101"/>
+      <c r="W8" s="100"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="30"/>
       <c r="Z8" s="30"/>
@@ -2258,26 +2261,26 @@
       <c r="AK8" s="30"/>
       <c r="AL8" s="30"/>
       <c r="AM8" s="29"/>
-      <c r="AN8" s="110"/>
-      <c r="AO8" s="102"/>
-      <c r="AP8" s="102"/>
-      <c r="AQ8" s="101"/>
+      <c r="AN8" s="109"/>
+      <c r="AO8" s="101"/>
+      <c r="AP8" s="101"/>
+      <c r="AQ8" s="100"/>
       <c r="AR8" s="28"/>
       <c r="AS8" s="30"/>
       <c r="AT8" s="30"/>
       <c r="AU8" s="29"/>
       <c r="AV8" s="28"/>
       <c r="AW8" s="30"/>
-      <c r="AX8" s="100"/>
-      <c r="AY8" s="101"/>
-      <c r="AZ8" s="106"/>
+      <c r="AX8" s="99"/>
+      <c r="AY8" s="100"/>
+      <c r="AZ8" s="105"/>
       <c r="BB8" s="4"/>
       <c r="BC8" s="4"/>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A9" s="90"/>
-      <c r="B9" s="92"/>
-      <c r="C9" s="115"/>
+      <c r="A9" s="89"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="114"/>
       <c r="D9" s="39"/>
       <c r="E9" s="40"/>
       <c r="F9" s="54"/>
@@ -2294,10 +2297,10 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="12"/>
-      <c r="T9" s="110"/>
-      <c r="U9" s="102"/>
-      <c r="V9" s="102"/>
-      <c r="W9" s="101"/>
+      <c r="T9" s="109"/>
+      <c r="U9" s="101"/>
+      <c r="V9" s="101"/>
+      <c r="W9" s="100"/>
       <c r="X9" s="11"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
@@ -2314,30 +2317,30 @@
       <c r="AK9" s="3"/>
       <c r="AL9" s="32"/>
       <c r="AM9" s="12"/>
-      <c r="AN9" s="110"/>
-      <c r="AO9" s="102"/>
-      <c r="AP9" s="102"/>
-      <c r="AQ9" s="101"/>
+      <c r="AN9" s="109"/>
+      <c r="AO9" s="101"/>
+      <c r="AP9" s="101"/>
+      <c r="AQ9" s="100"/>
       <c r="AR9" s="11"/>
       <c r="AS9" s="3"/>
       <c r="AT9" s="3"/>
       <c r="AU9" s="12"/>
       <c r="AV9" s="11"/>
       <c r="AW9" s="3"/>
-      <c r="AX9" s="100"/>
-      <c r="AY9" s="101"/>
-      <c r="AZ9" s="106"/>
+      <c r="AX9" s="99"/>
+      <c r="AY9" s="100"/>
+      <c r="AZ9" s="105"/>
       <c r="BB9" s="4"/>
       <c r="BC9" s="4"/>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A10" s="83" t="s">
+      <c r="A10" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="85">
+      <c r="B10" s="84">
         <v>2</v>
       </c>
-      <c r="C10" s="87">
+      <c r="C10" s="86">
         <v>1</v>
       </c>
       <c r="D10" s="28"/>
@@ -2356,10 +2359,10 @@
       <c r="Q10" s="30"/>
       <c r="R10" s="30"/>
       <c r="S10" s="29"/>
-      <c r="T10" s="110"/>
-      <c r="U10" s="102"/>
-      <c r="V10" s="102"/>
-      <c r="W10" s="101"/>
+      <c r="T10" s="109"/>
+      <c r="U10" s="101"/>
+      <c r="V10" s="101"/>
+      <c r="W10" s="100"/>
       <c r="X10" s="28"/>
       <c r="Y10" s="30"/>
       <c r="Z10" s="30"/>
@@ -2376,26 +2379,26 @@
       <c r="AK10" s="30"/>
       <c r="AL10" s="5"/>
       <c r="AM10" s="29"/>
-      <c r="AN10" s="110"/>
-      <c r="AO10" s="102"/>
-      <c r="AP10" s="102"/>
-      <c r="AQ10" s="101"/>
+      <c r="AN10" s="109"/>
+      <c r="AO10" s="101"/>
+      <c r="AP10" s="101"/>
+      <c r="AQ10" s="100"/>
       <c r="AR10" s="28"/>
       <c r="AS10" s="30"/>
       <c r="AT10" s="30"/>
       <c r="AU10" s="29"/>
       <c r="AV10" s="28"/>
       <c r="AW10" s="30"/>
-      <c r="AX10" s="100"/>
-      <c r="AY10" s="101"/>
-      <c r="AZ10" s="106"/>
+      <c r="AX10" s="99"/>
+      <c r="AY10" s="100"/>
+      <c r="AZ10" s="105"/>
       <c r="BB10" s="4"/>
       <c r="BC10" s="4"/>
     </row>
     <row r="11" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="84"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="88"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="87"/>
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
       <c r="F11" s="53"/>
@@ -2412,10 +2415,10 @@
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="110"/>
-      <c r="U11" s="102"/>
-      <c r="V11" s="102"/>
-      <c r="W11" s="101"/>
+      <c r="T11" s="109"/>
+      <c r="U11" s="101"/>
+      <c r="V11" s="101"/>
+      <c r="W11" s="100"/>
       <c r="X11" s="8"/>
       <c r="Y11" s="9"/>
       <c r="Z11" s="9"/>
@@ -2432,28 +2435,28 @@
       <c r="AK11" s="9"/>
       <c r="AL11" s="9"/>
       <c r="AM11" s="10"/>
-      <c r="AN11" s="110"/>
-      <c r="AO11" s="102"/>
-      <c r="AP11" s="102"/>
-      <c r="AQ11" s="101"/>
+      <c r="AN11" s="109"/>
+      <c r="AO11" s="101"/>
+      <c r="AP11" s="101"/>
+      <c r="AQ11" s="100"/>
       <c r="AR11" s="8"/>
       <c r="AS11" s="9"/>
       <c r="AT11" s="9"/>
       <c r="AU11" s="10"/>
       <c r="AV11" s="8"/>
       <c r="AW11" s="9"/>
-      <c r="AX11" s="100"/>
-      <c r="AY11" s="101"/>
-      <c r="AZ11" s="119"/>
+      <c r="AX11" s="99"/>
+      <c r="AY11" s="100"/>
+      <c r="AZ11" s="118"/>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A12" s="89" t="s">
+      <c r="A12" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="91">
+      <c r="B12" s="90">
         <v>1.5</v>
       </c>
-      <c r="C12" s="93"/>
+      <c r="C12" s="92"/>
       <c r="D12" s="18"/>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
@@ -2470,10 +2473,10 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
       <c r="S12" s="17"/>
-      <c r="T12" s="110"/>
-      <c r="U12" s="102"/>
-      <c r="V12" s="102"/>
-      <c r="W12" s="101"/>
+      <c r="T12" s="109"/>
+      <c r="U12" s="101"/>
+      <c r="V12" s="101"/>
+      <c r="W12" s="100"/>
       <c r="X12" s="15"/>
       <c r="Y12" s="16"/>
       <c r="Z12" s="16"/>
@@ -2490,26 +2493,26 @@
       <c r="AK12" s="16"/>
       <c r="AL12" s="16"/>
       <c r="AM12" s="17"/>
-      <c r="AN12" s="110"/>
-      <c r="AO12" s="102"/>
-      <c r="AP12" s="102"/>
-      <c r="AQ12" s="101"/>
+      <c r="AN12" s="109"/>
+      <c r="AO12" s="101"/>
+      <c r="AP12" s="101"/>
+      <c r="AQ12" s="100"/>
       <c r="AR12" s="15"/>
       <c r="AS12" s="16"/>
       <c r="AT12" s="16"/>
       <c r="AU12" s="17"/>
       <c r="AV12" s="15"/>
       <c r="AW12" s="16"/>
-      <c r="AX12" s="100"/>
-      <c r="AY12" s="101"/>
-      <c r="AZ12" s="95" t="s">
+      <c r="AX12" s="99"/>
+      <c r="AY12" s="100"/>
+      <c r="AZ12" s="94" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A13" s="90"/>
-      <c r="B13" s="92"/>
-      <c r="C13" s="94"/>
+      <c r="A13" s="89"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="93"/>
       <c r="D13" s="42"/>
       <c r="E13" s="41"/>
       <c r="F13" s="43"/>
@@ -2526,10 +2529,10 @@
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="12"/>
-      <c r="T13" s="110"/>
-      <c r="U13" s="102"/>
-      <c r="V13" s="102"/>
-      <c r="W13" s="101"/>
+      <c r="T13" s="109"/>
+      <c r="U13" s="101"/>
+      <c r="V13" s="101"/>
+      <c r="W13" s="100"/>
       <c r="X13" s="11"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
@@ -2546,28 +2549,28 @@
       <c r="AK13" s="32"/>
       <c r="AL13" s="32"/>
       <c r="AM13" s="31"/>
-      <c r="AN13" s="110"/>
-      <c r="AO13" s="102"/>
-      <c r="AP13" s="102"/>
-      <c r="AQ13" s="101"/>
+      <c r="AN13" s="109"/>
+      <c r="AO13" s="101"/>
+      <c r="AP13" s="101"/>
+      <c r="AQ13" s="100"/>
       <c r="AR13" s="33"/>
       <c r="AS13" s="32"/>
       <c r="AT13" s="32"/>
       <c r="AU13" s="31"/>
       <c r="AV13" s="33"/>
       <c r="AW13" s="32"/>
-      <c r="AX13" s="100"/>
-      <c r="AY13" s="101"/>
-      <c r="AZ13" s="96"/>
+      <c r="AX13" s="99"/>
+      <c r="AY13" s="100"/>
+      <c r="AZ13" s="95"/>
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A14" s="83" t="s">
+      <c r="A14" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="85">
+      <c r="B14" s="84">
         <v>1.5</v>
       </c>
-      <c r="C14" s="117"/>
+      <c r="C14" s="116"/>
       <c r="D14" s="28"/>
       <c r="E14" s="5"/>
       <c r="F14" s="30"/>
@@ -2584,10 +2587,10 @@
       <c r="Q14" s="30"/>
       <c r="R14" s="30"/>
       <c r="S14" s="29"/>
-      <c r="T14" s="110"/>
-      <c r="U14" s="102"/>
-      <c r="V14" s="102"/>
-      <c r="W14" s="101"/>
+      <c r="T14" s="109"/>
+      <c r="U14" s="101"/>
+      <c r="V14" s="101"/>
+      <c r="W14" s="100"/>
       <c r="X14" s="28"/>
       <c r="Y14" s="30"/>
       <c r="Z14" s="30"/>
@@ -2604,24 +2607,24 @@
       <c r="AK14" s="5"/>
       <c r="AL14" s="5"/>
       <c r="AM14" s="7"/>
-      <c r="AN14" s="110"/>
-      <c r="AO14" s="102"/>
-      <c r="AP14" s="102"/>
-      <c r="AQ14" s="101"/>
+      <c r="AN14" s="109"/>
+      <c r="AO14" s="101"/>
+      <c r="AP14" s="101"/>
+      <c r="AQ14" s="100"/>
       <c r="AR14" s="6"/>
       <c r="AS14" s="5"/>
       <c r="AT14" s="5"/>
       <c r="AU14" s="7"/>
       <c r="AV14" s="6"/>
       <c r="AW14" s="5"/>
-      <c r="AX14" s="100"/>
-      <c r="AY14" s="101"/>
-      <c r="AZ14" s="96"/>
+      <c r="AX14" s="99"/>
+      <c r="AY14" s="100"/>
+      <c r="AZ14" s="95"/>
     </row>
     <row r="15" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="84"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="88"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="87"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -2638,10 +2641,10 @@
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="110"/>
-      <c r="U15" s="102"/>
-      <c r="V15" s="102"/>
-      <c r="W15" s="101"/>
+      <c r="T15" s="109"/>
+      <c r="U15" s="101"/>
+      <c r="V15" s="101"/>
+      <c r="W15" s="100"/>
       <c r="X15" s="8"/>
       <c r="Y15" s="9"/>
       <c r="Z15" s="9"/>
@@ -2658,28 +2661,28 @@
       <c r="AK15" s="9"/>
       <c r="AL15" s="9"/>
       <c r="AM15" s="10"/>
-      <c r="AN15" s="110"/>
-      <c r="AO15" s="102"/>
-      <c r="AP15" s="102"/>
-      <c r="AQ15" s="101"/>
+      <c r="AN15" s="109"/>
+      <c r="AO15" s="101"/>
+      <c r="AP15" s="101"/>
+      <c r="AQ15" s="100"/>
       <c r="AR15" s="8"/>
       <c r="AS15" s="9"/>
       <c r="AT15" s="9"/>
       <c r="AU15" s="10"/>
       <c r="AV15" s="8"/>
       <c r="AW15" s="9"/>
-      <c r="AX15" s="100"/>
-      <c r="AY15" s="101"/>
-      <c r="AZ15" s="97"/>
+      <c r="AX15" s="99"/>
+      <c r="AY15" s="100"/>
+      <c r="AZ15" s="96"/>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A16" s="89" t="s">
+      <c r="A16" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="91">
+      <c r="B16" s="90">
         <v>1</v>
       </c>
-      <c r="C16" s="93"/>
+      <c r="C16" s="92"/>
       <c r="D16" s="15"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
@@ -2696,10 +2699,10 @@
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
       <c r="S16" s="17"/>
-      <c r="T16" s="110"/>
-      <c r="U16" s="102"/>
-      <c r="V16" s="102"/>
-      <c r="W16" s="101"/>
+      <c r="T16" s="109"/>
+      <c r="U16" s="101"/>
+      <c r="V16" s="101"/>
+      <c r="W16" s="100"/>
       <c r="X16" s="15"/>
       <c r="Y16" s="16"/>
       <c r="Z16" s="16"/>
@@ -2716,26 +2719,26 @@
       <c r="AK16" s="16"/>
       <c r="AL16" s="16"/>
       <c r="AM16" s="17"/>
-      <c r="AN16" s="110"/>
-      <c r="AO16" s="102"/>
-      <c r="AP16" s="102"/>
-      <c r="AQ16" s="101"/>
+      <c r="AN16" s="109"/>
+      <c r="AO16" s="101"/>
+      <c r="AP16" s="101"/>
+      <c r="AQ16" s="100"/>
       <c r="AR16" s="15"/>
       <c r="AS16" s="16"/>
       <c r="AT16" s="16"/>
       <c r="AU16" s="17"/>
       <c r="AV16" s="15"/>
       <c r="AW16" s="16"/>
-      <c r="AX16" s="100"/>
-      <c r="AY16" s="101"/>
-      <c r="AZ16" s="95" t="s">
+      <c r="AX16" s="99"/>
+      <c r="AY16" s="100"/>
+      <c r="AZ16" s="94" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A17" s="113"/>
-      <c r="B17" s="92"/>
-      <c r="C17" s="94"/>
+      <c r="A17" s="112"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="93"/>
       <c r="D17" s="11"/>
       <c r="E17" s="3"/>
       <c r="F17" s="32"/>
@@ -2752,10 +2755,10 @@
       <c r="Q17" s="3"/>
       <c r="R17" s="32"/>
       <c r="S17" s="12"/>
-      <c r="T17" s="110"/>
-      <c r="U17" s="102"/>
-      <c r="V17" s="102"/>
-      <c r="W17" s="101"/>
+      <c r="T17" s="109"/>
+      <c r="U17" s="101"/>
+      <c r="V17" s="101"/>
+      <c r="W17" s="100"/>
       <c r="X17" s="33"/>
       <c r="Y17" s="32"/>
       <c r="Z17" s="32"/>
@@ -2772,28 +2775,28 @@
       <c r="AK17" s="32"/>
       <c r="AL17" s="32"/>
       <c r="AM17" s="31"/>
-      <c r="AN17" s="110"/>
-      <c r="AO17" s="102"/>
-      <c r="AP17" s="102"/>
-      <c r="AQ17" s="101"/>
+      <c r="AN17" s="109"/>
+      <c r="AO17" s="101"/>
+      <c r="AP17" s="101"/>
+      <c r="AQ17" s="100"/>
       <c r="AR17" s="33"/>
       <c r="AS17" s="32"/>
       <c r="AT17" s="32"/>
       <c r="AU17" s="31"/>
       <c r="AV17" s="33"/>
       <c r="AW17" s="3"/>
-      <c r="AX17" s="100"/>
-      <c r="AY17" s="101"/>
-      <c r="AZ17" s="96"/>
+      <c r="AX17" s="99"/>
+      <c r="AY17" s="100"/>
+      <c r="AZ17" s="95"/>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A18" s="116" t="s">
+      <c r="A18" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="85">
+      <c r="B18" s="84">
         <v>2</v>
       </c>
-      <c r="C18" s="117"/>
+      <c r="C18" s="116"/>
       <c r="D18" s="28"/>
       <c r="E18" s="30"/>
       <c r="F18" s="5"/>
@@ -2810,10 +2813,10 @@
       <c r="Q18" s="30"/>
       <c r="R18" s="5"/>
       <c r="S18" s="29"/>
-      <c r="T18" s="110"/>
-      <c r="U18" s="102"/>
-      <c r="V18" s="102"/>
-      <c r="W18" s="101"/>
+      <c r="T18" s="109"/>
+      <c r="U18" s="101"/>
+      <c r="V18" s="101"/>
+      <c r="W18" s="100"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
@@ -2830,24 +2833,24 @@
       <c r="AK18" s="5"/>
       <c r="AL18" s="5"/>
       <c r="AM18" s="7"/>
-      <c r="AN18" s="110"/>
-      <c r="AO18" s="102"/>
-      <c r="AP18" s="102"/>
-      <c r="AQ18" s="101"/>
+      <c r="AN18" s="109"/>
+      <c r="AO18" s="101"/>
+      <c r="AP18" s="101"/>
+      <c r="AQ18" s="100"/>
       <c r="AR18" s="6"/>
       <c r="AS18" s="5"/>
       <c r="AT18" s="5"/>
       <c r="AU18" s="7"/>
       <c r="AV18" s="6"/>
       <c r="AW18" s="30"/>
-      <c r="AX18" s="100"/>
-      <c r="AY18" s="101"/>
-      <c r="AZ18" s="96"/>
+      <c r="AX18" s="99"/>
+      <c r="AY18" s="100"/>
+      <c r="AZ18" s="95"/>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A19" s="90"/>
-      <c r="B19" s="92"/>
-      <c r="C19" s="94"/>
+      <c r="A19" s="89"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="93"/>
       <c r="D19" s="11"/>
       <c r="E19" s="3"/>
       <c r="F19" s="32"/>
@@ -2856,7 +2859,7 @@
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
       <c r="K19" s="31"/>
-      <c r="L19" s="33"/>
+      <c r="L19" s="57"/>
       <c r="M19" s="32"/>
       <c r="N19" s="32"/>
       <c r="O19" s="31"/>
@@ -2864,10 +2867,10 @@
       <c r="Q19" s="32"/>
       <c r="R19" s="3"/>
       <c r="S19" s="31"/>
-      <c r="T19" s="110"/>
-      <c r="U19" s="102"/>
-      <c r="V19" s="102"/>
-      <c r="W19" s="101"/>
+      <c r="T19" s="109"/>
+      <c r="U19" s="101"/>
+      <c r="V19" s="101"/>
+      <c r="W19" s="100"/>
       <c r="X19" s="33"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
@@ -2884,28 +2887,28 @@
       <c r="AK19" s="32"/>
       <c r="AL19" s="32"/>
       <c r="AM19" s="31"/>
-      <c r="AN19" s="110"/>
-      <c r="AO19" s="102"/>
-      <c r="AP19" s="102"/>
-      <c r="AQ19" s="101"/>
+      <c r="AN19" s="109"/>
+      <c r="AO19" s="101"/>
+      <c r="AP19" s="101"/>
+      <c r="AQ19" s="100"/>
       <c r="AR19" s="33"/>
       <c r="AS19" s="3"/>
       <c r="AT19" s="32"/>
       <c r="AU19" s="31"/>
       <c r="AV19" s="33"/>
       <c r="AW19" s="32"/>
-      <c r="AX19" s="100"/>
-      <c r="AY19" s="101"/>
-      <c r="AZ19" s="96"/>
+      <c r="AX19" s="99"/>
+      <c r="AY19" s="100"/>
+      <c r="AZ19" s="95"/>
     </row>
     <row r="20" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A20" s="116" t="s">
+      <c r="A20" s="115" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="85">
+      <c r="B20" s="84">
         <v>0.5</v>
       </c>
-      <c r="C20" s="117"/>
+      <c r="C20" s="116"/>
       <c r="D20" s="28"/>
       <c r="E20" s="30"/>
       <c r="F20" s="5"/>
@@ -2915,17 +2918,17 @@
       <c r="J20" s="5"/>
       <c r="K20" s="7"/>
       <c r="L20" s="6"/>
-      <c r="M20" s="24"/>
+      <c r="M20" s="119"/>
       <c r="N20" s="5"/>
       <c r="O20" s="7"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="30"/>
       <c r="S20" s="7"/>
-      <c r="T20" s="110"/>
-      <c r="U20" s="102"/>
-      <c r="V20" s="102"/>
-      <c r="W20" s="101"/>
+      <c r="T20" s="109"/>
+      <c r="U20" s="101"/>
+      <c r="V20" s="101"/>
+      <c r="W20" s="100"/>
       <c r="X20" s="6"/>
       <c r="Y20" s="30"/>
       <c r="Z20" s="30"/>
@@ -2942,24 +2945,24 @@
       <c r="AK20" s="5"/>
       <c r="AL20" s="5"/>
       <c r="AM20" s="7"/>
-      <c r="AN20" s="110"/>
-      <c r="AO20" s="102"/>
-      <c r="AP20" s="102"/>
-      <c r="AQ20" s="101"/>
+      <c r="AN20" s="109"/>
+      <c r="AO20" s="101"/>
+      <c r="AP20" s="101"/>
+      <c r="AQ20" s="100"/>
       <c r="AR20" s="6"/>
       <c r="AS20" s="30"/>
       <c r="AT20" s="5"/>
       <c r="AU20" s="7"/>
       <c r="AV20" s="6"/>
       <c r="AW20" s="5"/>
-      <c r="AX20" s="100"/>
-      <c r="AY20" s="101"/>
-      <c r="AZ20" s="96"/>
+      <c r="AX20" s="99"/>
+      <c r="AY20" s="100"/>
+      <c r="AZ20" s="95"/>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A21" s="90"/>
-      <c r="B21" s="92"/>
-      <c r="C21" s="94"/>
+      <c r="A21" s="89"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="93"/>
       <c r="D21" s="33"/>
       <c r="E21" s="32"/>
       <c r="F21" s="32"/>
@@ -2976,10 +2979,10 @@
       <c r="Q21" s="32"/>
       <c r="R21" s="32"/>
       <c r="S21" s="31"/>
-      <c r="T21" s="110"/>
-      <c r="U21" s="102"/>
-      <c r="V21" s="102"/>
-      <c r="W21" s="101"/>
+      <c r="T21" s="109"/>
+      <c r="U21" s="101"/>
+      <c r="V21" s="101"/>
+      <c r="W21" s="100"/>
       <c r="X21" s="33"/>
       <c r="Y21" s="32"/>
       <c r="Z21" s="32"/>
@@ -2996,28 +2999,28 @@
       <c r="AK21" s="32"/>
       <c r="AL21" s="32"/>
       <c r="AM21" s="31"/>
-      <c r="AN21" s="110"/>
-      <c r="AO21" s="102"/>
-      <c r="AP21" s="102"/>
-      <c r="AQ21" s="101"/>
+      <c r="AN21" s="109"/>
+      <c r="AO21" s="101"/>
+      <c r="AP21" s="101"/>
+      <c r="AQ21" s="100"/>
       <c r="AR21" s="33"/>
       <c r="AS21" s="32"/>
       <c r="AT21" s="32"/>
       <c r="AU21" s="31"/>
       <c r="AV21" s="33"/>
       <c r="AW21" s="32"/>
-      <c r="AX21" s="100"/>
-      <c r="AY21" s="101"/>
-      <c r="AZ21" s="96"/>
+      <c r="AX21" s="99"/>
+      <c r="AY21" s="100"/>
+      <c r="AZ21" s="95"/>
     </row>
     <row r="22" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A22" s="116" t="s">
+      <c r="A22" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="85">
+      <c r="B22" s="84">
         <v>1</v>
       </c>
-      <c r="C22" s="117"/>
+      <c r="C22" s="116"/>
       <c r="D22" s="6"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -3027,17 +3030,17 @@
       <c r="J22" s="5"/>
       <c r="K22" s="7"/>
       <c r="L22" s="6"/>
-      <c r="M22" s="24"/>
+      <c r="M22" s="119"/>
       <c r="N22" s="5"/>
       <c r="O22" s="7"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
       <c r="S22" s="7"/>
-      <c r="T22" s="110"/>
-      <c r="U22" s="102"/>
-      <c r="V22" s="102"/>
-      <c r="W22" s="101"/>
+      <c r="T22" s="109"/>
+      <c r="U22" s="101"/>
+      <c r="V22" s="101"/>
+      <c r="W22" s="100"/>
       <c r="X22" s="6"/>
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
@@ -3054,24 +3057,24 @@
       <c r="AK22" s="5"/>
       <c r="AL22" s="5"/>
       <c r="AM22" s="7"/>
-      <c r="AN22" s="110"/>
-      <c r="AO22" s="102"/>
-      <c r="AP22" s="102"/>
-      <c r="AQ22" s="101"/>
+      <c r="AN22" s="109"/>
+      <c r="AO22" s="101"/>
+      <c r="AP22" s="101"/>
+      <c r="AQ22" s="100"/>
       <c r="AR22" s="6"/>
       <c r="AS22" s="5"/>
       <c r="AT22" s="5"/>
       <c r="AU22" s="7"/>
       <c r="AV22" s="6"/>
       <c r="AW22" s="5"/>
-      <c r="AX22" s="100"/>
-      <c r="AY22" s="101"/>
-      <c r="AZ22" s="96"/>
+      <c r="AX22" s="99"/>
+      <c r="AY22" s="100"/>
+      <c r="AZ22" s="95"/>
     </row>
     <row r="23" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A23" s="90"/>
-      <c r="B23" s="92"/>
-      <c r="C23" s="94"/>
+      <c r="A23" s="89"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="93"/>
       <c r="D23" s="11"/>
       <c r="E23" s="3"/>
       <c r="F23" s="32"/>
@@ -3088,10 +3091,10 @@
       <c r="Q23" s="32"/>
       <c r="R23" s="32"/>
       <c r="S23" s="31"/>
-      <c r="T23" s="110"/>
-      <c r="U23" s="102"/>
-      <c r="V23" s="102"/>
-      <c r="W23" s="101"/>
+      <c r="T23" s="109"/>
+      <c r="U23" s="101"/>
+      <c r="V23" s="101"/>
+      <c r="W23" s="100"/>
       <c r="X23" s="33"/>
       <c r="Y23" s="32"/>
       <c r="Z23" s="32"/>
@@ -3108,28 +3111,28 @@
       <c r="AK23" s="3"/>
       <c r="AL23" s="3"/>
       <c r="AM23" s="12"/>
-      <c r="AN23" s="110"/>
-      <c r="AO23" s="102"/>
-      <c r="AP23" s="102"/>
-      <c r="AQ23" s="101"/>
+      <c r="AN23" s="109"/>
+      <c r="AO23" s="101"/>
+      <c r="AP23" s="101"/>
+      <c r="AQ23" s="100"/>
       <c r="AR23" s="11"/>
       <c r="AS23" s="3"/>
       <c r="AT23" s="32"/>
       <c r="AU23" s="31"/>
       <c r="AV23" s="33"/>
       <c r="AW23" s="3"/>
-      <c r="AX23" s="100"/>
-      <c r="AY23" s="101"/>
-      <c r="AZ23" s="96"/>
+      <c r="AX23" s="99"/>
+      <c r="AY23" s="100"/>
+      <c r="AZ23" s="95"/>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A24" s="116" t="s">
+      <c r="A24" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="85">
+      <c r="B24" s="84">
         <v>1</v>
       </c>
-      <c r="C24" s="117"/>
+      <c r="C24" s="116"/>
       <c r="D24" s="28"/>
       <c r="E24" s="30"/>
       <c r="F24" s="5"/>
@@ -3139,17 +3142,17 @@
       <c r="J24" s="5"/>
       <c r="K24" s="7"/>
       <c r="L24" s="6"/>
-      <c r="M24" s="55"/>
-      <c r="N24" s="24"/>
+      <c r="M24" s="120"/>
+      <c r="N24" s="119"/>
       <c r="O24" s="7"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
       <c r="S24" s="7"/>
-      <c r="T24" s="110"/>
-      <c r="U24" s="102"/>
-      <c r="V24" s="102"/>
-      <c r="W24" s="101"/>
+      <c r="T24" s="109"/>
+      <c r="U24" s="101"/>
+      <c r="V24" s="101"/>
+      <c r="W24" s="100"/>
       <c r="X24" s="6"/>
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
@@ -3166,24 +3169,24 @@
       <c r="AK24" s="30"/>
       <c r="AL24" s="30"/>
       <c r="AM24" s="29"/>
-      <c r="AN24" s="110"/>
-      <c r="AO24" s="102"/>
-      <c r="AP24" s="102"/>
-      <c r="AQ24" s="101"/>
+      <c r="AN24" s="109"/>
+      <c r="AO24" s="101"/>
+      <c r="AP24" s="101"/>
+      <c r="AQ24" s="100"/>
       <c r="AR24" s="28"/>
       <c r="AS24" s="30"/>
       <c r="AT24" s="5"/>
       <c r="AU24" s="7"/>
       <c r="AV24" s="6"/>
       <c r="AW24" s="30"/>
-      <c r="AX24" s="100"/>
-      <c r="AY24" s="101"/>
-      <c r="AZ24" s="96"/>
+      <c r="AX24" s="99"/>
+      <c r="AY24" s="100"/>
+      <c r="AZ24" s="95"/>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A25" s="90"/>
-      <c r="B25" s="114"/>
-      <c r="C25" s="115"/>
+      <c r="A25" s="89"/>
+      <c r="B25" s="113"/>
+      <c r="C25" s="114"/>
       <c r="D25" s="33"/>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
@@ -3200,10 +3203,10 @@
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="31"/>
-      <c r="T25" s="110"/>
-      <c r="U25" s="102"/>
-      <c r="V25" s="102"/>
-      <c r="W25" s="101"/>
+      <c r="T25" s="109"/>
+      <c r="U25" s="101"/>
+      <c r="V25" s="101"/>
+      <c r="W25" s="100"/>
       <c r="X25" s="33"/>
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
@@ -3220,28 +3223,28 @@
       <c r="AK25" s="3"/>
       <c r="AL25" s="3"/>
       <c r="AM25" s="12"/>
-      <c r="AN25" s="110"/>
-      <c r="AO25" s="102"/>
-      <c r="AP25" s="102"/>
-      <c r="AQ25" s="101"/>
+      <c r="AN25" s="109"/>
+      <c r="AO25" s="101"/>
+      <c r="AP25" s="101"/>
+      <c r="AQ25" s="100"/>
       <c r="AR25" s="11"/>
       <c r="AS25" s="3"/>
       <c r="AT25" s="3"/>
       <c r="AU25" s="12"/>
       <c r="AV25" s="11"/>
       <c r="AW25" s="3"/>
-      <c r="AX25" s="100"/>
-      <c r="AY25" s="101"/>
-      <c r="AZ25" s="96"/>
+      <c r="AX25" s="99"/>
+      <c r="AY25" s="100"/>
+      <c r="AZ25" s="95"/>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A26" s="83" t="s">
+      <c r="A26" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="118">
+      <c r="B26" s="117">
         <v>2</v>
       </c>
-      <c r="C26" s="87"/>
+      <c r="C26" s="86"/>
       <c r="D26" s="6"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -3253,15 +3256,15 @@
       <c r="L26" s="6"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="66"/>
+      <c r="O26" s="121"/>
       <c r="P26" s="28"/>
       <c r="Q26" s="30"/>
       <c r="R26" s="30"/>
       <c r="S26" s="7"/>
-      <c r="T26" s="110"/>
-      <c r="U26" s="102"/>
-      <c r="V26" s="102"/>
-      <c r="W26" s="101"/>
+      <c r="T26" s="109"/>
+      <c r="U26" s="101"/>
+      <c r="V26" s="101"/>
+      <c r="W26" s="100"/>
       <c r="X26" s="6"/>
       <c r="Y26" s="30"/>
       <c r="Z26" s="30"/>
@@ -3278,24 +3281,24 @@
       <c r="AK26" s="30"/>
       <c r="AL26" s="30"/>
       <c r="AM26" s="29"/>
-      <c r="AN26" s="110"/>
-      <c r="AO26" s="102"/>
-      <c r="AP26" s="102"/>
-      <c r="AQ26" s="101"/>
+      <c r="AN26" s="109"/>
+      <c r="AO26" s="101"/>
+      <c r="AP26" s="101"/>
+      <c r="AQ26" s="100"/>
       <c r="AR26" s="28"/>
       <c r="AS26" s="30"/>
       <c r="AT26" s="30"/>
       <c r="AU26" s="29"/>
       <c r="AV26" s="28"/>
       <c r="AW26" s="30"/>
-      <c r="AX26" s="100"/>
-      <c r="AY26" s="101"/>
-      <c r="AZ26" s="96"/>
+      <c r="AX26" s="99"/>
+      <c r="AY26" s="100"/>
+      <c r="AZ26" s="95"/>
     </row>
     <row r="27" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="84"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="88"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="87"/>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
@@ -3312,10 +3315,10 @@
       <c r="Q27" s="9"/>
       <c r="R27" s="9"/>
       <c r="S27" s="10"/>
-      <c r="T27" s="110"/>
-      <c r="U27" s="102"/>
-      <c r="V27" s="102"/>
-      <c r="W27" s="101"/>
+      <c r="T27" s="109"/>
+      <c r="U27" s="101"/>
+      <c r="V27" s="101"/>
+      <c r="W27" s="100"/>
       <c r="X27" s="8"/>
       <c r="Y27" s="9"/>
       <c r="Z27" s="9"/>
@@ -3332,28 +3335,28 @@
       <c r="AK27" s="9"/>
       <c r="AL27" s="9"/>
       <c r="AM27" s="10"/>
-      <c r="AN27" s="110"/>
-      <c r="AO27" s="102"/>
-      <c r="AP27" s="102"/>
-      <c r="AQ27" s="101"/>
+      <c r="AN27" s="109"/>
+      <c r="AO27" s="101"/>
+      <c r="AP27" s="101"/>
+      <c r="AQ27" s="100"/>
       <c r="AR27" s="8"/>
       <c r="AS27" s="9"/>
       <c r="AT27" s="9"/>
       <c r="AU27" s="10"/>
       <c r="AV27" s="8"/>
       <c r="AW27" s="9"/>
-      <c r="AX27" s="100"/>
-      <c r="AY27" s="101"/>
-      <c r="AZ27" s="97"/>
+      <c r="AX27" s="99"/>
+      <c r="AY27" s="100"/>
+      <c r="AZ27" s="96"/>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A28" s="89" t="s">
+      <c r="A28" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="91">
+      <c r="B28" s="90">
         <v>0.5</v>
       </c>
-      <c r="C28" s="93"/>
+      <c r="C28" s="92"/>
       <c r="D28" s="15"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
@@ -3370,10 +3373,10 @@
       <c r="Q28" s="16"/>
       <c r="R28" s="16"/>
       <c r="S28" s="17"/>
-      <c r="T28" s="110"/>
-      <c r="U28" s="102"/>
-      <c r="V28" s="102"/>
-      <c r="W28" s="101"/>
+      <c r="T28" s="109"/>
+      <c r="U28" s="101"/>
+      <c r="V28" s="101"/>
+      <c r="W28" s="100"/>
       <c r="X28" s="15"/>
       <c r="Y28" s="16"/>
       <c r="Z28" s="16"/>
@@ -3390,26 +3393,26 @@
       <c r="AK28" s="16"/>
       <c r="AL28" s="16"/>
       <c r="AM28" s="17"/>
-      <c r="AN28" s="110"/>
-      <c r="AO28" s="102"/>
-      <c r="AP28" s="102"/>
-      <c r="AQ28" s="101"/>
+      <c r="AN28" s="109"/>
+      <c r="AO28" s="101"/>
+      <c r="AP28" s="101"/>
+      <c r="AQ28" s="100"/>
       <c r="AR28" s="15"/>
       <c r="AS28" s="16"/>
       <c r="AT28" s="16"/>
       <c r="AU28" s="17"/>
       <c r="AV28" s="15"/>
       <c r="AW28" s="17"/>
-      <c r="AX28" s="102"/>
-      <c r="AY28" s="101"/>
-      <c r="AZ28" s="80" t="s">
+      <c r="AX28" s="101"/>
+      <c r="AY28" s="100"/>
+      <c r="AZ28" s="79" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="84"/>
-      <c r="B29" s="86"/>
-      <c r="C29" s="88"/>
+      <c r="A29" s="83"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="87"/>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
@@ -3426,10 +3429,10 @@
       <c r="Q29" s="9"/>
       <c r="R29" s="9"/>
       <c r="S29" s="10"/>
-      <c r="T29" s="110"/>
-      <c r="U29" s="102"/>
-      <c r="V29" s="102"/>
-      <c r="W29" s="101"/>
+      <c r="T29" s="109"/>
+      <c r="U29" s="101"/>
+      <c r="V29" s="101"/>
+      <c r="W29" s="100"/>
       <c r="X29" s="8"/>
       <c r="Y29" s="9"/>
       <c r="Z29" s="9"/>
@@ -3446,28 +3449,28 @@
       <c r="AK29" s="9"/>
       <c r="AL29" s="9"/>
       <c r="AM29" s="10"/>
-      <c r="AN29" s="110"/>
-      <c r="AO29" s="102"/>
-      <c r="AP29" s="102"/>
-      <c r="AQ29" s="101"/>
+      <c r="AN29" s="109"/>
+      <c r="AO29" s="101"/>
+      <c r="AP29" s="101"/>
+      <c r="AQ29" s="100"/>
       <c r="AR29" s="8"/>
       <c r="AS29" s="9"/>
       <c r="AT29" s="9"/>
       <c r="AU29" s="10"/>
       <c r="AV29" s="8"/>
       <c r="AW29" s="10"/>
-      <c r="AX29" s="102"/>
-      <c r="AY29" s="101"/>
-      <c r="AZ29" s="81"/>
+      <c r="AX29" s="101"/>
+      <c r="AY29" s="100"/>
+      <c r="AZ29" s="80"/>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A30" s="83" t="s">
+      <c r="A30" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="118">
+      <c r="B30" s="117">
         <v>0.5</v>
       </c>
-      <c r="C30" s="87"/>
+      <c r="C30" s="86"/>
       <c r="D30" s="6"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -3484,10 +3487,10 @@
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
       <c r="S30" s="7"/>
-      <c r="T30" s="110"/>
-      <c r="U30" s="102"/>
-      <c r="V30" s="102"/>
-      <c r="W30" s="101"/>
+      <c r="T30" s="109"/>
+      <c r="U30" s="101"/>
+      <c r="V30" s="101"/>
+      <c r="W30" s="100"/>
       <c r="X30" s="6"/>
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
@@ -3504,26 +3507,26 @@
       <c r="AK30" s="5"/>
       <c r="AL30" s="5"/>
       <c r="AM30" s="7"/>
-      <c r="AN30" s="110"/>
-      <c r="AO30" s="102"/>
-      <c r="AP30" s="102"/>
-      <c r="AQ30" s="101"/>
+      <c r="AN30" s="109"/>
+      <c r="AO30" s="101"/>
+      <c r="AP30" s="101"/>
+      <c r="AQ30" s="100"/>
       <c r="AR30" s="6"/>
       <c r="AS30" s="5"/>
       <c r="AT30" s="5"/>
       <c r="AU30" s="7"/>
       <c r="AV30" s="6"/>
       <c r="AW30" s="5"/>
-      <c r="AX30" s="100"/>
-      <c r="AY30" s="101"/>
-      <c r="AZ30" s="80" t="s">
+      <c r="AX30" s="99"/>
+      <c r="AY30" s="100"/>
+      <c r="AZ30" s="79" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A31" s="90"/>
-      <c r="B31" s="92"/>
-      <c r="C31" s="94"/>
+      <c r="A31" s="89"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="93"/>
       <c r="D31" s="11"/>
       <c r="E31" s="32"/>
       <c r="F31" s="3"/>
@@ -3540,10 +3543,10 @@
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
       <c r="S31" s="31"/>
-      <c r="T31" s="110"/>
-      <c r="U31" s="102"/>
-      <c r="V31" s="102"/>
-      <c r="W31" s="101"/>
+      <c r="T31" s="109"/>
+      <c r="U31" s="101"/>
+      <c r="V31" s="101"/>
+      <c r="W31" s="100"/>
       <c r="X31" s="33"/>
       <c r="Y31" s="32"/>
       <c r="Z31" s="32"/>
@@ -3560,28 +3563,28 @@
       <c r="AK31" s="32"/>
       <c r="AL31" s="32"/>
       <c r="AM31" s="31"/>
-      <c r="AN31" s="110"/>
-      <c r="AO31" s="102"/>
-      <c r="AP31" s="102"/>
-      <c r="AQ31" s="101"/>
+      <c r="AN31" s="109"/>
+      <c r="AO31" s="101"/>
+      <c r="AP31" s="101"/>
+      <c r="AQ31" s="100"/>
       <c r="AR31" s="33"/>
       <c r="AS31" s="32"/>
       <c r="AT31" s="32"/>
       <c r="AU31" s="31"/>
       <c r="AV31" s="33"/>
       <c r="AW31" s="32"/>
-      <c r="AX31" s="100"/>
-      <c r="AY31" s="101"/>
-      <c r="AZ31" s="82"/>
+      <c r="AX31" s="99"/>
+      <c r="AY31" s="100"/>
+      <c r="AZ31" s="81"/>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A32" s="116" t="s">
+      <c r="A32" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="85">
+      <c r="B32" s="84">
         <v>1</v>
       </c>
-      <c r="C32" s="117"/>
+      <c r="C32" s="116"/>
       <c r="D32" s="28"/>
       <c r="E32" s="5"/>
       <c r="F32" s="30"/>
@@ -3598,10 +3601,10 @@
       <c r="Q32" s="34"/>
       <c r="R32" s="30"/>
       <c r="S32" s="7"/>
-      <c r="T32" s="110"/>
-      <c r="U32" s="102"/>
-      <c r="V32" s="102"/>
-      <c r="W32" s="101"/>
+      <c r="T32" s="109"/>
+      <c r="U32" s="101"/>
+      <c r="V32" s="101"/>
+      <c r="W32" s="100"/>
       <c r="X32" s="6"/>
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
@@ -3618,24 +3621,24 @@
       <c r="AK32" s="5"/>
       <c r="AL32" s="5"/>
       <c r="AM32" s="7"/>
-      <c r="AN32" s="110"/>
-      <c r="AO32" s="102"/>
-      <c r="AP32" s="102"/>
-      <c r="AQ32" s="101"/>
+      <c r="AN32" s="109"/>
+      <c r="AO32" s="101"/>
+      <c r="AP32" s="101"/>
+      <c r="AQ32" s="100"/>
       <c r="AR32" s="6"/>
       <c r="AS32" s="5"/>
       <c r="AT32" s="5"/>
       <c r="AU32" s="7"/>
       <c r="AV32" s="6"/>
       <c r="AW32" s="5"/>
-      <c r="AX32" s="100"/>
-      <c r="AY32" s="101"/>
-      <c r="AZ32" s="82"/>
+      <c r="AX32" s="99"/>
+      <c r="AY32" s="100"/>
+      <c r="AZ32" s="81"/>
     </row>
     <row r="33" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A33" s="90"/>
-      <c r="B33" s="114"/>
-      <c r="C33" s="115"/>
+      <c r="A33" s="89"/>
+      <c r="B33" s="113"/>
+      <c r="C33" s="114"/>
       <c r="D33" s="33"/>
       <c r="E33" s="32"/>
       <c r="F33" s="3"/>
@@ -3652,10 +3655,10 @@
       <c r="Q33" s="32"/>
       <c r="R33" s="32"/>
       <c r="S33" s="31"/>
-      <c r="T33" s="110"/>
-      <c r="U33" s="102"/>
-      <c r="V33" s="102"/>
-      <c r="W33" s="101"/>
+      <c r="T33" s="109"/>
+      <c r="U33" s="101"/>
+      <c r="V33" s="101"/>
+      <c r="W33" s="100"/>
       <c r="X33" s="33"/>
       <c r="Y33" s="3"/>
       <c r="Z33" s="32"/>
@@ -3672,28 +3675,28 @@
       <c r="AK33" s="32"/>
       <c r="AL33" s="32"/>
       <c r="AM33" s="31"/>
-      <c r="AN33" s="110"/>
-      <c r="AO33" s="102"/>
-      <c r="AP33" s="102"/>
-      <c r="AQ33" s="101"/>
+      <c r="AN33" s="109"/>
+      <c r="AO33" s="101"/>
+      <c r="AP33" s="101"/>
+      <c r="AQ33" s="100"/>
       <c r="AR33" s="33"/>
       <c r="AS33" s="3"/>
       <c r="AT33" s="3"/>
       <c r="AU33" s="12"/>
       <c r="AV33" s="11"/>
       <c r="AW33" s="32"/>
-      <c r="AX33" s="100"/>
-      <c r="AY33" s="101"/>
-      <c r="AZ33" s="82"/>
+      <c r="AX33" s="99"/>
+      <c r="AY33" s="100"/>
+      <c r="AZ33" s="81"/>
     </row>
     <row r="34" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A34" s="116" t="s">
+      <c r="A34" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="85">
+      <c r="B34" s="84">
         <v>1</v>
       </c>
-      <c r="C34" s="87"/>
+      <c r="C34" s="86"/>
       <c r="D34" s="6"/>
       <c r="E34" s="5"/>
       <c r="F34" s="30"/>
@@ -3710,10 +3713,10 @@
       <c r="Q34" s="55"/>
       <c r="R34" s="24"/>
       <c r="S34" s="7"/>
-      <c r="T34" s="110"/>
-      <c r="U34" s="102"/>
-      <c r="V34" s="102"/>
-      <c r="W34" s="101"/>
+      <c r="T34" s="109"/>
+      <c r="U34" s="101"/>
+      <c r="V34" s="101"/>
+      <c r="W34" s="100"/>
       <c r="X34" s="6"/>
       <c r="Y34" s="30"/>
       <c r="Z34" s="5"/>
@@ -3730,24 +3733,24 @@
       <c r="AK34" s="5"/>
       <c r="AL34" s="5"/>
       <c r="AM34" s="7"/>
-      <c r="AN34" s="110"/>
-      <c r="AO34" s="102"/>
-      <c r="AP34" s="102"/>
-      <c r="AQ34" s="101"/>
+      <c r="AN34" s="109"/>
+      <c r="AO34" s="101"/>
+      <c r="AP34" s="101"/>
+      <c r="AQ34" s="100"/>
       <c r="AR34" s="6"/>
       <c r="AS34" s="30"/>
       <c r="AT34" s="30"/>
       <c r="AU34" s="29"/>
       <c r="AV34" s="28"/>
       <c r="AW34" s="5"/>
-      <c r="AX34" s="100"/>
-      <c r="AY34" s="101"/>
-      <c r="AZ34" s="82"/>
+      <c r="AX34" s="99"/>
+      <c r="AY34" s="100"/>
+      <c r="AZ34" s="81"/>
     </row>
     <row r="35" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A35" s="90"/>
-      <c r="B35" s="114"/>
-      <c r="C35" s="94"/>
+      <c r="A35" s="89"/>
+      <c r="B35" s="113"/>
+      <c r="C35" s="93"/>
       <c r="D35" s="33"/>
       <c r="E35" s="32"/>
       <c r="F35" s="32"/>
@@ -3764,10 +3767,10 @@
       <c r="Q35" s="32"/>
       <c r="R35" s="3"/>
       <c r="S35" s="12"/>
-      <c r="T35" s="110"/>
-      <c r="U35" s="102"/>
-      <c r="V35" s="102"/>
-      <c r="W35" s="101"/>
+      <c r="T35" s="109"/>
+      <c r="U35" s="101"/>
+      <c r="V35" s="101"/>
+      <c r="W35" s="100"/>
       <c r="X35" s="11"/>
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
@@ -3784,28 +3787,28 @@
       <c r="AK35" s="3"/>
       <c r="AL35" s="3"/>
       <c r="AM35" s="12"/>
-      <c r="AN35" s="110"/>
-      <c r="AO35" s="102"/>
-      <c r="AP35" s="102"/>
-      <c r="AQ35" s="101"/>
+      <c r="AN35" s="109"/>
+      <c r="AO35" s="101"/>
+      <c r="AP35" s="101"/>
+      <c r="AQ35" s="100"/>
       <c r="AR35" s="33"/>
       <c r="AS35" s="3"/>
       <c r="AT35" s="32"/>
       <c r="AU35" s="31"/>
       <c r="AV35" s="33"/>
       <c r="AW35" s="3"/>
-      <c r="AX35" s="100"/>
-      <c r="AY35" s="101"/>
-      <c r="AZ35" s="82"/>
+      <c r="AX35" s="99"/>
+      <c r="AY35" s="100"/>
+      <c r="AZ35" s="81"/>
     </row>
     <row r="36" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A36" s="116" t="s">
+      <c r="A36" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="85">
+      <c r="B36" s="84">
         <v>1</v>
       </c>
-      <c r="C36" s="117"/>
+      <c r="C36" s="116"/>
       <c r="D36" s="6"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -3822,10 +3825,10 @@
       <c r="Q36" s="5"/>
       <c r="R36" s="30"/>
       <c r="S36" s="49"/>
-      <c r="T36" s="110"/>
-      <c r="U36" s="102"/>
-      <c r="V36" s="102"/>
-      <c r="W36" s="101"/>
+      <c r="T36" s="109"/>
+      <c r="U36" s="101"/>
+      <c r="V36" s="101"/>
+      <c r="W36" s="100"/>
       <c r="X36" s="28"/>
       <c r="Y36" s="30"/>
       <c r="Z36" s="30"/>
@@ -3842,24 +3845,24 @@
       <c r="AK36" s="30"/>
       <c r="AL36" s="30"/>
       <c r="AM36" s="29"/>
-      <c r="AN36" s="110"/>
-      <c r="AO36" s="102"/>
-      <c r="AP36" s="102"/>
-      <c r="AQ36" s="101"/>
+      <c r="AN36" s="109"/>
+      <c r="AO36" s="101"/>
+      <c r="AP36" s="101"/>
+      <c r="AQ36" s="100"/>
       <c r="AR36" s="6"/>
       <c r="AS36" s="30"/>
       <c r="AT36" s="5"/>
       <c r="AU36" s="7"/>
       <c r="AV36" s="6"/>
       <c r="AW36" s="30"/>
-      <c r="AX36" s="100"/>
-      <c r="AY36" s="101"/>
-      <c r="AZ36" s="82"/>
+      <c r="AX36" s="99"/>
+      <c r="AY36" s="100"/>
+      <c r="AZ36" s="81"/>
     </row>
     <row r="37" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A37" s="90"/>
-      <c r="B37" s="114"/>
-      <c r="C37" s="115"/>
+      <c r="A37" s="89"/>
+      <c r="B37" s="113"/>
+      <c r="C37" s="114"/>
       <c r="D37" s="33"/>
       <c r="E37" s="32"/>
       <c r="F37" s="3"/>
@@ -3876,10 +3879,10 @@
       <c r="Q37" s="32"/>
       <c r="R37" s="3"/>
       <c r="S37" s="31"/>
-      <c r="T37" s="110"/>
-      <c r="U37" s="102"/>
-      <c r="V37" s="102"/>
-      <c r="W37" s="101"/>
+      <c r="T37" s="109"/>
+      <c r="U37" s="101"/>
+      <c r="V37" s="101"/>
+      <c r="W37" s="100"/>
       <c r="X37" s="33"/>
       <c r="Y37" s="32"/>
       <c r="Z37" s="32"/>
@@ -3896,28 +3899,28 @@
       <c r="AK37" s="32"/>
       <c r="AL37" s="32"/>
       <c r="AM37" s="12"/>
-      <c r="AN37" s="110"/>
-      <c r="AO37" s="102"/>
-      <c r="AP37" s="102"/>
-      <c r="AQ37" s="101"/>
+      <c r="AN37" s="109"/>
+      <c r="AO37" s="101"/>
+      <c r="AP37" s="101"/>
+      <c r="AQ37" s="100"/>
       <c r="AR37" s="11"/>
       <c r="AS37" s="3"/>
       <c r="AT37" s="32"/>
       <c r="AU37" s="12"/>
       <c r="AV37" s="11"/>
       <c r="AW37" s="3"/>
-      <c r="AX37" s="100"/>
-      <c r="AY37" s="101"/>
-      <c r="AZ37" s="82"/>
+      <c r="AX37" s="99"/>
+      <c r="AY37" s="100"/>
+      <c r="AZ37" s="81"/>
     </row>
     <row r="38" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A38" s="83" t="s">
+      <c r="A38" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="85">
+      <c r="B38" s="84">
         <v>1</v>
       </c>
-      <c r="C38" s="117"/>
+      <c r="C38" s="116"/>
       <c r="D38" s="6"/>
       <c r="E38" s="5"/>
       <c r="F38" s="30"/>
@@ -3934,10 +3937,10 @@
       <c r="Q38" s="5"/>
       <c r="R38" s="30"/>
       <c r="S38" s="25"/>
-      <c r="T38" s="110"/>
-      <c r="U38" s="102"/>
-      <c r="V38" s="102"/>
-      <c r="W38" s="101"/>
+      <c r="T38" s="109"/>
+      <c r="U38" s="101"/>
+      <c r="V38" s="101"/>
+      <c r="W38" s="100"/>
       <c r="X38" s="6"/>
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
@@ -3954,24 +3957,24 @@
       <c r="AK38" s="5"/>
       <c r="AL38" s="5"/>
       <c r="AM38" s="29"/>
-      <c r="AN38" s="110"/>
-      <c r="AO38" s="102"/>
-      <c r="AP38" s="102"/>
-      <c r="AQ38" s="101"/>
+      <c r="AN38" s="109"/>
+      <c r="AO38" s="101"/>
+      <c r="AP38" s="101"/>
+      <c r="AQ38" s="100"/>
       <c r="AR38" s="28"/>
       <c r="AS38" s="30"/>
       <c r="AT38" s="5"/>
       <c r="AU38" s="29"/>
       <c r="AV38" s="28"/>
       <c r="AW38" s="30"/>
-      <c r="AX38" s="100"/>
-      <c r="AY38" s="101"/>
-      <c r="AZ38" s="82"/>
+      <c r="AX38" s="99"/>
+      <c r="AY38" s="100"/>
+      <c r="AZ38" s="81"/>
     </row>
     <row r="39" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A39" s="113"/>
-      <c r="B39" s="114"/>
-      <c r="C39" s="115"/>
+      <c r="A39" s="112"/>
+      <c r="B39" s="113"/>
+      <c r="C39" s="114"/>
       <c r="D39" s="11"/>
       <c r="E39" s="3"/>
       <c r="F39" s="32"/>
@@ -3988,10 +3991,10 @@
       <c r="Q39" s="32"/>
       <c r="R39" s="3"/>
       <c r="S39" s="12"/>
-      <c r="T39" s="110"/>
-      <c r="U39" s="102"/>
-      <c r="V39" s="102"/>
-      <c r="W39" s="101"/>
+      <c r="T39" s="109"/>
+      <c r="U39" s="101"/>
+      <c r="V39" s="101"/>
+      <c r="W39" s="100"/>
       <c r="X39" s="11"/>
       <c r="Y39" s="32"/>
       <c r="Z39" s="32"/>
@@ -4008,28 +4011,28 @@
       <c r="AK39" s="32"/>
       <c r="AL39" s="32"/>
       <c r="AM39" s="31"/>
-      <c r="AN39" s="110"/>
-      <c r="AO39" s="102"/>
-      <c r="AP39" s="102"/>
-      <c r="AQ39" s="101"/>
+      <c r="AN39" s="109"/>
+      <c r="AO39" s="101"/>
+      <c r="AP39" s="101"/>
+      <c r="AQ39" s="100"/>
       <c r="AR39" s="33"/>
       <c r="AS39" s="32"/>
       <c r="AT39" s="3"/>
       <c r="AU39" s="31"/>
       <c r="AV39" s="11"/>
       <c r="AW39" s="3"/>
-      <c r="AX39" s="100"/>
-      <c r="AY39" s="101"/>
-      <c r="AZ39" s="82"/>
+      <c r="AX39" s="99"/>
+      <c r="AY39" s="100"/>
+      <c r="AZ39" s="81"/>
     </row>
     <row r="40" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A40" s="116" t="s">
+      <c r="A40" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="85">
+      <c r="B40" s="84">
         <v>1</v>
       </c>
-      <c r="C40" s="117"/>
+      <c r="C40" s="116"/>
       <c r="D40" s="28"/>
       <c r="E40" s="30"/>
       <c r="F40" s="5"/>
@@ -4046,10 +4049,10 @@
       <c r="Q40" s="5"/>
       <c r="R40" s="30"/>
       <c r="S40" s="29"/>
-      <c r="T40" s="110"/>
-      <c r="U40" s="102"/>
-      <c r="V40" s="102"/>
-      <c r="W40" s="101"/>
+      <c r="T40" s="109"/>
+      <c r="U40" s="101"/>
+      <c r="V40" s="101"/>
+      <c r="W40" s="100"/>
       <c r="X40" s="38"/>
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
@@ -4066,24 +4069,24 @@
       <c r="AK40" s="5"/>
       <c r="AL40" s="5"/>
       <c r="AM40" s="7"/>
-      <c r="AN40" s="110"/>
-      <c r="AO40" s="102"/>
-      <c r="AP40" s="102"/>
-      <c r="AQ40" s="101"/>
+      <c r="AN40" s="109"/>
+      <c r="AO40" s="101"/>
+      <c r="AP40" s="101"/>
+      <c r="AQ40" s="100"/>
       <c r="AR40" s="6"/>
       <c r="AS40" s="5"/>
       <c r="AT40" s="30"/>
       <c r="AU40" s="7"/>
       <c r="AV40" s="28"/>
       <c r="AW40" s="30"/>
-      <c r="AX40" s="100"/>
-      <c r="AY40" s="101"/>
-      <c r="AZ40" s="82"/>
+      <c r="AX40" s="99"/>
+      <c r="AY40" s="100"/>
+      <c r="AZ40" s="81"/>
     </row>
     <row r="41" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A41" s="113"/>
-      <c r="B41" s="114"/>
-      <c r="C41" s="115"/>
+      <c r="A41" s="112"/>
+      <c r="B41" s="113"/>
+      <c r="C41" s="114"/>
       <c r="D41" s="33"/>
       <c r="E41" s="32"/>
       <c r="F41" s="32"/>
@@ -4100,10 +4103,10 @@
       <c r="Q41" s="32"/>
       <c r="R41" s="3"/>
       <c r="S41" s="12"/>
-      <c r="T41" s="110"/>
-      <c r="U41" s="102"/>
-      <c r="V41" s="102"/>
-      <c r="W41" s="101"/>
+      <c r="T41" s="109"/>
+      <c r="U41" s="101"/>
+      <c r="V41" s="101"/>
+      <c r="W41" s="100"/>
       <c r="X41" s="11"/>
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
@@ -4120,28 +4123,28 @@
       <c r="AK41" s="3"/>
       <c r="AL41" s="32"/>
       <c r="AM41" s="12"/>
-      <c r="AN41" s="110"/>
-      <c r="AO41" s="102"/>
-      <c r="AP41" s="102"/>
-      <c r="AQ41" s="101"/>
+      <c r="AN41" s="109"/>
+      <c r="AO41" s="101"/>
+      <c r="AP41" s="101"/>
+      <c r="AQ41" s="100"/>
       <c r="AR41" s="11"/>
       <c r="AS41" s="3"/>
       <c r="AT41" s="3"/>
       <c r="AU41" s="12"/>
       <c r="AV41" s="11"/>
       <c r="AW41" s="32"/>
-      <c r="AX41" s="100"/>
-      <c r="AY41" s="101"/>
-      <c r="AZ41" s="82"/>
+      <c r="AX41" s="99"/>
+      <c r="AY41" s="100"/>
+      <c r="AZ41" s="81"/>
     </row>
     <row r="42" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A42" s="116" t="s">
+      <c r="A42" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="85">
+      <c r="B42" s="84">
         <v>2</v>
       </c>
-      <c r="C42" s="117"/>
+      <c r="C42" s="116"/>
       <c r="D42" s="6"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -4158,10 +4161,10 @@
       <c r="Q42" s="5"/>
       <c r="R42" s="30"/>
       <c r="S42" s="29"/>
-      <c r="T42" s="110"/>
-      <c r="U42" s="102"/>
-      <c r="V42" s="102"/>
-      <c r="W42" s="101"/>
+      <c r="T42" s="109"/>
+      <c r="U42" s="101"/>
+      <c r="V42" s="101"/>
+      <c r="W42" s="100"/>
       <c r="X42" s="28"/>
       <c r="Y42" s="34"/>
       <c r="Z42" s="34"/>
@@ -4178,24 +4181,24 @@
       <c r="AK42" s="30"/>
       <c r="AL42" s="5"/>
       <c r="AM42" s="29"/>
-      <c r="AN42" s="110"/>
-      <c r="AO42" s="102"/>
-      <c r="AP42" s="102"/>
-      <c r="AQ42" s="101"/>
+      <c r="AN42" s="109"/>
+      <c r="AO42" s="101"/>
+      <c r="AP42" s="101"/>
+      <c r="AQ42" s="100"/>
       <c r="AR42" s="28"/>
       <c r="AS42" s="30"/>
       <c r="AT42" s="30"/>
       <c r="AU42" s="29"/>
       <c r="AV42" s="28"/>
       <c r="AW42" s="5"/>
-      <c r="AX42" s="100"/>
-      <c r="AY42" s="101"/>
-      <c r="AZ42" s="82"/>
+      <c r="AX42" s="99"/>
+      <c r="AY42" s="100"/>
+      <c r="AZ42" s="81"/>
     </row>
     <row r="43" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A43" s="90"/>
-      <c r="B43" s="114"/>
-      <c r="C43" s="115"/>
+      <c r="A43" s="89"/>
+      <c r="B43" s="113"/>
+      <c r="C43" s="114"/>
       <c r="D43" s="11"/>
       <c r="E43" s="32"/>
       <c r="F43" s="3"/>
@@ -4212,10 +4215,10 @@
       <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
       <c r="S43" s="31"/>
-      <c r="T43" s="110"/>
-      <c r="U43" s="102"/>
-      <c r="V43" s="102"/>
-      <c r="W43" s="101"/>
+      <c r="T43" s="109"/>
+      <c r="U43" s="101"/>
+      <c r="V43" s="101"/>
+      <c r="W43" s="100"/>
       <c r="X43" s="11"/>
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
@@ -4232,28 +4235,28 @@
       <c r="AK43" s="32"/>
       <c r="AL43" s="3"/>
       <c r="AM43" s="12"/>
-      <c r="AN43" s="110"/>
-      <c r="AO43" s="102"/>
-      <c r="AP43" s="102"/>
-      <c r="AQ43" s="101"/>
+      <c r="AN43" s="109"/>
+      <c r="AO43" s="101"/>
+      <c r="AP43" s="101"/>
+      <c r="AQ43" s="100"/>
       <c r="AR43" s="11"/>
       <c r="AS43" s="3"/>
       <c r="AT43" s="3"/>
       <c r="AU43" s="12"/>
       <c r="AV43" s="11"/>
       <c r="AW43" s="3"/>
-      <c r="AX43" s="100"/>
-      <c r="AY43" s="101"/>
-      <c r="AZ43" s="82"/>
+      <c r="AX43" s="99"/>
+      <c r="AY43" s="100"/>
+      <c r="AZ43" s="81"/>
     </row>
     <row r="44" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A44" s="116" t="s">
+      <c r="A44" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="118">
+      <c r="B44" s="117">
         <v>2.5</v>
       </c>
-      <c r="C44" s="117"/>
+      <c r="C44" s="116"/>
       <c r="D44" s="28"/>
       <c r="E44" s="5"/>
       <c r="F44" s="30"/>
@@ -4270,10 +4273,10 @@
       <c r="Q44" s="30"/>
       <c r="R44" s="30"/>
       <c r="S44" s="7"/>
-      <c r="T44" s="110"/>
-      <c r="U44" s="102"/>
-      <c r="V44" s="102"/>
-      <c r="W44" s="101"/>
+      <c r="T44" s="109"/>
+      <c r="U44" s="101"/>
+      <c r="V44" s="101"/>
+      <c r="W44" s="100"/>
       <c r="X44" s="28"/>
       <c r="Y44" s="30"/>
       <c r="Z44" s="34"/>
@@ -4290,24 +4293,24 @@
       <c r="AK44" s="5"/>
       <c r="AL44" s="30"/>
       <c r="AM44" s="29"/>
-      <c r="AN44" s="110"/>
-      <c r="AO44" s="102"/>
-      <c r="AP44" s="102"/>
-      <c r="AQ44" s="101"/>
+      <c r="AN44" s="109"/>
+      <c r="AO44" s="101"/>
+      <c r="AP44" s="101"/>
+      <c r="AQ44" s="100"/>
       <c r="AR44" s="28"/>
       <c r="AS44" s="30"/>
       <c r="AT44" s="30"/>
       <c r="AU44" s="29"/>
       <c r="AV44" s="28"/>
       <c r="AW44" s="30"/>
-      <c r="AX44" s="100"/>
-      <c r="AY44" s="101"/>
-      <c r="AZ44" s="82"/>
+      <c r="AX44" s="99"/>
+      <c r="AY44" s="100"/>
+      <c r="AZ44" s="81"/>
     </row>
     <row r="45" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A45" s="90"/>
-      <c r="B45" s="92"/>
-      <c r="C45" s="115"/>
+      <c r="A45" s="89"/>
+      <c r="B45" s="91"/>
+      <c r="C45" s="114"/>
       <c r="D45" s="11"/>
       <c r="E45" s="3"/>
       <c r="F45" s="32"/>
@@ -4324,10 +4327,10 @@
       <c r="Q45" s="3"/>
       <c r="R45" s="3"/>
       <c r="S45" s="12"/>
-      <c r="T45" s="110"/>
-      <c r="U45" s="102"/>
-      <c r="V45" s="102"/>
-      <c r="W45" s="101"/>
+      <c r="T45" s="109"/>
+      <c r="U45" s="101"/>
+      <c r="V45" s="101"/>
+      <c r="W45" s="100"/>
       <c r="X45" s="11"/>
       <c r="Y45" s="32"/>
       <c r="Z45" s="3"/>
@@ -4344,28 +4347,28 @@
       <c r="AK45" s="3"/>
       <c r="AL45" s="3"/>
       <c r="AM45" s="12"/>
-      <c r="AN45" s="110"/>
-      <c r="AO45" s="102"/>
-      <c r="AP45" s="102"/>
-      <c r="AQ45" s="101"/>
+      <c r="AN45" s="109"/>
+      <c r="AO45" s="101"/>
+      <c r="AP45" s="101"/>
+      <c r="AQ45" s="100"/>
       <c r="AR45" s="11"/>
       <c r="AS45" s="3"/>
       <c r="AT45" s="3"/>
       <c r="AU45" s="12"/>
       <c r="AV45" s="11"/>
       <c r="AW45" s="3"/>
-      <c r="AX45" s="100"/>
-      <c r="AY45" s="101"/>
-      <c r="AZ45" s="82"/>
+      <c r="AX45" s="99"/>
+      <c r="AY45" s="100"/>
+      <c r="AZ45" s="81"/>
     </row>
     <row r="46" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A46" s="83" t="s">
+      <c r="A46" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="85">
+      <c r="B46" s="84">
         <v>2</v>
       </c>
-      <c r="C46" s="87"/>
+      <c r="C46" s="86"/>
       <c r="D46" s="28"/>
       <c r="E46" s="30"/>
       <c r="F46" s="5"/>
@@ -4382,10 +4385,10 @@
       <c r="Q46" s="30"/>
       <c r="R46" s="30"/>
       <c r="S46" s="29"/>
-      <c r="T46" s="110"/>
-      <c r="U46" s="102"/>
-      <c r="V46" s="102"/>
-      <c r="W46" s="101"/>
+      <c r="T46" s="109"/>
+      <c r="U46" s="101"/>
+      <c r="V46" s="101"/>
+      <c r="W46" s="100"/>
       <c r="X46" s="28"/>
       <c r="Y46" s="5"/>
       <c r="Z46" s="30"/>
@@ -4402,24 +4405,24 @@
       <c r="AK46" s="30"/>
       <c r="AL46" s="30"/>
       <c r="AM46" s="29"/>
-      <c r="AN46" s="110"/>
-      <c r="AO46" s="102"/>
-      <c r="AP46" s="102"/>
-      <c r="AQ46" s="101"/>
+      <c r="AN46" s="109"/>
+      <c r="AO46" s="101"/>
+      <c r="AP46" s="101"/>
+      <c r="AQ46" s="100"/>
       <c r="AR46" s="28"/>
       <c r="AS46" s="30"/>
       <c r="AT46" s="30"/>
       <c r="AU46" s="29"/>
       <c r="AV46" s="28"/>
       <c r="AW46" s="30"/>
-      <c r="AX46" s="100"/>
-      <c r="AY46" s="101"/>
-      <c r="AZ46" s="82"/>
+      <c r="AX46" s="99"/>
+      <c r="AY46" s="100"/>
+      <c r="AZ46" s="81"/>
     </row>
     <row r="47" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A47" s="113"/>
-      <c r="B47" s="114"/>
-      <c r="C47" s="94"/>
+      <c r="A47" s="112"/>
+      <c r="B47" s="113"/>
+      <c r="C47" s="93"/>
       <c r="D47" s="11"/>
       <c r="E47" s="32"/>
       <c r="F47" s="3"/>
@@ -4436,10 +4439,10 @@
       <c r="Q47" s="3"/>
       <c r="R47" s="32"/>
       <c r="S47" s="12"/>
-      <c r="T47" s="110"/>
-      <c r="U47" s="102"/>
-      <c r="V47" s="102"/>
-      <c r="W47" s="101"/>
+      <c r="T47" s="109"/>
+      <c r="U47" s="101"/>
+      <c r="V47" s="101"/>
+      <c r="W47" s="100"/>
       <c r="X47" s="11"/>
       <c r="Y47" s="3"/>
       <c r="Z47" s="3"/>
@@ -4456,28 +4459,28 @@
       <c r="AK47" s="32"/>
       <c r="AL47" s="3"/>
       <c r="AM47" s="31"/>
-      <c r="AN47" s="110"/>
-      <c r="AO47" s="102"/>
-      <c r="AP47" s="102"/>
-      <c r="AQ47" s="101"/>
+      <c r="AN47" s="109"/>
+      <c r="AO47" s="101"/>
+      <c r="AP47" s="101"/>
+      <c r="AQ47" s="100"/>
       <c r="AR47" s="33"/>
       <c r="AS47" s="32"/>
       <c r="AT47" s="32"/>
       <c r="AU47" s="31"/>
       <c r="AV47" s="33"/>
       <c r="AW47" s="32"/>
-      <c r="AX47" s="100"/>
-      <c r="AY47" s="101"/>
-      <c r="AZ47" s="82"/>
+      <c r="AX47" s="99"/>
+      <c r="AY47" s="100"/>
+      <c r="AZ47" s="81"/>
     </row>
     <row r="48" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A48" s="116" t="s">
+      <c r="A48" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="118">
+      <c r="B48" s="117">
         <v>0.5</v>
       </c>
-      <c r="C48" s="117"/>
+      <c r="C48" s="116"/>
       <c r="D48" s="28"/>
       <c r="E48" s="5"/>
       <c r="F48" s="30"/>
@@ -4494,10 +4497,10 @@
       <c r="Q48" s="30"/>
       <c r="R48" s="5"/>
       <c r="S48" s="29"/>
-      <c r="T48" s="110"/>
-      <c r="U48" s="102"/>
-      <c r="V48" s="102"/>
-      <c r="W48" s="101"/>
+      <c r="T48" s="109"/>
+      <c r="U48" s="101"/>
+      <c r="V48" s="101"/>
+      <c r="W48" s="100"/>
       <c r="X48" s="28"/>
       <c r="Y48" s="30"/>
       <c r="Z48" s="30"/>
@@ -4514,24 +4517,24 @@
       <c r="AK48" s="5"/>
       <c r="AL48" s="30"/>
       <c r="AM48" s="7"/>
-      <c r="AN48" s="110"/>
-      <c r="AO48" s="102"/>
-      <c r="AP48" s="102"/>
-      <c r="AQ48" s="101"/>
+      <c r="AN48" s="109"/>
+      <c r="AO48" s="101"/>
+      <c r="AP48" s="101"/>
+      <c r="AQ48" s="100"/>
       <c r="AR48" s="6"/>
       <c r="AS48" s="5"/>
       <c r="AT48" s="5"/>
       <c r="AU48" s="7"/>
       <c r="AV48" s="6"/>
       <c r="AW48" s="5"/>
-      <c r="AX48" s="100"/>
-      <c r="AY48" s="101"/>
-      <c r="AZ48" s="82"/>
+      <c r="AX48" s="99"/>
+      <c r="AY48" s="100"/>
+      <c r="AZ48" s="81"/>
     </row>
     <row r="49" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A49" s="113"/>
-      <c r="B49" s="92"/>
-      <c r="C49" s="115"/>
+      <c r="A49" s="112"/>
+      <c r="B49" s="91"/>
+      <c r="C49" s="114"/>
       <c r="D49" s="33"/>
       <c r="E49" s="32"/>
       <c r="F49" s="32"/>
@@ -4548,10 +4551,10 @@
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
       <c r="S49" s="12"/>
-      <c r="T49" s="110"/>
-      <c r="U49" s="102"/>
-      <c r="V49" s="102"/>
-      <c r="W49" s="101"/>
+      <c r="T49" s="109"/>
+      <c r="U49" s="101"/>
+      <c r="V49" s="101"/>
+      <c r="W49" s="100"/>
       <c r="X49" s="11"/>
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
@@ -4568,28 +4571,28 @@
       <c r="AK49" s="3"/>
       <c r="AL49" s="3"/>
       <c r="AM49" s="12"/>
-      <c r="AN49" s="110"/>
-      <c r="AO49" s="102"/>
-      <c r="AP49" s="102"/>
-      <c r="AQ49" s="101"/>
+      <c r="AN49" s="109"/>
+      <c r="AO49" s="101"/>
+      <c r="AP49" s="101"/>
+      <c r="AQ49" s="100"/>
       <c r="AR49" s="33"/>
       <c r="AS49" s="3"/>
       <c r="AT49" s="32"/>
       <c r="AU49" s="31"/>
       <c r="AV49" s="11"/>
       <c r="AW49" s="3"/>
-      <c r="AX49" s="100"/>
-      <c r="AY49" s="101"/>
-      <c r="AZ49" s="82"/>
+      <c r="AX49" s="99"/>
+      <c r="AY49" s="100"/>
+      <c r="AZ49" s="81"/>
     </row>
     <row r="50" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A50" s="116" t="s">
+      <c r="A50" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="B50" s="85">
+      <c r="B50" s="84">
         <v>2.5</v>
       </c>
-      <c r="C50" s="117"/>
+      <c r="C50" s="116"/>
       <c r="D50" s="6"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -4606,10 +4609,10 @@
       <c r="Q50" s="30"/>
       <c r="R50" s="30"/>
       <c r="S50" s="29"/>
-      <c r="T50" s="110"/>
-      <c r="U50" s="102"/>
-      <c r="V50" s="102"/>
-      <c r="W50" s="101"/>
+      <c r="T50" s="109"/>
+      <c r="U50" s="101"/>
+      <c r="V50" s="101"/>
+      <c r="W50" s="100"/>
       <c r="X50" s="28"/>
       <c r="Y50" s="30"/>
       <c r="Z50" s="30"/>
@@ -4626,24 +4629,24 @@
       <c r="AK50" s="30"/>
       <c r="AL50" s="30"/>
       <c r="AM50" s="29"/>
-      <c r="AN50" s="110"/>
-      <c r="AO50" s="102"/>
-      <c r="AP50" s="102"/>
-      <c r="AQ50" s="101"/>
+      <c r="AN50" s="109"/>
+      <c r="AO50" s="101"/>
+      <c r="AP50" s="101"/>
+      <c r="AQ50" s="100"/>
       <c r="AR50" s="6"/>
       <c r="AS50" s="30"/>
       <c r="AT50" s="5"/>
       <c r="AU50" s="7"/>
       <c r="AV50" s="28"/>
       <c r="AW50" s="30"/>
-      <c r="AX50" s="100"/>
-      <c r="AY50" s="101"/>
-      <c r="AZ50" s="82"/>
+      <c r="AX50" s="99"/>
+      <c r="AY50" s="100"/>
+      <c r="AZ50" s="81"/>
     </row>
     <row r="51" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A51" s="90"/>
-      <c r="B51" s="114"/>
-      <c r="C51" s="115"/>
+      <c r="A51" s="89"/>
+      <c r="B51" s="113"/>
+      <c r="C51" s="114"/>
       <c r="D51" s="11"/>
       <c r="E51" s="32"/>
       <c r="F51" s="3"/>
@@ -4660,10 +4663,10 @@
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
       <c r="S51" s="12"/>
-      <c r="T51" s="110"/>
-      <c r="U51" s="102"/>
-      <c r="V51" s="102"/>
-      <c r="W51" s="101"/>
+      <c r="T51" s="109"/>
+      <c r="U51" s="101"/>
+      <c r="V51" s="101"/>
+      <c r="W51" s="100"/>
       <c r="X51" s="33"/>
       <c r="Y51" s="32"/>
       <c r="Z51" s="3"/>
@@ -4680,28 +4683,28 @@
       <c r="AK51" s="32"/>
       <c r="AL51" s="3"/>
       <c r="AM51" s="12"/>
-      <c r="AN51" s="110"/>
-      <c r="AO51" s="102"/>
-      <c r="AP51" s="102"/>
-      <c r="AQ51" s="101"/>
+      <c r="AN51" s="109"/>
+      <c r="AO51" s="101"/>
+      <c r="AP51" s="101"/>
+      <c r="AQ51" s="100"/>
       <c r="AR51" s="11"/>
       <c r="AS51" s="3"/>
       <c r="AT51" s="3"/>
       <c r="AU51" s="12"/>
       <c r="AV51" s="11"/>
       <c r="AW51" s="3"/>
-      <c r="AX51" s="100"/>
-      <c r="AY51" s="101"/>
-      <c r="AZ51" s="82"/>
+      <c r="AX51" s="99"/>
+      <c r="AY51" s="100"/>
+      <c r="AZ51" s="81"/>
     </row>
     <row r="52" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A52" s="83" t="s">
+      <c r="A52" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="85">
+      <c r="B52" s="84">
         <v>1.5</v>
       </c>
-      <c r="C52" s="117"/>
+      <c r="C52" s="116"/>
       <c r="D52" s="28"/>
       <c r="E52" s="5"/>
       <c r="F52" s="30"/>
@@ -4718,10 +4721,10 @@
       <c r="Q52" s="30"/>
       <c r="R52" s="30"/>
       <c r="S52" s="29"/>
-      <c r="T52" s="110"/>
-      <c r="U52" s="102"/>
-      <c r="V52" s="102"/>
-      <c r="W52" s="101"/>
+      <c r="T52" s="109"/>
+      <c r="U52" s="101"/>
+      <c r="V52" s="101"/>
+      <c r="W52" s="100"/>
       <c r="X52" s="6"/>
       <c r="Y52" s="5"/>
       <c r="Z52" s="30"/>
@@ -4738,24 +4741,24 @@
       <c r="AK52" s="5"/>
       <c r="AL52" s="30"/>
       <c r="AM52" s="29"/>
-      <c r="AN52" s="110"/>
-      <c r="AO52" s="102"/>
-      <c r="AP52" s="102"/>
-      <c r="AQ52" s="101"/>
+      <c r="AN52" s="109"/>
+      <c r="AO52" s="101"/>
+      <c r="AP52" s="101"/>
+      <c r="AQ52" s="100"/>
       <c r="AR52" s="28"/>
       <c r="AS52" s="30"/>
       <c r="AT52" s="30"/>
       <c r="AU52" s="29"/>
       <c r="AV52" s="28"/>
       <c r="AW52" s="30"/>
-      <c r="AX52" s="100"/>
-      <c r="AY52" s="101"/>
-      <c r="AZ52" s="82"/>
+      <c r="AX52" s="99"/>
+      <c r="AY52" s="100"/>
+      <c r="AZ52" s="81"/>
     </row>
     <row r="53" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A53" s="113"/>
-      <c r="B53" s="114"/>
-      <c r="C53" s="115"/>
+      <c r="A53" s="112"/>
+      <c r="B53" s="113"/>
+      <c r="C53" s="114"/>
       <c r="D53" s="33"/>
       <c r="E53" s="32"/>
       <c r="F53" s="32"/>
@@ -4772,10 +4775,10 @@
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
       <c r="S53" s="12"/>
-      <c r="T53" s="110"/>
-      <c r="U53" s="102"/>
-      <c r="V53" s="102"/>
-      <c r="W53" s="101"/>
+      <c r="T53" s="109"/>
+      <c r="U53" s="101"/>
+      <c r="V53" s="101"/>
+      <c r="W53" s="100"/>
       <c r="X53" s="11"/>
       <c r="Y53" s="32"/>
       <c r="Z53" s="3"/>
@@ -4792,28 +4795,28 @@
       <c r="AK53" s="3"/>
       <c r="AL53" s="3"/>
       <c r="AM53" s="12"/>
-      <c r="AN53" s="110"/>
-      <c r="AO53" s="102"/>
-      <c r="AP53" s="102"/>
-      <c r="AQ53" s="101"/>
+      <c r="AN53" s="109"/>
+      <c r="AO53" s="101"/>
+      <c r="AP53" s="101"/>
+      <c r="AQ53" s="100"/>
       <c r="AR53" s="11"/>
       <c r="AS53" s="3"/>
       <c r="AT53" s="3"/>
       <c r="AU53" s="12"/>
       <c r="AV53" s="11"/>
       <c r="AW53" s="3"/>
-      <c r="AX53" s="100"/>
-      <c r="AY53" s="101"/>
-      <c r="AZ53" s="82"/>
+      <c r="AX53" s="99"/>
+      <c r="AY53" s="100"/>
+      <c r="AZ53" s="81"/>
     </row>
     <row r="54" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A54" s="116" t="s">
+      <c r="A54" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="85">
+      <c r="B54" s="84">
         <v>1.5</v>
       </c>
-      <c r="C54" s="87"/>
+      <c r="C54" s="86"/>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
@@ -4830,10 +4833,10 @@
       <c r="Q54" s="30"/>
       <c r="R54" s="30"/>
       <c r="S54" s="29"/>
-      <c r="T54" s="110"/>
-      <c r="U54" s="102"/>
-      <c r="V54" s="102"/>
-      <c r="W54" s="101"/>
+      <c r="T54" s="109"/>
+      <c r="U54" s="101"/>
+      <c r="V54" s="101"/>
+      <c r="W54" s="100"/>
       <c r="X54" s="28"/>
       <c r="Y54" s="5"/>
       <c r="Z54" s="30"/>
@@ -4850,24 +4853,24 @@
       <c r="AK54" s="30"/>
       <c r="AL54" s="30"/>
       <c r="AM54" s="29"/>
-      <c r="AN54" s="110"/>
-      <c r="AO54" s="102"/>
-      <c r="AP54" s="102"/>
-      <c r="AQ54" s="101"/>
+      <c r="AN54" s="109"/>
+      <c r="AO54" s="101"/>
+      <c r="AP54" s="101"/>
+      <c r="AQ54" s="100"/>
       <c r="AR54" s="28"/>
       <c r="AS54" s="30"/>
       <c r="AT54" s="30"/>
       <c r="AU54" s="29"/>
       <c r="AV54" s="28"/>
       <c r="AW54" s="30"/>
-      <c r="AX54" s="100"/>
-      <c r="AY54" s="101"/>
-      <c r="AZ54" s="82"/>
+      <c r="AX54" s="99"/>
+      <c r="AY54" s="100"/>
+      <c r="AZ54" s="81"/>
     </row>
     <row r="55" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A55" s="90"/>
-      <c r="B55" s="114"/>
-      <c r="C55" s="94"/>
+      <c r="A55" s="89"/>
+      <c r="B55" s="113"/>
+      <c r="C55" s="93"/>
       <c r="D55" s="11"/>
       <c r="E55" s="32"/>
       <c r="F55" s="3"/>
@@ -4884,10 +4887,10 @@
       <c r="Q55" s="32"/>
       <c r="R55" s="3"/>
       <c r="S55" s="31"/>
-      <c r="T55" s="110"/>
-      <c r="U55" s="102"/>
-      <c r="V55" s="102"/>
-      <c r="W55" s="101"/>
+      <c r="T55" s="109"/>
+      <c r="U55" s="101"/>
+      <c r="V55" s="101"/>
+      <c r="W55" s="100"/>
       <c r="X55" s="11"/>
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
@@ -4904,28 +4907,28 @@
       <c r="AK55" s="32"/>
       <c r="AL55" s="32"/>
       <c r="AM55" s="31"/>
-      <c r="AN55" s="110"/>
-      <c r="AO55" s="102"/>
-      <c r="AP55" s="102"/>
-      <c r="AQ55" s="101"/>
+      <c r="AN55" s="109"/>
+      <c r="AO55" s="101"/>
+      <c r="AP55" s="101"/>
+      <c r="AQ55" s="100"/>
       <c r="AR55" s="33"/>
       <c r="AS55" s="32"/>
       <c r="AT55" s="32"/>
       <c r="AU55" s="12"/>
       <c r="AV55" s="11"/>
       <c r="AW55" s="3"/>
-      <c r="AX55" s="100"/>
-      <c r="AY55" s="101"/>
-      <c r="AZ55" s="82"/>
+      <c r="AX55" s="99"/>
+      <c r="AY55" s="100"/>
+      <c r="AZ55" s="81"/>
     </row>
     <row r="56" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A56" s="116" t="s">
+      <c r="A56" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="118">
+      <c r="B56" s="117">
         <v>2</v>
       </c>
-      <c r="C56" s="117"/>
+      <c r="C56" s="116"/>
       <c r="D56" s="28"/>
       <c r="E56" s="5"/>
       <c r="F56" s="30"/>
@@ -4942,10 +4945,10 @@
       <c r="Q56" s="5"/>
       <c r="R56" s="30"/>
       <c r="S56" s="7"/>
-      <c r="T56" s="110"/>
-      <c r="U56" s="102"/>
-      <c r="V56" s="102"/>
-      <c r="W56" s="101"/>
+      <c r="T56" s="109"/>
+      <c r="U56" s="101"/>
+      <c r="V56" s="101"/>
+      <c r="W56" s="100"/>
       <c r="X56" s="28"/>
       <c r="Y56" s="30"/>
       <c r="Z56" s="30"/>
@@ -4962,24 +4965,24 @@
       <c r="AK56" s="24"/>
       <c r="AL56" s="5"/>
       <c r="AM56" s="7"/>
-      <c r="AN56" s="110"/>
-      <c r="AO56" s="102"/>
-      <c r="AP56" s="102"/>
-      <c r="AQ56" s="101"/>
+      <c r="AN56" s="109"/>
+      <c r="AO56" s="101"/>
+      <c r="AP56" s="101"/>
+      <c r="AQ56" s="100"/>
       <c r="AR56" s="6"/>
       <c r="AS56" s="5"/>
       <c r="AT56" s="5"/>
       <c r="AU56" s="29"/>
       <c r="AV56" s="28"/>
       <c r="AW56" s="30"/>
-      <c r="AX56" s="100"/>
-      <c r="AY56" s="101"/>
-      <c r="AZ56" s="82"/>
+      <c r="AX56" s="99"/>
+      <c r="AY56" s="100"/>
+      <c r="AZ56" s="81"/>
     </row>
     <row r="57" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A57" s="90"/>
-      <c r="B57" s="92"/>
-      <c r="C57" s="94"/>
+      <c r="A57" s="89"/>
+      <c r="B57" s="91"/>
+      <c r="C57" s="93"/>
       <c r="D57" s="11"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -4996,10 +4999,10 @@
       <c r="Q57" s="3"/>
       <c r="R57" s="3"/>
       <c r="S57" s="12"/>
-      <c r="T57" s="110"/>
-      <c r="U57" s="102"/>
-      <c r="V57" s="102"/>
-      <c r="W57" s="101"/>
+      <c r="T57" s="109"/>
+      <c r="U57" s="101"/>
+      <c r="V57" s="101"/>
+      <c r="W57" s="100"/>
       <c r="X57" s="33"/>
       <c r="Y57" s="3"/>
       <c r="Z57" s="32"/>
@@ -5016,28 +5019,28 @@
       <c r="AK57" s="32"/>
       <c r="AL57" s="3"/>
       <c r="AM57" s="12"/>
-      <c r="AN57" s="110"/>
-      <c r="AO57" s="102"/>
-      <c r="AP57" s="102"/>
-      <c r="AQ57" s="101"/>
+      <c r="AN57" s="109"/>
+      <c r="AO57" s="101"/>
+      <c r="AP57" s="101"/>
+      <c r="AQ57" s="100"/>
       <c r="AR57" s="11"/>
       <c r="AS57" s="3"/>
       <c r="AT57" s="3"/>
       <c r="AU57" s="31"/>
       <c r="AV57" s="33"/>
       <c r="AW57" s="3"/>
-      <c r="AX57" s="100"/>
-      <c r="AY57" s="101"/>
-      <c r="AZ57" s="82"/>
+      <c r="AX57" s="99"/>
+      <c r="AY57" s="100"/>
+      <c r="AZ57" s="81"/>
     </row>
     <row r="58" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A58" s="83" t="s">
+      <c r="A58" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="85">
+      <c r="B58" s="84">
         <v>2</v>
       </c>
-      <c r="C58" s="117"/>
+      <c r="C58" s="116"/>
       <c r="D58" s="28"/>
       <c r="E58" s="30"/>
       <c r="F58" s="30"/>
@@ -5054,10 +5057,10 @@
       <c r="Q58" s="30"/>
       <c r="R58" s="30"/>
       <c r="S58" s="29"/>
-      <c r="T58" s="110"/>
-      <c r="U58" s="102"/>
-      <c r="V58" s="102"/>
-      <c r="W58" s="101"/>
+      <c r="T58" s="109"/>
+      <c r="U58" s="101"/>
+      <c r="V58" s="101"/>
+      <c r="W58" s="100"/>
       <c r="X58" s="6"/>
       <c r="Y58" s="30"/>
       <c r="Z58" s="5"/>
@@ -5074,24 +5077,24 @@
       <c r="AK58" s="5"/>
       <c r="AL58" s="34"/>
       <c r="AM58" s="59"/>
-      <c r="AN58" s="110"/>
-      <c r="AO58" s="102"/>
-      <c r="AP58" s="102"/>
-      <c r="AQ58" s="101"/>
+      <c r="AN58" s="109"/>
+      <c r="AO58" s="101"/>
+      <c r="AP58" s="101"/>
+      <c r="AQ58" s="100"/>
       <c r="AR58" s="28"/>
       <c r="AS58" s="30"/>
       <c r="AT58" s="30"/>
       <c r="AU58" s="7"/>
       <c r="AV58" s="6"/>
       <c r="AW58" s="30"/>
-      <c r="AX58" s="100"/>
-      <c r="AY58" s="101"/>
-      <c r="AZ58" s="82"/>
+      <c r="AX58" s="99"/>
+      <c r="AY58" s="100"/>
+      <c r="AZ58" s="81"/>
     </row>
     <row r="59" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="84"/>
-      <c r="B59" s="86"/>
-      <c r="C59" s="88"/>
+      <c r="A59" s="83"/>
+      <c r="B59" s="85"/>
+      <c r="C59" s="87"/>
       <c r="D59" s="8"/>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
@@ -5108,10 +5111,10 @@
       <c r="Q59" s="9"/>
       <c r="R59" s="9"/>
       <c r="S59" s="10"/>
-      <c r="T59" s="110"/>
-      <c r="U59" s="102"/>
-      <c r="V59" s="102"/>
-      <c r="W59" s="101"/>
+      <c r="T59" s="109"/>
+      <c r="U59" s="101"/>
+      <c r="V59" s="101"/>
+      <c r="W59" s="100"/>
       <c r="X59" s="8"/>
       <c r="Y59" s="9"/>
       <c r="Z59" s="9"/>
@@ -5128,28 +5131,28 @@
       <c r="AK59" s="9"/>
       <c r="AL59" s="9"/>
       <c r="AM59" s="10"/>
-      <c r="AN59" s="110"/>
-      <c r="AO59" s="102"/>
-      <c r="AP59" s="102"/>
-      <c r="AQ59" s="101"/>
+      <c r="AN59" s="109"/>
+      <c r="AO59" s="101"/>
+      <c r="AP59" s="101"/>
+      <c r="AQ59" s="100"/>
       <c r="AR59" s="8"/>
       <c r="AS59" s="9"/>
       <c r="AT59" s="9"/>
       <c r="AU59" s="10"/>
       <c r="AV59" s="8"/>
       <c r="AW59" s="9"/>
-      <c r="AX59" s="100"/>
-      <c r="AY59" s="101"/>
-      <c r="AZ59" s="81"/>
+      <c r="AX59" s="99"/>
+      <c r="AY59" s="100"/>
+      <c r="AZ59" s="80"/>
     </row>
     <row r="60" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A60" s="89" t="s">
+      <c r="A60" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="B60" s="91">
+      <c r="B60" s="90">
         <v>0.5</v>
       </c>
-      <c r="C60" s="93"/>
+      <c r="C60" s="92"/>
       <c r="D60" s="15"/>
       <c r="E60" s="16"/>
       <c r="F60" s="16"/>
@@ -5166,10 +5169,10 @@
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
       <c r="S60" s="17"/>
-      <c r="T60" s="110"/>
-      <c r="U60" s="102"/>
-      <c r="V60" s="102"/>
-      <c r="W60" s="101"/>
+      <c r="T60" s="109"/>
+      <c r="U60" s="101"/>
+      <c r="V60" s="101"/>
+      <c r="W60" s="100"/>
       <c r="X60" s="15"/>
       <c r="Y60" s="16"/>
       <c r="Z60" s="16"/>
@@ -5186,26 +5189,26 @@
       <c r="AK60" s="16"/>
       <c r="AL60" s="16"/>
       <c r="AM60" s="17"/>
-      <c r="AN60" s="110"/>
-      <c r="AO60" s="102"/>
-      <c r="AP60" s="102"/>
-      <c r="AQ60" s="101"/>
+      <c r="AN60" s="109"/>
+      <c r="AO60" s="101"/>
+      <c r="AP60" s="101"/>
+      <c r="AQ60" s="100"/>
       <c r="AR60" s="23"/>
       <c r="AS60" s="16"/>
       <c r="AT60" s="16"/>
       <c r="AU60" s="17"/>
       <c r="AV60" s="15"/>
       <c r="AW60" s="16"/>
-      <c r="AX60" s="100"/>
-      <c r="AY60" s="101"/>
-      <c r="AZ60" s="95" t="s">
+      <c r="AX60" s="99"/>
+      <c r="AY60" s="100"/>
+      <c r="AZ60" s="94" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A61" s="90"/>
-      <c r="B61" s="92"/>
-      <c r="C61" s="94"/>
+      <c r="A61" s="89"/>
+      <c r="B61" s="91"/>
+      <c r="C61" s="93"/>
       <c r="D61" s="11"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -5222,10 +5225,10 @@
       <c r="Q61" s="3"/>
       <c r="R61" s="3"/>
       <c r="S61" s="12"/>
-      <c r="T61" s="110"/>
-      <c r="U61" s="102"/>
-      <c r="V61" s="102"/>
-      <c r="W61" s="101"/>
+      <c r="T61" s="109"/>
+      <c r="U61" s="101"/>
+      <c r="V61" s="101"/>
+      <c r="W61" s="100"/>
       <c r="X61" s="11"/>
       <c r="Y61" s="3"/>
       <c r="Z61" s="3"/>
@@ -5242,28 +5245,28 @@
       <c r="AK61" s="32"/>
       <c r="AL61" s="3"/>
       <c r="AM61" s="12"/>
-      <c r="AN61" s="110"/>
-      <c r="AO61" s="102"/>
-      <c r="AP61" s="102"/>
-      <c r="AQ61" s="101"/>
+      <c r="AN61" s="109"/>
+      <c r="AO61" s="101"/>
+      <c r="AP61" s="101"/>
+      <c r="AQ61" s="100"/>
       <c r="AR61" s="11"/>
       <c r="AS61" s="3"/>
       <c r="AT61" s="3"/>
       <c r="AU61" s="12"/>
       <c r="AV61" s="33"/>
       <c r="AW61" s="3"/>
-      <c r="AX61" s="100"/>
-      <c r="AY61" s="101"/>
-      <c r="AZ61" s="96"/>
+      <c r="AX61" s="99"/>
+      <c r="AY61" s="100"/>
+      <c r="AZ61" s="95"/>
     </row>
     <row r="62" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A62" s="83" t="s">
+      <c r="A62" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="B62" s="85">
+      <c r="B62" s="84">
         <v>2</v>
       </c>
-      <c r="C62" s="117"/>
+      <c r="C62" s="116"/>
       <c r="D62" s="28"/>
       <c r="E62" s="30"/>
       <c r="F62" s="30"/>
@@ -5280,10 +5283,10 @@
       <c r="Q62" s="30"/>
       <c r="R62" s="30"/>
       <c r="S62" s="29"/>
-      <c r="T62" s="110"/>
-      <c r="U62" s="102"/>
-      <c r="V62" s="102"/>
-      <c r="W62" s="101"/>
+      <c r="T62" s="109"/>
+      <c r="U62" s="101"/>
+      <c r="V62" s="101"/>
+      <c r="W62" s="100"/>
       <c r="X62" s="28"/>
       <c r="Y62" s="30"/>
       <c r="Z62" s="30"/>
@@ -5300,24 +5303,24 @@
       <c r="AK62" s="5"/>
       <c r="AL62" s="30"/>
       <c r="AM62" s="29"/>
-      <c r="AN62" s="110"/>
-      <c r="AO62" s="102"/>
-      <c r="AP62" s="102"/>
-      <c r="AQ62" s="101"/>
+      <c r="AN62" s="109"/>
+      <c r="AO62" s="101"/>
+      <c r="AP62" s="101"/>
+      <c r="AQ62" s="100"/>
       <c r="AR62" s="38"/>
       <c r="AS62" s="34"/>
       <c r="AT62" s="30"/>
       <c r="AU62" s="29"/>
       <c r="AV62" s="6"/>
       <c r="AW62" s="30"/>
-      <c r="AX62" s="100"/>
-      <c r="AY62" s="101"/>
-      <c r="AZ62" s="96"/>
+      <c r="AX62" s="99"/>
+      <c r="AY62" s="100"/>
+      <c r="AZ62" s="95"/>
     </row>
     <row r="63" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="84"/>
-      <c r="B63" s="86"/>
-      <c r="C63" s="88"/>
+      <c r="A63" s="83"/>
+      <c r="B63" s="85"/>
+      <c r="C63" s="87"/>
       <c r="D63" s="8"/>
       <c r="E63" s="9"/>
       <c r="F63" s="9"/>
@@ -5334,10 +5337,10 @@
       <c r="Q63" s="9"/>
       <c r="R63" s="9"/>
       <c r="S63" s="10"/>
-      <c r="T63" s="110"/>
-      <c r="U63" s="102"/>
-      <c r="V63" s="102"/>
-      <c r="W63" s="101"/>
+      <c r="T63" s="109"/>
+      <c r="U63" s="101"/>
+      <c r="V63" s="101"/>
+      <c r="W63" s="100"/>
       <c r="X63" s="8"/>
       <c r="Y63" s="9"/>
       <c r="Z63" s="9"/>
@@ -5354,28 +5357,28 @@
       <c r="AK63" s="9"/>
       <c r="AL63" s="9"/>
       <c r="AM63" s="10"/>
-      <c r="AN63" s="110"/>
-      <c r="AO63" s="102"/>
-      <c r="AP63" s="102"/>
-      <c r="AQ63" s="101"/>
+      <c r="AN63" s="109"/>
+      <c r="AO63" s="101"/>
+      <c r="AP63" s="101"/>
+      <c r="AQ63" s="100"/>
       <c r="AR63" s="8"/>
       <c r="AS63" s="9"/>
       <c r="AT63" s="9"/>
       <c r="AU63" s="10"/>
       <c r="AV63" s="8"/>
       <c r="AW63" s="9"/>
-      <c r="AX63" s="100"/>
-      <c r="AY63" s="101"/>
-      <c r="AZ63" s="97"/>
+      <c r="AX63" s="99"/>
+      <c r="AY63" s="100"/>
+      <c r="AZ63" s="96"/>
     </row>
     <row r="64" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A64" s="89" t="s">
+      <c r="A64" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="B64" s="91">
+      <c r="B64" s="90">
         <v>2.5</v>
       </c>
-      <c r="C64" s="93"/>
+      <c r="C64" s="92"/>
       <c r="D64" s="15"/>
       <c r="E64" s="16"/>
       <c r="F64" s="16"/>
@@ -5392,10 +5395,10 @@
       <c r="Q64" s="16"/>
       <c r="R64" s="16"/>
       <c r="S64" s="17"/>
-      <c r="T64" s="110"/>
-      <c r="U64" s="102"/>
-      <c r="V64" s="102"/>
-      <c r="W64" s="101"/>
+      <c r="T64" s="109"/>
+      <c r="U64" s="101"/>
+      <c r="V64" s="101"/>
+      <c r="W64" s="100"/>
       <c r="X64" s="15"/>
       <c r="Y64" s="16"/>
       <c r="Z64" s="16"/>
@@ -5412,26 +5415,26 @@
       <c r="AK64" s="16"/>
       <c r="AL64" s="16"/>
       <c r="AM64" s="17"/>
-      <c r="AN64" s="110"/>
-      <c r="AO64" s="102"/>
-      <c r="AP64" s="102"/>
-      <c r="AQ64" s="101"/>
+      <c r="AN64" s="109"/>
+      <c r="AO64" s="101"/>
+      <c r="AP64" s="101"/>
+      <c r="AQ64" s="100"/>
       <c r="AR64" s="15"/>
       <c r="AS64" s="16"/>
       <c r="AT64" s="27"/>
       <c r="AU64" s="58"/>
       <c r="AV64" s="15"/>
       <c r="AW64" s="16"/>
-      <c r="AX64" s="100"/>
-      <c r="AY64" s="101"/>
-      <c r="AZ64" s="95" t="s">
+      <c r="AX64" s="99"/>
+      <c r="AY64" s="100"/>
+      <c r="AZ64" s="94" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="84"/>
-      <c r="B65" s="86"/>
-      <c r="C65" s="88"/>
+      <c r="A65" s="83"/>
+      <c r="B65" s="85"/>
+      <c r="C65" s="87"/>
       <c r="D65" s="8"/>
       <c r="E65" s="9"/>
       <c r="F65" s="9"/>
@@ -5448,10 +5451,10 @@
       <c r="Q65" s="9"/>
       <c r="R65" s="9"/>
       <c r="S65" s="10"/>
-      <c r="T65" s="111"/>
-      <c r="U65" s="112"/>
-      <c r="V65" s="112"/>
-      <c r="W65" s="104"/>
+      <c r="T65" s="110"/>
+      <c r="U65" s="111"/>
+      <c r="V65" s="111"/>
+      <c r="W65" s="103"/>
       <c r="X65" s="8"/>
       <c r="Y65" s="9"/>
       <c r="Z65" s="9"/>
@@ -5468,19 +5471,19 @@
       <c r="AK65" s="9"/>
       <c r="AL65" s="9"/>
       <c r="AM65" s="10"/>
-      <c r="AN65" s="111"/>
-      <c r="AO65" s="112"/>
-      <c r="AP65" s="112"/>
-      <c r="AQ65" s="104"/>
+      <c r="AN65" s="110"/>
+      <c r="AO65" s="111"/>
+      <c r="AP65" s="111"/>
+      <c r="AQ65" s="103"/>
       <c r="AR65" s="8"/>
       <c r="AS65" s="9"/>
       <c r="AT65" s="9"/>
       <c r="AU65" s="10"/>
       <c r="AV65" s="8"/>
       <c r="AW65" s="9"/>
-      <c r="AX65" s="103"/>
-      <c r="AY65" s="104"/>
-      <c r="AZ65" s="97"/>
+      <c r="AX65" s="102"/>
+      <c r="AY65" s="103"/>
+      <c r="AZ65" s="96"/>
     </row>
     <row r="66" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="14" t="s">

</xml_diff>

<commit_message>
Mit der entwicklung weit gekommen lediglich noch schwierigkeiten mit css aber alles was erstellt wrude funktioniert wen auch mit eins zwei schönheitsfehlern.
</commit_message>
<xml_diff>
--- a/Doku/Shannon_Neil_Schuerch_Zeitplan_IPA_2022.xlsx
+++ b/Doku/Shannon_Neil_Schuerch_Zeitplan_IPA_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Dashboard\Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20095296-03B1-4979-8F57-584E35EB148C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A62443-8FD1-467C-AB51-58E063C29111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28260" yWindow="-120" windowWidth="28380" windowHeight="14220" xr2:uid="{B08A1154-B080-432D-B17F-9B53C1DBF0AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14625" xr2:uid="{B08A1154-B080-432D-B17F-9B53C1DBF0AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1114,6 +1114,136 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1135,24 +1265,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1162,121 +1274,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1596,8 +1596,8 @@
   </sheetPr>
   <dimension ref="A1:BC66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R43" sqref="R43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,169 +1654,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="73" t="s">
+      <c r="C1" s="114"/>
+      <c r="D1" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="73" t="s">
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="73" t="s">
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="73" t="s">
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="73" t="s">
+      <c r="Q1" s="104"/>
+      <c r="R1" s="104"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="75"/>
-      <c r="X1" s="73" t="s">
+      <c r="U1" s="104"/>
+      <c r="V1" s="104"/>
+      <c r="W1" s="105"/>
+      <c r="X1" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="Y1" s="74"/>
-      <c r="Z1" s="74"/>
-      <c r="AA1" s="75"/>
-      <c r="AB1" s="73" t="s">
+      <c r="Y1" s="104"/>
+      <c r="Z1" s="104"/>
+      <c r="AA1" s="105"/>
+      <c r="AB1" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="AC1" s="74"/>
-      <c r="AD1" s="74"/>
-      <c r="AE1" s="75"/>
-      <c r="AF1" s="73" t="s">
+      <c r="AC1" s="104"/>
+      <c r="AD1" s="104"/>
+      <c r="AE1" s="105"/>
+      <c r="AF1" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="AG1" s="74"/>
-      <c r="AH1" s="74"/>
-      <c r="AI1" s="75"/>
-      <c r="AJ1" s="73" t="s">
+      <c r="AG1" s="104"/>
+      <c r="AH1" s="104"/>
+      <c r="AI1" s="105"/>
+      <c r="AJ1" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="AK1" s="74"/>
-      <c r="AL1" s="74"/>
-      <c r="AM1" s="75"/>
-      <c r="AN1" s="73" t="s">
+      <c r="AK1" s="104"/>
+      <c r="AL1" s="104"/>
+      <c r="AM1" s="105"/>
+      <c r="AN1" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="AO1" s="74"/>
-      <c r="AP1" s="74"/>
-      <c r="AQ1" s="75"/>
-      <c r="AR1" s="73" t="s">
+      <c r="AO1" s="104"/>
+      <c r="AP1" s="104"/>
+      <c r="AQ1" s="105"/>
+      <c r="AR1" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="AS1" s="74"/>
-      <c r="AT1" s="74"/>
-      <c r="AU1" s="75"/>
-      <c r="AV1" s="73" t="s">
+      <c r="AS1" s="104"/>
+      <c r="AT1" s="104"/>
+      <c r="AU1" s="105"/>
+      <c r="AV1" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="AW1" s="74"/>
-      <c r="AX1" s="74"/>
-      <c r="AY1" s="75"/>
-      <c r="AZ1" s="104" t="s">
+      <c r="AW1" s="104"/>
+      <c r="AX1" s="104"/>
+      <c r="AY1" s="105"/>
+      <c r="AZ1" s="82" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A2" s="67"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="76">
+      <c r="A2" s="111"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="106">
         <v>44627</v>
       </c>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="76">
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="106">
         <v>44628</v>
       </c>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="76">
+      <c r="I2" s="107"/>
+      <c r="J2" s="107"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="106">
         <v>44629</v>
       </c>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="76">
+      <c r="M2" s="107"/>
+      <c r="N2" s="107"/>
+      <c r="O2" s="108"/>
+      <c r="P2" s="106">
         <v>44630</v>
       </c>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="77"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="76">
+      <c r="Q2" s="107"/>
+      <c r="R2" s="107"/>
+      <c r="S2" s="108"/>
+      <c r="T2" s="106">
         <v>44631</v>
       </c>
-      <c r="U2" s="77"/>
-      <c r="V2" s="77"/>
-      <c r="W2" s="78"/>
-      <c r="X2" s="76">
+      <c r="U2" s="107"/>
+      <c r="V2" s="107"/>
+      <c r="W2" s="108"/>
+      <c r="X2" s="106">
         <v>44634</v>
       </c>
-      <c r="Y2" s="77"/>
-      <c r="Z2" s="77"/>
-      <c r="AA2" s="78"/>
-      <c r="AB2" s="76">
+      <c r="Y2" s="107"/>
+      <c r="Z2" s="107"/>
+      <c r="AA2" s="108"/>
+      <c r="AB2" s="106">
         <v>44635</v>
       </c>
-      <c r="AC2" s="77"/>
-      <c r="AD2" s="77"/>
-      <c r="AE2" s="78"/>
-      <c r="AF2" s="76">
+      <c r="AC2" s="107"/>
+      <c r="AD2" s="107"/>
+      <c r="AE2" s="108"/>
+      <c r="AF2" s="106">
         <v>44636</v>
       </c>
-      <c r="AG2" s="77"/>
-      <c r="AH2" s="77"/>
-      <c r="AI2" s="78"/>
-      <c r="AJ2" s="76">
+      <c r="AG2" s="107"/>
+      <c r="AH2" s="107"/>
+      <c r="AI2" s="108"/>
+      <c r="AJ2" s="106">
         <v>44637</v>
       </c>
-      <c r="AK2" s="77"/>
-      <c r="AL2" s="77"/>
-      <c r="AM2" s="78"/>
-      <c r="AN2" s="76">
+      <c r="AK2" s="107"/>
+      <c r="AL2" s="107"/>
+      <c r="AM2" s="108"/>
+      <c r="AN2" s="106">
         <v>44638</v>
       </c>
-      <c r="AO2" s="77"/>
-      <c r="AP2" s="77"/>
-      <c r="AQ2" s="78"/>
-      <c r="AR2" s="76">
+      <c r="AO2" s="107"/>
+      <c r="AP2" s="107"/>
+      <c r="AQ2" s="108"/>
+      <c r="AR2" s="106">
         <v>44641</v>
       </c>
-      <c r="AS2" s="77"/>
-      <c r="AT2" s="77"/>
-      <c r="AU2" s="78"/>
-      <c r="AV2" s="76">
+      <c r="AS2" s="107"/>
+      <c r="AT2" s="107"/>
+      <c r="AU2" s="108"/>
+      <c r="AV2" s="106">
         <v>44642</v>
       </c>
-      <c r="AW2" s="77"/>
-      <c r="AX2" s="77"/>
-      <c r="AY2" s="78"/>
-      <c r="AZ2" s="105"/>
+      <c r="AW2" s="107"/>
+      <c r="AX2" s="107"/>
+      <c r="AY2" s="108"/>
+      <c r="AZ2" s="83"/>
     </row>
     <row r="3" spans="1:55" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68"/>
+      <c r="A3" s="112"/>
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
@@ -1967,16 +1967,16 @@
       <c r="AY3" s="12">
         <v>17</v>
       </c>
-      <c r="AZ3" s="106"/>
+      <c r="AZ3" s="109"/>
     </row>
     <row r="4" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="90">
+      <c r="B4" s="78">
         <v>4</v>
       </c>
-      <c r="C4" s="92">
+      <c r="C4" s="80">
         <v>2</v>
       </c>
       <c r="D4" s="15"/>
@@ -1995,12 +1995,12 @@
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
       <c r="S4" s="17"/>
-      <c r="T4" s="107" t="s">
+      <c r="T4" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="U4" s="108"/>
-      <c r="V4" s="108"/>
-      <c r="W4" s="98"/>
+      <c r="U4" s="68"/>
+      <c r="V4" s="68"/>
+      <c r="W4" s="69"/>
       <c r="X4" s="15"/>
       <c r="Y4" s="16"/>
       <c r="Z4" s="16"/>
@@ -2017,32 +2017,32 @@
       <c r="AK4" s="16"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="17"/>
-      <c r="AN4" s="107" t="s">
+      <c r="AN4" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="AO4" s="108"/>
-      <c r="AP4" s="108"/>
-      <c r="AQ4" s="98"/>
+      <c r="AO4" s="68"/>
+      <c r="AP4" s="68"/>
+      <c r="AQ4" s="69"/>
       <c r="AR4" s="15"/>
       <c r="AS4" s="16"/>
       <c r="AT4" s="16"/>
       <c r="AU4" s="17"/>
       <c r="AV4" s="15"/>
       <c r="AW4" s="16"/>
-      <c r="AX4" s="97" t="s">
+      <c r="AX4" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="AY4" s="98"/>
-      <c r="AZ4" s="104"/>
+      <c r="AY4" s="69"/>
+      <c r="AZ4" s="82"/>
       <c r="BB4" s="60" t="s">
         <v>50</v>
       </c>
       <c r="BC4" s="61"/>
     </row>
     <row r="5" spans="1:55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="112"/>
-      <c r="B5" s="113"/>
-      <c r="C5" s="114"/>
+      <c r="A5" s="96"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="98"/>
       <c r="D5" s="33"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -2059,10 +2059,10 @@
       <c r="Q5" s="32"/>
       <c r="R5" s="3"/>
       <c r="S5" s="12"/>
-      <c r="T5" s="109"/>
-      <c r="U5" s="101"/>
-      <c r="V5" s="101"/>
-      <c r="W5" s="100"/>
+      <c r="T5" s="70"/>
+      <c r="U5" s="71"/>
+      <c r="V5" s="71"/>
+      <c r="W5" s="72"/>
       <c r="X5" s="11"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="32"/>
@@ -2079,32 +2079,32 @@
       <c r="AK5" s="3"/>
       <c r="AL5" s="3"/>
       <c r="AM5" s="12"/>
-      <c r="AN5" s="109"/>
-      <c r="AO5" s="101"/>
-      <c r="AP5" s="101"/>
-      <c r="AQ5" s="100"/>
+      <c r="AN5" s="70"/>
+      <c r="AO5" s="71"/>
+      <c r="AP5" s="71"/>
+      <c r="AQ5" s="72"/>
       <c r="AR5" s="11"/>
       <c r="AS5" s="3"/>
       <c r="AT5" s="3"/>
       <c r="AU5" s="12"/>
       <c r="AV5" s="11"/>
       <c r="AW5" s="3"/>
-      <c r="AX5" s="99"/>
-      <c r="AY5" s="100"/>
-      <c r="AZ5" s="105"/>
+      <c r="AX5" s="101"/>
+      <c r="AY5" s="72"/>
+      <c r="AZ5" s="83"/>
       <c r="BB5" s="62" t="s">
         <v>51</v>
       </c>
       <c r="BC5" s="63"/>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A6" s="115" t="s">
+      <c r="A6" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="84">
+      <c r="B6" s="92">
         <v>32</v>
       </c>
-      <c r="C6" s="116"/>
+      <c r="C6" s="93"/>
       <c r="D6" s="13"/>
       <c r="E6" s="35"/>
       <c r="F6" s="30"/>
@@ -2121,10 +2121,10 @@
       <c r="Q6" s="24"/>
       <c r="R6" s="47"/>
       <c r="S6" s="48"/>
-      <c r="T6" s="109"/>
-      <c r="U6" s="101"/>
-      <c r="V6" s="101"/>
-      <c r="W6" s="100"/>
+      <c r="T6" s="70"/>
+      <c r="U6" s="71"/>
+      <c r="V6" s="71"/>
+      <c r="W6" s="72"/>
       <c r="X6" s="38"/>
       <c r="Y6" s="34"/>
       <c r="Z6" s="24"/>
@@ -2141,28 +2141,28 @@
       <c r="AK6" s="34"/>
       <c r="AL6" s="34"/>
       <c r="AM6" s="49"/>
-      <c r="AN6" s="109"/>
-      <c r="AO6" s="101"/>
-      <c r="AP6" s="101"/>
-      <c r="AQ6" s="100"/>
+      <c r="AN6" s="70"/>
+      <c r="AO6" s="71"/>
+      <c r="AP6" s="71"/>
+      <c r="AQ6" s="72"/>
       <c r="AR6" s="38"/>
       <c r="AS6" s="34"/>
       <c r="AT6" s="34"/>
       <c r="AU6" s="49"/>
       <c r="AV6" s="38"/>
       <c r="AW6" s="34"/>
-      <c r="AX6" s="99"/>
-      <c r="AY6" s="100"/>
-      <c r="AZ6" s="105"/>
+      <c r="AX6" s="101"/>
+      <c r="AY6" s="72"/>
+      <c r="AZ6" s="83"/>
       <c r="BB6" s="62" t="s">
         <v>52</v>
       </c>
       <c r="BC6" s="64"/>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A7" s="112"/>
-      <c r="B7" s="113"/>
-      <c r="C7" s="114"/>
+      <c r="A7" s="96"/>
+      <c r="B7" s="97"/>
+      <c r="C7" s="98"/>
       <c r="D7" s="33"/>
       <c r="E7" s="32"/>
       <c r="F7" s="3"/>
@@ -2174,15 +2174,15 @@
       <c r="L7" s="39"/>
       <c r="M7" s="40"/>
       <c r="N7" s="40"/>
-      <c r="O7" s="122"/>
+      <c r="O7" s="66"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="12"/>
-      <c r="T7" s="109"/>
-      <c r="U7" s="101"/>
-      <c r="V7" s="101"/>
-      <c r="W7" s="100"/>
+      <c r="T7" s="70"/>
+      <c r="U7" s="71"/>
+      <c r="V7" s="71"/>
+      <c r="W7" s="72"/>
       <c r="X7" s="33"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
@@ -2199,30 +2199,30 @@
       <c r="AK7" s="3"/>
       <c r="AL7" s="3"/>
       <c r="AM7" s="12"/>
-      <c r="AN7" s="109"/>
-      <c r="AO7" s="101"/>
-      <c r="AP7" s="101"/>
-      <c r="AQ7" s="100"/>
+      <c r="AN7" s="70"/>
+      <c r="AO7" s="71"/>
+      <c r="AP7" s="71"/>
+      <c r="AQ7" s="72"/>
       <c r="AR7" s="11"/>
       <c r="AS7" s="3"/>
       <c r="AT7" s="3"/>
       <c r="AU7" s="12"/>
       <c r="AV7" s="11"/>
       <c r="AW7" s="3"/>
-      <c r="AX7" s="99"/>
-      <c r="AY7" s="100"/>
-      <c r="AZ7" s="105"/>
+      <c r="AX7" s="101"/>
+      <c r="AY7" s="72"/>
+      <c r="AZ7" s="83"/>
       <c r="BB7" s="4"/>
       <c r="BC7" s="4"/>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A8" s="115" t="s">
+      <c r="A8" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="117">
+      <c r="B8" s="95">
         <v>4</v>
       </c>
-      <c r="C8" s="116">
+      <c r="C8" s="93">
         <v>5</v>
       </c>
       <c r="D8" s="26"/>
@@ -2241,10 +2241,10 @@
       <c r="Q8" s="30"/>
       <c r="R8" s="30"/>
       <c r="S8" s="29"/>
-      <c r="T8" s="109"/>
-      <c r="U8" s="101"/>
-      <c r="V8" s="101"/>
-      <c r="W8" s="100"/>
+      <c r="T8" s="70"/>
+      <c r="U8" s="71"/>
+      <c r="V8" s="71"/>
+      <c r="W8" s="72"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="30"/>
       <c r="Z8" s="30"/>
@@ -2261,26 +2261,26 @@
       <c r="AK8" s="30"/>
       <c r="AL8" s="30"/>
       <c r="AM8" s="29"/>
-      <c r="AN8" s="109"/>
-      <c r="AO8" s="101"/>
-      <c r="AP8" s="101"/>
-      <c r="AQ8" s="100"/>
+      <c r="AN8" s="70"/>
+      <c r="AO8" s="71"/>
+      <c r="AP8" s="71"/>
+      <c r="AQ8" s="72"/>
       <c r="AR8" s="28"/>
       <c r="AS8" s="30"/>
       <c r="AT8" s="30"/>
       <c r="AU8" s="29"/>
       <c r="AV8" s="28"/>
       <c r="AW8" s="30"/>
-      <c r="AX8" s="99"/>
-      <c r="AY8" s="100"/>
-      <c r="AZ8" s="105"/>
+      <c r="AX8" s="101"/>
+      <c r="AY8" s="72"/>
+      <c r="AZ8" s="83"/>
       <c r="BB8" s="4"/>
       <c r="BC8" s="4"/>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A9" s="89"/>
-      <c r="B9" s="91"/>
-      <c r="C9" s="114"/>
+      <c r="A9" s="88"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="98"/>
       <c r="D9" s="39"/>
       <c r="E9" s="40"/>
       <c r="F9" s="54"/>
@@ -2297,10 +2297,10 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="12"/>
-      <c r="T9" s="109"/>
-      <c r="U9" s="101"/>
-      <c r="V9" s="101"/>
-      <c r="W9" s="100"/>
+      <c r="T9" s="70"/>
+      <c r="U9" s="71"/>
+      <c r="V9" s="71"/>
+      <c r="W9" s="72"/>
       <c r="X9" s="11"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
@@ -2317,30 +2317,30 @@
       <c r="AK9" s="3"/>
       <c r="AL9" s="32"/>
       <c r="AM9" s="12"/>
-      <c r="AN9" s="109"/>
-      <c r="AO9" s="101"/>
-      <c r="AP9" s="101"/>
-      <c r="AQ9" s="100"/>
+      <c r="AN9" s="70"/>
+      <c r="AO9" s="71"/>
+      <c r="AP9" s="71"/>
+      <c r="AQ9" s="72"/>
       <c r="AR9" s="11"/>
       <c r="AS9" s="3"/>
       <c r="AT9" s="3"/>
       <c r="AU9" s="12"/>
       <c r="AV9" s="11"/>
       <c r="AW9" s="3"/>
-      <c r="AX9" s="99"/>
-      <c r="AY9" s="100"/>
-      <c r="AZ9" s="105"/>
+      <c r="AX9" s="101"/>
+      <c r="AY9" s="72"/>
+      <c r="AZ9" s="83"/>
       <c r="BB9" s="4"/>
       <c r="BC9" s="4"/>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="84">
+      <c r="B10" s="92">
         <v>2</v>
       </c>
-      <c r="C10" s="86">
+      <c r="C10" s="99">
         <v>1</v>
       </c>
       <c r="D10" s="28"/>
@@ -2359,10 +2359,10 @@
       <c r="Q10" s="30"/>
       <c r="R10" s="30"/>
       <c r="S10" s="29"/>
-      <c r="T10" s="109"/>
-      <c r="U10" s="101"/>
-      <c r="V10" s="101"/>
-      <c r="W10" s="100"/>
+      <c r="T10" s="70"/>
+      <c r="U10" s="71"/>
+      <c r="V10" s="71"/>
+      <c r="W10" s="72"/>
       <c r="X10" s="28"/>
       <c r="Y10" s="30"/>
       <c r="Z10" s="30"/>
@@ -2379,26 +2379,26 @@
       <c r="AK10" s="30"/>
       <c r="AL10" s="5"/>
       <c r="AM10" s="29"/>
-      <c r="AN10" s="109"/>
-      <c r="AO10" s="101"/>
-      <c r="AP10" s="101"/>
-      <c r="AQ10" s="100"/>
+      <c r="AN10" s="70"/>
+      <c r="AO10" s="71"/>
+      <c r="AP10" s="71"/>
+      <c r="AQ10" s="72"/>
       <c r="AR10" s="28"/>
       <c r="AS10" s="30"/>
       <c r="AT10" s="30"/>
       <c r="AU10" s="29"/>
       <c r="AV10" s="28"/>
       <c r="AW10" s="30"/>
-      <c r="AX10" s="99"/>
-      <c r="AY10" s="100"/>
-      <c r="AZ10" s="105"/>
+      <c r="AX10" s="101"/>
+      <c r="AY10" s="72"/>
+      <c r="AZ10" s="83"/>
       <c r="BB10" s="4"/>
       <c r="BC10" s="4"/>
     </row>
     <row r="11" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="83"/>
-      <c r="B11" s="85"/>
-      <c r="C11" s="87"/>
+      <c r="A11" s="77"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="81"/>
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
       <c r="F11" s="53"/>
@@ -2415,10 +2415,10 @@
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="109"/>
-      <c r="U11" s="101"/>
-      <c r="V11" s="101"/>
-      <c r="W11" s="100"/>
+      <c r="T11" s="70"/>
+      <c r="U11" s="71"/>
+      <c r="V11" s="71"/>
+      <c r="W11" s="72"/>
       <c r="X11" s="8"/>
       <c r="Y11" s="9"/>
       <c r="Z11" s="9"/>
@@ -2435,28 +2435,28 @@
       <c r="AK11" s="9"/>
       <c r="AL11" s="9"/>
       <c r="AM11" s="10"/>
-      <c r="AN11" s="109"/>
-      <c r="AO11" s="101"/>
-      <c r="AP11" s="101"/>
-      <c r="AQ11" s="100"/>
+      <c r="AN11" s="70"/>
+      <c r="AO11" s="71"/>
+      <c r="AP11" s="71"/>
+      <c r="AQ11" s="72"/>
       <c r="AR11" s="8"/>
       <c r="AS11" s="9"/>
       <c r="AT11" s="9"/>
       <c r="AU11" s="10"/>
       <c r="AV11" s="8"/>
       <c r="AW11" s="9"/>
-      <c r="AX11" s="99"/>
-      <c r="AY11" s="100"/>
-      <c r="AZ11" s="118"/>
+      <c r="AX11" s="101"/>
+      <c r="AY11" s="72"/>
+      <c r="AZ11" s="84"/>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="90">
+      <c r="B12" s="78">
         <v>1.5</v>
       </c>
-      <c r="C12" s="92"/>
+      <c r="C12" s="80"/>
       <c r="D12" s="18"/>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
@@ -2473,10 +2473,10 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
       <c r="S12" s="17"/>
-      <c r="T12" s="109"/>
-      <c r="U12" s="101"/>
-      <c r="V12" s="101"/>
-      <c r="W12" s="100"/>
+      <c r="T12" s="70"/>
+      <c r="U12" s="71"/>
+      <c r="V12" s="71"/>
+      <c r="W12" s="72"/>
       <c r="X12" s="15"/>
       <c r="Y12" s="16"/>
       <c r="Z12" s="16"/>
@@ -2493,26 +2493,26 @@
       <c r="AK12" s="16"/>
       <c r="AL12" s="16"/>
       <c r="AM12" s="17"/>
-      <c r="AN12" s="109"/>
-      <c r="AO12" s="101"/>
-      <c r="AP12" s="101"/>
-      <c r="AQ12" s="100"/>
+      <c r="AN12" s="70"/>
+      <c r="AO12" s="71"/>
+      <c r="AP12" s="71"/>
+      <c r="AQ12" s="72"/>
       <c r="AR12" s="15"/>
       <c r="AS12" s="16"/>
       <c r="AT12" s="16"/>
       <c r="AU12" s="17"/>
       <c r="AV12" s="15"/>
       <c r="AW12" s="16"/>
-      <c r="AX12" s="99"/>
-      <c r="AY12" s="100"/>
-      <c r="AZ12" s="94" t="s">
+      <c r="AX12" s="101"/>
+      <c r="AY12" s="72"/>
+      <c r="AZ12" s="85" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A13" s="89"/>
-      <c r="B13" s="91"/>
-      <c r="C13" s="93"/>
+      <c r="A13" s="88"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="90"/>
       <c r="D13" s="42"/>
       <c r="E13" s="41"/>
       <c r="F13" s="43"/>
@@ -2529,10 +2529,10 @@
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="12"/>
-      <c r="T13" s="109"/>
-      <c r="U13" s="101"/>
-      <c r="V13" s="101"/>
-      <c r="W13" s="100"/>
+      <c r="T13" s="70"/>
+      <c r="U13" s="71"/>
+      <c r="V13" s="71"/>
+      <c r="W13" s="72"/>
       <c r="X13" s="11"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
@@ -2549,28 +2549,28 @@
       <c r="AK13" s="32"/>
       <c r="AL13" s="32"/>
       <c r="AM13" s="31"/>
-      <c r="AN13" s="109"/>
-      <c r="AO13" s="101"/>
-      <c r="AP13" s="101"/>
-      <c r="AQ13" s="100"/>
+      <c r="AN13" s="70"/>
+      <c r="AO13" s="71"/>
+      <c r="AP13" s="71"/>
+      <c r="AQ13" s="72"/>
       <c r="AR13" s="33"/>
       <c r="AS13" s="32"/>
       <c r="AT13" s="32"/>
       <c r="AU13" s="31"/>
       <c r="AV13" s="33"/>
       <c r="AW13" s="32"/>
-      <c r="AX13" s="99"/>
-      <c r="AY13" s="100"/>
-      <c r="AZ13" s="95"/>
+      <c r="AX13" s="101"/>
+      <c r="AY13" s="72"/>
+      <c r="AZ13" s="86"/>
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A14" s="82" t="s">
+      <c r="A14" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="84">
+      <c r="B14" s="92">
         <v>1.5</v>
       </c>
-      <c r="C14" s="116"/>
+      <c r="C14" s="93"/>
       <c r="D14" s="28"/>
       <c r="E14" s="5"/>
       <c r="F14" s="30"/>
@@ -2587,10 +2587,10 @@
       <c r="Q14" s="30"/>
       <c r="R14" s="30"/>
       <c r="S14" s="29"/>
-      <c r="T14" s="109"/>
-      <c r="U14" s="101"/>
-      <c r="V14" s="101"/>
-      <c r="W14" s="100"/>
+      <c r="T14" s="70"/>
+      <c r="U14" s="71"/>
+      <c r="V14" s="71"/>
+      <c r="W14" s="72"/>
       <c r="X14" s="28"/>
       <c r="Y14" s="30"/>
       <c r="Z14" s="30"/>
@@ -2607,24 +2607,24 @@
       <c r="AK14" s="5"/>
       <c r="AL14" s="5"/>
       <c r="AM14" s="7"/>
-      <c r="AN14" s="109"/>
-      <c r="AO14" s="101"/>
-      <c r="AP14" s="101"/>
-      <c r="AQ14" s="100"/>
+      <c r="AN14" s="70"/>
+      <c r="AO14" s="71"/>
+      <c r="AP14" s="71"/>
+      <c r="AQ14" s="72"/>
       <c r="AR14" s="6"/>
       <c r="AS14" s="5"/>
       <c r="AT14" s="5"/>
       <c r="AU14" s="7"/>
       <c r="AV14" s="6"/>
       <c r="AW14" s="5"/>
-      <c r="AX14" s="99"/>
-      <c r="AY14" s="100"/>
-      <c r="AZ14" s="95"/>
+      <c r="AX14" s="101"/>
+      <c r="AY14" s="72"/>
+      <c r="AZ14" s="86"/>
     </row>
     <row r="15" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="83"/>
-      <c r="B15" s="85"/>
-      <c r="C15" s="87"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="81"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -2641,10 +2641,10 @@
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="109"/>
-      <c r="U15" s="101"/>
-      <c r="V15" s="101"/>
-      <c r="W15" s="100"/>
+      <c r="T15" s="70"/>
+      <c r="U15" s="71"/>
+      <c r="V15" s="71"/>
+      <c r="W15" s="72"/>
       <c r="X15" s="8"/>
       <c r="Y15" s="9"/>
       <c r="Z15" s="9"/>
@@ -2661,28 +2661,28 @@
       <c r="AK15" s="9"/>
       <c r="AL15" s="9"/>
       <c r="AM15" s="10"/>
-      <c r="AN15" s="109"/>
-      <c r="AO15" s="101"/>
-      <c r="AP15" s="101"/>
-      <c r="AQ15" s="100"/>
+      <c r="AN15" s="70"/>
+      <c r="AO15" s="71"/>
+      <c r="AP15" s="71"/>
+      <c r="AQ15" s="72"/>
       <c r="AR15" s="8"/>
       <c r="AS15" s="9"/>
       <c r="AT15" s="9"/>
       <c r="AU15" s="10"/>
       <c r="AV15" s="8"/>
       <c r="AW15" s="9"/>
-      <c r="AX15" s="99"/>
-      <c r="AY15" s="100"/>
-      <c r="AZ15" s="96"/>
+      <c r="AX15" s="101"/>
+      <c r="AY15" s="72"/>
+      <c r="AZ15" s="87"/>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="90">
+      <c r="B16" s="78">
         <v>1</v>
       </c>
-      <c r="C16" s="92"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="15"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
@@ -2699,10 +2699,10 @@
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
       <c r="S16" s="17"/>
-      <c r="T16" s="109"/>
-      <c r="U16" s="101"/>
-      <c r="V16" s="101"/>
-      <c r="W16" s="100"/>
+      <c r="T16" s="70"/>
+      <c r="U16" s="71"/>
+      <c r="V16" s="71"/>
+      <c r="W16" s="72"/>
       <c r="X16" s="15"/>
       <c r="Y16" s="16"/>
       <c r="Z16" s="16"/>
@@ -2719,26 +2719,26 @@
       <c r="AK16" s="16"/>
       <c r="AL16" s="16"/>
       <c r="AM16" s="17"/>
-      <c r="AN16" s="109"/>
-      <c r="AO16" s="101"/>
-      <c r="AP16" s="101"/>
-      <c r="AQ16" s="100"/>
+      <c r="AN16" s="70"/>
+      <c r="AO16" s="71"/>
+      <c r="AP16" s="71"/>
+      <c r="AQ16" s="72"/>
       <c r="AR16" s="15"/>
       <c r="AS16" s="16"/>
       <c r="AT16" s="16"/>
       <c r="AU16" s="17"/>
       <c r="AV16" s="15"/>
       <c r="AW16" s="16"/>
-      <c r="AX16" s="99"/>
-      <c r="AY16" s="100"/>
-      <c r="AZ16" s="94" t="s">
+      <c r="AX16" s="101"/>
+      <c r="AY16" s="72"/>
+      <c r="AZ16" s="85" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A17" s="112"/>
-      <c r="B17" s="91"/>
-      <c r="C17" s="93"/>
+      <c r="A17" s="96"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="90"/>
       <c r="D17" s="11"/>
       <c r="E17" s="3"/>
       <c r="F17" s="32"/>
@@ -2755,10 +2755,10 @@
       <c r="Q17" s="3"/>
       <c r="R17" s="32"/>
       <c r="S17" s="12"/>
-      <c r="T17" s="109"/>
-      <c r="U17" s="101"/>
-      <c r="V17" s="101"/>
-      <c r="W17" s="100"/>
+      <c r="T17" s="70"/>
+      <c r="U17" s="71"/>
+      <c r="V17" s="71"/>
+      <c r="W17" s="72"/>
       <c r="X17" s="33"/>
       <c r="Y17" s="32"/>
       <c r="Z17" s="32"/>
@@ -2775,28 +2775,28 @@
       <c r="AK17" s="32"/>
       <c r="AL17" s="32"/>
       <c r="AM17" s="31"/>
-      <c r="AN17" s="109"/>
-      <c r="AO17" s="101"/>
-      <c r="AP17" s="101"/>
-      <c r="AQ17" s="100"/>
+      <c r="AN17" s="70"/>
+      <c r="AO17" s="71"/>
+      <c r="AP17" s="71"/>
+      <c r="AQ17" s="72"/>
       <c r="AR17" s="33"/>
       <c r="AS17" s="32"/>
       <c r="AT17" s="32"/>
       <c r="AU17" s="31"/>
       <c r="AV17" s="33"/>
       <c r="AW17" s="3"/>
-      <c r="AX17" s="99"/>
-      <c r="AY17" s="100"/>
-      <c r="AZ17" s="95"/>
+      <c r="AX17" s="101"/>
+      <c r="AY17" s="72"/>
+      <c r="AZ17" s="86"/>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A18" s="115" t="s">
+      <c r="A18" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="84">
+      <c r="B18" s="92">
         <v>2</v>
       </c>
-      <c r="C18" s="116"/>
+      <c r="C18" s="93"/>
       <c r="D18" s="28"/>
       <c r="E18" s="30"/>
       <c r="F18" s="5"/>
@@ -2813,10 +2813,10 @@
       <c r="Q18" s="30"/>
       <c r="R18" s="5"/>
       <c r="S18" s="29"/>
-      <c r="T18" s="109"/>
-      <c r="U18" s="101"/>
-      <c r="V18" s="101"/>
-      <c r="W18" s="100"/>
+      <c r="T18" s="70"/>
+      <c r="U18" s="71"/>
+      <c r="V18" s="71"/>
+      <c r="W18" s="72"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
@@ -2833,24 +2833,24 @@
       <c r="AK18" s="5"/>
       <c r="AL18" s="5"/>
       <c r="AM18" s="7"/>
-      <c r="AN18" s="109"/>
-      <c r="AO18" s="101"/>
-      <c r="AP18" s="101"/>
-      <c r="AQ18" s="100"/>
+      <c r="AN18" s="70"/>
+      <c r="AO18" s="71"/>
+      <c r="AP18" s="71"/>
+      <c r="AQ18" s="72"/>
       <c r="AR18" s="6"/>
       <c r="AS18" s="5"/>
       <c r="AT18" s="5"/>
       <c r="AU18" s="7"/>
       <c r="AV18" s="6"/>
       <c r="AW18" s="30"/>
-      <c r="AX18" s="99"/>
-      <c r="AY18" s="100"/>
-      <c r="AZ18" s="95"/>
+      <c r="AX18" s="101"/>
+      <c r="AY18" s="72"/>
+      <c r="AZ18" s="86"/>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A19" s="89"/>
-      <c r="B19" s="91"/>
-      <c r="C19" s="93"/>
+      <c r="A19" s="88"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="90"/>
       <c r="D19" s="11"/>
       <c r="E19" s="3"/>
       <c r="F19" s="32"/>
@@ -2867,10 +2867,10 @@
       <c r="Q19" s="32"/>
       <c r="R19" s="3"/>
       <c r="S19" s="31"/>
-      <c r="T19" s="109"/>
-      <c r="U19" s="101"/>
-      <c r="V19" s="101"/>
-      <c r="W19" s="100"/>
+      <c r="T19" s="70"/>
+      <c r="U19" s="71"/>
+      <c r="V19" s="71"/>
+      <c r="W19" s="72"/>
       <c r="X19" s="33"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
@@ -2887,28 +2887,28 @@
       <c r="AK19" s="32"/>
       <c r="AL19" s="32"/>
       <c r="AM19" s="31"/>
-      <c r="AN19" s="109"/>
-      <c r="AO19" s="101"/>
-      <c r="AP19" s="101"/>
-      <c r="AQ19" s="100"/>
+      <c r="AN19" s="70"/>
+      <c r="AO19" s="71"/>
+      <c r="AP19" s="71"/>
+      <c r="AQ19" s="72"/>
       <c r="AR19" s="33"/>
       <c r="AS19" s="3"/>
       <c r="AT19" s="32"/>
       <c r="AU19" s="31"/>
       <c r="AV19" s="33"/>
       <c r="AW19" s="32"/>
-      <c r="AX19" s="99"/>
-      <c r="AY19" s="100"/>
-      <c r="AZ19" s="95"/>
+      <c r="AX19" s="101"/>
+      <c r="AY19" s="72"/>
+      <c r="AZ19" s="86"/>
     </row>
     <row r="20" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A20" s="115" t="s">
+      <c r="A20" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="84">
+      <c r="B20" s="92">
         <v>0.5</v>
       </c>
-      <c r="C20" s="116"/>
+      <c r="C20" s="93"/>
       <c r="D20" s="28"/>
       <c r="E20" s="30"/>
       <c r="F20" s="5"/>
@@ -2918,17 +2918,17 @@
       <c r="J20" s="5"/>
       <c r="K20" s="7"/>
       <c r="L20" s="6"/>
-      <c r="M20" s="119"/>
+      <c r="M20" s="24"/>
       <c r="N20" s="5"/>
       <c r="O20" s="7"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="30"/>
       <c r="S20" s="7"/>
-      <c r="T20" s="109"/>
-      <c r="U20" s="101"/>
-      <c r="V20" s="101"/>
-      <c r="W20" s="100"/>
+      <c r="T20" s="70"/>
+      <c r="U20" s="71"/>
+      <c r="V20" s="71"/>
+      <c r="W20" s="72"/>
       <c r="X20" s="6"/>
       <c r="Y20" s="30"/>
       <c r="Z20" s="30"/>
@@ -2945,24 +2945,24 @@
       <c r="AK20" s="5"/>
       <c r="AL20" s="5"/>
       <c r="AM20" s="7"/>
-      <c r="AN20" s="109"/>
-      <c r="AO20" s="101"/>
-      <c r="AP20" s="101"/>
-      <c r="AQ20" s="100"/>
+      <c r="AN20" s="70"/>
+      <c r="AO20" s="71"/>
+      <c r="AP20" s="71"/>
+      <c r="AQ20" s="72"/>
       <c r="AR20" s="6"/>
       <c r="AS20" s="30"/>
       <c r="AT20" s="5"/>
       <c r="AU20" s="7"/>
       <c r="AV20" s="6"/>
       <c r="AW20" s="5"/>
-      <c r="AX20" s="99"/>
-      <c r="AY20" s="100"/>
-      <c r="AZ20" s="95"/>
+      <c r="AX20" s="101"/>
+      <c r="AY20" s="72"/>
+      <c r="AZ20" s="86"/>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A21" s="89"/>
-      <c r="B21" s="91"/>
-      <c r="C21" s="93"/>
+      <c r="A21" s="88"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="90"/>
       <c r="D21" s="33"/>
       <c r="E21" s="32"/>
       <c r="F21" s="32"/>
@@ -2972,17 +2972,17 @@
       <c r="J21" s="32"/>
       <c r="K21" s="31"/>
       <c r="L21" s="33"/>
-      <c r="M21" s="32"/>
+      <c r="M21" s="54"/>
       <c r="N21" s="32"/>
       <c r="O21" s="31"/>
       <c r="P21" s="33"/>
       <c r="Q21" s="32"/>
       <c r="R21" s="32"/>
       <c r="S21" s="31"/>
-      <c r="T21" s="109"/>
-      <c r="U21" s="101"/>
-      <c r="V21" s="101"/>
-      <c r="W21" s="100"/>
+      <c r="T21" s="70"/>
+      <c r="U21" s="71"/>
+      <c r="V21" s="71"/>
+      <c r="W21" s="72"/>
       <c r="X21" s="33"/>
       <c r="Y21" s="32"/>
       <c r="Z21" s="32"/>
@@ -2999,28 +2999,28 @@
       <c r="AK21" s="32"/>
       <c r="AL21" s="32"/>
       <c r="AM21" s="31"/>
-      <c r="AN21" s="109"/>
-      <c r="AO21" s="101"/>
-      <c r="AP21" s="101"/>
-      <c r="AQ21" s="100"/>
+      <c r="AN21" s="70"/>
+      <c r="AO21" s="71"/>
+      <c r="AP21" s="71"/>
+      <c r="AQ21" s="72"/>
       <c r="AR21" s="33"/>
       <c r="AS21" s="32"/>
       <c r="AT21" s="32"/>
       <c r="AU21" s="31"/>
       <c r="AV21" s="33"/>
       <c r="AW21" s="32"/>
-      <c r="AX21" s="99"/>
-      <c r="AY21" s="100"/>
-      <c r="AZ21" s="95"/>
+      <c r="AX21" s="101"/>
+      <c r="AY21" s="72"/>
+      <c r="AZ21" s="86"/>
     </row>
     <row r="22" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A22" s="115" t="s">
+      <c r="A22" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="84">
+      <c r="B22" s="92">
         <v>1</v>
       </c>
-      <c r="C22" s="116"/>
+      <c r="C22" s="93"/>
       <c r="D22" s="6"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -3030,17 +3030,17 @@
       <c r="J22" s="5"/>
       <c r="K22" s="7"/>
       <c r="L22" s="6"/>
-      <c r="M22" s="119"/>
+      <c r="M22" s="24"/>
       <c r="N22" s="5"/>
       <c r="O22" s="7"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
       <c r="S22" s="7"/>
-      <c r="T22" s="109"/>
-      <c r="U22" s="101"/>
-      <c r="V22" s="101"/>
-      <c r="W22" s="100"/>
+      <c r="T22" s="70"/>
+      <c r="U22" s="71"/>
+      <c r="V22" s="71"/>
+      <c r="W22" s="72"/>
       <c r="X22" s="6"/>
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
@@ -3057,24 +3057,24 @@
       <c r="AK22" s="5"/>
       <c r="AL22" s="5"/>
       <c r="AM22" s="7"/>
-      <c r="AN22" s="109"/>
-      <c r="AO22" s="101"/>
-      <c r="AP22" s="101"/>
-      <c r="AQ22" s="100"/>
+      <c r="AN22" s="70"/>
+      <c r="AO22" s="71"/>
+      <c r="AP22" s="71"/>
+      <c r="AQ22" s="72"/>
       <c r="AR22" s="6"/>
       <c r="AS22" s="5"/>
       <c r="AT22" s="5"/>
       <c r="AU22" s="7"/>
       <c r="AV22" s="6"/>
       <c r="AW22" s="5"/>
-      <c r="AX22" s="99"/>
-      <c r="AY22" s="100"/>
-      <c r="AZ22" s="95"/>
+      <c r="AX22" s="101"/>
+      <c r="AY22" s="72"/>
+      <c r="AZ22" s="86"/>
     </row>
     <row r="23" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A23" s="89"/>
-      <c r="B23" s="91"/>
-      <c r="C23" s="93"/>
+      <c r="A23" s="88"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="90"/>
       <c r="D23" s="11"/>
       <c r="E23" s="3"/>
       <c r="F23" s="32"/>
@@ -3084,17 +3084,17 @@
       <c r="J23" s="32"/>
       <c r="K23" s="31"/>
       <c r="L23" s="33"/>
-      <c r="M23" s="32"/>
+      <c r="M23" s="54"/>
       <c r="N23" s="32"/>
       <c r="O23" s="31"/>
       <c r="P23" s="33"/>
       <c r="Q23" s="32"/>
       <c r="R23" s="32"/>
       <c r="S23" s="31"/>
-      <c r="T23" s="109"/>
-      <c r="U23" s="101"/>
-      <c r="V23" s="101"/>
-      <c r="W23" s="100"/>
+      <c r="T23" s="70"/>
+      <c r="U23" s="71"/>
+      <c r="V23" s="71"/>
+      <c r="W23" s="72"/>
       <c r="X23" s="33"/>
       <c r="Y23" s="32"/>
       <c r="Z23" s="32"/>
@@ -3111,28 +3111,28 @@
       <c r="AK23" s="3"/>
       <c r="AL23" s="3"/>
       <c r="AM23" s="12"/>
-      <c r="AN23" s="109"/>
-      <c r="AO23" s="101"/>
-      <c r="AP23" s="101"/>
-      <c r="AQ23" s="100"/>
+      <c r="AN23" s="70"/>
+      <c r="AO23" s="71"/>
+      <c r="AP23" s="71"/>
+      <c r="AQ23" s="72"/>
       <c r="AR23" s="11"/>
       <c r="AS23" s="3"/>
       <c r="AT23" s="32"/>
       <c r="AU23" s="31"/>
       <c r="AV23" s="33"/>
       <c r="AW23" s="3"/>
-      <c r="AX23" s="99"/>
-      <c r="AY23" s="100"/>
-      <c r="AZ23" s="95"/>
+      <c r="AX23" s="101"/>
+      <c r="AY23" s="72"/>
+      <c r="AZ23" s="86"/>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A24" s="115" t="s">
+      <c r="A24" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="84">
+      <c r="B24" s="92">
         <v>1</v>
       </c>
-      <c r="C24" s="116"/>
+      <c r="C24" s="93"/>
       <c r="D24" s="28"/>
       <c r="E24" s="30"/>
       <c r="F24" s="5"/>
@@ -3142,17 +3142,17 @@
       <c r="J24" s="5"/>
       <c r="K24" s="7"/>
       <c r="L24" s="6"/>
-      <c r="M24" s="120"/>
-      <c r="N24" s="119"/>
+      <c r="M24" s="55"/>
+      <c r="N24" s="24"/>
       <c r="O24" s="7"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
       <c r="S24" s="7"/>
-      <c r="T24" s="109"/>
-      <c r="U24" s="101"/>
-      <c r="V24" s="101"/>
-      <c r="W24" s="100"/>
+      <c r="T24" s="70"/>
+      <c r="U24" s="71"/>
+      <c r="V24" s="71"/>
+      <c r="W24" s="72"/>
       <c r="X24" s="6"/>
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
@@ -3169,24 +3169,24 @@
       <c r="AK24" s="30"/>
       <c r="AL24" s="30"/>
       <c r="AM24" s="29"/>
-      <c r="AN24" s="109"/>
-      <c r="AO24" s="101"/>
-      <c r="AP24" s="101"/>
-      <c r="AQ24" s="100"/>
+      <c r="AN24" s="70"/>
+      <c r="AO24" s="71"/>
+      <c r="AP24" s="71"/>
+      <c r="AQ24" s="72"/>
       <c r="AR24" s="28"/>
       <c r="AS24" s="30"/>
       <c r="AT24" s="5"/>
       <c r="AU24" s="7"/>
       <c r="AV24" s="6"/>
       <c r="AW24" s="30"/>
-      <c r="AX24" s="99"/>
-      <c r="AY24" s="100"/>
-      <c r="AZ24" s="95"/>
+      <c r="AX24" s="101"/>
+      <c r="AY24" s="72"/>
+      <c r="AZ24" s="86"/>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A25" s="89"/>
-      <c r="B25" s="113"/>
-      <c r="C25" s="114"/>
+      <c r="A25" s="88"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="98"/>
       <c r="D25" s="33"/>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
@@ -3196,17 +3196,17 @@
       <c r="J25" s="3"/>
       <c r="K25" s="31"/>
       <c r="L25" s="33"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
       <c r="O25" s="31"/>
       <c r="P25" s="11"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="31"/>
-      <c r="T25" s="109"/>
-      <c r="U25" s="101"/>
-      <c r="V25" s="101"/>
-      <c r="W25" s="100"/>
+      <c r="T25" s="70"/>
+      <c r="U25" s="71"/>
+      <c r="V25" s="71"/>
+      <c r="W25" s="72"/>
       <c r="X25" s="33"/>
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
@@ -3223,28 +3223,28 @@
       <c r="AK25" s="3"/>
       <c r="AL25" s="3"/>
       <c r="AM25" s="12"/>
-      <c r="AN25" s="109"/>
-      <c r="AO25" s="101"/>
-      <c r="AP25" s="101"/>
-      <c r="AQ25" s="100"/>
+      <c r="AN25" s="70"/>
+      <c r="AO25" s="71"/>
+      <c r="AP25" s="71"/>
+      <c r="AQ25" s="72"/>
       <c r="AR25" s="11"/>
       <c r="AS25" s="3"/>
       <c r="AT25" s="3"/>
       <c r="AU25" s="12"/>
       <c r="AV25" s="11"/>
       <c r="AW25" s="3"/>
-      <c r="AX25" s="99"/>
-      <c r="AY25" s="100"/>
-      <c r="AZ25" s="95"/>
+      <c r="AX25" s="101"/>
+      <c r="AY25" s="72"/>
+      <c r="AZ25" s="86"/>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A26" s="82" t="s">
+      <c r="A26" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="117">
+      <c r="B26" s="95">
         <v>2</v>
       </c>
-      <c r="C26" s="86"/>
+      <c r="C26" s="99"/>
       <c r="D26" s="6"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -3261,10 +3261,10 @@
       <c r="Q26" s="30"/>
       <c r="R26" s="30"/>
       <c r="S26" s="7"/>
-      <c r="T26" s="109"/>
-      <c r="U26" s="101"/>
-      <c r="V26" s="101"/>
-      <c r="W26" s="100"/>
+      <c r="T26" s="70"/>
+      <c r="U26" s="71"/>
+      <c r="V26" s="71"/>
+      <c r="W26" s="72"/>
       <c r="X26" s="6"/>
       <c r="Y26" s="30"/>
       <c r="Z26" s="30"/>
@@ -3281,24 +3281,24 @@
       <c r="AK26" s="30"/>
       <c r="AL26" s="30"/>
       <c r="AM26" s="29"/>
-      <c r="AN26" s="109"/>
-      <c r="AO26" s="101"/>
-      <c r="AP26" s="101"/>
-      <c r="AQ26" s="100"/>
+      <c r="AN26" s="70"/>
+      <c r="AO26" s="71"/>
+      <c r="AP26" s="71"/>
+      <c r="AQ26" s="72"/>
       <c r="AR26" s="28"/>
       <c r="AS26" s="30"/>
       <c r="AT26" s="30"/>
       <c r="AU26" s="29"/>
       <c r="AV26" s="28"/>
       <c r="AW26" s="30"/>
-      <c r="AX26" s="99"/>
-      <c r="AY26" s="100"/>
-      <c r="AZ26" s="95"/>
+      <c r="AX26" s="101"/>
+      <c r="AY26" s="72"/>
+      <c r="AZ26" s="86"/>
     </row>
     <row r="27" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="83"/>
-      <c r="B27" s="85"/>
-      <c r="C27" s="87"/>
+      <c r="A27" s="77"/>
+      <c r="B27" s="79"/>
+      <c r="C27" s="81"/>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
@@ -3310,15 +3310,15 @@
       <c r="L27" s="8"/>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
-      <c r="O27" s="10"/>
+      <c r="O27" s="120"/>
       <c r="P27" s="8"/>
       <c r="Q27" s="9"/>
       <c r="R27" s="9"/>
       <c r="S27" s="10"/>
-      <c r="T27" s="109"/>
-      <c r="U27" s="101"/>
-      <c r="V27" s="101"/>
-      <c r="W27" s="100"/>
+      <c r="T27" s="70"/>
+      <c r="U27" s="71"/>
+      <c r="V27" s="71"/>
+      <c r="W27" s="72"/>
       <c r="X27" s="8"/>
       <c r="Y27" s="9"/>
       <c r="Z27" s="9"/>
@@ -3335,28 +3335,28 @@
       <c r="AK27" s="9"/>
       <c r="AL27" s="9"/>
       <c r="AM27" s="10"/>
-      <c r="AN27" s="109"/>
-      <c r="AO27" s="101"/>
-      <c r="AP27" s="101"/>
-      <c r="AQ27" s="100"/>
+      <c r="AN27" s="70"/>
+      <c r="AO27" s="71"/>
+      <c r="AP27" s="71"/>
+      <c r="AQ27" s="72"/>
       <c r="AR27" s="8"/>
       <c r="AS27" s="9"/>
       <c r="AT27" s="9"/>
       <c r="AU27" s="10"/>
       <c r="AV27" s="8"/>
       <c r="AW27" s="9"/>
-      <c r="AX27" s="99"/>
-      <c r="AY27" s="100"/>
-      <c r="AZ27" s="96"/>
+      <c r="AX27" s="101"/>
+      <c r="AY27" s="72"/>
+      <c r="AZ27" s="87"/>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A28" s="88" t="s">
+      <c r="A28" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="90">
+      <c r="B28" s="78">
         <v>0.5</v>
       </c>
-      <c r="C28" s="92"/>
+      <c r="C28" s="80"/>
       <c r="D28" s="15"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
@@ -3373,10 +3373,10 @@
       <c r="Q28" s="16"/>
       <c r="R28" s="16"/>
       <c r="S28" s="17"/>
-      <c r="T28" s="109"/>
-      <c r="U28" s="101"/>
-      <c r="V28" s="101"/>
-      <c r="W28" s="100"/>
+      <c r="T28" s="70"/>
+      <c r="U28" s="71"/>
+      <c r="V28" s="71"/>
+      <c r="W28" s="72"/>
       <c r="X28" s="15"/>
       <c r="Y28" s="16"/>
       <c r="Z28" s="16"/>
@@ -3393,26 +3393,26 @@
       <c r="AK28" s="16"/>
       <c r="AL28" s="16"/>
       <c r="AM28" s="17"/>
-      <c r="AN28" s="109"/>
-      <c r="AO28" s="101"/>
-      <c r="AP28" s="101"/>
-      <c r="AQ28" s="100"/>
+      <c r="AN28" s="70"/>
+      <c r="AO28" s="71"/>
+      <c r="AP28" s="71"/>
+      <c r="AQ28" s="72"/>
       <c r="AR28" s="15"/>
       <c r="AS28" s="16"/>
       <c r="AT28" s="16"/>
       <c r="AU28" s="17"/>
       <c r="AV28" s="15"/>
       <c r="AW28" s="17"/>
-      <c r="AX28" s="101"/>
-      <c r="AY28" s="100"/>
-      <c r="AZ28" s="79" t="s">
+      <c r="AX28" s="71"/>
+      <c r="AY28" s="72"/>
+      <c r="AZ28" s="117" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="83"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="87"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="79"/>
+      <c r="C29" s="81"/>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
@@ -3425,14 +3425,14 @@
       <c r="M29" s="9"/>
       <c r="N29" s="50"/>
       <c r="O29" s="51"/>
-      <c r="P29" s="8"/>
+      <c r="P29" s="122"/>
       <c r="Q29" s="9"/>
       <c r="R29" s="9"/>
       <c r="S29" s="10"/>
-      <c r="T29" s="109"/>
-      <c r="U29" s="101"/>
-      <c r="V29" s="101"/>
-      <c r="W29" s="100"/>
+      <c r="T29" s="70"/>
+      <c r="U29" s="71"/>
+      <c r="V29" s="71"/>
+      <c r="W29" s="72"/>
       <c r="X29" s="8"/>
       <c r="Y29" s="9"/>
       <c r="Z29" s="9"/>
@@ -3449,28 +3449,28 @@
       <c r="AK29" s="9"/>
       <c r="AL29" s="9"/>
       <c r="AM29" s="10"/>
-      <c r="AN29" s="109"/>
-      <c r="AO29" s="101"/>
-      <c r="AP29" s="101"/>
-      <c r="AQ29" s="100"/>
+      <c r="AN29" s="70"/>
+      <c r="AO29" s="71"/>
+      <c r="AP29" s="71"/>
+      <c r="AQ29" s="72"/>
       <c r="AR29" s="8"/>
       <c r="AS29" s="9"/>
       <c r="AT29" s="9"/>
       <c r="AU29" s="10"/>
       <c r="AV29" s="8"/>
       <c r="AW29" s="10"/>
-      <c r="AX29" s="101"/>
-      <c r="AY29" s="100"/>
-      <c r="AZ29" s="80"/>
+      <c r="AX29" s="71"/>
+      <c r="AY29" s="72"/>
+      <c r="AZ29" s="118"/>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A30" s="82" t="s">
+      <c r="A30" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="117">
+      <c r="B30" s="95">
         <v>0.5</v>
       </c>
-      <c r="C30" s="86"/>
+      <c r="C30" s="99"/>
       <c r="D30" s="6"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -3487,10 +3487,10 @@
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
       <c r="S30" s="7"/>
-      <c r="T30" s="109"/>
-      <c r="U30" s="101"/>
-      <c r="V30" s="101"/>
-      <c r="W30" s="100"/>
+      <c r="T30" s="70"/>
+      <c r="U30" s="71"/>
+      <c r="V30" s="71"/>
+      <c r="W30" s="72"/>
       <c r="X30" s="6"/>
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
@@ -3507,26 +3507,26 @@
       <c r="AK30" s="5"/>
       <c r="AL30" s="5"/>
       <c r="AM30" s="7"/>
-      <c r="AN30" s="109"/>
-      <c r="AO30" s="101"/>
-      <c r="AP30" s="101"/>
-      <c r="AQ30" s="100"/>
+      <c r="AN30" s="70"/>
+      <c r="AO30" s="71"/>
+      <c r="AP30" s="71"/>
+      <c r="AQ30" s="72"/>
       <c r="AR30" s="6"/>
       <c r="AS30" s="5"/>
       <c r="AT30" s="5"/>
       <c r="AU30" s="7"/>
       <c r="AV30" s="6"/>
       <c r="AW30" s="5"/>
-      <c r="AX30" s="99"/>
-      <c r="AY30" s="100"/>
-      <c r="AZ30" s="79" t="s">
+      <c r="AX30" s="101"/>
+      <c r="AY30" s="72"/>
+      <c r="AZ30" s="117" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A31" s="89"/>
-      <c r="B31" s="91"/>
-      <c r="C31" s="93"/>
+      <c r="A31" s="88"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="90"/>
       <c r="D31" s="11"/>
       <c r="E31" s="32"/>
       <c r="F31" s="3"/>
@@ -3536,17 +3536,17 @@
       <c r="J31" s="32"/>
       <c r="K31" s="12"/>
       <c r="L31" s="11"/>
-      <c r="M31" s="3"/>
+      <c r="M31" s="40"/>
       <c r="N31" s="3"/>
       <c r="O31" s="12"/>
       <c r="P31" s="11"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
       <c r="S31" s="31"/>
-      <c r="T31" s="109"/>
-      <c r="U31" s="101"/>
-      <c r="V31" s="101"/>
-      <c r="W31" s="100"/>
+      <c r="T31" s="70"/>
+      <c r="U31" s="71"/>
+      <c r="V31" s="71"/>
+      <c r="W31" s="72"/>
       <c r="X31" s="33"/>
       <c r="Y31" s="32"/>
       <c r="Z31" s="32"/>
@@ -3563,28 +3563,28 @@
       <c r="AK31" s="32"/>
       <c r="AL31" s="32"/>
       <c r="AM31" s="31"/>
-      <c r="AN31" s="109"/>
-      <c r="AO31" s="101"/>
-      <c r="AP31" s="101"/>
-      <c r="AQ31" s="100"/>
+      <c r="AN31" s="70"/>
+      <c r="AO31" s="71"/>
+      <c r="AP31" s="71"/>
+      <c r="AQ31" s="72"/>
       <c r="AR31" s="33"/>
       <c r="AS31" s="32"/>
       <c r="AT31" s="32"/>
       <c r="AU31" s="31"/>
       <c r="AV31" s="33"/>
       <c r="AW31" s="32"/>
-      <c r="AX31" s="99"/>
-      <c r="AY31" s="100"/>
-      <c r="AZ31" s="81"/>
+      <c r="AX31" s="101"/>
+      <c r="AY31" s="72"/>
+      <c r="AZ31" s="119"/>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A32" s="115" t="s">
+      <c r="A32" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="84">
+      <c r="B32" s="92">
         <v>1</v>
       </c>
-      <c r="C32" s="116"/>
+      <c r="C32" s="93"/>
       <c r="D32" s="28"/>
       <c r="E32" s="5"/>
       <c r="F32" s="30"/>
@@ -3601,10 +3601,10 @@
       <c r="Q32" s="34"/>
       <c r="R32" s="30"/>
       <c r="S32" s="7"/>
-      <c r="T32" s="109"/>
-      <c r="U32" s="101"/>
-      <c r="V32" s="101"/>
-      <c r="W32" s="100"/>
+      <c r="T32" s="70"/>
+      <c r="U32" s="71"/>
+      <c r="V32" s="71"/>
+      <c r="W32" s="72"/>
       <c r="X32" s="6"/>
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
@@ -3621,24 +3621,24 @@
       <c r="AK32" s="5"/>
       <c r="AL32" s="5"/>
       <c r="AM32" s="7"/>
-      <c r="AN32" s="109"/>
-      <c r="AO32" s="101"/>
-      <c r="AP32" s="101"/>
-      <c r="AQ32" s="100"/>
+      <c r="AN32" s="70"/>
+      <c r="AO32" s="71"/>
+      <c r="AP32" s="71"/>
+      <c r="AQ32" s="72"/>
       <c r="AR32" s="6"/>
       <c r="AS32" s="5"/>
       <c r="AT32" s="5"/>
       <c r="AU32" s="7"/>
       <c r="AV32" s="6"/>
       <c r="AW32" s="5"/>
-      <c r="AX32" s="99"/>
-      <c r="AY32" s="100"/>
-      <c r="AZ32" s="81"/>
+      <c r="AX32" s="101"/>
+      <c r="AY32" s="72"/>
+      <c r="AZ32" s="119"/>
     </row>
     <row r="33" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A33" s="89"/>
-      <c r="B33" s="113"/>
-      <c r="C33" s="114"/>
+      <c r="A33" s="88"/>
+      <c r="B33" s="97"/>
+      <c r="C33" s="98"/>
       <c r="D33" s="33"/>
       <c r="E33" s="32"/>
       <c r="F33" s="3"/>
@@ -3651,14 +3651,14 @@
       <c r="M33" s="32"/>
       <c r="N33" s="3"/>
       <c r="O33" s="31"/>
-      <c r="P33" s="33"/>
-      <c r="Q33" s="32"/>
+      <c r="P33" s="57"/>
+      <c r="Q33" s="54"/>
       <c r="R33" s="32"/>
       <c r="S33" s="31"/>
-      <c r="T33" s="109"/>
-      <c r="U33" s="101"/>
-      <c r="V33" s="101"/>
-      <c r="W33" s="100"/>
+      <c r="T33" s="70"/>
+      <c r="U33" s="71"/>
+      <c r="V33" s="71"/>
+      <c r="W33" s="72"/>
       <c r="X33" s="33"/>
       <c r="Y33" s="3"/>
       <c r="Z33" s="32"/>
@@ -3675,28 +3675,28 @@
       <c r="AK33" s="32"/>
       <c r="AL33" s="32"/>
       <c r="AM33" s="31"/>
-      <c r="AN33" s="109"/>
-      <c r="AO33" s="101"/>
-      <c r="AP33" s="101"/>
-      <c r="AQ33" s="100"/>
+      <c r="AN33" s="70"/>
+      <c r="AO33" s="71"/>
+      <c r="AP33" s="71"/>
+      <c r="AQ33" s="72"/>
       <c r="AR33" s="33"/>
       <c r="AS33" s="3"/>
       <c r="AT33" s="3"/>
       <c r="AU33" s="12"/>
       <c r="AV33" s="11"/>
       <c r="AW33" s="32"/>
-      <c r="AX33" s="99"/>
-      <c r="AY33" s="100"/>
-      <c r="AZ33" s="81"/>
+      <c r="AX33" s="101"/>
+      <c r="AY33" s="72"/>
+      <c r="AZ33" s="119"/>
     </row>
     <row r="34" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A34" s="115" t="s">
+      <c r="A34" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="84">
+      <c r="B34" s="92">
         <v>1</v>
       </c>
-      <c r="C34" s="86"/>
+      <c r="C34" s="99"/>
       <c r="D34" s="6"/>
       <c r="E34" s="5"/>
       <c r="F34" s="30"/>
@@ -3713,10 +3713,10 @@
       <c r="Q34" s="55"/>
       <c r="R34" s="24"/>
       <c r="S34" s="7"/>
-      <c r="T34" s="109"/>
-      <c r="U34" s="101"/>
-      <c r="V34" s="101"/>
-      <c r="W34" s="100"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="71"/>
+      <c r="V34" s="71"/>
+      <c r="W34" s="72"/>
       <c r="X34" s="6"/>
       <c r="Y34" s="30"/>
       <c r="Z34" s="5"/>
@@ -3733,24 +3733,24 @@
       <c r="AK34" s="5"/>
       <c r="AL34" s="5"/>
       <c r="AM34" s="7"/>
-      <c r="AN34" s="109"/>
-      <c r="AO34" s="101"/>
-      <c r="AP34" s="101"/>
-      <c r="AQ34" s="100"/>
+      <c r="AN34" s="70"/>
+      <c r="AO34" s="71"/>
+      <c r="AP34" s="71"/>
+      <c r="AQ34" s="72"/>
       <c r="AR34" s="6"/>
       <c r="AS34" s="30"/>
       <c r="AT34" s="30"/>
       <c r="AU34" s="29"/>
       <c r="AV34" s="28"/>
       <c r="AW34" s="5"/>
-      <c r="AX34" s="99"/>
-      <c r="AY34" s="100"/>
-      <c r="AZ34" s="81"/>
+      <c r="AX34" s="101"/>
+      <c r="AY34" s="72"/>
+      <c r="AZ34" s="119"/>
     </row>
     <row r="35" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A35" s="89"/>
-      <c r="B35" s="113"/>
-      <c r="C35" s="93"/>
+      <c r="A35" s="88"/>
+      <c r="B35" s="97"/>
+      <c r="C35" s="90"/>
       <c r="D35" s="33"/>
       <c r="E35" s="32"/>
       <c r="F35" s="32"/>
@@ -3764,13 +3764,13 @@
       <c r="N35" s="3"/>
       <c r="O35" s="31"/>
       <c r="P35" s="33"/>
-      <c r="Q35" s="32"/>
-      <c r="R35" s="3"/>
+      <c r="Q35" s="54"/>
+      <c r="R35" s="40"/>
       <c r="S35" s="12"/>
-      <c r="T35" s="109"/>
-      <c r="U35" s="101"/>
-      <c r="V35" s="101"/>
-      <c r="W35" s="100"/>
+      <c r="T35" s="70"/>
+      <c r="U35" s="71"/>
+      <c r="V35" s="71"/>
+      <c r="W35" s="72"/>
       <c r="X35" s="11"/>
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
@@ -3787,28 +3787,28 @@
       <c r="AK35" s="3"/>
       <c r="AL35" s="3"/>
       <c r="AM35" s="12"/>
-      <c r="AN35" s="109"/>
-      <c r="AO35" s="101"/>
-      <c r="AP35" s="101"/>
-      <c r="AQ35" s="100"/>
+      <c r="AN35" s="70"/>
+      <c r="AO35" s="71"/>
+      <c r="AP35" s="71"/>
+      <c r="AQ35" s="72"/>
       <c r="AR35" s="33"/>
       <c r="AS35" s="3"/>
       <c r="AT35" s="32"/>
       <c r="AU35" s="31"/>
       <c r="AV35" s="33"/>
       <c r="AW35" s="3"/>
-      <c r="AX35" s="99"/>
-      <c r="AY35" s="100"/>
-      <c r="AZ35" s="81"/>
+      <c r="AX35" s="101"/>
+      <c r="AY35" s="72"/>
+      <c r="AZ35" s="119"/>
     </row>
     <row r="36" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A36" s="115" t="s">
+      <c r="A36" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="84">
+      <c r="B36" s="92">
         <v>1</v>
       </c>
-      <c r="C36" s="116"/>
+      <c r="C36" s="93"/>
       <c r="D36" s="6"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -3825,10 +3825,10 @@
       <c r="Q36" s="5"/>
       <c r="R36" s="30"/>
       <c r="S36" s="49"/>
-      <c r="T36" s="109"/>
-      <c r="U36" s="101"/>
-      <c r="V36" s="101"/>
-      <c r="W36" s="100"/>
+      <c r="T36" s="70"/>
+      <c r="U36" s="71"/>
+      <c r="V36" s="71"/>
+      <c r="W36" s="72"/>
       <c r="X36" s="28"/>
       <c r="Y36" s="30"/>
       <c r="Z36" s="30"/>
@@ -3845,24 +3845,24 @@
       <c r="AK36" s="30"/>
       <c r="AL36" s="30"/>
       <c r="AM36" s="29"/>
-      <c r="AN36" s="109"/>
-      <c r="AO36" s="101"/>
-      <c r="AP36" s="101"/>
-      <c r="AQ36" s="100"/>
+      <c r="AN36" s="70"/>
+      <c r="AO36" s="71"/>
+      <c r="AP36" s="71"/>
+      <c r="AQ36" s="72"/>
       <c r="AR36" s="6"/>
       <c r="AS36" s="30"/>
       <c r="AT36" s="5"/>
       <c r="AU36" s="7"/>
       <c r="AV36" s="6"/>
       <c r="AW36" s="30"/>
-      <c r="AX36" s="99"/>
-      <c r="AY36" s="100"/>
-      <c r="AZ36" s="81"/>
+      <c r="AX36" s="101"/>
+      <c r="AY36" s="72"/>
+      <c r="AZ36" s="119"/>
     </row>
     <row r="37" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A37" s="89"/>
-      <c r="B37" s="113"/>
-      <c r="C37" s="114"/>
+      <c r="A37" s="88"/>
+      <c r="B37" s="97"/>
+      <c r="C37" s="98"/>
       <c r="D37" s="33"/>
       <c r="E37" s="32"/>
       <c r="F37" s="3"/>
@@ -3878,11 +3878,11 @@
       <c r="P37" s="33"/>
       <c r="Q37" s="32"/>
       <c r="R37" s="3"/>
-      <c r="S37" s="31"/>
-      <c r="T37" s="109"/>
-      <c r="U37" s="101"/>
-      <c r="V37" s="101"/>
-      <c r="W37" s="100"/>
+      <c r="S37" s="66"/>
+      <c r="T37" s="70"/>
+      <c r="U37" s="71"/>
+      <c r="V37" s="71"/>
+      <c r="W37" s="72"/>
       <c r="X37" s="33"/>
       <c r="Y37" s="32"/>
       <c r="Z37" s="32"/>
@@ -3899,28 +3899,28 @@
       <c r="AK37" s="32"/>
       <c r="AL37" s="32"/>
       <c r="AM37" s="12"/>
-      <c r="AN37" s="109"/>
-      <c r="AO37" s="101"/>
-      <c r="AP37" s="101"/>
-      <c r="AQ37" s="100"/>
+      <c r="AN37" s="70"/>
+      <c r="AO37" s="71"/>
+      <c r="AP37" s="71"/>
+      <c r="AQ37" s="72"/>
       <c r="AR37" s="11"/>
       <c r="AS37" s="3"/>
       <c r="AT37" s="32"/>
       <c r="AU37" s="12"/>
       <c r="AV37" s="11"/>
       <c r="AW37" s="3"/>
-      <c r="AX37" s="99"/>
-      <c r="AY37" s="100"/>
-      <c r="AZ37" s="81"/>
+      <c r="AX37" s="101"/>
+      <c r="AY37" s="72"/>
+      <c r="AZ37" s="119"/>
     </row>
     <row r="38" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A38" s="82" t="s">
+      <c r="A38" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="84">
+      <c r="B38" s="92">
         <v>1</v>
       </c>
-      <c r="C38" s="116"/>
+      <c r="C38" s="93"/>
       <c r="D38" s="6"/>
       <c r="E38" s="5"/>
       <c r="F38" s="30"/>
@@ -3937,10 +3937,10 @@
       <c r="Q38" s="5"/>
       <c r="R38" s="30"/>
       <c r="S38" s="25"/>
-      <c r="T38" s="109"/>
-      <c r="U38" s="101"/>
-      <c r="V38" s="101"/>
-      <c r="W38" s="100"/>
+      <c r="T38" s="70"/>
+      <c r="U38" s="71"/>
+      <c r="V38" s="71"/>
+      <c r="W38" s="72"/>
       <c r="X38" s="6"/>
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
@@ -3957,24 +3957,24 @@
       <c r="AK38" s="5"/>
       <c r="AL38" s="5"/>
       <c r="AM38" s="29"/>
-      <c r="AN38" s="109"/>
-      <c r="AO38" s="101"/>
-      <c r="AP38" s="101"/>
-      <c r="AQ38" s="100"/>
+      <c r="AN38" s="70"/>
+      <c r="AO38" s="71"/>
+      <c r="AP38" s="71"/>
+      <c r="AQ38" s="72"/>
       <c r="AR38" s="28"/>
       <c r="AS38" s="30"/>
       <c r="AT38" s="5"/>
       <c r="AU38" s="29"/>
       <c r="AV38" s="28"/>
       <c r="AW38" s="30"/>
-      <c r="AX38" s="99"/>
-      <c r="AY38" s="100"/>
-      <c r="AZ38" s="81"/>
+      <c r="AX38" s="101"/>
+      <c r="AY38" s="72"/>
+      <c r="AZ38" s="119"/>
     </row>
     <row r="39" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A39" s="112"/>
-      <c r="B39" s="113"/>
-      <c r="C39" s="114"/>
+      <c r="A39" s="96"/>
+      <c r="B39" s="97"/>
+      <c r="C39" s="98"/>
       <c r="D39" s="11"/>
       <c r="E39" s="3"/>
       <c r="F39" s="32"/>
@@ -3991,10 +3991,10 @@
       <c r="Q39" s="32"/>
       <c r="R39" s="3"/>
       <c r="S39" s="12"/>
-      <c r="T39" s="109"/>
-      <c r="U39" s="101"/>
-      <c r="V39" s="101"/>
-      <c r="W39" s="100"/>
+      <c r="T39" s="70"/>
+      <c r="U39" s="71"/>
+      <c r="V39" s="71"/>
+      <c r="W39" s="72"/>
       <c r="X39" s="11"/>
       <c r="Y39" s="32"/>
       <c r="Z39" s="32"/>
@@ -4011,28 +4011,28 @@
       <c r="AK39" s="32"/>
       <c r="AL39" s="32"/>
       <c r="AM39" s="31"/>
-      <c r="AN39" s="109"/>
-      <c r="AO39" s="101"/>
-      <c r="AP39" s="101"/>
-      <c r="AQ39" s="100"/>
+      <c r="AN39" s="70"/>
+      <c r="AO39" s="71"/>
+      <c r="AP39" s="71"/>
+      <c r="AQ39" s="72"/>
       <c r="AR39" s="33"/>
       <c r="AS39" s="32"/>
       <c r="AT39" s="3"/>
       <c r="AU39" s="31"/>
       <c r="AV39" s="11"/>
       <c r="AW39" s="3"/>
-      <c r="AX39" s="99"/>
-      <c r="AY39" s="100"/>
-      <c r="AZ39" s="81"/>
+      <c r="AX39" s="101"/>
+      <c r="AY39" s="72"/>
+      <c r="AZ39" s="119"/>
     </row>
     <row r="40" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A40" s="115" t="s">
+      <c r="A40" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="84">
+      <c r="B40" s="92">
         <v>1</v>
       </c>
-      <c r="C40" s="116"/>
+      <c r="C40" s="93"/>
       <c r="D40" s="28"/>
       <c r="E40" s="30"/>
       <c r="F40" s="5"/>
@@ -4049,10 +4049,10 @@
       <c r="Q40" s="5"/>
       <c r="R40" s="30"/>
       <c r="S40" s="29"/>
-      <c r="T40" s="109"/>
-      <c r="U40" s="101"/>
-      <c r="V40" s="101"/>
-      <c r="W40" s="100"/>
+      <c r="T40" s="70"/>
+      <c r="U40" s="71"/>
+      <c r="V40" s="71"/>
+      <c r="W40" s="72"/>
       <c r="X40" s="38"/>
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
@@ -4069,24 +4069,24 @@
       <c r="AK40" s="5"/>
       <c r="AL40" s="5"/>
       <c r="AM40" s="7"/>
-      <c r="AN40" s="109"/>
-      <c r="AO40" s="101"/>
-      <c r="AP40" s="101"/>
-      <c r="AQ40" s="100"/>
+      <c r="AN40" s="70"/>
+      <c r="AO40" s="71"/>
+      <c r="AP40" s="71"/>
+      <c r="AQ40" s="72"/>
       <c r="AR40" s="6"/>
       <c r="AS40" s="5"/>
       <c r="AT40" s="30"/>
       <c r="AU40" s="7"/>
       <c r="AV40" s="28"/>
       <c r="AW40" s="30"/>
-      <c r="AX40" s="99"/>
-      <c r="AY40" s="100"/>
-      <c r="AZ40" s="81"/>
+      <c r="AX40" s="101"/>
+      <c r="AY40" s="72"/>
+      <c r="AZ40" s="119"/>
     </row>
     <row r="41" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A41" s="112"/>
-      <c r="B41" s="113"/>
-      <c r="C41" s="114"/>
+      <c r="A41" s="96"/>
+      <c r="B41" s="97"/>
+      <c r="C41" s="98"/>
       <c r="D41" s="33"/>
       <c r="E41" s="32"/>
       <c r="F41" s="32"/>
@@ -4103,10 +4103,10 @@
       <c r="Q41" s="32"/>
       <c r="R41" s="3"/>
       <c r="S41" s="12"/>
-      <c r="T41" s="109"/>
-      <c r="U41" s="101"/>
-      <c r="V41" s="101"/>
-      <c r="W41" s="100"/>
+      <c r="T41" s="70"/>
+      <c r="U41" s="71"/>
+      <c r="V41" s="71"/>
+      <c r="W41" s="72"/>
       <c r="X41" s="11"/>
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
@@ -4123,28 +4123,28 @@
       <c r="AK41" s="3"/>
       <c r="AL41" s="32"/>
       <c r="AM41" s="12"/>
-      <c r="AN41" s="109"/>
-      <c r="AO41" s="101"/>
-      <c r="AP41" s="101"/>
-      <c r="AQ41" s="100"/>
+      <c r="AN41" s="70"/>
+      <c r="AO41" s="71"/>
+      <c r="AP41" s="71"/>
+      <c r="AQ41" s="72"/>
       <c r="AR41" s="11"/>
       <c r="AS41" s="3"/>
       <c r="AT41" s="3"/>
       <c r="AU41" s="12"/>
       <c r="AV41" s="11"/>
       <c r="AW41" s="32"/>
-      <c r="AX41" s="99"/>
-      <c r="AY41" s="100"/>
-      <c r="AZ41" s="81"/>
+      <c r="AX41" s="101"/>
+      <c r="AY41" s="72"/>
+      <c r="AZ41" s="119"/>
     </row>
     <row r="42" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A42" s="115" t="s">
+      <c r="A42" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="84">
+      <c r="B42" s="92">
         <v>2</v>
       </c>
-      <c r="C42" s="116"/>
+      <c r="C42" s="93"/>
       <c r="D42" s="6"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -4161,10 +4161,10 @@
       <c r="Q42" s="5"/>
       <c r="R42" s="30"/>
       <c r="S42" s="29"/>
-      <c r="T42" s="109"/>
-      <c r="U42" s="101"/>
-      <c r="V42" s="101"/>
-      <c r="W42" s="100"/>
+      <c r="T42" s="70"/>
+      <c r="U42" s="71"/>
+      <c r="V42" s="71"/>
+      <c r="W42" s="72"/>
       <c r="X42" s="28"/>
       <c r="Y42" s="34"/>
       <c r="Z42" s="34"/>
@@ -4181,24 +4181,24 @@
       <c r="AK42" s="30"/>
       <c r="AL42" s="5"/>
       <c r="AM42" s="29"/>
-      <c r="AN42" s="109"/>
-      <c r="AO42" s="101"/>
-      <c r="AP42" s="101"/>
-      <c r="AQ42" s="100"/>
+      <c r="AN42" s="70"/>
+      <c r="AO42" s="71"/>
+      <c r="AP42" s="71"/>
+      <c r="AQ42" s="72"/>
       <c r="AR42" s="28"/>
       <c r="AS42" s="30"/>
       <c r="AT42" s="30"/>
       <c r="AU42" s="29"/>
       <c r="AV42" s="28"/>
       <c r="AW42" s="5"/>
-      <c r="AX42" s="99"/>
-      <c r="AY42" s="100"/>
-      <c r="AZ42" s="81"/>
+      <c r="AX42" s="101"/>
+      <c r="AY42" s="72"/>
+      <c r="AZ42" s="119"/>
     </row>
     <row r="43" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A43" s="89"/>
-      <c r="B43" s="113"/>
-      <c r="C43" s="114"/>
+      <c r="A43" s="88"/>
+      <c r="B43" s="97"/>
+      <c r="C43" s="98"/>
       <c r="D43" s="11"/>
       <c r="E43" s="32"/>
       <c r="F43" s="3"/>
@@ -4214,11 +4214,11 @@
       <c r="P43" s="11"/>
       <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
-      <c r="S43" s="31"/>
-      <c r="T43" s="109"/>
-      <c r="U43" s="101"/>
-      <c r="V43" s="101"/>
-      <c r="W43" s="100"/>
+      <c r="S43" s="66"/>
+      <c r="T43" s="70"/>
+      <c r="U43" s="71"/>
+      <c r="V43" s="71"/>
+      <c r="W43" s="72"/>
       <c r="X43" s="11"/>
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
@@ -4235,28 +4235,28 @@
       <c r="AK43" s="32"/>
       <c r="AL43" s="3"/>
       <c r="AM43" s="12"/>
-      <c r="AN43" s="109"/>
-      <c r="AO43" s="101"/>
-      <c r="AP43" s="101"/>
-      <c r="AQ43" s="100"/>
+      <c r="AN43" s="70"/>
+      <c r="AO43" s="71"/>
+      <c r="AP43" s="71"/>
+      <c r="AQ43" s="72"/>
       <c r="AR43" s="11"/>
       <c r="AS43" s="3"/>
       <c r="AT43" s="3"/>
       <c r="AU43" s="12"/>
       <c r="AV43" s="11"/>
       <c r="AW43" s="3"/>
-      <c r="AX43" s="99"/>
-      <c r="AY43" s="100"/>
-      <c r="AZ43" s="81"/>
+      <c r="AX43" s="101"/>
+      <c r="AY43" s="72"/>
+      <c r="AZ43" s="119"/>
     </row>
     <row r="44" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A44" s="115" t="s">
+      <c r="A44" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="117">
+      <c r="B44" s="95">
         <v>2.5</v>
       </c>
-      <c r="C44" s="116"/>
+      <c r="C44" s="93"/>
       <c r="D44" s="28"/>
       <c r="E44" s="5"/>
       <c r="F44" s="30"/>
@@ -4273,10 +4273,10 @@
       <c r="Q44" s="30"/>
       <c r="R44" s="30"/>
       <c r="S44" s="7"/>
-      <c r="T44" s="109"/>
-      <c r="U44" s="101"/>
-      <c r="V44" s="101"/>
-      <c r="W44" s="100"/>
+      <c r="T44" s="70"/>
+      <c r="U44" s="71"/>
+      <c r="V44" s="71"/>
+      <c r="W44" s="72"/>
       <c r="X44" s="28"/>
       <c r="Y44" s="30"/>
       <c r="Z44" s="34"/>
@@ -4293,24 +4293,24 @@
       <c r="AK44" s="5"/>
       <c r="AL44" s="30"/>
       <c r="AM44" s="29"/>
-      <c r="AN44" s="109"/>
-      <c r="AO44" s="101"/>
-      <c r="AP44" s="101"/>
-      <c r="AQ44" s="100"/>
+      <c r="AN44" s="70"/>
+      <c r="AO44" s="71"/>
+      <c r="AP44" s="71"/>
+      <c r="AQ44" s="72"/>
       <c r="AR44" s="28"/>
       <c r="AS44" s="30"/>
       <c r="AT44" s="30"/>
       <c r="AU44" s="29"/>
       <c r="AV44" s="28"/>
       <c r="AW44" s="30"/>
-      <c r="AX44" s="99"/>
-      <c r="AY44" s="100"/>
-      <c r="AZ44" s="81"/>
+      <c r="AX44" s="101"/>
+      <c r="AY44" s="72"/>
+      <c r="AZ44" s="119"/>
     </row>
     <row r="45" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A45" s="89"/>
-      <c r="B45" s="91"/>
-      <c r="C45" s="114"/>
+      <c r="A45" s="88"/>
+      <c r="B45" s="89"/>
+      <c r="C45" s="98"/>
       <c r="D45" s="11"/>
       <c r="E45" s="3"/>
       <c r="F45" s="32"/>
@@ -4326,11 +4326,11 @@
       <c r="P45" s="11"/>
       <c r="Q45" s="3"/>
       <c r="R45" s="3"/>
-      <c r="S45" s="12"/>
-      <c r="T45" s="109"/>
-      <c r="U45" s="101"/>
-      <c r="V45" s="101"/>
-      <c r="W45" s="100"/>
+      <c r="S45" s="65"/>
+      <c r="T45" s="70"/>
+      <c r="U45" s="71"/>
+      <c r="V45" s="71"/>
+      <c r="W45" s="72"/>
       <c r="X45" s="11"/>
       <c r="Y45" s="32"/>
       <c r="Z45" s="3"/>
@@ -4347,28 +4347,28 @@
       <c r="AK45" s="3"/>
       <c r="AL45" s="3"/>
       <c r="AM45" s="12"/>
-      <c r="AN45" s="109"/>
-      <c r="AO45" s="101"/>
-      <c r="AP45" s="101"/>
-      <c r="AQ45" s="100"/>
+      <c r="AN45" s="70"/>
+      <c r="AO45" s="71"/>
+      <c r="AP45" s="71"/>
+      <c r="AQ45" s="72"/>
       <c r="AR45" s="11"/>
       <c r="AS45" s="3"/>
       <c r="AT45" s="3"/>
       <c r="AU45" s="12"/>
       <c r="AV45" s="11"/>
       <c r="AW45" s="3"/>
-      <c r="AX45" s="99"/>
-      <c r="AY45" s="100"/>
-      <c r="AZ45" s="81"/>
+      <c r="AX45" s="101"/>
+      <c r="AY45" s="72"/>
+      <c r="AZ45" s="119"/>
     </row>
     <row r="46" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A46" s="82" t="s">
+      <c r="A46" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="84">
+      <c r="B46" s="92">
         <v>2</v>
       </c>
-      <c r="C46" s="86"/>
+      <c r="C46" s="99"/>
       <c r="D46" s="28"/>
       <c r="E46" s="30"/>
       <c r="F46" s="5"/>
@@ -4385,10 +4385,10 @@
       <c r="Q46" s="30"/>
       <c r="R46" s="30"/>
       <c r="S46" s="29"/>
-      <c r="T46" s="109"/>
-      <c r="U46" s="101"/>
-      <c r="V46" s="101"/>
-      <c r="W46" s="100"/>
+      <c r="T46" s="70"/>
+      <c r="U46" s="71"/>
+      <c r="V46" s="71"/>
+      <c r="W46" s="72"/>
       <c r="X46" s="28"/>
       <c r="Y46" s="5"/>
       <c r="Z46" s="30"/>
@@ -4405,24 +4405,24 @@
       <c r="AK46" s="30"/>
       <c r="AL46" s="30"/>
       <c r="AM46" s="29"/>
-      <c r="AN46" s="109"/>
-      <c r="AO46" s="101"/>
-      <c r="AP46" s="101"/>
-      <c r="AQ46" s="100"/>
+      <c r="AN46" s="70"/>
+      <c r="AO46" s="71"/>
+      <c r="AP46" s="71"/>
+      <c r="AQ46" s="72"/>
       <c r="AR46" s="28"/>
       <c r="AS46" s="30"/>
       <c r="AT46" s="30"/>
       <c r="AU46" s="29"/>
       <c r="AV46" s="28"/>
       <c r="AW46" s="30"/>
-      <c r="AX46" s="99"/>
-      <c r="AY46" s="100"/>
-      <c r="AZ46" s="81"/>
+      <c r="AX46" s="101"/>
+      <c r="AY46" s="72"/>
+      <c r="AZ46" s="119"/>
     </row>
     <row r="47" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A47" s="112"/>
-      <c r="B47" s="113"/>
-      <c r="C47" s="93"/>
+      <c r="A47" s="96"/>
+      <c r="B47" s="97"/>
+      <c r="C47" s="90"/>
       <c r="D47" s="11"/>
       <c r="E47" s="32"/>
       <c r="F47" s="3"/>
@@ -4439,10 +4439,10 @@
       <c r="Q47" s="3"/>
       <c r="R47" s="32"/>
       <c r="S47" s="12"/>
-      <c r="T47" s="109"/>
-      <c r="U47" s="101"/>
-      <c r="V47" s="101"/>
-      <c r="W47" s="100"/>
+      <c r="T47" s="70"/>
+      <c r="U47" s="71"/>
+      <c r="V47" s="71"/>
+      <c r="W47" s="72"/>
       <c r="X47" s="11"/>
       <c r="Y47" s="3"/>
       <c r="Z47" s="3"/>
@@ -4459,28 +4459,28 @@
       <c r="AK47" s="32"/>
       <c r="AL47" s="3"/>
       <c r="AM47" s="31"/>
-      <c r="AN47" s="109"/>
-      <c r="AO47" s="101"/>
-      <c r="AP47" s="101"/>
-      <c r="AQ47" s="100"/>
+      <c r="AN47" s="70"/>
+      <c r="AO47" s="71"/>
+      <c r="AP47" s="71"/>
+      <c r="AQ47" s="72"/>
       <c r="AR47" s="33"/>
       <c r="AS47" s="32"/>
       <c r="AT47" s="32"/>
       <c r="AU47" s="31"/>
       <c r="AV47" s="33"/>
       <c r="AW47" s="32"/>
-      <c r="AX47" s="99"/>
-      <c r="AY47" s="100"/>
-      <c r="AZ47" s="81"/>
+      <c r="AX47" s="101"/>
+      <c r="AY47" s="72"/>
+      <c r="AZ47" s="119"/>
     </row>
     <row r="48" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A48" s="115" t="s">
+      <c r="A48" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="117">
+      <c r="B48" s="95">
         <v>0.5</v>
       </c>
-      <c r="C48" s="116"/>
+      <c r="C48" s="93"/>
       <c r="D48" s="28"/>
       <c r="E48" s="5"/>
       <c r="F48" s="30"/>
@@ -4497,10 +4497,10 @@
       <c r="Q48" s="30"/>
       <c r="R48" s="5"/>
       <c r="S48" s="29"/>
-      <c r="T48" s="109"/>
-      <c r="U48" s="101"/>
-      <c r="V48" s="101"/>
-      <c r="W48" s="100"/>
+      <c r="T48" s="70"/>
+      <c r="U48" s="71"/>
+      <c r="V48" s="71"/>
+      <c r="W48" s="72"/>
       <c r="X48" s="28"/>
       <c r="Y48" s="30"/>
       <c r="Z48" s="30"/>
@@ -4517,24 +4517,24 @@
       <c r="AK48" s="5"/>
       <c r="AL48" s="30"/>
       <c r="AM48" s="7"/>
-      <c r="AN48" s="109"/>
-      <c r="AO48" s="101"/>
-      <c r="AP48" s="101"/>
-      <c r="AQ48" s="100"/>
+      <c r="AN48" s="70"/>
+      <c r="AO48" s="71"/>
+      <c r="AP48" s="71"/>
+      <c r="AQ48" s="72"/>
       <c r="AR48" s="6"/>
       <c r="AS48" s="5"/>
       <c r="AT48" s="5"/>
       <c r="AU48" s="7"/>
       <c r="AV48" s="6"/>
       <c r="AW48" s="5"/>
-      <c r="AX48" s="99"/>
-      <c r="AY48" s="100"/>
-      <c r="AZ48" s="81"/>
+      <c r="AX48" s="101"/>
+      <c r="AY48" s="72"/>
+      <c r="AZ48" s="119"/>
     </row>
     <row r="49" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A49" s="112"/>
-      <c r="B49" s="91"/>
-      <c r="C49" s="114"/>
+      <c r="A49" s="96"/>
+      <c r="B49" s="89"/>
+      <c r="C49" s="98"/>
       <c r="D49" s="33"/>
       <c r="E49" s="32"/>
       <c r="F49" s="32"/>
@@ -4551,10 +4551,10 @@
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
       <c r="S49" s="12"/>
-      <c r="T49" s="109"/>
-      <c r="U49" s="101"/>
-      <c r="V49" s="101"/>
-      <c r="W49" s="100"/>
+      <c r="T49" s="70"/>
+      <c r="U49" s="71"/>
+      <c r="V49" s="71"/>
+      <c r="W49" s="72"/>
       <c r="X49" s="11"/>
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
@@ -4571,28 +4571,28 @@
       <c r="AK49" s="3"/>
       <c r="AL49" s="3"/>
       <c r="AM49" s="12"/>
-      <c r="AN49" s="109"/>
-      <c r="AO49" s="101"/>
-      <c r="AP49" s="101"/>
-      <c r="AQ49" s="100"/>
+      <c r="AN49" s="70"/>
+      <c r="AO49" s="71"/>
+      <c r="AP49" s="71"/>
+      <c r="AQ49" s="72"/>
       <c r="AR49" s="33"/>
       <c r="AS49" s="3"/>
       <c r="AT49" s="32"/>
       <c r="AU49" s="31"/>
       <c r="AV49" s="11"/>
       <c r="AW49" s="3"/>
-      <c r="AX49" s="99"/>
-      <c r="AY49" s="100"/>
-      <c r="AZ49" s="81"/>
+      <c r="AX49" s="101"/>
+      <c r="AY49" s="72"/>
+      <c r="AZ49" s="119"/>
     </row>
     <row r="50" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A50" s="115" t="s">
+      <c r="A50" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="B50" s="84">
+      <c r="B50" s="92">
         <v>2.5</v>
       </c>
-      <c r="C50" s="116"/>
+      <c r="C50" s="93"/>
       <c r="D50" s="6"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -4609,10 +4609,10 @@
       <c r="Q50" s="30"/>
       <c r="R50" s="30"/>
       <c r="S50" s="29"/>
-      <c r="T50" s="109"/>
-      <c r="U50" s="101"/>
-      <c r="V50" s="101"/>
-      <c r="W50" s="100"/>
+      <c r="T50" s="70"/>
+      <c r="U50" s="71"/>
+      <c r="V50" s="71"/>
+      <c r="W50" s="72"/>
       <c r="X50" s="28"/>
       <c r="Y50" s="30"/>
       <c r="Z50" s="30"/>
@@ -4629,24 +4629,24 @@
       <c r="AK50" s="30"/>
       <c r="AL50" s="30"/>
       <c r="AM50" s="29"/>
-      <c r="AN50" s="109"/>
-      <c r="AO50" s="101"/>
-      <c r="AP50" s="101"/>
-      <c r="AQ50" s="100"/>
+      <c r="AN50" s="70"/>
+      <c r="AO50" s="71"/>
+      <c r="AP50" s="71"/>
+      <c r="AQ50" s="72"/>
       <c r="AR50" s="6"/>
       <c r="AS50" s="30"/>
       <c r="AT50" s="5"/>
       <c r="AU50" s="7"/>
       <c r="AV50" s="28"/>
       <c r="AW50" s="30"/>
-      <c r="AX50" s="99"/>
-      <c r="AY50" s="100"/>
-      <c r="AZ50" s="81"/>
+      <c r="AX50" s="101"/>
+      <c r="AY50" s="72"/>
+      <c r="AZ50" s="119"/>
     </row>
     <row r="51" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A51" s="89"/>
-      <c r="B51" s="113"/>
-      <c r="C51" s="114"/>
+      <c r="A51" s="88"/>
+      <c r="B51" s="97"/>
+      <c r="C51" s="98"/>
       <c r="D51" s="11"/>
       <c r="E51" s="32"/>
       <c r="F51" s="3"/>
@@ -4663,10 +4663,10 @@
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
       <c r="S51" s="12"/>
-      <c r="T51" s="109"/>
-      <c r="U51" s="101"/>
-      <c r="V51" s="101"/>
-      <c r="W51" s="100"/>
+      <c r="T51" s="70"/>
+      <c r="U51" s="71"/>
+      <c r="V51" s="71"/>
+      <c r="W51" s="72"/>
       <c r="X51" s="33"/>
       <c r="Y51" s="32"/>
       <c r="Z51" s="3"/>
@@ -4683,28 +4683,28 @@
       <c r="AK51" s="32"/>
       <c r="AL51" s="3"/>
       <c r="AM51" s="12"/>
-      <c r="AN51" s="109"/>
-      <c r="AO51" s="101"/>
-      <c r="AP51" s="101"/>
-      <c r="AQ51" s="100"/>
+      <c r="AN51" s="70"/>
+      <c r="AO51" s="71"/>
+      <c r="AP51" s="71"/>
+      <c r="AQ51" s="72"/>
       <c r="AR51" s="11"/>
       <c r="AS51" s="3"/>
       <c r="AT51" s="3"/>
       <c r="AU51" s="12"/>
       <c r="AV51" s="11"/>
       <c r="AW51" s="3"/>
-      <c r="AX51" s="99"/>
-      <c r="AY51" s="100"/>
-      <c r="AZ51" s="81"/>
+      <c r="AX51" s="101"/>
+      <c r="AY51" s="72"/>
+      <c r="AZ51" s="119"/>
     </row>
     <row r="52" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A52" s="82" t="s">
+      <c r="A52" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="84">
+      <c r="B52" s="92">
         <v>1.5</v>
       </c>
-      <c r="C52" s="116"/>
+      <c r="C52" s="93"/>
       <c r="D52" s="28"/>
       <c r="E52" s="5"/>
       <c r="F52" s="30"/>
@@ -4721,10 +4721,10 @@
       <c r="Q52" s="30"/>
       <c r="R52" s="30"/>
       <c r="S52" s="29"/>
-      <c r="T52" s="109"/>
-      <c r="U52" s="101"/>
-      <c r="V52" s="101"/>
-      <c r="W52" s="100"/>
+      <c r="T52" s="70"/>
+      <c r="U52" s="71"/>
+      <c r="V52" s="71"/>
+      <c r="W52" s="72"/>
       <c r="X52" s="6"/>
       <c r="Y52" s="5"/>
       <c r="Z52" s="30"/>
@@ -4741,24 +4741,24 @@
       <c r="AK52" s="5"/>
       <c r="AL52" s="30"/>
       <c r="AM52" s="29"/>
-      <c r="AN52" s="109"/>
-      <c r="AO52" s="101"/>
-      <c r="AP52" s="101"/>
-      <c r="AQ52" s="100"/>
+      <c r="AN52" s="70"/>
+      <c r="AO52" s="71"/>
+      <c r="AP52" s="71"/>
+      <c r="AQ52" s="72"/>
       <c r="AR52" s="28"/>
       <c r="AS52" s="30"/>
       <c r="AT52" s="30"/>
       <c r="AU52" s="29"/>
       <c r="AV52" s="28"/>
       <c r="AW52" s="30"/>
-      <c r="AX52" s="99"/>
-      <c r="AY52" s="100"/>
-      <c r="AZ52" s="81"/>
+      <c r="AX52" s="101"/>
+      <c r="AY52" s="72"/>
+      <c r="AZ52" s="119"/>
     </row>
     <row r="53" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A53" s="112"/>
-      <c r="B53" s="113"/>
-      <c r="C53" s="114"/>
+      <c r="A53" s="96"/>
+      <c r="B53" s="97"/>
+      <c r="C53" s="98"/>
       <c r="D53" s="33"/>
       <c r="E53" s="32"/>
       <c r="F53" s="32"/>
@@ -4775,10 +4775,10 @@
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
       <c r="S53" s="12"/>
-      <c r="T53" s="109"/>
-      <c r="U53" s="101"/>
-      <c r="V53" s="101"/>
-      <c r="W53" s="100"/>
+      <c r="T53" s="70"/>
+      <c r="U53" s="71"/>
+      <c r="V53" s="71"/>
+      <c r="W53" s="72"/>
       <c r="X53" s="11"/>
       <c r="Y53" s="32"/>
       <c r="Z53" s="3"/>
@@ -4795,28 +4795,28 @@
       <c r="AK53" s="3"/>
       <c r="AL53" s="3"/>
       <c r="AM53" s="12"/>
-      <c r="AN53" s="109"/>
-      <c r="AO53" s="101"/>
-      <c r="AP53" s="101"/>
-      <c r="AQ53" s="100"/>
+      <c r="AN53" s="70"/>
+      <c r="AO53" s="71"/>
+      <c r="AP53" s="71"/>
+      <c r="AQ53" s="72"/>
       <c r="AR53" s="11"/>
       <c r="AS53" s="3"/>
       <c r="AT53" s="3"/>
       <c r="AU53" s="12"/>
       <c r="AV53" s="11"/>
       <c r="AW53" s="3"/>
-      <c r="AX53" s="99"/>
-      <c r="AY53" s="100"/>
-      <c r="AZ53" s="81"/>
+      <c r="AX53" s="101"/>
+      <c r="AY53" s="72"/>
+      <c r="AZ53" s="119"/>
     </row>
     <row r="54" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A54" s="115" t="s">
+      <c r="A54" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="84">
+      <c r="B54" s="92">
         <v>1.5</v>
       </c>
-      <c r="C54" s="86"/>
+      <c r="C54" s="99"/>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
@@ -4833,10 +4833,10 @@
       <c r="Q54" s="30"/>
       <c r="R54" s="30"/>
       <c r="S54" s="29"/>
-      <c r="T54" s="109"/>
-      <c r="U54" s="101"/>
-      <c r="V54" s="101"/>
-      <c r="W54" s="100"/>
+      <c r="T54" s="70"/>
+      <c r="U54" s="71"/>
+      <c r="V54" s="71"/>
+      <c r="W54" s="72"/>
       <c r="X54" s="28"/>
       <c r="Y54" s="5"/>
       <c r="Z54" s="30"/>
@@ -4853,24 +4853,24 @@
       <c r="AK54" s="30"/>
       <c r="AL54" s="30"/>
       <c r="AM54" s="29"/>
-      <c r="AN54" s="109"/>
-      <c r="AO54" s="101"/>
-      <c r="AP54" s="101"/>
-      <c r="AQ54" s="100"/>
+      <c r="AN54" s="70"/>
+      <c r="AO54" s="71"/>
+      <c r="AP54" s="71"/>
+      <c r="AQ54" s="72"/>
       <c r="AR54" s="28"/>
       <c r="AS54" s="30"/>
       <c r="AT54" s="30"/>
       <c r="AU54" s="29"/>
       <c r="AV54" s="28"/>
       <c r="AW54" s="30"/>
-      <c r="AX54" s="99"/>
-      <c r="AY54" s="100"/>
-      <c r="AZ54" s="81"/>
+      <c r="AX54" s="101"/>
+      <c r="AY54" s="72"/>
+      <c r="AZ54" s="119"/>
     </row>
     <row r="55" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A55" s="89"/>
-      <c r="B55" s="113"/>
-      <c r="C55" s="93"/>
+      <c r="A55" s="88"/>
+      <c r="B55" s="97"/>
+      <c r="C55" s="90"/>
       <c r="D55" s="11"/>
       <c r="E55" s="32"/>
       <c r="F55" s="3"/>
@@ -4887,10 +4887,10 @@
       <c r="Q55" s="32"/>
       <c r="R55" s="3"/>
       <c r="S55" s="31"/>
-      <c r="T55" s="109"/>
-      <c r="U55" s="101"/>
-      <c r="V55" s="101"/>
-      <c r="W55" s="100"/>
+      <c r="T55" s="70"/>
+      <c r="U55" s="71"/>
+      <c r="V55" s="71"/>
+      <c r="W55" s="72"/>
       <c r="X55" s="11"/>
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
@@ -4907,28 +4907,28 @@
       <c r="AK55" s="32"/>
       <c r="AL55" s="32"/>
       <c r="AM55" s="31"/>
-      <c r="AN55" s="109"/>
-      <c r="AO55" s="101"/>
-      <c r="AP55" s="101"/>
-      <c r="AQ55" s="100"/>
+      <c r="AN55" s="70"/>
+      <c r="AO55" s="71"/>
+      <c r="AP55" s="71"/>
+      <c r="AQ55" s="72"/>
       <c r="AR55" s="33"/>
       <c r="AS55" s="32"/>
       <c r="AT55" s="32"/>
       <c r="AU55" s="12"/>
       <c r="AV55" s="11"/>
       <c r="AW55" s="3"/>
-      <c r="AX55" s="99"/>
-      <c r="AY55" s="100"/>
-      <c r="AZ55" s="81"/>
+      <c r="AX55" s="101"/>
+      <c r="AY55" s="72"/>
+      <c r="AZ55" s="119"/>
     </row>
     <row r="56" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A56" s="115" t="s">
+      <c r="A56" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="117">
+      <c r="B56" s="95">
         <v>2</v>
       </c>
-      <c r="C56" s="116"/>
+      <c r="C56" s="93"/>
       <c r="D56" s="28"/>
       <c r="E56" s="5"/>
       <c r="F56" s="30"/>
@@ -4945,10 +4945,10 @@
       <c r="Q56" s="5"/>
       <c r="R56" s="30"/>
       <c r="S56" s="7"/>
-      <c r="T56" s="109"/>
-      <c r="U56" s="101"/>
-      <c r="V56" s="101"/>
-      <c r="W56" s="100"/>
+      <c r="T56" s="70"/>
+      <c r="U56" s="71"/>
+      <c r="V56" s="71"/>
+      <c r="W56" s="72"/>
       <c r="X56" s="28"/>
       <c r="Y56" s="30"/>
       <c r="Z56" s="30"/>
@@ -4965,24 +4965,24 @@
       <c r="AK56" s="24"/>
       <c r="AL56" s="5"/>
       <c r="AM56" s="7"/>
-      <c r="AN56" s="109"/>
-      <c r="AO56" s="101"/>
-      <c r="AP56" s="101"/>
-      <c r="AQ56" s="100"/>
+      <c r="AN56" s="70"/>
+      <c r="AO56" s="71"/>
+      <c r="AP56" s="71"/>
+      <c r="AQ56" s="72"/>
       <c r="AR56" s="6"/>
       <c r="AS56" s="5"/>
       <c r="AT56" s="5"/>
       <c r="AU56" s="29"/>
       <c r="AV56" s="28"/>
       <c r="AW56" s="30"/>
-      <c r="AX56" s="99"/>
-      <c r="AY56" s="100"/>
-      <c r="AZ56" s="81"/>
+      <c r="AX56" s="101"/>
+      <c r="AY56" s="72"/>
+      <c r="AZ56" s="119"/>
     </row>
     <row r="57" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A57" s="89"/>
-      <c r="B57" s="91"/>
-      <c r="C57" s="93"/>
+      <c r="A57" s="88"/>
+      <c r="B57" s="89"/>
+      <c r="C57" s="90"/>
       <c r="D57" s="11"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -4999,10 +4999,10 @@
       <c r="Q57" s="3"/>
       <c r="R57" s="3"/>
       <c r="S57" s="12"/>
-      <c r="T57" s="109"/>
-      <c r="U57" s="101"/>
-      <c r="V57" s="101"/>
-      <c r="W57" s="100"/>
+      <c r="T57" s="70"/>
+      <c r="U57" s="71"/>
+      <c r="V57" s="71"/>
+      <c r="W57" s="72"/>
       <c r="X57" s="33"/>
       <c r="Y57" s="3"/>
       <c r="Z57" s="32"/>
@@ -5019,28 +5019,28 @@
       <c r="AK57" s="32"/>
       <c r="AL57" s="3"/>
       <c r="AM57" s="12"/>
-      <c r="AN57" s="109"/>
-      <c r="AO57" s="101"/>
-      <c r="AP57" s="101"/>
-      <c r="AQ57" s="100"/>
+      <c r="AN57" s="70"/>
+      <c r="AO57" s="71"/>
+      <c r="AP57" s="71"/>
+      <c r="AQ57" s="72"/>
       <c r="AR57" s="11"/>
       <c r="AS57" s="3"/>
       <c r="AT57" s="3"/>
       <c r="AU57" s="31"/>
       <c r="AV57" s="33"/>
       <c r="AW57" s="3"/>
-      <c r="AX57" s="99"/>
-      <c r="AY57" s="100"/>
-      <c r="AZ57" s="81"/>
+      <c r="AX57" s="101"/>
+      <c r="AY57" s="72"/>
+      <c r="AZ57" s="119"/>
     </row>
     <row r="58" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A58" s="82" t="s">
+      <c r="A58" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="84">
+      <c r="B58" s="92">
         <v>2</v>
       </c>
-      <c r="C58" s="116"/>
+      <c r="C58" s="93"/>
       <c r="D58" s="28"/>
       <c r="E58" s="30"/>
       <c r="F58" s="30"/>
@@ -5057,10 +5057,10 @@
       <c r="Q58" s="30"/>
       <c r="R58" s="30"/>
       <c r="S58" s="29"/>
-      <c r="T58" s="109"/>
-      <c r="U58" s="101"/>
-      <c r="V58" s="101"/>
-      <c r="W58" s="100"/>
+      <c r="T58" s="70"/>
+      <c r="U58" s="71"/>
+      <c r="V58" s="71"/>
+      <c r="W58" s="72"/>
       <c r="X58" s="6"/>
       <c r="Y58" s="30"/>
       <c r="Z58" s="5"/>
@@ -5077,24 +5077,24 @@
       <c r="AK58" s="5"/>
       <c r="AL58" s="34"/>
       <c r="AM58" s="59"/>
-      <c r="AN58" s="109"/>
-      <c r="AO58" s="101"/>
-      <c r="AP58" s="101"/>
-      <c r="AQ58" s="100"/>
+      <c r="AN58" s="70"/>
+      <c r="AO58" s="71"/>
+      <c r="AP58" s="71"/>
+      <c r="AQ58" s="72"/>
       <c r="AR58" s="28"/>
       <c r="AS58" s="30"/>
       <c r="AT58" s="30"/>
       <c r="AU58" s="7"/>
       <c r="AV58" s="6"/>
       <c r="AW58" s="30"/>
-      <c r="AX58" s="99"/>
-      <c r="AY58" s="100"/>
-      <c r="AZ58" s="81"/>
+      <c r="AX58" s="101"/>
+      <c r="AY58" s="72"/>
+      <c r="AZ58" s="119"/>
     </row>
     <row r="59" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="83"/>
-      <c r="B59" s="85"/>
-      <c r="C59" s="87"/>
+      <c r="A59" s="77"/>
+      <c r="B59" s="79"/>
+      <c r="C59" s="81"/>
       <c r="D59" s="8"/>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
@@ -5111,10 +5111,10 @@
       <c r="Q59" s="9"/>
       <c r="R59" s="9"/>
       <c r="S59" s="10"/>
-      <c r="T59" s="109"/>
-      <c r="U59" s="101"/>
-      <c r="V59" s="101"/>
-      <c r="W59" s="100"/>
+      <c r="T59" s="70"/>
+      <c r="U59" s="71"/>
+      <c r="V59" s="71"/>
+      <c r="W59" s="72"/>
       <c r="X59" s="8"/>
       <c r="Y59" s="9"/>
       <c r="Z59" s="9"/>
@@ -5131,28 +5131,28 @@
       <c r="AK59" s="9"/>
       <c r="AL59" s="9"/>
       <c r="AM59" s="10"/>
-      <c r="AN59" s="109"/>
-      <c r="AO59" s="101"/>
-      <c r="AP59" s="101"/>
-      <c r="AQ59" s="100"/>
+      <c r="AN59" s="70"/>
+      <c r="AO59" s="71"/>
+      <c r="AP59" s="71"/>
+      <c r="AQ59" s="72"/>
       <c r="AR59" s="8"/>
       <c r="AS59" s="9"/>
       <c r="AT59" s="9"/>
       <c r="AU59" s="10"/>
       <c r="AV59" s="8"/>
       <c r="AW59" s="9"/>
-      <c r="AX59" s="99"/>
-      <c r="AY59" s="100"/>
-      <c r="AZ59" s="80"/>
+      <c r="AX59" s="101"/>
+      <c r="AY59" s="72"/>
+      <c r="AZ59" s="118"/>
     </row>
     <row r="60" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A60" s="88" t="s">
+      <c r="A60" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="B60" s="90">
+      <c r="B60" s="78">
         <v>0.5</v>
       </c>
-      <c r="C60" s="92"/>
+      <c r="C60" s="80"/>
       <c r="D60" s="15"/>
       <c r="E60" s="16"/>
       <c r="F60" s="16"/>
@@ -5169,10 +5169,10 @@
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
       <c r="S60" s="17"/>
-      <c r="T60" s="109"/>
-      <c r="U60" s="101"/>
-      <c r="V60" s="101"/>
-      <c r="W60" s="100"/>
+      <c r="T60" s="70"/>
+      <c r="U60" s="71"/>
+      <c r="V60" s="71"/>
+      <c r="W60" s="72"/>
       <c r="X60" s="15"/>
       <c r="Y60" s="16"/>
       <c r="Z60" s="16"/>
@@ -5189,26 +5189,26 @@
       <c r="AK60" s="16"/>
       <c r="AL60" s="16"/>
       <c r="AM60" s="17"/>
-      <c r="AN60" s="109"/>
-      <c r="AO60" s="101"/>
-      <c r="AP60" s="101"/>
-      <c r="AQ60" s="100"/>
+      <c r="AN60" s="70"/>
+      <c r="AO60" s="71"/>
+      <c r="AP60" s="71"/>
+      <c r="AQ60" s="72"/>
       <c r="AR60" s="23"/>
       <c r="AS60" s="16"/>
       <c r="AT60" s="16"/>
       <c r="AU60" s="17"/>
       <c r="AV60" s="15"/>
       <c r="AW60" s="16"/>
-      <c r="AX60" s="99"/>
-      <c r="AY60" s="100"/>
-      <c r="AZ60" s="94" t="s">
+      <c r="AX60" s="101"/>
+      <c r="AY60" s="72"/>
+      <c r="AZ60" s="85" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A61" s="89"/>
-      <c r="B61" s="91"/>
-      <c r="C61" s="93"/>
+      <c r="A61" s="88"/>
+      <c r="B61" s="89"/>
+      <c r="C61" s="90"/>
       <c r="D61" s="11"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -5225,10 +5225,10 @@
       <c r="Q61" s="3"/>
       <c r="R61" s="3"/>
       <c r="S61" s="12"/>
-      <c r="T61" s="109"/>
-      <c r="U61" s="101"/>
-      <c r="V61" s="101"/>
-      <c r="W61" s="100"/>
+      <c r="T61" s="70"/>
+      <c r="U61" s="71"/>
+      <c r="V61" s="71"/>
+      <c r="W61" s="72"/>
       <c r="X61" s="11"/>
       <c r="Y61" s="3"/>
       <c r="Z61" s="3"/>
@@ -5245,28 +5245,28 @@
       <c r="AK61" s="32"/>
       <c r="AL61" s="3"/>
       <c r="AM61" s="12"/>
-      <c r="AN61" s="109"/>
-      <c r="AO61" s="101"/>
-      <c r="AP61" s="101"/>
-      <c r="AQ61" s="100"/>
+      <c r="AN61" s="70"/>
+      <c r="AO61" s="71"/>
+      <c r="AP61" s="71"/>
+      <c r="AQ61" s="72"/>
       <c r="AR61" s="11"/>
       <c r="AS61" s="3"/>
       <c r="AT61" s="3"/>
       <c r="AU61" s="12"/>
       <c r="AV61" s="33"/>
       <c r="AW61" s="3"/>
-      <c r="AX61" s="99"/>
-      <c r="AY61" s="100"/>
-      <c r="AZ61" s="95"/>
+      <c r="AX61" s="101"/>
+      <c r="AY61" s="72"/>
+      <c r="AZ61" s="86"/>
     </row>
     <row r="62" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A62" s="82" t="s">
+      <c r="A62" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="B62" s="84">
+      <c r="B62" s="92">
         <v>2</v>
       </c>
-      <c r="C62" s="116"/>
+      <c r="C62" s="93"/>
       <c r="D62" s="28"/>
       <c r="E62" s="30"/>
       <c r="F62" s="30"/>
@@ -5283,10 +5283,10 @@
       <c r="Q62" s="30"/>
       <c r="R62" s="30"/>
       <c r="S62" s="29"/>
-      <c r="T62" s="109"/>
-      <c r="U62" s="101"/>
-      <c r="V62" s="101"/>
-      <c r="W62" s="100"/>
+      <c r="T62" s="70"/>
+      <c r="U62" s="71"/>
+      <c r="V62" s="71"/>
+      <c r="W62" s="72"/>
       <c r="X62" s="28"/>
       <c r="Y62" s="30"/>
       <c r="Z62" s="30"/>
@@ -5303,24 +5303,24 @@
       <c r="AK62" s="5"/>
       <c r="AL62" s="30"/>
       <c r="AM62" s="29"/>
-      <c r="AN62" s="109"/>
-      <c r="AO62" s="101"/>
-      <c r="AP62" s="101"/>
-      <c r="AQ62" s="100"/>
+      <c r="AN62" s="70"/>
+      <c r="AO62" s="71"/>
+      <c r="AP62" s="71"/>
+      <c r="AQ62" s="72"/>
       <c r="AR62" s="38"/>
       <c r="AS62" s="34"/>
       <c r="AT62" s="30"/>
       <c r="AU62" s="29"/>
       <c r="AV62" s="6"/>
       <c r="AW62" s="30"/>
-      <c r="AX62" s="99"/>
-      <c r="AY62" s="100"/>
-      <c r="AZ62" s="95"/>
+      <c r="AX62" s="101"/>
+      <c r="AY62" s="72"/>
+      <c r="AZ62" s="86"/>
     </row>
     <row r="63" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="83"/>
-      <c r="B63" s="85"/>
-      <c r="C63" s="87"/>
+      <c r="A63" s="77"/>
+      <c r="B63" s="79"/>
+      <c r="C63" s="81"/>
       <c r="D63" s="8"/>
       <c r="E63" s="9"/>
       <c r="F63" s="9"/>
@@ -5337,10 +5337,10 @@
       <c r="Q63" s="9"/>
       <c r="R63" s="9"/>
       <c r="S63" s="10"/>
-      <c r="T63" s="109"/>
-      <c r="U63" s="101"/>
-      <c r="V63" s="101"/>
-      <c r="W63" s="100"/>
+      <c r="T63" s="70"/>
+      <c r="U63" s="71"/>
+      <c r="V63" s="71"/>
+      <c r="W63" s="72"/>
       <c r="X63" s="8"/>
       <c r="Y63" s="9"/>
       <c r="Z63" s="9"/>
@@ -5357,28 +5357,28 @@
       <c r="AK63" s="9"/>
       <c r="AL63" s="9"/>
       <c r="AM63" s="10"/>
-      <c r="AN63" s="109"/>
-      <c r="AO63" s="101"/>
-      <c r="AP63" s="101"/>
-      <c r="AQ63" s="100"/>
+      <c r="AN63" s="70"/>
+      <c r="AO63" s="71"/>
+      <c r="AP63" s="71"/>
+      <c r="AQ63" s="72"/>
       <c r="AR63" s="8"/>
       <c r="AS63" s="9"/>
       <c r="AT63" s="9"/>
       <c r="AU63" s="10"/>
       <c r="AV63" s="8"/>
       <c r="AW63" s="9"/>
-      <c r="AX63" s="99"/>
-      <c r="AY63" s="100"/>
-      <c r="AZ63" s="96"/>
+      <c r="AX63" s="101"/>
+      <c r="AY63" s="72"/>
+      <c r="AZ63" s="87"/>
     </row>
     <row r="64" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A64" s="88" t="s">
+      <c r="A64" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="B64" s="90">
+      <c r="B64" s="78">
         <v>2.5</v>
       </c>
-      <c r="C64" s="92"/>
+      <c r="C64" s="80"/>
       <c r="D64" s="15"/>
       <c r="E64" s="16"/>
       <c r="F64" s="16"/>
@@ -5395,10 +5395,10 @@
       <c r="Q64" s="16"/>
       <c r="R64" s="16"/>
       <c r="S64" s="17"/>
-      <c r="T64" s="109"/>
-      <c r="U64" s="101"/>
-      <c r="V64" s="101"/>
-      <c r="W64" s="100"/>
+      <c r="T64" s="70"/>
+      <c r="U64" s="71"/>
+      <c r="V64" s="71"/>
+      <c r="W64" s="72"/>
       <c r="X64" s="15"/>
       <c r="Y64" s="16"/>
       <c r="Z64" s="16"/>
@@ -5415,26 +5415,26 @@
       <c r="AK64" s="16"/>
       <c r="AL64" s="16"/>
       <c r="AM64" s="17"/>
-      <c r="AN64" s="109"/>
-      <c r="AO64" s="101"/>
-      <c r="AP64" s="101"/>
-      <c r="AQ64" s="100"/>
+      <c r="AN64" s="70"/>
+      <c r="AO64" s="71"/>
+      <c r="AP64" s="71"/>
+      <c r="AQ64" s="72"/>
       <c r="AR64" s="15"/>
       <c r="AS64" s="16"/>
       <c r="AT64" s="27"/>
       <c r="AU64" s="58"/>
       <c r="AV64" s="15"/>
       <c r="AW64" s="16"/>
-      <c r="AX64" s="99"/>
-      <c r="AY64" s="100"/>
-      <c r="AZ64" s="94" t="s">
+      <c r="AX64" s="101"/>
+      <c r="AY64" s="72"/>
+      <c r="AZ64" s="85" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="83"/>
-      <c r="B65" s="85"/>
-      <c r="C65" s="87"/>
+      <c r="A65" s="77"/>
+      <c r="B65" s="79"/>
+      <c r="C65" s="81"/>
       <c r="D65" s="8"/>
       <c r="E65" s="9"/>
       <c r="F65" s="9"/>
@@ -5451,10 +5451,10 @@
       <c r="Q65" s="9"/>
       <c r="R65" s="9"/>
       <c r="S65" s="10"/>
-      <c r="T65" s="110"/>
-      <c r="U65" s="111"/>
-      <c r="V65" s="111"/>
-      <c r="W65" s="103"/>
+      <c r="T65" s="73"/>
+      <c r="U65" s="74"/>
+      <c r="V65" s="74"/>
+      <c r="W65" s="75"/>
       <c r="X65" s="8"/>
       <c r="Y65" s="9"/>
       <c r="Z65" s="9"/>
@@ -5471,10 +5471,10 @@
       <c r="AK65" s="9"/>
       <c r="AL65" s="9"/>
       <c r="AM65" s="10"/>
-      <c r="AN65" s="110"/>
-      <c r="AO65" s="111"/>
-      <c r="AP65" s="111"/>
-      <c r="AQ65" s="103"/>
+      <c r="AN65" s="73"/>
+      <c r="AO65" s="74"/>
+      <c r="AP65" s="74"/>
+      <c r="AQ65" s="75"/>
       <c r="AR65" s="8"/>
       <c r="AS65" s="9"/>
       <c r="AT65" s="9"/>
@@ -5482,8 +5482,8 @@
       <c r="AV65" s="8"/>
       <c r="AW65" s="9"/>
       <c r="AX65" s="102"/>
-      <c r="AY65" s="103"/>
-      <c r="AZ65" s="96"/>
+      <c r="AY65" s="75"/>
+      <c r="AZ65" s="87"/>
     </row>
     <row r="66" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="14" t="s">
@@ -5549,6 +5549,112 @@
     </row>
   </sheetData>
   <mergeCells count="130">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="AZ28:AZ29"/>
+    <mergeCell ref="AZ30:AZ59"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="X1:AA1"/>
+    <mergeCell ref="X2:AA2"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="AZ60:AZ63"/>
+    <mergeCell ref="AZ64:AZ65"/>
+    <mergeCell ref="AX4:AY65"/>
+    <mergeCell ref="AR1:AU1"/>
+    <mergeCell ref="AR2:AU2"/>
+    <mergeCell ref="AV1:AY1"/>
+    <mergeCell ref="AV2:AY2"/>
+    <mergeCell ref="AZ1:AZ3"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AF2:AI2"/>
+    <mergeCell ref="AJ1:AM1"/>
+    <mergeCell ref="AJ2:AM2"/>
+    <mergeCell ref="AN1:AQ1"/>
+    <mergeCell ref="AN2:AQ2"/>
+    <mergeCell ref="AN4:AQ65"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C46:C47"/>
     <mergeCell ref="T4:W65"/>
     <mergeCell ref="A64:A65"/>
     <mergeCell ref="B64:B65"/>
@@ -5573,112 +5679,6 @@
     <mergeCell ref="C52:C53"/>
     <mergeCell ref="A54:A55"/>
     <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="AZ60:AZ63"/>
-    <mergeCell ref="AZ64:AZ65"/>
-    <mergeCell ref="AX4:AY65"/>
-    <mergeCell ref="AR1:AU1"/>
-    <mergeCell ref="AR2:AU2"/>
-    <mergeCell ref="AV1:AY1"/>
-    <mergeCell ref="AV2:AY2"/>
-    <mergeCell ref="AZ1:AZ3"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AF2:AI2"/>
-    <mergeCell ref="AJ1:AM1"/>
-    <mergeCell ref="AJ2:AM2"/>
-    <mergeCell ref="AN1:AQ1"/>
-    <mergeCell ref="AN2:AQ2"/>
-    <mergeCell ref="AN4:AQ65"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="AZ28:AZ29"/>
-    <mergeCell ref="AZ30:AZ59"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="T2:W2"/>
-    <mergeCell ref="X1:AA1"/>
-    <mergeCell ref="X2:AA2"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="47" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Super tag keine schwierigkeiten mit GIT
</commit_message>
<xml_diff>
--- a/Doku/Shannon_Neil_Schuerch_Zeitplan_IPA_2022.xlsx
+++ b/Doku/Shannon_Neil_Schuerch_Zeitplan_IPA_2022.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Dashboard\Doku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Dashboardd\Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A62443-8FD1-467C-AB51-58E063C29111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED9A8AD-839F-499D-9241-DF5901445F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14625" xr2:uid="{B08A1154-B080-432D-B17F-9B53C1DBF0AA}"/>
   </bookViews>
@@ -1115,135 +1115,9 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1265,6 +1139,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1274,9 +1166,117 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1596,8 +1596,8 @@
   </sheetPr>
   <dimension ref="A1:BC66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R43" sqref="R43"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI55" sqref="AI55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,169 +1654,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="D1" s="103" t="s">
+      <c r="C1" s="74"/>
+      <c r="D1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="103" t="s">
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="103" t="s">
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="104"/>
-      <c r="N1" s="104"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="103" t="s">
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="104"/>
-      <c r="R1" s="104"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="103" t="s">
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="104"/>
-      <c r="V1" s="104"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="103" t="s">
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="79"/>
+      <c r="X1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="Y1" s="104"/>
-      <c r="Z1" s="104"/>
-      <c r="AA1" s="105"/>
-      <c r="AB1" s="103" t="s">
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="79"/>
+      <c r="AB1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="AC1" s="104"/>
-      <c r="AD1" s="104"/>
-      <c r="AE1" s="105"/>
-      <c r="AF1" s="103" t="s">
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="79"/>
+      <c r="AF1" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="AG1" s="104"/>
-      <c r="AH1" s="104"/>
-      <c r="AI1" s="105"/>
-      <c r="AJ1" s="103" t="s">
+      <c r="AG1" s="78"/>
+      <c r="AH1" s="78"/>
+      <c r="AI1" s="79"/>
+      <c r="AJ1" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="AK1" s="104"/>
-      <c r="AL1" s="104"/>
-      <c r="AM1" s="105"/>
-      <c r="AN1" s="103" t="s">
+      <c r="AK1" s="78"/>
+      <c r="AL1" s="78"/>
+      <c r="AM1" s="79"/>
+      <c r="AN1" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="AO1" s="104"/>
-      <c r="AP1" s="104"/>
-      <c r="AQ1" s="105"/>
-      <c r="AR1" s="103" t="s">
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="78"/>
+      <c r="AQ1" s="79"/>
+      <c r="AR1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="AS1" s="104"/>
-      <c r="AT1" s="104"/>
-      <c r="AU1" s="105"/>
-      <c r="AV1" s="103" t="s">
+      <c r="AS1" s="78"/>
+      <c r="AT1" s="78"/>
+      <c r="AU1" s="79"/>
+      <c r="AV1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="AW1" s="104"/>
-      <c r="AX1" s="104"/>
-      <c r="AY1" s="105"/>
-      <c r="AZ1" s="82" t="s">
+      <c r="AW1" s="78"/>
+      <c r="AX1" s="78"/>
+      <c r="AY1" s="79"/>
+      <c r="AZ1" s="108" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A2" s="111"/>
-      <c r="B2" s="115"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="106">
+      <c r="A2" s="71"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="80">
         <v>44627</v>
       </c>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="106">
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="80">
         <v>44628</v>
       </c>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="106">
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="80">
         <v>44629</v>
       </c>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="108"/>
-      <c r="P2" s="106">
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="80">
         <v>44630</v>
       </c>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="107"/>
-      <c r="S2" s="108"/>
-      <c r="T2" s="106">
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="80">
         <v>44631</v>
       </c>
-      <c r="U2" s="107"/>
-      <c r="V2" s="107"/>
-      <c r="W2" s="108"/>
-      <c r="X2" s="106">
+      <c r="U2" s="81"/>
+      <c r="V2" s="81"/>
+      <c r="W2" s="82"/>
+      <c r="X2" s="80">
         <v>44634</v>
       </c>
-      <c r="Y2" s="107"/>
-      <c r="Z2" s="107"/>
-      <c r="AA2" s="108"/>
-      <c r="AB2" s="106">
+      <c r="Y2" s="81"/>
+      <c r="Z2" s="81"/>
+      <c r="AA2" s="82"/>
+      <c r="AB2" s="80">
         <v>44635</v>
       </c>
-      <c r="AC2" s="107"/>
-      <c r="AD2" s="107"/>
-      <c r="AE2" s="108"/>
-      <c r="AF2" s="106">
+      <c r="AC2" s="81"/>
+      <c r="AD2" s="81"/>
+      <c r="AE2" s="82"/>
+      <c r="AF2" s="80">
         <v>44636</v>
       </c>
-      <c r="AG2" s="107"/>
-      <c r="AH2" s="107"/>
-      <c r="AI2" s="108"/>
-      <c r="AJ2" s="106">
+      <c r="AG2" s="81"/>
+      <c r="AH2" s="81"/>
+      <c r="AI2" s="82"/>
+      <c r="AJ2" s="80">
         <v>44637</v>
       </c>
-      <c r="AK2" s="107"/>
-      <c r="AL2" s="107"/>
-      <c r="AM2" s="108"/>
-      <c r="AN2" s="106">
+      <c r="AK2" s="81"/>
+      <c r="AL2" s="81"/>
+      <c r="AM2" s="82"/>
+      <c r="AN2" s="80">
         <v>44638</v>
       </c>
-      <c r="AO2" s="107"/>
-      <c r="AP2" s="107"/>
-      <c r="AQ2" s="108"/>
-      <c r="AR2" s="106">
+      <c r="AO2" s="81"/>
+      <c r="AP2" s="81"/>
+      <c r="AQ2" s="82"/>
+      <c r="AR2" s="80">
         <v>44641</v>
       </c>
-      <c r="AS2" s="107"/>
-      <c r="AT2" s="107"/>
-      <c r="AU2" s="108"/>
-      <c r="AV2" s="106">
+      <c r="AS2" s="81"/>
+      <c r="AT2" s="81"/>
+      <c r="AU2" s="82"/>
+      <c r="AV2" s="80">
         <v>44642</v>
       </c>
-      <c r="AW2" s="107"/>
-      <c r="AX2" s="107"/>
-      <c r="AY2" s="108"/>
-      <c r="AZ2" s="83"/>
+      <c r="AW2" s="81"/>
+      <c r="AX2" s="81"/>
+      <c r="AY2" s="82"/>
+      <c r="AZ2" s="109"/>
     </row>
     <row r="3" spans="1:55" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="112"/>
+      <c r="A3" s="72"/>
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
@@ -1967,16 +1967,16 @@
       <c r="AY3" s="12">
         <v>17</v>
       </c>
-      <c r="AZ3" s="109"/>
+      <c r="AZ3" s="110"/>
     </row>
     <row r="4" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="78">
+      <c r="B4" s="94">
         <v>4</v>
       </c>
-      <c r="C4" s="80">
+      <c r="C4" s="96">
         <v>2</v>
       </c>
       <c r="D4" s="15"/>
@@ -1995,12 +1995,12 @@
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
       <c r="S4" s="17"/>
-      <c r="T4" s="67" t="s">
+      <c r="T4" s="111" t="s">
         <v>43</v>
       </c>
-      <c r="U4" s="68"/>
-      <c r="V4" s="68"/>
-      <c r="W4" s="69"/>
+      <c r="U4" s="112"/>
+      <c r="V4" s="112"/>
+      <c r="W4" s="102"/>
       <c r="X4" s="15"/>
       <c r="Y4" s="16"/>
       <c r="Z4" s="16"/>
@@ -2017,32 +2017,32 @@
       <c r="AK4" s="16"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="17"/>
-      <c r="AN4" s="67" t="s">
+      <c r="AN4" s="111" t="s">
         <v>43</v>
       </c>
-      <c r="AO4" s="68"/>
-      <c r="AP4" s="68"/>
-      <c r="AQ4" s="69"/>
+      <c r="AO4" s="112"/>
+      <c r="AP4" s="112"/>
+      <c r="AQ4" s="102"/>
       <c r="AR4" s="15"/>
       <c r="AS4" s="16"/>
       <c r="AT4" s="16"/>
       <c r="AU4" s="17"/>
       <c r="AV4" s="15"/>
       <c r="AW4" s="16"/>
-      <c r="AX4" s="100" t="s">
+      <c r="AX4" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="AY4" s="69"/>
-      <c r="AZ4" s="82"/>
+      <c r="AY4" s="102"/>
+      <c r="AZ4" s="108"/>
       <c r="BB4" s="60" t="s">
         <v>50</v>
       </c>
       <c r="BC4" s="61"/>
     </row>
     <row r="5" spans="1:55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96"/>
-      <c r="B5" s="97"/>
-      <c r="C5" s="98"/>
+      <c r="A5" s="116"/>
+      <c r="B5" s="117"/>
+      <c r="C5" s="118"/>
       <c r="D5" s="33"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -2059,10 +2059,10 @@
       <c r="Q5" s="32"/>
       <c r="R5" s="3"/>
       <c r="S5" s="12"/>
-      <c r="T5" s="70"/>
-      <c r="U5" s="71"/>
-      <c r="V5" s="71"/>
-      <c r="W5" s="72"/>
+      <c r="T5" s="113"/>
+      <c r="U5" s="105"/>
+      <c r="V5" s="105"/>
+      <c r="W5" s="104"/>
       <c r="X5" s="11"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="32"/>
@@ -2079,32 +2079,32 @@
       <c r="AK5" s="3"/>
       <c r="AL5" s="3"/>
       <c r="AM5" s="12"/>
-      <c r="AN5" s="70"/>
-      <c r="AO5" s="71"/>
-      <c r="AP5" s="71"/>
-      <c r="AQ5" s="72"/>
+      <c r="AN5" s="113"/>
+      <c r="AO5" s="105"/>
+      <c r="AP5" s="105"/>
+      <c r="AQ5" s="104"/>
       <c r="AR5" s="11"/>
       <c r="AS5" s="3"/>
       <c r="AT5" s="3"/>
       <c r="AU5" s="12"/>
       <c r="AV5" s="11"/>
       <c r="AW5" s="3"/>
-      <c r="AX5" s="101"/>
-      <c r="AY5" s="72"/>
-      <c r="AZ5" s="83"/>
+      <c r="AX5" s="103"/>
+      <c r="AY5" s="104"/>
+      <c r="AZ5" s="109"/>
       <c r="BB5" s="62" t="s">
         <v>51</v>
       </c>
       <c r="BC5" s="63"/>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="92">
+      <c r="B6" s="88">
         <v>32</v>
       </c>
-      <c r="C6" s="93"/>
+      <c r="C6" s="120"/>
       <c r="D6" s="13"/>
       <c r="E6" s="35"/>
       <c r="F6" s="30"/>
@@ -2121,10 +2121,10 @@
       <c r="Q6" s="24"/>
       <c r="R6" s="47"/>
       <c r="S6" s="48"/>
-      <c r="T6" s="70"/>
-      <c r="U6" s="71"/>
-      <c r="V6" s="71"/>
-      <c r="W6" s="72"/>
+      <c r="T6" s="113"/>
+      <c r="U6" s="105"/>
+      <c r="V6" s="105"/>
+      <c r="W6" s="104"/>
       <c r="X6" s="38"/>
       <c r="Y6" s="34"/>
       <c r="Z6" s="24"/>
@@ -2141,28 +2141,28 @@
       <c r="AK6" s="34"/>
       <c r="AL6" s="34"/>
       <c r="AM6" s="49"/>
-      <c r="AN6" s="70"/>
-      <c r="AO6" s="71"/>
-      <c r="AP6" s="71"/>
-      <c r="AQ6" s="72"/>
+      <c r="AN6" s="113"/>
+      <c r="AO6" s="105"/>
+      <c r="AP6" s="105"/>
+      <c r="AQ6" s="104"/>
       <c r="AR6" s="38"/>
       <c r="AS6" s="34"/>
       <c r="AT6" s="34"/>
       <c r="AU6" s="49"/>
       <c r="AV6" s="38"/>
       <c r="AW6" s="34"/>
-      <c r="AX6" s="101"/>
-      <c r="AY6" s="72"/>
-      <c r="AZ6" s="83"/>
+      <c r="AX6" s="103"/>
+      <c r="AY6" s="104"/>
+      <c r="AZ6" s="109"/>
       <c r="BB6" s="62" t="s">
         <v>52</v>
       </c>
       <c r="BC6" s="64"/>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A7" s="96"/>
-      <c r="B7" s="97"/>
-      <c r="C7" s="98"/>
+      <c r="A7" s="116"/>
+      <c r="B7" s="117"/>
+      <c r="C7" s="118"/>
       <c r="D7" s="33"/>
       <c r="E7" s="32"/>
       <c r="F7" s="3"/>
@@ -2175,54 +2175,54 @@
       <c r="M7" s="40"/>
       <c r="N7" s="40"/>
       <c r="O7" s="66"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="70"/>
-      <c r="U7" s="71"/>
-      <c r="V7" s="71"/>
-      <c r="W7" s="72"/>
-      <c r="X7" s="33"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="12"/>
-      <c r="AB7" s="33"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="12"/>
-      <c r="AF7" s="11"/>
-      <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
-      <c r="AI7" s="12"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="65"/>
+      <c r="T7" s="113"/>
+      <c r="U7" s="105"/>
+      <c r="V7" s="105"/>
+      <c r="W7" s="104"/>
+      <c r="X7" s="57"/>
+      <c r="Y7" s="40"/>
+      <c r="Z7" s="40"/>
+      <c r="AA7" s="65"/>
+      <c r="AB7" s="57"/>
+      <c r="AC7" s="40"/>
+      <c r="AD7" s="40"/>
+      <c r="AE7" s="65"/>
+      <c r="AF7" s="39"/>
+      <c r="AG7" s="40"/>
+      <c r="AH7" s="40"/>
+      <c r="AI7" s="65"/>
       <c r="AJ7" s="11"/>
       <c r="AK7" s="3"/>
       <c r="AL7" s="3"/>
       <c r="AM7" s="12"/>
-      <c r="AN7" s="70"/>
-      <c r="AO7" s="71"/>
-      <c r="AP7" s="71"/>
-      <c r="AQ7" s="72"/>
+      <c r="AN7" s="113"/>
+      <c r="AO7" s="105"/>
+      <c r="AP7" s="105"/>
+      <c r="AQ7" s="104"/>
       <c r="AR7" s="11"/>
       <c r="AS7" s="3"/>
       <c r="AT7" s="3"/>
       <c r="AU7" s="12"/>
       <c r="AV7" s="11"/>
       <c r="AW7" s="3"/>
-      <c r="AX7" s="101"/>
-      <c r="AY7" s="72"/>
-      <c r="AZ7" s="83"/>
+      <c r="AX7" s="103"/>
+      <c r="AY7" s="104"/>
+      <c r="AZ7" s="109"/>
       <c r="BB7" s="4"/>
       <c r="BC7" s="4"/>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="95">
+      <c r="B8" s="121">
         <v>4</v>
       </c>
-      <c r="C8" s="93">
+      <c r="C8" s="120">
         <v>5</v>
       </c>
       <c r="D8" s="26"/>
@@ -2241,10 +2241,10 @@
       <c r="Q8" s="30"/>
       <c r="R8" s="30"/>
       <c r="S8" s="29"/>
-      <c r="T8" s="70"/>
-      <c r="U8" s="71"/>
-      <c r="V8" s="71"/>
-      <c r="W8" s="72"/>
+      <c r="T8" s="113"/>
+      <c r="U8" s="105"/>
+      <c r="V8" s="105"/>
+      <c r="W8" s="104"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="30"/>
       <c r="Z8" s="30"/>
@@ -2261,26 +2261,26 @@
       <c r="AK8" s="30"/>
       <c r="AL8" s="30"/>
       <c r="AM8" s="29"/>
-      <c r="AN8" s="70"/>
-      <c r="AO8" s="71"/>
-      <c r="AP8" s="71"/>
-      <c r="AQ8" s="72"/>
+      <c r="AN8" s="113"/>
+      <c r="AO8" s="105"/>
+      <c r="AP8" s="105"/>
+      <c r="AQ8" s="104"/>
       <c r="AR8" s="28"/>
       <c r="AS8" s="30"/>
       <c r="AT8" s="30"/>
       <c r="AU8" s="29"/>
       <c r="AV8" s="28"/>
       <c r="AW8" s="30"/>
-      <c r="AX8" s="101"/>
-      <c r="AY8" s="72"/>
-      <c r="AZ8" s="83"/>
+      <c r="AX8" s="103"/>
+      <c r="AY8" s="104"/>
+      <c r="AZ8" s="109"/>
       <c r="BB8" s="4"/>
       <c r="BC8" s="4"/>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A9" s="88"/>
-      <c r="B9" s="89"/>
-      <c r="C9" s="98"/>
+      <c r="A9" s="93"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="118"/>
       <c r="D9" s="39"/>
       <c r="E9" s="40"/>
       <c r="F9" s="54"/>
@@ -2297,10 +2297,10 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="12"/>
-      <c r="T9" s="70"/>
-      <c r="U9" s="71"/>
-      <c r="V9" s="71"/>
-      <c r="W9" s="72"/>
+      <c r="T9" s="113"/>
+      <c r="U9" s="105"/>
+      <c r="V9" s="105"/>
+      <c r="W9" s="104"/>
       <c r="X9" s="11"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
@@ -2317,30 +2317,30 @@
       <c r="AK9" s="3"/>
       <c r="AL9" s="32"/>
       <c r="AM9" s="12"/>
-      <c r="AN9" s="70"/>
-      <c r="AO9" s="71"/>
-      <c r="AP9" s="71"/>
-      <c r="AQ9" s="72"/>
+      <c r="AN9" s="113"/>
+      <c r="AO9" s="105"/>
+      <c r="AP9" s="105"/>
+      <c r="AQ9" s="104"/>
       <c r="AR9" s="11"/>
       <c r="AS9" s="3"/>
       <c r="AT9" s="3"/>
       <c r="AU9" s="12"/>
       <c r="AV9" s="11"/>
       <c r="AW9" s="3"/>
-      <c r="AX9" s="101"/>
-      <c r="AY9" s="72"/>
-      <c r="AZ9" s="83"/>
+      <c r="AX9" s="103"/>
+      <c r="AY9" s="104"/>
+      <c r="AZ9" s="109"/>
       <c r="BB9" s="4"/>
       <c r="BC9" s="4"/>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="92">
+      <c r="B10" s="88">
         <v>2</v>
       </c>
-      <c r="C10" s="99">
+      <c r="C10" s="90">
         <v>1</v>
       </c>
       <c r="D10" s="28"/>
@@ -2359,10 +2359,10 @@
       <c r="Q10" s="30"/>
       <c r="R10" s="30"/>
       <c r="S10" s="29"/>
-      <c r="T10" s="70"/>
-      <c r="U10" s="71"/>
-      <c r="V10" s="71"/>
-      <c r="W10" s="72"/>
+      <c r="T10" s="113"/>
+      <c r="U10" s="105"/>
+      <c r="V10" s="105"/>
+      <c r="W10" s="104"/>
       <c r="X10" s="28"/>
       <c r="Y10" s="30"/>
       <c r="Z10" s="30"/>
@@ -2379,26 +2379,26 @@
       <c r="AK10" s="30"/>
       <c r="AL10" s="5"/>
       <c r="AM10" s="29"/>
-      <c r="AN10" s="70"/>
-      <c r="AO10" s="71"/>
-      <c r="AP10" s="71"/>
-      <c r="AQ10" s="72"/>
+      <c r="AN10" s="113"/>
+      <c r="AO10" s="105"/>
+      <c r="AP10" s="105"/>
+      <c r="AQ10" s="104"/>
       <c r="AR10" s="28"/>
       <c r="AS10" s="30"/>
       <c r="AT10" s="30"/>
       <c r="AU10" s="29"/>
       <c r="AV10" s="28"/>
       <c r="AW10" s="30"/>
-      <c r="AX10" s="101"/>
-      <c r="AY10" s="72"/>
-      <c r="AZ10" s="83"/>
+      <c r="AX10" s="103"/>
+      <c r="AY10" s="104"/>
+      <c r="AZ10" s="109"/>
       <c r="BB10" s="4"/>
       <c r="BC10" s="4"/>
     </row>
     <row r="11" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="77"/>
-      <c r="B11" s="79"/>
-      <c r="C11" s="81"/>
+      <c r="A11" s="87"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
       <c r="F11" s="53"/>
@@ -2415,10 +2415,10 @@
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="70"/>
-      <c r="U11" s="71"/>
-      <c r="V11" s="71"/>
-      <c r="W11" s="72"/>
+      <c r="T11" s="113"/>
+      <c r="U11" s="105"/>
+      <c r="V11" s="105"/>
+      <c r="W11" s="104"/>
       <c r="X11" s="8"/>
       <c r="Y11" s="9"/>
       <c r="Z11" s="9"/>
@@ -2435,28 +2435,28 @@
       <c r="AK11" s="9"/>
       <c r="AL11" s="9"/>
       <c r="AM11" s="10"/>
-      <c r="AN11" s="70"/>
-      <c r="AO11" s="71"/>
-      <c r="AP11" s="71"/>
-      <c r="AQ11" s="72"/>
+      <c r="AN11" s="113"/>
+      <c r="AO11" s="105"/>
+      <c r="AP11" s="105"/>
+      <c r="AQ11" s="104"/>
       <c r="AR11" s="8"/>
       <c r="AS11" s="9"/>
       <c r="AT11" s="9"/>
       <c r="AU11" s="10"/>
       <c r="AV11" s="8"/>
       <c r="AW11" s="9"/>
-      <c r="AX11" s="101"/>
-      <c r="AY11" s="72"/>
-      <c r="AZ11" s="84"/>
+      <c r="AX11" s="103"/>
+      <c r="AY11" s="104"/>
+      <c r="AZ11" s="122"/>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A12" s="76" t="s">
+      <c r="A12" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="78">
+      <c r="B12" s="94">
         <v>1.5</v>
       </c>
-      <c r="C12" s="80"/>
+      <c r="C12" s="96"/>
       <c r="D12" s="18"/>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
@@ -2473,10 +2473,10 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
       <c r="S12" s="17"/>
-      <c r="T12" s="70"/>
-      <c r="U12" s="71"/>
-      <c r="V12" s="71"/>
-      <c r="W12" s="72"/>
+      <c r="T12" s="113"/>
+      <c r="U12" s="105"/>
+      <c r="V12" s="105"/>
+      <c r="W12" s="104"/>
       <c r="X12" s="15"/>
       <c r="Y12" s="16"/>
       <c r="Z12" s="16"/>
@@ -2493,26 +2493,26 @@
       <c r="AK12" s="16"/>
       <c r="AL12" s="16"/>
       <c r="AM12" s="17"/>
-      <c r="AN12" s="70"/>
-      <c r="AO12" s="71"/>
-      <c r="AP12" s="71"/>
-      <c r="AQ12" s="72"/>
+      <c r="AN12" s="113"/>
+      <c r="AO12" s="105"/>
+      <c r="AP12" s="105"/>
+      <c r="AQ12" s="104"/>
       <c r="AR12" s="15"/>
       <c r="AS12" s="16"/>
       <c r="AT12" s="16"/>
       <c r="AU12" s="17"/>
       <c r="AV12" s="15"/>
       <c r="AW12" s="16"/>
-      <c r="AX12" s="101"/>
-      <c r="AY12" s="72"/>
-      <c r="AZ12" s="85" t="s">
+      <c r="AX12" s="103"/>
+      <c r="AY12" s="104"/>
+      <c r="AZ12" s="98" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A13" s="88"/>
-      <c r="B13" s="89"/>
-      <c r="C13" s="90"/>
+      <c r="A13" s="93"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="42"/>
       <c r="E13" s="41"/>
       <c r="F13" s="43"/>
@@ -2529,10 +2529,10 @@
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="12"/>
-      <c r="T13" s="70"/>
-      <c r="U13" s="71"/>
-      <c r="V13" s="71"/>
-      <c r="W13" s="72"/>
+      <c r="T13" s="113"/>
+      <c r="U13" s="105"/>
+      <c r="V13" s="105"/>
+      <c r="W13" s="104"/>
       <c r="X13" s="11"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
@@ -2549,28 +2549,28 @@
       <c r="AK13" s="32"/>
       <c r="AL13" s="32"/>
       <c r="AM13" s="31"/>
-      <c r="AN13" s="70"/>
-      <c r="AO13" s="71"/>
-      <c r="AP13" s="71"/>
-      <c r="AQ13" s="72"/>
+      <c r="AN13" s="113"/>
+      <c r="AO13" s="105"/>
+      <c r="AP13" s="105"/>
+      <c r="AQ13" s="104"/>
       <c r="AR13" s="33"/>
       <c r="AS13" s="32"/>
       <c r="AT13" s="32"/>
       <c r="AU13" s="31"/>
       <c r="AV13" s="33"/>
       <c r="AW13" s="32"/>
-      <c r="AX13" s="101"/>
-      <c r="AY13" s="72"/>
-      <c r="AZ13" s="86"/>
+      <c r="AX13" s="103"/>
+      <c r="AY13" s="104"/>
+      <c r="AZ13" s="99"/>
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A14" s="91" t="s">
+      <c r="A14" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="92">
+      <c r="B14" s="88">
         <v>1.5</v>
       </c>
-      <c r="C14" s="93"/>
+      <c r="C14" s="120"/>
       <c r="D14" s="28"/>
       <c r="E14" s="5"/>
       <c r="F14" s="30"/>
@@ -2587,10 +2587,10 @@
       <c r="Q14" s="30"/>
       <c r="R14" s="30"/>
       <c r="S14" s="29"/>
-      <c r="T14" s="70"/>
-      <c r="U14" s="71"/>
-      <c r="V14" s="71"/>
-      <c r="W14" s="72"/>
+      <c r="T14" s="113"/>
+      <c r="U14" s="105"/>
+      <c r="V14" s="105"/>
+      <c r="W14" s="104"/>
       <c r="X14" s="28"/>
       <c r="Y14" s="30"/>
       <c r="Z14" s="30"/>
@@ -2607,24 +2607,24 @@
       <c r="AK14" s="5"/>
       <c r="AL14" s="5"/>
       <c r="AM14" s="7"/>
-      <c r="AN14" s="70"/>
-      <c r="AO14" s="71"/>
-      <c r="AP14" s="71"/>
-      <c r="AQ14" s="72"/>
+      <c r="AN14" s="113"/>
+      <c r="AO14" s="105"/>
+      <c r="AP14" s="105"/>
+      <c r="AQ14" s="104"/>
       <c r="AR14" s="6"/>
       <c r="AS14" s="5"/>
       <c r="AT14" s="5"/>
       <c r="AU14" s="7"/>
       <c r="AV14" s="6"/>
       <c r="AW14" s="5"/>
-      <c r="AX14" s="101"/>
-      <c r="AY14" s="72"/>
-      <c r="AZ14" s="86"/>
+      <c r="AX14" s="103"/>
+      <c r="AY14" s="104"/>
+      <c r="AZ14" s="99"/>
     </row>
     <row r="15" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="77"/>
-      <c r="B15" s="79"/>
-      <c r="C15" s="81"/>
+      <c r="A15" s="87"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="91"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -2641,10 +2641,10 @@
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="70"/>
-      <c r="U15" s="71"/>
-      <c r="V15" s="71"/>
-      <c r="W15" s="72"/>
+      <c r="T15" s="113"/>
+      <c r="U15" s="105"/>
+      <c r="V15" s="105"/>
+      <c r="W15" s="104"/>
       <c r="X15" s="8"/>
       <c r="Y15" s="9"/>
       <c r="Z15" s="9"/>
@@ -2661,28 +2661,28 @@
       <c r="AK15" s="9"/>
       <c r="AL15" s="9"/>
       <c r="AM15" s="10"/>
-      <c r="AN15" s="70"/>
-      <c r="AO15" s="71"/>
-      <c r="AP15" s="71"/>
-      <c r="AQ15" s="72"/>
+      <c r="AN15" s="113"/>
+      <c r="AO15" s="105"/>
+      <c r="AP15" s="105"/>
+      <c r="AQ15" s="104"/>
       <c r="AR15" s="8"/>
       <c r="AS15" s="9"/>
       <c r="AT15" s="9"/>
       <c r="AU15" s="10"/>
       <c r="AV15" s="8"/>
       <c r="AW15" s="9"/>
-      <c r="AX15" s="101"/>
-      <c r="AY15" s="72"/>
-      <c r="AZ15" s="87"/>
+      <c r="AX15" s="103"/>
+      <c r="AY15" s="104"/>
+      <c r="AZ15" s="100"/>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A16" s="76" t="s">
+      <c r="A16" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="78">
+      <c r="B16" s="94">
         <v>1</v>
       </c>
-      <c r="C16" s="80"/>
+      <c r="C16" s="96"/>
       <c r="D16" s="15"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
@@ -2699,10 +2699,10 @@
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
       <c r="S16" s="17"/>
-      <c r="T16" s="70"/>
-      <c r="U16" s="71"/>
-      <c r="V16" s="71"/>
-      <c r="W16" s="72"/>
+      <c r="T16" s="113"/>
+      <c r="U16" s="105"/>
+      <c r="V16" s="105"/>
+      <c r="W16" s="104"/>
       <c r="X16" s="15"/>
       <c r="Y16" s="16"/>
       <c r="Z16" s="16"/>
@@ -2719,26 +2719,26 @@
       <c r="AK16" s="16"/>
       <c r="AL16" s="16"/>
       <c r="AM16" s="17"/>
-      <c r="AN16" s="70"/>
-      <c r="AO16" s="71"/>
-      <c r="AP16" s="71"/>
-      <c r="AQ16" s="72"/>
+      <c r="AN16" s="113"/>
+      <c r="AO16" s="105"/>
+      <c r="AP16" s="105"/>
+      <c r="AQ16" s="104"/>
       <c r="AR16" s="15"/>
       <c r="AS16" s="16"/>
       <c r="AT16" s="16"/>
       <c r="AU16" s="17"/>
       <c r="AV16" s="15"/>
       <c r="AW16" s="16"/>
-      <c r="AX16" s="101"/>
-      <c r="AY16" s="72"/>
-      <c r="AZ16" s="85" t="s">
+      <c r="AX16" s="103"/>
+      <c r="AY16" s="104"/>
+      <c r="AZ16" s="98" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A17" s="96"/>
-      <c r="B17" s="89"/>
-      <c r="C17" s="90"/>
+      <c r="A17" s="116"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="97"/>
       <c r="D17" s="11"/>
       <c r="E17" s="3"/>
       <c r="F17" s="32"/>
@@ -2755,10 +2755,10 @@
       <c r="Q17" s="3"/>
       <c r="R17" s="32"/>
       <c r="S17" s="12"/>
-      <c r="T17" s="70"/>
-      <c r="U17" s="71"/>
-      <c r="V17" s="71"/>
-      <c r="W17" s="72"/>
+      <c r="T17" s="113"/>
+      <c r="U17" s="105"/>
+      <c r="V17" s="105"/>
+      <c r="W17" s="104"/>
       <c r="X17" s="33"/>
       <c r="Y17" s="32"/>
       <c r="Z17" s="32"/>
@@ -2775,28 +2775,28 @@
       <c r="AK17" s="32"/>
       <c r="AL17" s="32"/>
       <c r="AM17" s="31"/>
-      <c r="AN17" s="70"/>
-      <c r="AO17" s="71"/>
-      <c r="AP17" s="71"/>
-      <c r="AQ17" s="72"/>
+      <c r="AN17" s="113"/>
+      <c r="AO17" s="105"/>
+      <c r="AP17" s="105"/>
+      <c r="AQ17" s="104"/>
       <c r="AR17" s="33"/>
       <c r="AS17" s="32"/>
       <c r="AT17" s="32"/>
       <c r="AU17" s="31"/>
       <c r="AV17" s="33"/>
       <c r="AW17" s="3"/>
-      <c r="AX17" s="101"/>
-      <c r="AY17" s="72"/>
-      <c r="AZ17" s="86"/>
+      <c r="AX17" s="103"/>
+      <c r="AY17" s="104"/>
+      <c r="AZ17" s="99"/>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A18" s="94" t="s">
+      <c r="A18" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="92">
+      <c r="B18" s="88">
         <v>2</v>
       </c>
-      <c r="C18" s="93"/>
+      <c r="C18" s="120"/>
       <c r="D18" s="28"/>
       <c r="E18" s="30"/>
       <c r="F18" s="5"/>
@@ -2813,10 +2813,10 @@
       <c r="Q18" s="30"/>
       <c r="R18" s="5"/>
       <c r="S18" s="29"/>
-      <c r="T18" s="70"/>
-      <c r="U18" s="71"/>
-      <c r="V18" s="71"/>
-      <c r="W18" s="72"/>
+      <c r="T18" s="113"/>
+      <c r="U18" s="105"/>
+      <c r="V18" s="105"/>
+      <c r="W18" s="104"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
@@ -2833,24 +2833,24 @@
       <c r="AK18" s="5"/>
       <c r="AL18" s="5"/>
       <c r="AM18" s="7"/>
-      <c r="AN18" s="70"/>
-      <c r="AO18" s="71"/>
-      <c r="AP18" s="71"/>
-      <c r="AQ18" s="72"/>
+      <c r="AN18" s="113"/>
+      <c r="AO18" s="105"/>
+      <c r="AP18" s="105"/>
+      <c r="AQ18" s="104"/>
       <c r="AR18" s="6"/>
       <c r="AS18" s="5"/>
       <c r="AT18" s="5"/>
       <c r="AU18" s="7"/>
       <c r="AV18" s="6"/>
       <c r="AW18" s="30"/>
-      <c r="AX18" s="101"/>
-      <c r="AY18" s="72"/>
-      <c r="AZ18" s="86"/>
+      <c r="AX18" s="103"/>
+      <c r="AY18" s="104"/>
+      <c r="AZ18" s="99"/>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A19" s="88"/>
-      <c r="B19" s="89"/>
-      <c r="C19" s="90"/>
+      <c r="A19" s="93"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="97"/>
       <c r="D19" s="11"/>
       <c r="E19" s="3"/>
       <c r="F19" s="32"/>
@@ -2867,10 +2867,10 @@
       <c r="Q19" s="32"/>
       <c r="R19" s="3"/>
       <c r="S19" s="31"/>
-      <c r="T19" s="70"/>
-      <c r="U19" s="71"/>
-      <c r="V19" s="71"/>
-      <c r="W19" s="72"/>
+      <c r="T19" s="113"/>
+      <c r="U19" s="105"/>
+      <c r="V19" s="105"/>
+      <c r="W19" s="104"/>
       <c r="X19" s="33"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
@@ -2887,28 +2887,28 @@
       <c r="AK19" s="32"/>
       <c r="AL19" s="32"/>
       <c r="AM19" s="31"/>
-      <c r="AN19" s="70"/>
-      <c r="AO19" s="71"/>
-      <c r="AP19" s="71"/>
-      <c r="AQ19" s="72"/>
+      <c r="AN19" s="113"/>
+      <c r="AO19" s="105"/>
+      <c r="AP19" s="105"/>
+      <c r="AQ19" s="104"/>
       <c r="AR19" s="33"/>
       <c r="AS19" s="3"/>
       <c r="AT19" s="32"/>
       <c r="AU19" s="31"/>
       <c r="AV19" s="33"/>
       <c r="AW19" s="32"/>
-      <c r="AX19" s="101"/>
-      <c r="AY19" s="72"/>
-      <c r="AZ19" s="86"/>
+      <c r="AX19" s="103"/>
+      <c r="AY19" s="104"/>
+      <c r="AZ19" s="99"/>
     </row>
     <row r="20" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A20" s="94" t="s">
+      <c r="A20" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="92">
+      <c r="B20" s="88">
         <v>0.5</v>
       </c>
-      <c r="C20" s="93"/>
+      <c r="C20" s="120"/>
       <c r="D20" s="28"/>
       <c r="E20" s="30"/>
       <c r="F20" s="5"/>
@@ -2925,10 +2925,10 @@
       <c r="Q20" s="5"/>
       <c r="R20" s="30"/>
       <c r="S20" s="7"/>
-      <c r="T20" s="70"/>
-      <c r="U20" s="71"/>
-      <c r="V20" s="71"/>
-      <c r="W20" s="72"/>
+      <c r="T20" s="113"/>
+      <c r="U20" s="105"/>
+      <c r="V20" s="105"/>
+      <c r="W20" s="104"/>
       <c r="X20" s="6"/>
       <c r="Y20" s="30"/>
       <c r="Z20" s="30"/>
@@ -2945,24 +2945,24 @@
       <c r="AK20" s="5"/>
       <c r="AL20" s="5"/>
       <c r="AM20" s="7"/>
-      <c r="AN20" s="70"/>
-      <c r="AO20" s="71"/>
-      <c r="AP20" s="71"/>
-      <c r="AQ20" s="72"/>
+      <c r="AN20" s="113"/>
+      <c r="AO20" s="105"/>
+      <c r="AP20" s="105"/>
+      <c r="AQ20" s="104"/>
       <c r="AR20" s="6"/>
       <c r="AS20" s="30"/>
       <c r="AT20" s="5"/>
       <c r="AU20" s="7"/>
       <c r="AV20" s="6"/>
       <c r="AW20" s="5"/>
-      <c r="AX20" s="101"/>
-      <c r="AY20" s="72"/>
-      <c r="AZ20" s="86"/>
+      <c r="AX20" s="103"/>
+      <c r="AY20" s="104"/>
+      <c r="AZ20" s="99"/>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A21" s="88"/>
-      <c r="B21" s="89"/>
-      <c r="C21" s="90"/>
+      <c r="A21" s="93"/>
+      <c r="B21" s="95"/>
+      <c r="C21" s="97"/>
       <c r="D21" s="33"/>
       <c r="E21" s="32"/>
       <c r="F21" s="32"/>
@@ -2979,10 +2979,10 @@
       <c r="Q21" s="32"/>
       <c r="R21" s="32"/>
       <c r="S21" s="31"/>
-      <c r="T21" s="70"/>
-      <c r="U21" s="71"/>
-      <c r="V21" s="71"/>
-      <c r="W21" s="72"/>
+      <c r="T21" s="113"/>
+      <c r="U21" s="105"/>
+      <c r="V21" s="105"/>
+      <c r="W21" s="104"/>
       <c r="X21" s="33"/>
       <c r="Y21" s="32"/>
       <c r="Z21" s="32"/>
@@ -2999,28 +2999,28 @@
       <c r="AK21" s="32"/>
       <c r="AL21" s="32"/>
       <c r="AM21" s="31"/>
-      <c r="AN21" s="70"/>
-      <c r="AO21" s="71"/>
-      <c r="AP21" s="71"/>
-      <c r="AQ21" s="72"/>
+      <c r="AN21" s="113"/>
+      <c r="AO21" s="105"/>
+      <c r="AP21" s="105"/>
+      <c r="AQ21" s="104"/>
       <c r="AR21" s="33"/>
       <c r="AS21" s="32"/>
       <c r="AT21" s="32"/>
       <c r="AU21" s="31"/>
       <c r="AV21" s="33"/>
       <c r="AW21" s="32"/>
-      <c r="AX21" s="101"/>
-      <c r="AY21" s="72"/>
-      <c r="AZ21" s="86"/>
+      <c r="AX21" s="103"/>
+      <c r="AY21" s="104"/>
+      <c r="AZ21" s="99"/>
     </row>
     <row r="22" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="92">
+      <c r="B22" s="88">
         <v>1</v>
       </c>
-      <c r="C22" s="93"/>
+      <c r="C22" s="120"/>
       <c r="D22" s="6"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -3037,10 +3037,10 @@
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
       <c r="S22" s="7"/>
-      <c r="T22" s="70"/>
-      <c r="U22" s="71"/>
-      <c r="V22" s="71"/>
-      <c r="W22" s="72"/>
+      <c r="T22" s="113"/>
+      <c r="U22" s="105"/>
+      <c r="V22" s="105"/>
+      <c r="W22" s="104"/>
       <c r="X22" s="6"/>
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
@@ -3057,24 +3057,24 @@
       <c r="AK22" s="5"/>
       <c r="AL22" s="5"/>
       <c r="AM22" s="7"/>
-      <c r="AN22" s="70"/>
-      <c r="AO22" s="71"/>
-      <c r="AP22" s="71"/>
-      <c r="AQ22" s="72"/>
+      <c r="AN22" s="113"/>
+      <c r="AO22" s="105"/>
+      <c r="AP22" s="105"/>
+      <c r="AQ22" s="104"/>
       <c r="AR22" s="6"/>
       <c r="AS22" s="5"/>
       <c r="AT22" s="5"/>
       <c r="AU22" s="7"/>
       <c r="AV22" s="6"/>
       <c r="AW22" s="5"/>
-      <c r="AX22" s="101"/>
-      <c r="AY22" s="72"/>
-      <c r="AZ22" s="86"/>
+      <c r="AX22" s="103"/>
+      <c r="AY22" s="104"/>
+      <c r="AZ22" s="99"/>
     </row>
     <row r="23" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A23" s="88"/>
-      <c r="B23" s="89"/>
-      <c r="C23" s="90"/>
+      <c r="A23" s="93"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="97"/>
       <c r="D23" s="11"/>
       <c r="E23" s="3"/>
       <c r="F23" s="32"/>
@@ -3091,10 +3091,10 @@
       <c r="Q23" s="32"/>
       <c r="R23" s="32"/>
       <c r="S23" s="31"/>
-      <c r="T23" s="70"/>
-      <c r="U23" s="71"/>
-      <c r="V23" s="71"/>
-      <c r="W23" s="72"/>
+      <c r="T23" s="113"/>
+      <c r="U23" s="105"/>
+      <c r="V23" s="105"/>
+      <c r="W23" s="104"/>
       <c r="X23" s="33"/>
       <c r="Y23" s="32"/>
       <c r="Z23" s="32"/>
@@ -3111,28 +3111,28 @@
       <c r="AK23" s="3"/>
       <c r="AL23" s="3"/>
       <c r="AM23" s="12"/>
-      <c r="AN23" s="70"/>
-      <c r="AO23" s="71"/>
-      <c r="AP23" s="71"/>
-      <c r="AQ23" s="72"/>
+      <c r="AN23" s="113"/>
+      <c r="AO23" s="105"/>
+      <c r="AP23" s="105"/>
+      <c r="AQ23" s="104"/>
       <c r="AR23" s="11"/>
       <c r="AS23" s="3"/>
       <c r="AT23" s="32"/>
       <c r="AU23" s="31"/>
       <c r="AV23" s="33"/>
       <c r="AW23" s="3"/>
-      <c r="AX23" s="101"/>
-      <c r="AY23" s="72"/>
-      <c r="AZ23" s="86"/>
+      <c r="AX23" s="103"/>
+      <c r="AY23" s="104"/>
+      <c r="AZ23" s="99"/>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A24" s="94" t="s">
+      <c r="A24" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="92">
+      <c r="B24" s="88">
         <v>1</v>
       </c>
-      <c r="C24" s="93"/>
+      <c r="C24" s="120"/>
       <c r="D24" s="28"/>
       <c r="E24" s="30"/>
       <c r="F24" s="5"/>
@@ -3149,10 +3149,10 @@
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
       <c r="S24" s="7"/>
-      <c r="T24" s="70"/>
-      <c r="U24" s="71"/>
-      <c r="V24" s="71"/>
-      <c r="W24" s="72"/>
+      <c r="T24" s="113"/>
+      <c r="U24" s="105"/>
+      <c r="V24" s="105"/>
+      <c r="W24" s="104"/>
       <c r="X24" s="6"/>
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
@@ -3169,24 +3169,24 @@
       <c r="AK24" s="30"/>
       <c r="AL24" s="30"/>
       <c r="AM24" s="29"/>
-      <c r="AN24" s="70"/>
-      <c r="AO24" s="71"/>
-      <c r="AP24" s="71"/>
-      <c r="AQ24" s="72"/>
+      <c r="AN24" s="113"/>
+      <c r="AO24" s="105"/>
+      <c r="AP24" s="105"/>
+      <c r="AQ24" s="104"/>
       <c r="AR24" s="28"/>
       <c r="AS24" s="30"/>
       <c r="AT24" s="5"/>
       <c r="AU24" s="7"/>
       <c r="AV24" s="6"/>
       <c r="AW24" s="30"/>
-      <c r="AX24" s="101"/>
-      <c r="AY24" s="72"/>
-      <c r="AZ24" s="86"/>
+      <c r="AX24" s="103"/>
+      <c r="AY24" s="104"/>
+      <c r="AZ24" s="99"/>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A25" s="88"/>
-      <c r="B25" s="97"/>
-      <c r="C25" s="98"/>
+      <c r="A25" s="93"/>
+      <c r="B25" s="117"/>
+      <c r="C25" s="118"/>
       <c r="D25" s="33"/>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
@@ -3203,10 +3203,10 @@
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="31"/>
-      <c r="T25" s="70"/>
-      <c r="U25" s="71"/>
-      <c r="V25" s="71"/>
-      <c r="W25" s="72"/>
+      <c r="T25" s="113"/>
+      <c r="U25" s="105"/>
+      <c r="V25" s="105"/>
+      <c r="W25" s="104"/>
       <c r="X25" s="33"/>
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
@@ -3223,28 +3223,28 @@
       <c r="AK25" s="3"/>
       <c r="AL25" s="3"/>
       <c r="AM25" s="12"/>
-      <c r="AN25" s="70"/>
-      <c r="AO25" s="71"/>
-      <c r="AP25" s="71"/>
-      <c r="AQ25" s="72"/>
+      <c r="AN25" s="113"/>
+      <c r="AO25" s="105"/>
+      <c r="AP25" s="105"/>
+      <c r="AQ25" s="104"/>
       <c r="AR25" s="11"/>
       <c r="AS25" s="3"/>
       <c r="AT25" s="3"/>
       <c r="AU25" s="12"/>
       <c r="AV25" s="11"/>
       <c r="AW25" s="3"/>
-      <c r="AX25" s="101"/>
-      <c r="AY25" s="72"/>
-      <c r="AZ25" s="86"/>
+      <c r="AX25" s="103"/>
+      <c r="AY25" s="104"/>
+      <c r="AZ25" s="99"/>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A26" s="91" t="s">
+      <c r="A26" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="95">
+      <c r="B26" s="121">
         <v>2</v>
       </c>
-      <c r="C26" s="99"/>
+      <c r="C26" s="90"/>
       <c r="D26" s="6"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -3256,15 +3256,15 @@
       <c r="L26" s="6"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="121"/>
+      <c r="O26" s="68"/>
       <c r="P26" s="28"/>
       <c r="Q26" s="30"/>
       <c r="R26" s="30"/>
       <c r="S26" s="7"/>
-      <c r="T26" s="70"/>
-      <c r="U26" s="71"/>
-      <c r="V26" s="71"/>
-      <c r="W26" s="72"/>
+      <c r="T26" s="113"/>
+      <c r="U26" s="105"/>
+      <c r="V26" s="105"/>
+      <c r="W26" s="104"/>
       <c r="X26" s="6"/>
       <c r="Y26" s="30"/>
       <c r="Z26" s="30"/>
@@ -3281,24 +3281,24 @@
       <c r="AK26" s="30"/>
       <c r="AL26" s="30"/>
       <c r="AM26" s="29"/>
-      <c r="AN26" s="70"/>
-      <c r="AO26" s="71"/>
-      <c r="AP26" s="71"/>
-      <c r="AQ26" s="72"/>
+      <c r="AN26" s="113"/>
+      <c r="AO26" s="105"/>
+      <c r="AP26" s="105"/>
+      <c r="AQ26" s="104"/>
       <c r="AR26" s="28"/>
       <c r="AS26" s="30"/>
       <c r="AT26" s="30"/>
       <c r="AU26" s="29"/>
       <c r="AV26" s="28"/>
       <c r="AW26" s="30"/>
-      <c r="AX26" s="101"/>
-      <c r="AY26" s="72"/>
-      <c r="AZ26" s="86"/>
+      <c r="AX26" s="103"/>
+      <c r="AY26" s="104"/>
+      <c r="AZ26" s="99"/>
     </row>
     <row r="27" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="77"/>
-      <c r="B27" s="79"/>
-      <c r="C27" s="81"/>
+      <c r="A27" s="87"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="91"/>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
@@ -3310,15 +3310,15 @@
       <c r="L27" s="8"/>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
-      <c r="O27" s="120"/>
+      <c r="O27" s="67"/>
       <c r="P27" s="8"/>
       <c r="Q27" s="9"/>
       <c r="R27" s="9"/>
       <c r="S27" s="10"/>
-      <c r="T27" s="70"/>
-      <c r="U27" s="71"/>
-      <c r="V27" s="71"/>
-      <c r="W27" s="72"/>
+      <c r="T27" s="113"/>
+      <c r="U27" s="105"/>
+      <c r="V27" s="105"/>
+      <c r="W27" s="104"/>
       <c r="X27" s="8"/>
       <c r="Y27" s="9"/>
       <c r="Z27" s="9"/>
@@ -3335,28 +3335,28 @@
       <c r="AK27" s="9"/>
       <c r="AL27" s="9"/>
       <c r="AM27" s="10"/>
-      <c r="AN27" s="70"/>
-      <c r="AO27" s="71"/>
-      <c r="AP27" s="71"/>
-      <c r="AQ27" s="72"/>
+      <c r="AN27" s="113"/>
+      <c r="AO27" s="105"/>
+      <c r="AP27" s="105"/>
+      <c r="AQ27" s="104"/>
       <c r="AR27" s="8"/>
       <c r="AS27" s="9"/>
       <c r="AT27" s="9"/>
       <c r="AU27" s="10"/>
       <c r="AV27" s="8"/>
       <c r="AW27" s="9"/>
-      <c r="AX27" s="101"/>
-      <c r="AY27" s="72"/>
-      <c r="AZ27" s="87"/>
+      <c r="AX27" s="103"/>
+      <c r="AY27" s="104"/>
+      <c r="AZ27" s="100"/>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A28" s="76" t="s">
+      <c r="A28" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="78">
+      <c r="B28" s="94">
         <v>0.5</v>
       </c>
-      <c r="C28" s="80"/>
+      <c r="C28" s="96"/>
       <c r="D28" s="15"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
@@ -3373,10 +3373,10 @@
       <c r="Q28" s="16"/>
       <c r="R28" s="16"/>
       <c r="S28" s="17"/>
-      <c r="T28" s="70"/>
-      <c r="U28" s="71"/>
-      <c r="V28" s="71"/>
-      <c r="W28" s="72"/>
+      <c r="T28" s="113"/>
+      <c r="U28" s="105"/>
+      <c r="V28" s="105"/>
+      <c r="W28" s="104"/>
       <c r="X28" s="15"/>
       <c r="Y28" s="16"/>
       <c r="Z28" s="16"/>
@@ -3393,26 +3393,26 @@
       <c r="AK28" s="16"/>
       <c r="AL28" s="16"/>
       <c r="AM28" s="17"/>
-      <c r="AN28" s="70"/>
-      <c r="AO28" s="71"/>
-      <c r="AP28" s="71"/>
-      <c r="AQ28" s="72"/>
+      <c r="AN28" s="113"/>
+      <c r="AO28" s="105"/>
+      <c r="AP28" s="105"/>
+      <c r="AQ28" s="104"/>
       <c r="AR28" s="15"/>
       <c r="AS28" s="16"/>
       <c r="AT28" s="16"/>
       <c r="AU28" s="17"/>
       <c r="AV28" s="15"/>
       <c r="AW28" s="17"/>
-      <c r="AX28" s="71"/>
-      <c r="AY28" s="72"/>
-      <c r="AZ28" s="117" t="s">
+      <c r="AX28" s="105"/>
+      <c r="AY28" s="104"/>
+      <c r="AZ28" s="83" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="77"/>
-      <c r="B29" s="79"/>
-      <c r="C29" s="81"/>
+      <c r="A29" s="87"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="91"/>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
@@ -3425,14 +3425,14 @@
       <c r="M29" s="9"/>
       <c r="N29" s="50"/>
       <c r="O29" s="51"/>
-      <c r="P29" s="122"/>
+      <c r="P29" s="69"/>
       <c r="Q29" s="9"/>
       <c r="R29" s="9"/>
       <c r="S29" s="10"/>
-      <c r="T29" s="70"/>
-      <c r="U29" s="71"/>
-      <c r="V29" s="71"/>
-      <c r="W29" s="72"/>
+      <c r="T29" s="113"/>
+      <c r="U29" s="105"/>
+      <c r="V29" s="105"/>
+      <c r="W29" s="104"/>
       <c r="X29" s="8"/>
       <c r="Y29" s="9"/>
       <c r="Z29" s="9"/>
@@ -3449,28 +3449,28 @@
       <c r="AK29" s="9"/>
       <c r="AL29" s="9"/>
       <c r="AM29" s="10"/>
-      <c r="AN29" s="70"/>
-      <c r="AO29" s="71"/>
-      <c r="AP29" s="71"/>
-      <c r="AQ29" s="72"/>
+      <c r="AN29" s="113"/>
+      <c r="AO29" s="105"/>
+      <c r="AP29" s="105"/>
+      <c r="AQ29" s="104"/>
       <c r="AR29" s="8"/>
       <c r="AS29" s="9"/>
       <c r="AT29" s="9"/>
       <c r="AU29" s="10"/>
       <c r="AV29" s="8"/>
       <c r="AW29" s="10"/>
-      <c r="AX29" s="71"/>
-      <c r="AY29" s="72"/>
-      <c r="AZ29" s="118"/>
+      <c r="AX29" s="105"/>
+      <c r="AY29" s="104"/>
+      <c r="AZ29" s="84"/>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A30" s="91" t="s">
+      <c r="A30" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="95">
+      <c r="B30" s="121">
         <v>0.5</v>
       </c>
-      <c r="C30" s="99"/>
+      <c r="C30" s="90"/>
       <c r="D30" s="6"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -3487,10 +3487,10 @@
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
       <c r="S30" s="7"/>
-      <c r="T30" s="70"/>
-      <c r="U30" s="71"/>
-      <c r="V30" s="71"/>
-      <c r="W30" s="72"/>
+      <c r="T30" s="113"/>
+      <c r="U30" s="105"/>
+      <c r="V30" s="105"/>
+      <c r="W30" s="104"/>
       <c r="X30" s="6"/>
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
@@ -3507,26 +3507,26 @@
       <c r="AK30" s="5"/>
       <c r="AL30" s="5"/>
       <c r="AM30" s="7"/>
-      <c r="AN30" s="70"/>
-      <c r="AO30" s="71"/>
-      <c r="AP30" s="71"/>
-      <c r="AQ30" s="72"/>
+      <c r="AN30" s="113"/>
+      <c r="AO30" s="105"/>
+      <c r="AP30" s="105"/>
+      <c r="AQ30" s="104"/>
       <c r="AR30" s="6"/>
       <c r="AS30" s="5"/>
       <c r="AT30" s="5"/>
       <c r="AU30" s="7"/>
       <c r="AV30" s="6"/>
       <c r="AW30" s="5"/>
-      <c r="AX30" s="101"/>
-      <c r="AY30" s="72"/>
-      <c r="AZ30" s="117" t="s">
+      <c r="AX30" s="103"/>
+      <c r="AY30" s="104"/>
+      <c r="AZ30" s="83" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A31" s="88"/>
-      <c r="B31" s="89"/>
-      <c r="C31" s="90"/>
+      <c r="A31" s="93"/>
+      <c r="B31" s="95"/>
+      <c r="C31" s="97"/>
       <c r="D31" s="11"/>
       <c r="E31" s="32"/>
       <c r="F31" s="3"/>
@@ -3543,10 +3543,10 @@
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
       <c r="S31" s="31"/>
-      <c r="T31" s="70"/>
-      <c r="U31" s="71"/>
-      <c r="V31" s="71"/>
-      <c r="W31" s="72"/>
+      <c r="T31" s="113"/>
+      <c r="U31" s="105"/>
+      <c r="V31" s="105"/>
+      <c r="W31" s="104"/>
       <c r="X31" s="33"/>
       <c r="Y31" s="32"/>
       <c r="Z31" s="32"/>
@@ -3563,28 +3563,28 @@
       <c r="AK31" s="32"/>
       <c r="AL31" s="32"/>
       <c r="AM31" s="31"/>
-      <c r="AN31" s="70"/>
-      <c r="AO31" s="71"/>
-      <c r="AP31" s="71"/>
-      <c r="AQ31" s="72"/>
+      <c r="AN31" s="113"/>
+      <c r="AO31" s="105"/>
+      <c r="AP31" s="105"/>
+      <c r="AQ31" s="104"/>
       <c r="AR31" s="33"/>
       <c r="AS31" s="32"/>
       <c r="AT31" s="32"/>
       <c r="AU31" s="31"/>
       <c r="AV31" s="33"/>
       <c r="AW31" s="32"/>
-      <c r="AX31" s="101"/>
-      <c r="AY31" s="72"/>
-      <c r="AZ31" s="119"/>
+      <c r="AX31" s="103"/>
+      <c r="AY31" s="104"/>
+      <c r="AZ31" s="85"/>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A32" s="94" t="s">
+      <c r="A32" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="92">
+      <c r="B32" s="88">
         <v>1</v>
       </c>
-      <c r="C32" s="93"/>
+      <c r="C32" s="120"/>
       <c r="D32" s="28"/>
       <c r="E32" s="5"/>
       <c r="F32" s="30"/>
@@ -3601,10 +3601,10 @@
       <c r="Q32" s="34"/>
       <c r="R32" s="30"/>
       <c r="S32" s="7"/>
-      <c r="T32" s="70"/>
-      <c r="U32" s="71"/>
-      <c r="V32" s="71"/>
-      <c r="W32" s="72"/>
+      <c r="T32" s="113"/>
+      <c r="U32" s="105"/>
+      <c r="V32" s="105"/>
+      <c r="W32" s="104"/>
       <c r="X32" s="6"/>
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
@@ -3621,24 +3621,24 @@
       <c r="AK32" s="5"/>
       <c r="AL32" s="5"/>
       <c r="AM32" s="7"/>
-      <c r="AN32" s="70"/>
-      <c r="AO32" s="71"/>
-      <c r="AP32" s="71"/>
-      <c r="AQ32" s="72"/>
+      <c r="AN32" s="113"/>
+      <c r="AO32" s="105"/>
+      <c r="AP32" s="105"/>
+      <c r="AQ32" s="104"/>
       <c r="AR32" s="6"/>
       <c r="AS32" s="5"/>
       <c r="AT32" s="5"/>
       <c r="AU32" s="7"/>
       <c r="AV32" s="6"/>
       <c r="AW32" s="5"/>
-      <c r="AX32" s="101"/>
-      <c r="AY32" s="72"/>
-      <c r="AZ32" s="119"/>
+      <c r="AX32" s="103"/>
+      <c r="AY32" s="104"/>
+      <c r="AZ32" s="85"/>
     </row>
     <row r="33" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A33" s="88"/>
-      <c r="B33" s="97"/>
-      <c r="C33" s="98"/>
+      <c r="A33" s="93"/>
+      <c r="B33" s="117"/>
+      <c r="C33" s="118"/>
       <c r="D33" s="33"/>
       <c r="E33" s="32"/>
       <c r="F33" s="3"/>
@@ -3655,10 +3655,10 @@
       <c r="Q33" s="54"/>
       <c r="R33" s="32"/>
       <c r="S33" s="31"/>
-      <c r="T33" s="70"/>
-      <c r="U33" s="71"/>
-      <c r="V33" s="71"/>
-      <c r="W33" s="72"/>
+      <c r="T33" s="113"/>
+      <c r="U33" s="105"/>
+      <c r="V33" s="105"/>
+      <c r="W33" s="104"/>
       <c r="X33" s="33"/>
       <c r="Y33" s="3"/>
       <c r="Z33" s="32"/>
@@ -3675,28 +3675,28 @@
       <c r="AK33" s="32"/>
       <c r="AL33" s="32"/>
       <c r="AM33" s="31"/>
-      <c r="AN33" s="70"/>
-      <c r="AO33" s="71"/>
-      <c r="AP33" s="71"/>
-      <c r="AQ33" s="72"/>
+      <c r="AN33" s="113"/>
+      <c r="AO33" s="105"/>
+      <c r="AP33" s="105"/>
+      <c r="AQ33" s="104"/>
       <c r="AR33" s="33"/>
       <c r="AS33" s="3"/>
       <c r="AT33" s="3"/>
       <c r="AU33" s="12"/>
       <c r="AV33" s="11"/>
       <c r="AW33" s="32"/>
-      <c r="AX33" s="101"/>
-      <c r="AY33" s="72"/>
-      <c r="AZ33" s="119"/>
+      <c r="AX33" s="103"/>
+      <c r="AY33" s="104"/>
+      <c r="AZ33" s="85"/>
     </row>
     <row r="34" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A34" s="94" t="s">
+      <c r="A34" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="92">
+      <c r="B34" s="88">
         <v>1</v>
       </c>
-      <c r="C34" s="99"/>
+      <c r="C34" s="90"/>
       <c r="D34" s="6"/>
       <c r="E34" s="5"/>
       <c r="F34" s="30"/>
@@ -3713,10 +3713,10 @@
       <c r="Q34" s="55"/>
       <c r="R34" s="24"/>
       <c r="S34" s="7"/>
-      <c r="T34" s="70"/>
-      <c r="U34" s="71"/>
-      <c r="V34" s="71"/>
-      <c r="W34" s="72"/>
+      <c r="T34" s="113"/>
+      <c r="U34" s="105"/>
+      <c r="V34" s="105"/>
+      <c r="W34" s="104"/>
       <c r="X34" s="6"/>
       <c r="Y34" s="30"/>
       <c r="Z34" s="5"/>
@@ -3733,24 +3733,24 @@
       <c r="AK34" s="5"/>
       <c r="AL34" s="5"/>
       <c r="AM34" s="7"/>
-      <c r="AN34" s="70"/>
-      <c r="AO34" s="71"/>
-      <c r="AP34" s="71"/>
-      <c r="AQ34" s="72"/>
+      <c r="AN34" s="113"/>
+      <c r="AO34" s="105"/>
+      <c r="AP34" s="105"/>
+      <c r="AQ34" s="104"/>
       <c r="AR34" s="6"/>
       <c r="AS34" s="30"/>
       <c r="AT34" s="30"/>
       <c r="AU34" s="29"/>
       <c r="AV34" s="28"/>
       <c r="AW34" s="5"/>
-      <c r="AX34" s="101"/>
-      <c r="AY34" s="72"/>
-      <c r="AZ34" s="119"/>
+      <c r="AX34" s="103"/>
+      <c r="AY34" s="104"/>
+      <c r="AZ34" s="85"/>
     </row>
     <row r="35" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A35" s="88"/>
-      <c r="B35" s="97"/>
-      <c r="C35" s="90"/>
+      <c r="A35" s="93"/>
+      <c r="B35" s="117"/>
+      <c r="C35" s="97"/>
       <c r="D35" s="33"/>
       <c r="E35" s="32"/>
       <c r="F35" s="32"/>
@@ -3767,10 +3767,10 @@
       <c r="Q35" s="54"/>
       <c r="R35" s="40"/>
       <c r="S35" s="12"/>
-      <c r="T35" s="70"/>
-      <c r="U35" s="71"/>
-      <c r="V35" s="71"/>
-      <c r="W35" s="72"/>
+      <c r="T35" s="113"/>
+      <c r="U35" s="105"/>
+      <c r="V35" s="105"/>
+      <c r="W35" s="104"/>
       <c r="X35" s="11"/>
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
@@ -3787,28 +3787,28 @@
       <c r="AK35" s="3"/>
       <c r="AL35" s="3"/>
       <c r="AM35" s="12"/>
-      <c r="AN35" s="70"/>
-      <c r="AO35" s="71"/>
-      <c r="AP35" s="71"/>
-      <c r="AQ35" s="72"/>
+      <c r="AN35" s="113"/>
+      <c r="AO35" s="105"/>
+      <c r="AP35" s="105"/>
+      <c r="AQ35" s="104"/>
       <c r="AR35" s="33"/>
       <c r="AS35" s="3"/>
       <c r="AT35" s="32"/>
       <c r="AU35" s="31"/>
       <c r="AV35" s="33"/>
       <c r="AW35" s="3"/>
-      <c r="AX35" s="101"/>
-      <c r="AY35" s="72"/>
-      <c r="AZ35" s="119"/>
+      <c r="AX35" s="103"/>
+      <c r="AY35" s="104"/>
+      <c r="AZ35" s="85"/>
     </row>
     <row r="36" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A36" s="94" t="s">
+      <c r="A36" s="119" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="92">
+      <c r="B36" s="88">
         <v>1</v>
       </c>
-      <c r="C36" s="93"/>
+      <c r="C36" s="120"/>
       <c r="D36" s="6"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -3825,10 +3825,10 @@
       <c r="Q36" s="5"/>
       <c r="R36" s="30"/>
       <c r="S36" s="49"/>
-      <c r="T36" s="70"/>
-      <c r="U36" s="71"/>
-      <c r="V36" s="71"/>
-      <c r="W36" s="72"/>
+      <c r="T36" s="113"/>
+      <c r="U36" s="105"/>
+      <c r="V36" s="105"/>
+      <c r="W36" s="104"/>
       <c r="X36" s="28"/>
       <c r="Y36" s="30"/>
       <c r="Z36" s="30"/>
@@ -3845,24 +3845,24 @@
       <c r="AK36" s="30"/>
       <c r="AL36" s="30"/>
       <c r="AM36" s="29"/>
-      <c r="AN36" s="70"/>
-      <c r="AO36" s="71"/>
-      <c r="AP36" s="71"/>
-      <c r="AQ36" s="72"/>
+      <c r="AN36" s="113"/>
+      <c r="AO36" s="105"/>
+      <c r="AP36" s="105"/>
+      <c r="AQ36" s="104"/>
       <c r="AR36" s="6"/>
       <c r="AS36" s="30"/>
       <c r="AT36" s="5"/>
       <c r="AU36" s="7"/>
       <c r="AV36" s="6"/>
       <c r="AW36" s="30"/>
-      <c r="AX36" s="101"/>
-      <c r="AY36" s="72"/>
-      <c r="AZ36" s="119"/>
+      <c r="AX36" s="103"/>
+      <c r="AY36" s="104"/>
+      <c r="AZ36" s="85"/>
     </row>
     <row r="37" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A37" s="88"/>
-      <c r="B37" s="97"/>
-      <c r="C37" s="98"/>
+      <c r="A37" s="93"/>
+      <c r="B37" s="117"/>
+      <c r="C37" s="118"/>
       <c r="D37" s="33"/>
       <c r="E37" s="32"/>
       <c r="F37" s="3"/>
@@ -3879,10 +3879,10 @@
       <c r="Q37" s="32"/>
       <c r="R37" s="3"/>
       <c r="S37" s="66"/>
-      <c r="T37" s="70"/>
-      <c r="U37" s="71"/>
-      <c r="V37" s="71"/>
-      <c r="W37" s="72"/>
+      <c r="T37" s="113"/>
+      <c r="U37" s="105"/>
+      <c r="V37" s="105"/>
+      <c r="W37" s="104"/>
       <c r="X37" s="33"/>
       <c r="Y37" s="32"/>
       <c r="Z37" s="32"/>
@@ -3899,28 +3899,28 @@
       <c r="AK37" s="32"/>
       <c r="AL37" s="32"/>
       <c r="AM37" s="12"/>
-      <c r="AN37" s="70"/>
-      <c r="AO37" s="71"/>
-      <c r="AP37" s="71"/>
-      <c r="AQ37" s="72"/>
+      <c r="AN37" s="113"/>
+      <c r="AO37" s="105"/>
+      <c r="AP37" s="105"/>
+      <c r="AQ37" s="104"/>
       <c r="AR37" s="11"/>
       <c r="AS37" s="3"/>
       <c r="AT37" s="32"/>
       <c r="AU37" s="12"/>
       <c r="AV37" s="11"/>
       <c r="AW37" s="3"/>
-      <c r="AX37" s="101"/>
-      <c r="AY37" s="72"/>
-      <c r="AZ37" s="119"/>
+      <c r="AX37" s="103"/>
+      <c r="AY37" s="104"/>
+      <c r="AZ37" s="85"/>
     </row>
     <row r="38" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A38" s="91" t="s">
+      <c r="A38" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="92">
+      <c r="B38" s="88">
         <v>1</v>
       </c>
-      <c r="C38" s="93"/>
+      <c r="C38" s="120"/>
       <c r="D38" s="6"/>
       <c r="E38" s="5"/>
       <c r="F38" s="30"/>
@@ -3937,10 +3937,10 @@
       <c r="Q38" s="5"/>
       <c r="R38" s="30"/>
       <c r="S38" s="25"/>
-      <c r="T38" s="70"/>
-      <c r="U38" s="71"/>
-      <c r="V38" s="71"/>
-      <c r="W38" s="72"/>
+      <c r="T38" s="113"/>
+      <c r="U38" s="105"/>
+      <c r="V38" s="105"/>
+      <c r="W38" s="104"/>
       <c r="X38" s="6"/>
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
@@ -3957,24 +3957,24 @@
       <c r="AK38" s="5"/>
       <c r="AL38" s="5"/>
       <c r="AM38" s="29"/>
-      <c r="AN38" s="70"/>
-      <c r="AO38" s="71"/>
-      <c r="AP38" s="71"/>
-      <c r="AQ38" s="72"/>
+      <c r="AN38" s="113"/>
+      <c r="AO38" s="105"/>
+      <c r="AP38" s="105"/>
+      <c r="AQ38" s="104"/>
       <c r="AR38" s="28"/>
       <c r="AS38" s="30"/>
       <c r="AT38" s="5"/>
       <c r="AU38" s="29"/>
       <c r="AV38" s="28"/>
       <c r="AW38" s="30"/>
-      <c r="AX38" s="101"/>
-      <c r="AY38" s="72"/>
-      <c r="AZ38" s="119"/>
+      <c r="AX38" s="103"/>
+      <c r="AY38" s="104"/>
+      <c r="AZ38" s="85"/>
     </row>
     <row r="39" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A39" s="96"/>
-      <c r="B39" s="97"/>
-      <c r="C39" s="98"/>
+      <c r="A39" s="116"/>
+      <c r="B39" s="117"/>
+      <c r="C39" s="118"/>
       <c r="D39" s="11"/>
       <c r="E39" s="3"/>
       <c r="F39" s="32"/>
@@ -3991,12 +3991,12 @@
       <c r="Q39" s="32"/>
       <c r="R39" s="3"/>
       <c r="S39" s="12"/>
-      <c r="T39" s="70"/>
-      <c r="U39" s="71"/>
-      <c r="V39" s="71"/>
-      <c r="W39" s="72"/>
-      <c r="X39" s="11"/>
-      <c r="Y39" s="32"/>
+      <c r="T39" s="113"/>
+      <c r="U39" s="105"/>
+      <c r="V39" s="105"/>
+      <c r="W39" s="104"/>
+      <c r="X39" s="39"/>
+      <c r="Y39" s="54"/>
       <c r="Z39" s="32"/>
       <c r="AA39" s="12"/>
       <c r="AB39" s="33"/>
@@ -4011,28 +4011,28 @@
       <c r="AK39" s="32"/>
       <c r="AL39" s="32"/>
       <c r="AM39" s="31"/>
-      <c r="AN39" s="70"/>
-      <c r="AO39" s="71"/>
-      <c r="AP39" s="71"/>
-      <c r="AQ39" s="72"/>
+      <c r="AN39" s="113"/>
+      <c r="AO39" s="105"/>
+      <c r="AP39" s="105"/>
+      <c r="AQ39" s="104"/>
       <c r="AR39" s="33"/>
       <c r="AS39" s="32"/>
       <c r="AT39" s="3"/>
       <c r="AU39" s="31"/>
       <c r="AV39" s="11"/>
       <c r="AW39" s="3"/>
-      <c r="AX39" s="101"/>
-      <c r="AY39" s="72"/>
-      <c r="AZ39" s="119"/>
+      <c r="AX39" s="103"/>
+      <c r="AY39" s="104"/>
+      <c r="AZ39" s="85"/>
     </row>
     <row r="40" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A40" s="94" t="s">
+      <c r="A40" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="92">
+      <c r="B40" s="88">
         <v>1</v>
       </c>
-      <c r="C40" s="93"/>
+      <c r="C40" s="120"/>
       <c r="D40" s="28"/>
       <c r="E40" s="30"/>
       <c r="F40" s="5"/>
@@ -4049,10 +4049,10 @@
       <c r="Q40" s="5"/>
       <c r="R40" s="30"/>
       <c r="S40" s="29"/>
-      <c r="T40" s="70"/>
-      <c r="U40" s="71"/>
-      <c r="V40" s="71"/>
-      <c r="W40" s="72"/>
+      <c r="T40" s="113"/>
+      <c r="U40" s="105"/>
+      <c r="V40" s="105"/>
+      <c r="W40" s="104"/>
       <c r="X40" s="38"/>
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
@@ -4069,24 +4069,24 @@
       <c r="AK40" s="5"/>
       <c r="AL40" s="5"/>
       <c r="AM40" s="7"/>
-      <c r="AN40" s="70"/>
-      <c r="AO40" s="71"/>
-      <c r="AP40" s="71"/>
-      <c r="AQ40" s="72"/>
+      <c r="AN40" s="113"/>
+      <c r="AO40" s="105"/>
+      <c r="AP40" s="105"/>
+      <c r="AQ40" s="104"/>
       <c r="AR40" s="6"/>
       <c r="AS40" s="5"/>
       <c r="AT40" s="30"/>
       <c r="AU40" s="7"/>
       <c r="AV40" s="28"/>
       <c r="AW40" s="30"/>
-      <c r="AX40" s="101"/>
-      <c r="AY40" s="72"/>
-      <c r="AZ40" s="119"/>
+      <c r="AX40" s="103"/>
+      <c r="AY40" s="104"/>
+      <c r="AZ40" s="85"/>
     </row>
     <row r="41" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A41" s="96"/>
-      <c r="B41" s="97"/>
-      <c r="C41" s="98"/>
+      <c r="A41" s="116"/>
+      <c r="B41" s="117"/>
+      <c r="C41" s="118"/>
       <c r="D41" s="33"/>
       <c r="E41" s="32"/>
       <c r="F41" s="32"/>
@@ -4103,12 +4103,12 @@
       <c r="Q41" s="32"/>
       <c r="R41" s="3"/>
       <c r="S41" s="12"/>
-      <c r="T41" s="70"/>
-      <c r="U41" s="71"/>
-      <c r="V41" s="71"/>
-      <c r="W41" s="72"/>
-      <c r="X41" s="11"/>
-      <c r="Y41" s="3"/>
+      <c r="T41" s="113"/>
+      <c r="U41" s="105"/>
+      <c r="V41" s="105"/>
+      <c r="W41" s="104"/>
+      <c r="X41" s="39"/>
+      <c r="Y41" s="40"/>
       <c r="Z41" s="3"/>
       <c r="AA41" s="12"/>
       <c r="AB41" s="11"/>
@@ -4123,28 +4123,28 @@
       <c r="AK41" s="3"/>
       <c r="AL41" s="32"/>
       <c r="AM41" s="12"/>
-      <c r="AN41" s="70"/>
-      <c r="AO41" s="71"/>
-      <c r="AP41" s="71"/>
-      <c r="AQ41" s="72"/>
+      <c r="AN41" s="113"/>
+      <c r="AO41" s="105"/>
+      <c r="AP41" s="105"/>
+      <c r="AQ41" s="104"/>
       <c r="AR41" s="11"/>
       <c r="AS41" s="3"/>
       <c r="AT41" s="3"/>
       <c r="AU41" s="12"/>
       <c r="AV41" s="11"/>
       <c r="AW41" s="32"/>
-      <c r="AX41" s="101"/>
-      <c r="AY41" s="72"/>
-      <c r="AZ41" s="119"/>
+      <c r="AX41" s="103"/>
+      <c r="AY41" s="104"/>
+      <c r="AZ41" s="85"/>
     </row>
     <row r="42" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A42" s="94" t="s">
+      <c r="A42" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="92">
+      <c r="B42" s="88">
         <v>2</v>
       </c>
-      <c r="C42" s="93"/>
+      <c r="C42" s="120"/>
       <c r="D42" s="6"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -4161,10 +4161,10 @@
       <c r="Q42" s="5"/>
       <c r="R42" s="30"/>
       <c r="S42" s="29"/>
-      <c r="T42" s="70"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
-      <c r="W42" s="72"/>
+      <c r="T42" s="113"/>
+      <c r="U42" s="105"/>
+      <c r="V42" s="105"/>
+      <c r="W42" s="104"/>
       <c r="X42" s="28"/>
       <c r="Y42" s="34"/>
       <c r="Z42" s="34"/>
@@ -4181,24 +4181,24 @@
       <c r="AK42" s="30"/>
       <c r="AL42" s="5"/>
       <c r="AM42" s="29"/>
-      <c r="AN42" s="70"/>
-      <c r="AO42" s="71"/>
-      <c r="AP42" s="71"/>
-      <c r="AQ42" s="72"/>
+      <c r="AN42" s="113"/>
+      <c r="AO42" s="105"/>
+      <c r="AP42" s="105"/>
+      <c r="AQ42" s="104"/>
       <c r="AR42" s="28"/>
       <c r="AS42" s="30"/>
       <c r="AT42" s="30"/>
       <c r="AU42" s="29"/>
       <c r="AV42" s="28"/>
       <c r="AW42" s="5"/>
-      <c r="AX42" s="101"/>
-      <c r="AY42" s="72"/>
-      <c r="AZ42" s="119"/>
+      <c r="AX42" s="103"/>
+      <c r="AY42" s="104"/>
+      <c r="AZ42" s="85"/>
     </row>
     <row r="43" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A43" s="88"/>
-      <c r="B43" s="97"/>
-      <c r="C43" s="98"/>
+      <c r="A43" s="93"/>
+      <c r="B43" s="117"/>
+      <c r="C43" s="118"/>
       <c r="D43" s="11"/>
       <c r="E43" s="32"/>
       <c r="F43" s="3"/>
@@ -4215,10 +4215,10 @@
       <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
       <c r="S43" s="66"/>
-      <c r="T43" s="70"/>
-      <c r="U43" s="71"/>
-      <c r="V43" s="71"/>
-      <c r="W43" s="72"/>
+      <c r="T43" s="113"/>
+      <c r="U43" s="105"/>
+      <c r="V43" s="105"/>
+      <c r="W43" s="104"/>
       <c r="X43" s="11"/>
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
@@ -4235,28 +4235,28 @@
       <c r="AK43" s="32"/>
       <c r="AL43" s="3"/>
       <c r="AM43" s="12"/>
-      <c r="AN43" s="70"/>
-      <c r="AO43" s="71"/>
-      <c r="AP43" s="71"/>
-      <c r="AQ43" s="72"/>
+      <c r="AN43" s="113"/>
+      <c r="AO43" s="105"/>
+      <c r="AP43" s="105"/>
+      <c r="AQ43" s="104"/>
       <c r="AR43" s="11"/>
       <c r="AS43" s="3"/>
       <c r="AT43" s="3"/>
       <c r="AU43" s="12"/>
       <c r="AV43" s="11"/>
       <c r="AW43" s="3"/>
-      <c r="AX43" s="101"/>
-      <c r="AY43" s="72"/>
-      <c r="AZ43" s="119"/>
+      <c r="AX43" s="103"/>
+      <c r="AY43" s="104"/>
+      <c r="AZ43" s="85"/>
     </row>
     <row r="44" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A44" s="94" t="s">
+      <c r="A44" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="95">
+      <c r="B44" s="121">
         <v>2.5</v>
       </c>
-      <c r="C44" s="93"/>
+      <c r="C44" s="120"/>
       <c r="D44" s="28"/>
       <c r="E44" s="5"/>
       <c r="F44" s="30"/>
@@ -4273,10 +4273,10 @@
       <c r="Q44" s="30"/>
       <c r="R44" s="30"/>
       <c r="S44" s="7"/>
-      <c r="T44" s="70"/>
-      <c r="U44" s="71"/>
-      <c r="V44" s="71"/>
-      <c r="W44" s="72"/>
+      <c r="T44" s="113"/>
+      <c r="U44" s="105"/>
+      <c r="V44" s="105"/>
+      <c r="W44" s="104"/>
       <c r="X44" s="28"/>
       <c r="Y44" s="30"/>
       <c r="Z44" s="34"/>
@@ -4293,24 +4293,24 @@
       <c r="AK44" s="5"/>
       <c r="AL44" s="30"/>
       <c r="AM44" s="29"/>
-      <c r="AN44" s="70"/>
-      <c r="AO44" s="71"/>
-      <c r="AP44" s="71"/>
-      <c r="AQ44" s="72"/>
+      <c r="AN44" s="113"/>
+      <c r="AO44" s="105"/>
+      <c r="AP44" s="105"/>
+      <c r="AQ44" s="104"/>
       <c r="AR44" s="28"/>
       <c r="AS44" s="30"/>
       <c r="AT44" s="30"/>
       <c r="AU44" s="29"/>
       <c r="AV44" s="28"/>
       <c r="AW44" s="30"/>
-      <c r="AX44" s="101"/>
-      <c r="AY44" s="72"/>
-      <c r="AZ44" s="119"/>
+      <c r="AX44" s="103"/>
+      <c r="AY44" s="104"/>
+      <c r="AZ44" s="85"/>
     </row>
     <row r="45" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A45" s="88"/>
-      <c r="B45" s="89"/>
-      <c r="C45" s="98"/>
+      <c r="A45" s="93"/>
+      <c r="B45" s="95"/>
+      <c r="C45" s="118"/>
       <c r="D45" s="11"/>
       <c r="E45" s="3"/>
       <c r="F45" s="32"/>
@@ -4327,10 +4327,10 @@
       <c r="Q45" s="3"/>
       <c r="R45" s="3"/>
       <c r="S45" s="65"/>
-      <c r="T45" s="70"/>
-      <c r="U45" s="71"/>
-      <c r="V45" s="71"/>
-      <c r="W45" s="72"/>
+      <c r="T45" s="113"/>
+      <c r="U45" s="105"/>
+      <c r="V45" s="105"/>
+      <c r="W45" s="104"/>
       <c r="X45" s="11"/>
       <c r="Y45" s="32"/>
       <c r="Z45" s="3"/>
@@ -4347,28 +4347,28 @@
       <c r="AK45" s="3"/>
       <c r="AL45" s="3"/>
       <c r="AM45" s="12"/>
-      <c r="AN45" s="70"/>
-      <c r="AO45" s="71"/>
-      <c r="AP45" s="71"/>
-      <c r="AQ45" s="72"/>
+      <c r="AN45" s="113"/>
+      <c r="AO45" s="105"/>
+      <c r="AP45" s="105"/>
+      <c r="AQ45" s="104"/>
       <c r="AR45" s="11"/>
       <c r="AS45" s="3"/>
       <c r="AT45" s="3"/>
       <c r="AU45" s="12"/>
       <c r="AV45" s="11"/>
       <c r="AW45" s="3"/>
-      <c r="AX45" s="101"/>
-      <c r="AY45" s="72"/>
-      <c r="AZ45" s="119"/>
+      <c r="AX45" s="103"/>
+      <c r="AY45" s="104"/>
+      <c r="AZ45" s="85"/>
     </row>
     <row r="46" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A46" s="91" t="s">
+      <c r="A46" s="86" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="92">
+      <c r="B46" s="88">
         <v>2</v>
       </c>
-      <c r="C46" s="99"/>
+      <c r="C46" s="90"/>
       <c r="D46" s="28"/>
       <c r="E46" s="30"/>
       <c r="F46" s="5"/>
@@ -4385,10 +4385,10 @@
       <c r="Q46" s="30"/>
       <c r="R46" s="30"/>
       <c r="S46" s="29"/>
-      <c r="T46" s="70"/>
-      <c r="U46" s="71"/>
-      <c r="V46" s="71"/>
-      <c r="W46" s="72"/>
+      <c r="T46" s="113"/>
+      <c r="U46" s="105"/>
+      <c r="V46" s="105"/>
+      <c r="W46" s="104"/>
       <c r="X46" s="28"/>
       <c r="Y46" s="5"/>
       <c r="Z46" s="30"/>
@@ -4405,24 +4405,24 @@
       <c r="AK46" s="30"/>
       <c r="AL46" s="30"/>
       <c r="AM46" s="29"/>
-      <c r="AN46" s="70"/>
-      <c r="AO46" s="71"/>
-      <c r="AP46" s="71"/>
-      <c r="AQ46" s="72"/>
+      <c r="AN46" s="113"/>
+      <c r="AO46" s="105"/>
+      <c r="AP46" s="105"/>
+      <c r="AQ46" s="104"/>
       <c r="AR46" s="28"/>
       <c r="AS46" s="30"/>
       <c r="AT46" s="30"/>
       <c r="AU46" s="29"/>
       <c r="AV46" s="28"/>
       <c r="AW46" s="30"/>
-      <c r="AX46" s="101"/>
-      <c r="AY46" s="72"/>
-      <c r="AZ46" s="119"/>
+      <c r="AX46" s="103"/>
+      <c r="AY46" s="104"/>
+      <c r="AZ46" s="85"/>
     </row>
     <row r="47" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A47" s="96"/>
-      <c r="B47" s="97"/>
-      <c r="C47" s="90"/>
+      <c r="A47" s="116"/>
+      <c r="B47" s="117"/>
+      <c r="C47" s="97"/>
       <c r="D47" s="11"/>
       <c r="E47" s="32"/>
       <c r="F47" s="3"/>
@@ -4439,15 +4439,15 @@
       <c r="Q47" s="3"/>
       <c r="R47" s="32"/>
       <c r="S47" s="12"/>
-      <c r="T47" s="70"/>
-      <c r="U47" s="71"/>
-      <c r="V47" s="71"/>
-      <c r="W47" s="72"/>
+      <c r="T47" s="113"/>
+      <c r="U47" s="105"/>
+      <c r="V47" s="105"/>
+      <c r="W47" s="104"/>
       <c r="X47" s="11"/>
       <c r="Y47" s="3"/>
       <c r="Z47" s="3"/>
       <c r="AA47" s="31"/>
-      <c r="AB47" s="11"/>
+      <c r="AB47" s="39"/>
       <c r="AC47" s="3"/>
       <c r="AD47" s="3"/>
       <c r="AE47" s="31"/>
@@ -4459,28 +4459,28 @@
       <c r="AK47" s="32"/>
       <c r="AL47" s="3"/>
       <c r="AM47" s="31"/>
-      <c r="AN47" s="70"/>
-      <c r="AO47" s="71"/>
-      <c r="AP47" s="71"/>
-      <c r="AQ47" s="72"/>
+      <c r="AN47" s="113"/>
+      <c r="AO47" s="105"/>
+      <c r="AP47" s="105"/>
+      <c r="AQ47" s="104"/>
       <c r="AR47" s="33"/>
       <c r="AS47" s="32"/>
       <c r="AT47" s="32"/>
       <c r="AU47" s="31"/>
       <c r="AV47" s="33"/>
       <c r="AW47" s="32"/>
-      <c r="AX47" s="101"/>
-      <c r="AY47" s="72"/>
-      <c r="AZ47" s="119"/>
+      <c r="AX47" s="103"/>
+      <c r="AY47" s="104"/>
+      <c r="AZ47" s="85"/>
     </row>
     <row r="48" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A48" s="94" t="s">
+      <c r="A48" s="119" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="95">
+      <c r="B48" s="121">
         <v>0.5</v>
       </c>
-      <c r="C48" s="93"/>
+      <c r="C48" s="120"/>
       <c r="D48" s="28"/>
       <c r="E48" s="5"/>
       <c r="F48" s="30"/>
@@ -4497,10 +4497,10 @@
       <c r="Q48" s="30"/>
       <c r="R48" s="5"/>
       <c r="S48" s="29"/>
-      <c r="T48" s="70"/>
-      <c r="U48" s="71"/>
-      <c r="V48" s="71"/>
-      <c r="W48" s="72"/>
+      <c r="T48" s="113"/>
+      <c r="U48" s="105"/>
+      <c r="V48" s="105"/>
+      <c r="W48" s="104"/>
       <c r="X48" s="28"/>
       <c r="Y48" s="30"/>
       <c r="Z48" s="30"/>
@@ -4517,24 +4517,24 @@
       <c r="AK48" s="5"/>
       <c r="AL48" s="30"/>
       <c r="AM48" s="7"/>
-      <c r="AN48" s="70"/>
-      <c r="AO48" s="71"/>
-      <c r="AP48" s="71"/>
-      <c r="AQ48" s="72"/>
+      <c r="AN48" s="113"/>
+      <c r="AO48" s="105"/>
+      <c r="AP48" s="105"/>
+      <c r="AQ48" s="104"/>
       <c r="AR48" s="6"/>
       <c r="AS48" s="5"/>
       <c r="AT48" s="5"/>
       <c r="AU48" s="7"/>
       <c r="AV48" s="6"/>
       <c r="AW48" s="5"/>
-      <c r="AX48" s="101"/>
-      <c r="AY48" s="72"/>
-      <c r="AZ48" s="119"/>
+      <c r="AX48" s="103"/>
+      <c r="AY48" s="104"/>
+      <c r="AZ48" s="85"/>
     </row>
     <row r="49" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A49" s="96"/>
-      <c r="B49" s="89"/>
-      <c r="C49" s="98"/>
+      <c r="A49" s="116"/>
+      <c r="B49" s="95"/>
+      <c r="C49" s="118"/>
       <c r="D49" s="33"/>
       <c r="E49" s="32"/>
       <c r="F49" s="32"/>
@@ -4551,16 +4551,16 @@
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
       <c r="S49" s="12"/>
-      <c r="T49" s="70"/>
-      <c r="U49" s="71"/>
-      <c r="V49" s="71"/>
-      <c r="W49" s="72"/>
+      <c r="T49" s="113"/>
+      <c r="U49" s="105"/>
+      <c r="V49" s="105"/>
+      <c r="W49" s="104"/>
       <c r="X49" s="11"/>
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
       <c r="AA49" s="12"/>
       <c r="AB49" s="11"/>
-      <c r="AC49" s="3"/>
+      <c r="AC49" s="40"/>
       <c r="AD49" s="3"/>
       <c r="AE49" s="12"/>
       <c r="AF49" s="11"/>
@@ -4571,28 +4571,28 @@
       <c r="AK49" s="3"/>
       <c r="AL49" s="3"/>
       <c r="AM49" s="12"/>
-      <c r="AN49" s="70"/>
-      <c r="AO49" s="71"/>
-      <c r="AP49" s="71"/>
-      <c r="AQ49" s="72"/>
+      <c r="AN49" s="113"/>
+      <c r="AO49" s="105"/>
+      <c r="AP49" s="105"/>
+      <c r="AQ49" s="104"/>
       <c r="AR49" s="33"/>
       <c r="AS49" s="3"/>
       <c r="AT49" s="32"/>
       <c r="AU49" s="31"/>
       <c r="AV49" s="11"/>
       <c r="AW49" s="3"/>
-      <c r="AX49" s="101"/>
-      <c r="AY49" s="72"/>
-      <c r="AZ49" s="119"/>
+      <c r="AX49" s="103"/>
+      <c r="AY49" s="104"/>
+      <c r="AZ49" s="85"/>
     </row>
     <row r="50" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A50" s="94" t="s">
+      <c r="A50" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="B50" s="92">
+      <c r="B50" s="88">
         <v>2.5</v>
       </c>
-      <c r="C50" s="93"/>
+      <c r="C50" s="120"/>
       <c r="D50" s="6"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -4609,10 +4609,10 @@
       <c r="Q50" s="30"/>
       <c r="R50" s="30"/>
       <c r="S50" s="29"/>
-      <c r="T50" s="70"/>
-      <c r="U50" s="71"/>
-      <c r="V50" s="71"/>
-      <c r="W50" s="72"/>
+      <c r="T50" s="113"/>
+      <c r="U50" s="105"/>
+      <c r="V50" s="105"/>
+      <c r="W50" s="104"/>
       <c r="X50" s="28"/>
       <c r="Y50" s="30"/>
       <c r="Z50" s="30"/>
@@ -4629,24 +4629,24 @@
       <c r="AK50" s="30"/>
       <c r="AL50" s="30"/>
       <c r="AM50" s="29"/>
-      <c r="AN50" s="70"/>
-      <c r="AO50" s="71"/>
-      <c r="AP50" s="71"/>
-      <c r="AQ50" s="72"/>
+      <c r="AN50" s="113"/>
+      <c r="AO50" s="105"/>
+      <c r="AP50" s="105"/>
+      <c r="AQ50" s="104"/>
       <c r="AR50" s="6"/>
       <c r="AS50" s="30"/>
       <c r="AT50" s="5"/>
       <c r="AU50" s="7"/>
       <c r="AV50" s="28"/>
       <c r="AW50" s="30"/>
-      <c r="AX50" s="101"/>
-      <c r="AY50" s="72"/>
-      <c r="AZ50" s="119"/>
+      <c r="AX50" s="103"/>
+      <c r="AY50" s="104"/>
+      <c r="AZ50" s="85"/>
     </row>
     <row r="51" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A51" s="88"/>
-      <c r="B51" s="97"/>
-      <c r="C51" s="98"/>
+      <c r="A51" s="93"/>
+      <c r="B51" s="117"/>
+      <c r="C51" s="118"/>
       <c r="D51" s="11"/>
       <c r="E51" s="32"/>
       <c r="F51" s="3"/>
@@ -4663,18 +4663,18 @@
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
       <c r="S51" s="12"/>
-      <c r="T51" s="70"/>
-      <c r="U51" s="71"/>
-      <c r="V51" s="71"/>
-      <c r="W51" s="72"/>
+      <c r="T51" s="113"/>
+      <c r="U51" s="105"/>
+      <c r="V51" s="105"/>
+      <c r="W51" s="104"/>
       <c r="X51" s="33"/>
       <c r="Y51" s="32"/>
       <c r="Z51" s="3"/>
       <c r="AA51" s="31"/>
       <c r="AB51" s="11"/>
       <c r="AC51" s="3"/>
-      <c r="AD51" s="3"/>
-      <c r="AE51" s="31"/>
+      <c r="AD51" s="40"/>
+      <c r="AE51" s="66"/>
       <c r="AF51" s="11"/>
       <c r="AG51" s="3"/>
       <c r="AH51" s="3"/>
@@ -4683,28 +4683,28 @@
       <c r="AK51" s="32"/>
       <c r="AL51" s="3"/>
       <c r="AM51" s="12"/>
-      <c r="AN51" s="70"/>
-      <c r="AO51" s="71"/>
-      <c r="AP51" s="71"/>
-      <c r="AQ51" s="72"/>
+      <c r="AN51" s="113"/>
+      <c r="AO51" s="105"/>
+      <c r="AP51" s="105"/>
+      <c r="AQ51" s="104"/>
       <c r="AR51" s="11"/>
       <c r="AS51" s="3"/>
       <c r="AT51" s="3"/>
       <c r="AU51" s="12"/>
       <c r="AV51" s="11"/>
       <c r="AW51" s="3"/>
-      <c r="AX51" s="101"/>
-      <c r="AY51" s="72"/>
-      <c r="AZ51" s="119"/>
+      <c r="AX51" s="103"/>
+      <c r="AY51" s="104"/>
+      <c r="AZ51" s="85"/>
     </row>
     <row r="52" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A52" s="91" t="s">
+      <c r="A52" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="92">
+      <c r="B52" s="88">
         <v>1.5</v>
       </c>
-      <c r="C52" s="93"/>
+      <c r="C52" s="120"/>
       <c r="D52" s="28"/>
       <c r="E52" s="5"/>
       <c r="F52" s="30"/>
@@ -4721,10 +4721,10 @@
       <c r="Q52" s="30"/>
       <c r="R52" s="30"/>
       <c r="S52" s="29"/>
-      <c r="T52" s="70"/>
-      <c r="U52" s="71"/>
-      <c r="V52" s="71"/>
-      <c r="W52" s="72"/>
+      <c r="T52" s="113"/>
+      <c r="U52" s="105"/>
+      <c r="V52" s="105"/>
+      <c r="W52" s="104"/>
       <c r="X52" s="6"/>
       <c r="Y52" s="5"/>
       <c r="Z52" s="30"/>
@@ -4741,24 +4741,24 @@
       <c r="AK52" s="5"/>
       <c r="AL52" s="30"/>
       <c r="AM52" s="29"/>
-      <c r="AN52" s="70"/>
-      <c r="AO52" s="71"/>
-      <c r="AP52" s="71"/>
-      <c r="AQ52" s="72"/>
+      <c r="AN52" s="113"/>
+      <c r="AO52" s="105"/>
+      <c r="AP52" s="105"/>
+      <c r="AQ52" s="104"/>
       <c r="AR52" s="28"/>
       <c r="AS52" s="30"/>
       <c r="AT52" s="30"/>
       <c r="AU52" s="29"/>
       <c r="AV52" s="28"/>
       <c r="AW52" s="30"/>
-      <c r="AX52" s="101"/>
-      <c r="AY52" s="72"/>
-      <c r="AZ52" s="119"/>
+      <c r="AX52" s="103"/>
+      <c r="AY52" s="104"/>
+      <c r="AZ52" s="85"/>
     </row>
     <row r="53" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A53" s="96"/>
-      <c r="B53" s="97"/>
-      <c r="C53" s="98"/>
+      <c r="A53" s="116"/>
+      <c r="B53" s="117"/>
+      <c r="C53" s="118"/>
       <c r="D53" s="33"/>
       <c r="E53" s="32"/>
       <c r="F53" s="32"/>
@@ -4775,10 +4775,10 @@
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
       <c r="S53" s="12"/>
-      <c r="T53" s="70"/>
-      <c r="U53" s="71"/>
-      <c r="V53" s="71"/>
-      <c r="W53" s="72"/>
+      <c r="T53" s="113"/>
+      <c r="U53" s="105"/>
+      <c r="V53" s="105"/>
+      <c r="W53" s="104"/>
       <c r="X53" s="11"/>
       <c r="Y53" s="32"/>
       <c r="Z53" s="3"/>
@@ -4788,35 +4788,35 @@
       <c r="AD53" s="3"/>
       <c r="AE53" s="12"/>
       <c r="AF53" s="11"/>
-      <c r="AG53" s="32"/>
-      <c r="AH53" s="3"/>
+      <c r="AG53" s="54"/>
+      <c r="AH53" s="40"/>
       <c r="AI53" s="31"/>
       <c r="AJ53" s="11"/>
       <c r="AK53" s="3"/>
       <c r="AL53" s="3"/>
       <c r="AM53" s="12"/>
-      <c r="AN53" s="70"/>
-      <c r="AO53" s="71"/>
-      <c r="AP53" s="71"/>
-      <c r="AQ53" s="72"/>
+      <c r="AN53" s="113"/>
+      <c r="AO53" s="105"/>
+      <c r="AP53" s="105"/>
+      <c r="AQ53" s="104"/>
       <c r="AR53" s="11"/>
       <c r="AS53" s="3"/>
       <c r="AT53" s="3"/>
       <c r="AU53" s="12"/>
       <c r="AV53" s="11"/>
       <c r="AW53" s="3"/>
-      <c r="AX53" s="101"/>
-      <c r="AY53" s="72"/>
-      <c r="AZ53" s="119"/>
+      <c r="AX53" s="103"/>
+      <c r="AY53" s="104"/>
+      <c r="AZ53" s="85"/>
     </row>
     <row r="54" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A54" s="94" t="s">
+      <c r="A54" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="92">
+      <c r="B54" s="88">
         <v>1.5</v>
       </c>
-      <c r="C54" s="99"/>
+      <c r="C54" s="90"/>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
@@ -4833,10 +4833,10 @@
       <c r="Q54" s="30"/>
       <c r="R54" s="30"/>
       <c r="S54" s="29"/>
-      <c r="T54" s="70"/>
-      <c r="U54" s="71"/>
-      <c r="V54" s="71"/>
-      <c r="W54" s="72"/>
+      <c r="T54" s="113"/>
+      <c r="U54" s="105"/>
+      <c r="V54" s="105"/>
+      <c r="W54" s="104"/>
       <c r="X54" s="28"/>
       <c r="Y54" s="5"/>
       <c r="Z54" s="30"/>
@@ -4853,24 +4853,24 @@
       <c r="AK54" s="30"/>
       <c r="AL54" s="30"/>
       <c r="AM54" s="29"/>
-      <c r="AN54" s="70"/>
-      <c r="AO54" s="71"/>
-      <c r="AP54" s="71"/>
-      <c r="AQ54" s="72"/>
+      <c r="AN54" s="113"/>
+      <c r="AO54" s="105"/>
+      <c r="AP54" s="105"/>
+      <c r="AQ54" s="104"/>
       <c r="AR54" s="28"/>
       <c r="AS54" s="30"/>
       <c r="AT54" s="30"/>
       <c r="AU54" s="29"/>
       <c r="AV54" s="28"/>
       <c r="AW54" s="30"/>
-      <c r="AX54" s="101"/>
-      <c r="AY54" s="72"/>
-      <c r="AZ54" s="119"/>
+      <c r="AX54" s="103"/>
+      <c r="AY54" s="104"/>
+      <c r="AZ54" s="85"/>
     </row>
     <row r="55" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A55" s="88"/>
-      <c r="B55" s="97"/>
-      <c r="C55" s="90"/>
+      <c r="A55" s="93"/>
+      <c r="B55" s="117"/>
+      <c r="C55" s="97"/>
       <c r="D55" s="11"/>
       <c r="E55" s="32"/>
       <c r="F55" s="3"/>
@@ -4887,10 +4887,10 @@
       <c r="Q55" s="32"/>
       <c r="R55" s="3"/>
       <c r="S55" s="31"/>
-      <c r="T55" s="70"/>
-      <c r="U55" s="71"/>
-      <c r="V55" s="71"/>
-      <c r="W55" s="72"/>
+      <c r="T55" s="113"/>
+      <c r="U55" s="105"/>
+      <c r="V55" s="105"/>
+      <c r="W55" s="104"/>
       <c r="X55" s="11"/>
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
@@ -4902,33 +4902,33 @@
       <c r="AF55" s="33"/>
       <c r="AG55" s="32"/>
       <c r="AH55" s="32"/>
-      <c r="AI55" s="31"/>
+      <c r="AI55" s="66"/>
       <c r="AJ55" s="33"/>
       <c r="AK55" s="32"/>
       <c r="AL55" s="32"/>
       <c r="AM55" s="31"/>
-      <c r="AN55" s="70"/>
-      <c r="AO55" s="71"/>
-      <c r="AP55" s="71"/>
-      <c r="AQ55" s="72"/>
+      <c r="AN55" s="113"/>
+      <c r="AO55" s="105"/>
+      <c r="AP55" s="105"/>
+      <c r="AQ55" s="104"/>
       <c r="AR55" s="33"/>
       <c r="AS55" s="32"/>
       <c r="AT55" s="32"/>
       <c r="AU55" s="12"/>
       <c r="AV55" s="11"/>
       <c r="AW55" s="3"/>
-      <c r="AX55" s="101"/>
-      <c r="AY55" s="72"/>
-      <c r="AZ55" s="119"/>
+      <c r="AX55" s="103"/>
+      <c r="AY55" s="104"/>
+      <c r="AZ55" s="85"/>
     </row>
     <row r="56" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A56" s="94" t="s">
+      <c r="A56" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="95">
+      <c r="B56" s="121">
         <v>2</v>
       </c>
-      <c r="C56" s="93"/>
+      <c r="C56" s="120"/>
       <c r="D56" s="28"/>
       <c r="E56" s="5"/>
       <c r="F56" s="30"/>
@@ -4945,10 +4945,10 @@
       <c r="Q56" s="5"/>
       <c r="R56" s="30"/>
       <c r="S56" s="7"/>
-      <c r="T56" s="70"/>
-      <c r="U56" s="71"/>
-      <c r="V56" s="71"/>
-      <c r="W56" s="72"/>
+      <c r="T56" s="113"/>
+      <c r="U56" s="105"/>
+      <c r="V56" s="105"/>
+      <c r="W56" s="104"/>
       <c r="X56" s="28"/>
       <c r="Y56" s="30"/>
       <c r="Z56" s="30"/>
@@ -4965,24 +4965,24 @@
       <c r="AK56" s="24"/>
       <c r="AL56" s="5"/>
       <c r="AM56" s="7"/>
-      <c r="AN56" s="70"/>
-      <c r="AO56" s="71"/>
-      <c r="AP56" s="71"/>
-      <c r="AQ56" s="72"/>
+      <c r="AN56" s="113"/>
+      <c r="AO56" s="105"/>
+      <c r="AP56" s="105"/>
+      <c r="AQ56" s="104"/>
       <c r="AR56" s="6"/>
       <c r="AS56" s="5"/>
       <c r="AT56" s="5"/>
       <c r="AU56" s="29"/>
       <c r="AV56" s="28"/>
       <c r="AW56" s="30"/>
-      <c r="AX56" s="101"/>
-      <c r="AY56" s="72"/>
-      <c r="AZ56" s="119"/>
+      <c r="AX56" s="103"/>
+      <c r="AY56" s="104"/>
+      <c r="AZ56" s="85"/>
     </row>
     <row r="57" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A57" s="88"/>
-      <c r="B57" s="89"/>
-      <c r="C57" s="90"/>
+      <c r="A57" s="93"/>
+      <c r="B57" s="95"/>
+      <c r="C57" s="97"/>
       <c r="D57" s="11"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -4999,10 +4999,10 @@
       <c r="Q57" s="3"/>
       <c r="R57" s="3"/>
       <c r="S57" s="12"/>
-      <c r="T57" s="70"/>
-      <c r="U57" s="71"/>
-      <c r="V57" s="71"/>
-      <c r="W57" s="72"/>
+      <c r="T57" s="113"/>
+      <c r="U57" s="105"/>
+      <c r="V57" s="105"/>
+      <c r="W57" s="104"/>
       <c r="X57" s="33"/>
       <c r="Y57" s="3"/>
       <c r="Z57" s="32"/>
@@ -5019,28 +5019,28 @@
       <c r="AK57" s="32"/>
       <c r="AL57" s="3"/>
       <c r="AM57" s="12"/>
-      <c r="AN57" s="70"/>
-      <c r="AO57" s="71"/>
-      <c r="AP57" s="71"/>
-      <c r="AQ57" s="72"/>
+      <c r="AN57" s="113"/>
+      <c r="AO57" s="105"/>
+      <c r="AP57" s="105"/>
+      <c r="AQ57" s="104"/>
       <c r="AR57" s="11"/>
       <c r="AS57" s="3"/>
       <c r="AT57" s="3"/>
       <c r="AU57" s="31"/>
       <c r="AV57" s="33"/>
       <c r="AW57" s="3"/>
-      <c r="AX57" s="101"/>
-      <c r="AY57" s="72"/>
-      <c r="AZ57" s="119"/>
+      <c r="AX57" s="103"/>
+      <c r="AY57" s="104"/>
+      <c r="AZ57" s="85"/>
     </row>
     <row r="58" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A58" s="91" t="s">
+      <c r="A58" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="92">
+      <c r="B58" s="88">
         <v>2</v>
       </c>
-      <c r="C58" s="93"/>
+      <c r="C58" s="120"/>
       <c r="D58" s="28"/>
       <c r="E58" s="30"/>
       <c r="F58" s="30"/>
@@ -5057,10 +5057,10 @@
       <c r="Q58" s="30"/>
       <c r="R58" s="30"/>
       <c r="S58" s="29"/>
-      <c r="T58" s="70"/>
-      <c r="U58" s="71"/>
-      <c r="V58" s="71"/>
-      <c r="W58" s="72"/>
+      <c r="T58" s="113"/>
+      <c r="U58" s="105"/>
+      <c r="V58" s="105"/>
+      <c r="W58" s="104"/>
       <c r="X58" s="6"/>
       <c r="Y58" s="30"/>
       <c r="Z58" s="5"/>
@@ -5077,24 +5077,24 @@
       <c r="AK58" s="5"/>
       <c r="AL58" s="34"/>
       <c r="AM58" s="59"/>
-      <c r="AN58" s="70"/>
-      <c r="AO58" s="71"/>
-      <c r="AP58" s="71"/>
-      <c r="AQ58" s="72"/>
+      <c r="AN58" s="113"/>
+      <c r="AO58" s="105"/>
+      <c r="AP58" s="105"/>
+      <c r="AQ58" s="104"/>
       <c r="AR58" s="28"/>
       <c r="AS58" s="30"/>
       <c r="AT58" s="30"/>
       <c r="AU58" s="7"/>
       <c r="AV58" s="6"/>
       <c r="AW58" s="30"/>
-      <c r="AX58" s="101"/>
-      <c r="AY58" s="72"/>
-      <c r="AZ58" s="119"/>
+      <c r="AX58" s="103"/>
+      <c r="AY58" s="104"/>
+      <c r="AZ58" s="85"/>
     </row>
     <row r="59" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="77"/>
-      <c r="B59" s="79"/>
-      <c r="C59" s="81"/>
+      <c r="A59" s="87"/>
+      <c r="B59" s="89"/>
+      <c r="C59" s="91"/>
       <c r="D59" s="8"/>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
@@ -5111,10 +5111,10 @@
       <c r="Q59" s="9"/>
       <c r="R59" s="9"/>
       <c r="S59" s="10"/>
-      <c r="T59" s="70"/>
-      <c r="U59" s="71"/>
-      <c r="V59" s="71"/>
-      <c r="W59" s="72"/>
+      <c r="T59" s="113"/>
+      <c r="U59" s="105"/>
+      <c r="V59" s="105"/>
+      <c r="W59" s="104"/>
       <c r="X59" s="8"/>
       <c r="Y59" s="9"/>
       <c r="Z59" s="9"/>
@@ -5131,28 +5131,28 @@
       <c r="AK59" s="9"/>
       <c r="AL59" s="9"/>
       <c r="AM59" s="10"/>
-      <c r="AN59" s="70"/>
-      <c r="AO59" s="71"/>
-      <c r="AP59" s="71"/>
-      <c r="AQ59" s="72"/>
+      <c r="AN59" s="113"/>
+      <c r="AO59" s="105"/>
+      <c r="AP59" s="105"/>
+      <c r="AQ59" s="104"/>
       <c r="AR59" s="8"/>
       <c r="AS59" s="9"/>
       <c r="AT59" s="9"/>
       <c r="AU59" s="10"/>
       <c r="AV59" s="8"/>
       <c r="AW59" s="9"/>
-      <c r="AX59" s="101"/>
-      <c r="AY59" s="72"/>
-      <c r="AZ59" s="118"/>
+      <c r="AX59" s="103"/>
+      <c r="AY59" s="104"/>
+      <c r="AZ59" s="84"/>
     </row>
     <row r="60" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A60" s="76" t="s">
+      <c r="A60" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="B60" s="78">
+      <c r="B60" s="94">
         <v>0.5</v>
       </c>
-      <c r="C60" s="80"/>
+      <c r="C60" s="96"/>
       <c r="D60" s="15"/>
       <c r="E60" s="16"/>
       <c r="F60" s="16"/>
@@ -5169,10 +5169,10 @@
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
       <c r="S60" s="17"/>
-      <c r="T60" s="70"/>
-      <c r="U60" s="71"/>
-      <c r="V60" s="71"/>
-      <c r="W60" s="72"/>
+      <c r="T60" s="113"/>
+      <c r="U60" s="105"/>
+      <c r="V60" s="105"/>
+      <c r="W60" s="104"/>
       <c r="X60" s="15"/>
       <c r="Y60" s="16"/>
       <c r="Z60" s="16"/>
@@ -5189,26 +5189,26 @@
       <c r="AK60" s="16"/>
       <c r="AL60" s="16"/>
       <c r="AM60" s="17"/>
-      <c r="AN60" s="70"/>
-      <c r="AO60" s="71"/>
-      <c r="AP60" s="71"/>
-      <c r="AQ60" s="72"/>
+      <c r="AN60" s="113"/>
+      <c r="AO60" s="105"/>
+      <c r="AP60" s="105"/>
+      <c r="AQ60" s="104"/>
       <c r="AR60" s="23"/>
       <c r="AS60" s="16"/>
       <c r="AT60" s="16"/>
       <c r="AU60" s="17"/>
       <c r="AV60" s="15"/>
       <c r="AW60" s="16"/>
-      <c r="AX60" s="101"/>
-      <c r="AY60" s="72"/>
-      <c r="AZ60" s="85" t="s">
+      <c r="AX60" s="103"/>
+      <c r="AY60" s="104"/>
+      <c r="AZ60" s="98" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A61" s="88"/>
-      <c r="B61" s="89"/>
-      <c r="C61" s="90"/>
+      <c r="A61" s="93"/>
+      <c r="B61" s="95"/>
+      <c r="C61" s="97"/>
       <c r="D61" s="11"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -5225,10 +5225,10 @@
       <c r="Q61" s="3"/>
       <c r="R61" s="3"/>
       <c r="S61" s="12"/>
-      <c r="T61" s="70"/>
-      <c r="U61" s="71"/>
-      <c r="V61" s="71"/>
-      <c r="W61" s="72"/>
+      <c r="T61" s="113"/>
+      <c r="U61" s="105"/>
+      <c r="V61" s="105"/>
+      <c r="W61" s="104"/>
       <c r="X61" s="11"/>
       <c r="Y61" s="3"/>
       <c r="Z61" s="3"/>
@@ -5245,28 +5245,28 @@
       <c r="AK61" s="32"/>
       <c r="AL61" s="3"/>
       <c r="AM61" s="12"/>
-      <c r="AN61" s="70"/>
-      <c r="AO61" s="71"/>
-      <c r="AP61" s="71"/>
-      <c r="AQ61" s="72"/>
+      <c r="AN61" s="113"/>
+      <c r="AO61" s="105"/>
+      <c r="AP61" s="105"/>
+      <c r="AQ61" s="104"/>
       <c r="AR61" s="11"/>
       <c r="AS61" s="3"/>
       <c r="AT61" s="3"/>
       <c r="AU61" s="12"/>
       <c r="AV61" s="33"/>
       <c r="AW61" s="3"/>
-      <c r="AX61" s="101"/>
-      <c r="AY61" s="72"/>
-      <c r="AZ61" s="86"/>
+      <c r="AX61" s="103"/>
+      <c r="AY61" s="104"/>
+      <c r="AZ61" s="99"/>
     </row>
     <row r="62" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A62" s="91" t="s">
+      <c r="A62" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="B62" s="92">
+      <c r="B62" s="88">
         <v>2</v>
       </c>
-      <c r="C62" s="93"/>
+      <c r="C62" s="120"/>
       <c r="D62" s="28"/>
       <c r="E62" s="30"/>
       <c r="F62" s="30"/>
@@ -5283,10 +5283,10 @@
       <c r="Q62" s="30"/>
       <c r="R62" s="30"/>
       <c r="S62" s="29"/>
-      <c r="T62" s="70"/>
-      <c r="U62" s="71"/>
-      <c r="V62" s="71"/>
-      <c r="W62" s="72"/>
+      <c r="T62" s="113"/>
+      <c r="U62" s="105"/>
+      <c r="V62" s="105"/>
+      <c r="W62" s="104"/>
       <c r="X62" s="28"/>
       <c r="Y62" s="30"/>
       <c r="Z62" s="30"/>
@@ -5303,24 +5303,24 @@
       <c r="AK62" s="5"/>
       <c r="AL62" s="30"/>
       <c r="AM62" s="29"/>
-      <c r="AN62" s="70"/>
-      <c r="AO62" s="71"/>
-      <c r="AP62" s="71"/>
-      <c r="AQ62" s="72"/>
+      <c r="AN62" s="113"/>
+      <c r="AO62" s="105"/>
+      <c r="AP62" s="105"/>
+      <c r="AQ62" s="104"/>
       <c r="AR62" s="38"/>
       <c r="AS62" s="34"/>
       <c r="AT62" s="30"/>
       <c r="AU62" s="29"/>
       <c r="AV62" s="6"/>
       <c r="AW62" s="30"/>
-      <c r="AX62" s="101"/>
-      <c r="AY62" s="72"/>
-      <c r="AZ62" s="86"/>
+      <c r="AX62" s="103"/>
+      <c r="AY62" s="104"/>
+      <c r="AZ62" s="99"/>
     </row>
     <row r="63" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="77"/>
-      <c r="B63" s="79"/>
-      <c r="C63" s="81"/>
+      <c r="A63" s="87"/>
+      <c r="B63" s="89"/>
+      <c r="C63" s="91"/>
       <c r="D63" s="8"/>
       <c r="E63" s="9"/>
       <c r="F63" s="9"/>
@@ -5337,10 +5337,10 @@
       <c r="Q63" s="9"/>
       <c r="R63" s="9"/>
       <c r="S63" s="10"/>
-      <c r="T63" s="70"/>
-      <c r="U63" s="71"/>
-      <c r="V63" s="71"/>
-      <c r="W63" s="72"/>
+      <c r="T63" s="113"/>
+      <c r="U63" s="105"/>
+      <c r="V63" s="105"/>
+      <c r="W63" s="104"/>
       <c r="X63" s="8"/>
       <c r="Y63" s="9"/>
       <c r="Z63" s="9"/>
@@ -5357,28 +5357,28 @@
       <c r="AK63" s="9"/>
       <c r="AL63" s="9"/>
       <c r="AM63" s="10"/>
-      <c r="AN63" s="70"/>
-      <c r="AO63" s="71"/>
-      <c r="AP63" s="71"/>
-      <c r="AQ63" s="72"/>
+      <c r="AN63" s="113"/>
+      <c r="AO63" s="105"/>
+      <c r="AP63" s="105"/>
+      <c r="AQ63" s="104"/>
       <c r="AR63" s="8"/>
       <c r="AS63" s="9"/>
       <c r="AT63" s="9"/>
       <c r="AU63" s="10"/>
       <c r="AV63" s="8"/>
       <c r="AW63" s="9"/>
-      <c r="AX63" s="101"/>
-      <c r="AY63" s="72"/>
-      <c r="AZ63" s="87"/>
+      <c r="AX63" s="103"/>
+      <c r="AY63" s="104"/>
+      <c r="AZ63" s="100"/>
     </row>
     <row r="64" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A64" s="76" t="s">
+      <c r="A64" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="B64" s="78">
+      <c r="B64" s="94">
         <v>2.5</v>
       </c>
-      <c r="C64" s="80"/>
+      <c r="C64" s="96"/>
       <c r="D64" s="15"/>
       <c r="E64" s="16"/>
       <c r="F64" s="16"/>
@@ -5395,10 +5395,10 @@
       <c r="Q64" s="16"/>
       <c r="R64" s="16"/>
       <c r="S64" s="17"/>
-      <c r="T64" s="70"/>
-      <c r="U64" s="71"/>
-      <c r="V64" s="71"/>
-      <c r="W64" s="72"/>
+      <c r="T64" s="113"/>
+      <c r="U64" s="105"/>
+      <c r="V64" s="105"/>
+      <c r="W64" s="104"/>
       <c r="X64" s="15"/>
       <c r="Y64" s="16"/>
       <c r="Z64" s="16"/>
@@ -5415,26 +5415,26 @@
       <c r="AK64" s="16"/>
       <c r="AL64" s="16"/>
       <c r="AM64" s="17"/>
-      <c r="AN64" s="70"/>
-      <c r="AO64" s="71"/>
-      <c r="AP64" s="71"/>
-      <c r="AQ64" s="72"/>
+      <c r="AN64" s="113"/>
+      <c r="AO64" s="105"/>
+      <c r="AP64" s="105"/>
+      <c r="AQ64" s="104"/>
       <c r="AR64" s="15"/>
       <c r="AS64" s="16"/>
       <c r="AT64" s="27"/>
       <c r="AU64" s="58"/>
       <c r="AV64" s="15"/>
       <c r="AW64" s="16"/>
-      <c r="AX64" s="101"/>
-      <c r="AY64" s="72"/>
-      <c r="AZ64" s="85" t="s">
+      <c r="AX64" s="103"/>
+      <c r="AY64" s="104"/>
+      <c r="AZ64" s="98" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="77"/>
-      <c r="B65" s="79"/>
-      <c r="C65" s="81"/>
+      <c r="A65" s="87"/>
+      <c r="B65" s="89"/>
+      <c r="C65" s="91"/>
       <c r="D65" s="8"/>
       <c r="E65" s="9"/>
       <c r="F65" s="9"/>
@@ -5451,10 +5451,10 @@
       <c r="Q65" s="9"/>
       <c r="R65" s="9"/>
       <c r="S65" s="10"/>
-      <c r="T65" s="73"/>
-      <c r="U65" s="74"/>
-      <c r="V65" s="74"/>
-      <c r="W65" s="75"/>
+      <c r="T65" s="114"/>
+      <c r="U65" s="115"/>
+      <c r="V65" s="115"/>
+      <c r="W65" s="107"/>
       <c r="X65" s="8"/>
       <c r="Y65" s="9"/>
       <c r="Z65" s="9"/>
@@ -5471,19 +5471,19 @@
       <c r="AK65" s="9"/>
       <c r="AL65" s="9"/>
       <c r="AM65" s="10"/>
-      <c r="AN65" s="73"/>
-      <c r="AO65" s="74"/>
-      <c r="AP65" s="74"/>
-      <c r="AQ65" s="75"/>
+      <c r="AN65" s="114"/>
+      <c r="AO65" s="115"/>
+      <c r="AP65" s="115"/>
+      <c r="AQ65" s="107"/>
       <c r="AR65" s="8"/>
       <c r="AS65" s="9"/>
       <c r="AT65" s="9"/>
       <c r="AU65" s="10"/>
       <c r="AV65" s="8"/>
       <c r="AW65" s="9"/>
-      <c r="AX65" s="102"/>
-      <c r="AY65" s="75"/>
-      <c r="AZ65" s="87"/>
+      <c r="AX65" s="106"/>
+      <c r="AY65" s="107"/>
+      <c r="AZ65" s="100"/>
     </row>
     <row r="66" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="14" t="s">
@@ -5549,6 +5549,112 @@
     </row>
   </sheetData>
   <mergeCells count="130">
+    <mergeCell ref="T4:W65"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="AZ12:AZ15"/>
+    <mergeCell ref="AZ16:AZ27"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="AZ60:AZ63"/>
+    <mergeCell ref="AZ64:AZ65"/>
+    <mergeCell ref="AX4:AY65"/>
+    <mergeCell ref="AR1:AU1"/>
+    <mergeCell ref="AR2:AU2"/>
+    <mergeCell ref="AV1:AY1"/>
+    <mergeCell ref="AV2:AY2"/>
+    <mergeCell ref="AZ1:AZ3"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AF2:AI2"/>
+    <mergeCell ref="AJ1:AM1"/>
+    <mergeCell ref="AJ2:AM2"/>
+    <mergeCell ref="AN1:AQ1"/>
+    <mergeCell ref="AN2:AQ2"/>
+    <mergeCell ref="AN4:AQ65"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:C2"/>
     <mergeCell ref="D1:G1"/>
@@ -5573,112 +5679,6 @@
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
-    <mergeCell ref="AZ60:AZ63"/>
-    <mergeCell ref="AZ64:AZ65"/>
-    <mergeCell ref="AX4:AY65"/>
-    <mergeCell ref="AR1:AU1"/>
-    <mergeCell ref="AR2:AU2"/>
-    <mergeCell ref="AV1:AY1"/>
-    <mergeCell ref="AV2:AY2"/>
-    <mergeCell ref="AZ1:AZ3"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AF2:AI2"/>
-    <mergeCell ref="AJ1:AM1"/>
-    <mergeCell ref="AJ2:AM2"/>
-    <mergeCell ref="AN1:AQ1"/>
-    <mergeCell ref="AN2:AQ2"/>
-    <mergeCell ref="AN4:AQ65"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="T4:W65"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="AZ12:AZ15"/>
-    <mergeCell ref="AZ16:AZ27"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="47" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
super tag habe viel text verfasst ausserdem ist meine applikation jetzt von redundantem code empfernt und fehler sind behendelt
</commit_message>
<xml_diff>
--- a/Doku/Shannon_Neil_Schuerch_Zeitplan_IPA_2022.xlsx
+++ b/Doku/Shannon_Neil_Schuerch_Zeitplan_IPA_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Dashboardd\Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED9A8AD-839F-499D-9241-DF5901445F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498C9E64-8935-4376-ACF8-501047E5DB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14625" xr2:uid="{B08A1154-B080-432D-B17F-9B53C1DBF0AA}"/>
   </bookViews>
@@ -1118,6 +1118,135 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1139,24 +1268,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1165,117 +1276,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1596,8 +1596,8 @@
   </sheetPr>
   <dimension ref="A1:BC66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI55" sqref="AI55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="BD28" sqref="BD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,169 +1654,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="77" t="s">
+      <c r="C1" s="117"/>
+      <c r="D1" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="77" t="s">
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="77" t="s">
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="77" t="s">
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="77" t="s">
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="108"/>
+      <c r="T1" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="79"/>
-      <c r="X1" s="77" t="s">
+      <c r="U1" s="107"/>
+      <c r="V1" s="107"/>
+      <c r="W1" s="108"/>
+      <c r="X1" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="79"/>
-      <c r="AB1" s="77" t="s">
+      <c r="Y1" s="107"/>
+      <c r="Z1" s="107"/>
+      <c r="AA1" s="108"/>
+      <c r="AB1" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="79"/>
-      <c r="AF1" s="77" t="s">
+      <c r="AC1" s="107"/>
+      <c r="AD1" s="107"/>
+      <c r="AE1" s="108"/>
+      <c r="AF1" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="AG1" s="78"/>
-      <c r="AH1" s="78"/>
-      <c r="AI1" s="79"/>
-      <c r="AJ1" s="77" t="s">
+      <c r="AG1" s="107"/>
+      <c r="AH1" s="107"/>
+      <c r="AI1" s="108"/>
+      <c r="AJ1" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="AK1" s="78"/>
-      <c r="AL1" s="78"/>
-      <c r="AM1" s="79"/>
-      <c r="AN1" s="77" t="s">
+      <c r="AK1" s="107"/>
+      <c r="AL1" s="107"/>
+      <c r="AM1" s="108"/>
+      <c r="AN1" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="AO1" s="78"/>
-      <c r="AP1" s="78"/>
-      <c r="AQ1" s="79"/>
-      <c r="AR1" s="77" t="s">
+      <c r="AO1" s="107"/>
+      <c r="AP1" s="107"/>
+      <c r="AQ1" s="108"/>
+      <c r="AR1" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="AS1" s="78"/>
-      <c r="AT1" s="78"/>
-      <c r="AU1" s="79"/>
-      <c r="AV1" s="77" t="s">
+      <c r="AS1" s="107"/>
+      <c r="AT1" s="107"/>
+      <c r="AU1" s="108"/>
+      <c r="AV1" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="AW1" s="78"/>
-      <c r="AX1" s="78"/>
-      <c r="AY1" s="79"/>
-      <c r="AZ1" s="108" t="s">
+      <c r="AW1" s="107"/>
+      <c r="AX1" s="107"/>
+      <c r="AY1" s="108"/>
+      <c r="AZ1" s="85" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A2" s="71"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="80">
+      <c r="A2" s="114"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="109">
         <v>44627</v>
       </c>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="80">
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="109">
         <v>44628</v>
       </c>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="80">
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="109">
         <v>44629</v>
       </c>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="80">
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="109">
         <v>44630</v>
       </c>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
-      <c r="S2" s="82"/>
-      <c r="T2" s="80">
+      <c r="Q2" s="110"/>
+      <c r="R2" s="110"/>
+      <c r="S2" s="111"/>
+      <c r="T2" s="109">
         <v>44631</v>
       </c>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="82"/>
-      <c r="X2" s="80">
+      <c r="U2" s="110"/>
+      <c r="V2" s="110"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="109">
         <v>44634</v>
       </c>
-      <c r="Y2" s="81"/>
-      <c r="Z2" s="81"/>
-      <c r="AA2" s="82"/>
-      <c r="AB2" s="80">
+      <c r="Y2" s="110"/>
+      <c r="Z2" s="110"/>
+      <c r="AA2" s="111"/>
+      <c r="AB2" s="109">
         <v>44635</v>
       </c>
-      <c r="AC2" s="81"/>
-      <c r="AD2" s="81"/>
-      <c r="AE2" s="82"/>
-      <c r="AF2" s="80">
+      <c r="AC2" s="110"/>
+      <c r="AD2" s="110"/>
+      <c r="AE2" s="111"/>
+      <c r="AF2" s="109">
         <v>44636</v>
       </c>
-      <c r="AG2" s="81"/>
-      <c r="AH2" s="81"/>
-      <c r="AI2" s="82"/>
-      <c r="AJ2" s="80">
+      <c r="AG2" s="110"/>
+      <c r="AH2" s="110"/>
+      <c r="AI2" s="111"/>
+      <c r="AJ2" s="109">
         <v>44637</v>
       </c>
-      <c r="AK2" s="81"/>
-      <c r="AL2" s="81"/>
-      <c r="AM2" s="82"/>
-      <c r="AN2" s="80">
+      <c r="AK2" s="110"/>
+      <c r="AL2" s="110"/>
+      <c r="AM2" s="111"/>
+      <c r="AN2" s="109">
         <v>44638</v>
       </c>
-      <c r="AO2" s="81"/>
-      <c r="AP2" s="81"/>
-      <c r="AQ2" s="82"/>
-      <c r="AR2" s="80">
+      <c r="AO2" s="110"/>
+      <c r="AP2" s="110"/>
+      <c r="AQ2" s="111"/>
+      <c r="AR2" s="109">
         <v>44641</v>
       </c>
-      <c r="AS2" s="81"/>
-      <c r="AT2" s="81"/>
-      <c r="AU2" s="82"/>
-      <c r="AV2" s="80">
+      <c r="AS2" s="110"/>
+      <c r="AT2" s="110"/>
+      <c r="AU2" s="111"/>
+      <c r="AV2" s="109">
         <v>44642</v>
       </c>
-      <c r="AW2" s="81"/>
-      <c r="AX2" s="81"/>
-      <c r="AY2" s="82"/>
-      <c r="AZ2" s="109"/>
+      <c r="AW2" s="110"/>
+      <c r="AX2" s="110"/>
+      <c r="AY2" s="111"/>
+      <c r="AZ2" s="86"/>
     </row>
     <row r="3" spans="1:55" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="72"/>
+      <c r="A3" s="115"/>
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
@@ -1967,17 +1967,17 @@
       <c r="AY3" s="12">
         <v>17</v>
       </c>
-      <c r="AZ3" s="110"/>
+      <c r="AZ3" s="112"/>
     </row>
     <row r="4" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="94">
+      <c r="B4" s="81">
         <v>4</v>
       </c>
-      <c r="C4" s="96">
-        <v>2</v>
+      <c r="C4" s="83">
+        <v>4</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="16"/>
@@ -1995,12 +1995,12 @@
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
       <c r="S4" s="17"/>
-      <c r="T4" s="111" t="s">
+      <c r="T4" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="102"/>
+      <c r="U4" s="71"/>
+      <c r="V4" s="71"/>
+      <c r="W4" s="72"/>
       <c r="X4" s="15"/>
       <c r="Y4" s="16"/>
       <c r="Z4" s="16"/>
@@ -2017,32 +2017,32 @@
       <c r="AK4" s="16"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="17"/>
-      <c r="AN4" s="111" t="s">
+      <c r="AN4" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="AO4" s="112"/>
-      <c r="AP4" s="112"/>
-      <c r="AQ4" s="102"/>
+      <c r="AO4" s="71"/>
+      <c r="AP4" s="71"/>
+      <c r="AQ4" s="72"/>
       <c r="AR4" s="15"/>
       <c r="AS4" s="16"/>
       <c r="AT4" s="16"/>
       <c r="AU4" s="17"/>
       <c r="AV4" s="15"/>
       <c r="AW4" s="16"/>
-      <c r="AX4" s="101" t="s">
+      <c r="AX4" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="AY4" s="102"/>
-      <c r="AZ4" s="108"/>
+      <c r="AY4" s="72"/>
+      <c r="AZ4" s="85"/>
       <c r="BB4" s="60" t="s">
         <v>50</v>
       </c>
       <c r="BC4" s="61"/>
     </row>
     <row r="5" spans="1:55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="116"/>
-      <c r="B5" s="117"/>
-      <c r="C5" s="118"/>
+      <c r="A5" s="99"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="101"/>
       <c r="D5" s="33"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -2059,10 +2059,10 @@
       <c r="Q5" s="32"/>
       <c r="R5" s="3"/>
       <c r="S5" s="12"/>
-      <c r="T5" s="113"/>
-      <c r="U5" s="105"/>
-      <c r="V5" s="105"/>
-      <c r="W5" s="104"/>
+      <c r="T5" s="73"/>
+      <c r="U5" s="74"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="75"/>
       <c r="X5" s="11"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="32"/>
@@ -2079,32 +2079,34 @@
       <c r="AK5" s="3"/>
       <c r="AL5" s="3"/>
       <c r="AM5" s="12"/>
-      <c r="AN5" s="113"/>
-      <c r="AO5" s="105"/>
-      <c r="AP5" s="105"/>
-      <c r="AQ5" s="104"/>
+      <c r="AN5" s="73"/>
+      <c r="AO5" s="74"/>
+      <c r="AP5" s="74"/>
+      <c r="AQ5" s="75"/>
       <c r="AR5" s="11"/>
       <c r="AS5" s="3"/>
       <c r="AT5" s="3"/>
       <c r="AU5" s="12"/>
       <c r="AV5" s="11"/>
       <c r="AW5" s="3"/>
-      <c r="AX5" s="103"/>
-      <c r="AY5" s="104"/>
-      <c r="AZ5" s="109"/>
+      <c r="AX5" s="104"/>
+      <c r="AY5" s="75"/>
+      <c r="AZ5" s="86"/>
       <c r="BB5" s="62" t="s">
         <v>51</v>
       </c>
       <c r="BC5" s="63"/>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A6" s="119" t="s">
+      <c r="A6" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="88">
+      <c r="B6" s="95">
         <v>32</v>
       </c>
-      <c r="C6" s="120"/>
+      <c r="C6" s="96">
+        <v>26.5</v>
+      </c>
       <c r="D6" s="13"/>
       <c r="E6" s="35"/>
       <c r="F6" s="30"/>
@@ -2121,10 +2123,10 @@
       <c r="Q6" s="24"/>
       <c r="R6" s="47"/>
       <c r="S6" s="48"/>
-      <c r="T6" s="113"/>
-      <c r="U6" s="105"/>
-      <c r="V6" s="105"/>
-      <c r="W6" s="104"/>
+      <c r="T6" s="73"/>
+      <c r="U6" s="74"/>
+      <c r="V6" s="74"/>
+      <c r="W6" s="75"/>
       <c r="X6" s="38"/>
       <c r="Y6" s="34"/>
       <c r="Z6" s="24"/>
@@ -2141,28 +2143,28 @@
       <c r="AK6" s="34"/>
       <c r="AL6" s="34"/>
       <c r="AM6" s="49"/>
-      <c r="AN6" s="113"/>
-      <c r="AO6" s="105"/>
-      <c r="AP6" s="105"/>
-      <c r="AQ6" s="104"/>
+      <c r="AN6" s="73"/>
+      <c r="AO6" s="74"/>
+      <c r="AP6" s="74"/>
+      <c r="AQ6" s="75"/>
       <c r="AR6" s="38"/>
       <c r="AS6" s="34"/>
       <c r="AT6" s="34"/>
       <c r="AU6" s="49"/>
       <c r="AV6" s="38"/>
       <c r="AW6" s="34"/>
-      <c r="AX6" s="103"/>
-      <c r="AY6" s="104"/>
-      <c r="AZ6" s="109"/>
+      <c r="AX6" s="104"/>
+      <c r="AY6" s="75"/>
+      <c r="AZ6" s="86"/>
       <c r="BB6" s="62" t="s">
         <v>52</v>
       </c>
       <c r="BC6" s="64"/>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A7" s="116"/>
-      <c r="B7" s="117"/>
-      <c r="C7" s="118"/>
+      <c r="A7" s="99"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="101"/>
       <c r="D7" s="33"/>
       <c r="E7" s="32"/>
       <c r="F7" s="3"/>
@@ -2179,10 +2181,10 @@
       <c r="Q7" s="40"/>
       <c r="R7" s="40"/>
       <c r="S7" s="65"/>
-      <c r="T7" s="113"/>
-      <c r="U7" s="105"/>
-      <c r="V7" s="105"/>
-      <c r="W7" s="104"/>
+      <c r="T7" s="73"/>
+      <c r="U7" s="74"/>
+      <c r="V7" s="74"/>
+      <c r="W7" s="75"/>
       <c r="X7" s="57"/>
       <c r="Y7" s="40"/>
       <c r="Z7" s="40"/>
@@ -2195,34 +2197,34 @@
       <c r="AG7" s="40"/>
       <c r="AH7" s="40"/>
       <c r="AI7" s="65"/>
-      <c r="AJ7" s="11"/>
-      <c r="AK7" s="3"/>
+      <c r="AJ7" s="39"/>
+      <c r="AK7" s="40"/>
       <c r="AL7" s="3"/>
       <c r="AM7" s="12"/>
-      <c r="AN7" s="113"/>
-      <c r="AO7" s="105"/>
-      <c r="AP7" s="105"/>
-      <c r="AQ7" s="104"/>
+      <c r="AN7" s="73"/>
+      <c r="AO7" s="74"/>
+      <c r="AP7" s="74"/>
+      <c r="AQ7" s="75"/>
       <c r="AR7" s="11"/>
       <c r="AS7" s="3"/>
       <c r="AT7" s="3"/>
       <c r="AU7" s="12"/>
       <c r="AV7" s="11"/>
       <c r="AW7" s="3"/>
-      <c r="AX7" s="103"/>
-      <c r="AY7" s="104"/>
-      <c r="AZ7" s="109"/>
+      <c r="AX7" s="104"/>
+      <c r="AY7" s="75"/>
+      <c r="AZ7" s="86"/>
       <c r="BB7" s="4"/>
       <c r="BC7" s="4"/>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A8" s="119" t="s">
+      <c r="A8" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="121">
+      <c r="B8" s="98">
         <v>4</v>
       </c>
-      <c r="C8" s="120">
+      <c r="C8" s="96">
         <v>5</v>
       </c>
       <c r="D8" s="26"/>
@@ -2241,10 +2243,10 @@
       <c r="Q8" s="30"/>
       <c r="R8" s="30"/>
       <c r="S8" s="29"/>
-      <c r="T8" s="113"/>
-      <c r="U8" s="105"/>
-      <c r="V8" s="105"/>
-      <c r="W8" s="104"/>
+      <c r="T8" s="73"/>
+      <c r="U8" s="74"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="75"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="30"/>
       <c r="Z8" s="30"/>
@@ -2261,26 +2263,26 @@
       <c r="AK8" s="30"/>
       <c r="AL8" s="30"/>
       <c r="AM8" s="29"/>
-      <c r="AN8" s="113"/>
-      <c r="AO8" s="105"/>
-      <c r="AP8" s="105"/>
-      <c r="AQ8" s="104"/>
+      <c r="AN8" s="73"/>
+      <c r="AO8" s="74"/>
+      <c r="AP8" s="74"/>
+      <c r="AQ8" s="75"/>
       <c r="AR8" s="28"/>
       <c r="AS8" s="30"/>
       <c r="AT8" s="30"/>
       <c r="AU8" s="29"/>
       <c r="AV8" s="28"/>
       <c r="AW8" s="30"/>
-      <c r="AX8" s="103"/>
-      <c r="AY8" s="104"/>
-      <c r="AZ8" s="109"/>
+      <c r="AX8" s="104"/>
+      <c r="AY8" s="75"/>
+      <c r="AZ8" s="86"/>
       <c r="BB8" s="4"/>
       <c r="BC8" s="4"/>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A9" s="93"/>
-      <c r="B9" s="95"/>
-      <c r="C9" s="118"/>
+      <c r="A9" s="91"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="101"/>
       <c r="D9" s="39"/>
       <c r="E9" s="40"/>
       <c r="F9" s="54"/>
@@ -2297,10 +2299,10 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="12"/>
-      <c r="T9" s="113"/>
-      <c r="U9" s="105"/>
-      <c r="V9" s="105"/>
-      <c r="W9" s="104"/>
+      <c r="T9" s="73"/>
+      <c r="U9" s="74"/>
+      <c r="V9" s="74"/>
+      <c r="W9" s="75"/>
       <c r="X9" s="11"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
@@ -2317,30 +2319,30 @@
       <c r="AK9" s="3"/>
       <c r="AL9" s="32"/>
       <c r="AM9" s="12"/>
-      <c r="AN9" s="113"/>
-      <c r="AO9" s="105"/>
-      <c r="AP9" s="105"/>
-      <c r="AQ9" s="104"/>
+      <c r="AN9" s="73"/>
+      <c r="AO9" s="74"/>
+      <c r="AP9" s="74"/>
+      <c r="AQ9" s="75"/>
       <c r="AR9" s="11"/>
       <c r="AS9" s="3"/>
       <c r="AT9" s="3"/>
       <c r="AU9" s="12"/>
       <c r="AV9" s="11"/>
       <c r="AW9" s="3"/>
-      <c r="AX9" s="103"/>
-      <c r="AY9" s="104"/>
-      <c r="AZ9" s="109"/>
+      <c r="AX9" s="104"/>
+      <c r="AY9" s="75"/>
+      <c r="AZ9" s="86"/>
       <c r="BB9" s="4"/>
       <c r="BC9" s="4"/>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A10" s="86" t="s">
+      <c r="A10" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="88">
+      <c r="B10" s="95">
         <v>2</v>
       </c>
-      <c r="C10" s="90">
+      <c r="C10" s="102">
         <v>1</v>
       </c>
       <c r="D10" s="28"/>
@@ -2359,10 +2361,10 @@
       <c r="Q10" s="30"/>
       <c r="R10" s="30"/>
       <c r="S10" s="29"/>
-      <c r="T10" s="113"/>
-      <c r="U10" s="105"/>
-      <c r="V10" s="105"/>
-      <c r="W10" s="104"/>
+      <c r="T10" s="73"/>
+      <c r="U10" s="74"/>
+      <c r="V10" s="74"/>
+      <c r="W10" s="75"/>
       <c r="X10" s="28"/>
       <c r="Y10" s="30"/>
       <c r="Z10" s="30"/>
@@ -2379,26 +2381,26 @@
       <c r="AK10" s="30"/>
       <c r="AL10" s="5"/>
       <c r="AM10" s="29"/>
-      <c r="AN10" s="113"/>
-      <c r="AO10" s="105"/>
-      <c r="AP10" s="105"/>
-      <c r="AQ10" s="104"/>
+      <c r="AN10" s="73"/>
+      <c r="AO10" s="74"/>
+      <c r="AP10" s="74"/>
+      <c r="AQ10" s="75"/>
       <c r="AR10" s="28"/>
       <c r="AS10" s="30"/>
       <c r="AT10" s="30"/>
       <c r="AU10" s="29"/>
       <c r="AV10" s="28"/>
       <c r="AW10" s="30"/>
-      <c r="AX10" s="103"/>
-      <c r="AY10" s="104"/>
-      <c r="AZ10" s="109"/>
+      <c r="AX10" s="104"/>
+      <c r="AY10" s="75"/>
+      <c r="AZ10" s="86"/>
       <c r="BB10" s="4"/>
       <c r="BC10" s="4"/>
     </row>
     <row r="11" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="87"/>
-      <c r="B11" s="89"/>
-      <c r="C11" s="91"/>
+      <c r="A11" s="80"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="84"/>
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
       <c r="F11" s="53"/>
@@ -2415,10 +2417,10 @@
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="113"/>
-      <c r="U11" s="105"/>
-      <c r="V11" s="105"/>
-      <c r="W11" s="104"/>
+      <c r="T11" s="73"/>
+      <c r="U11" s="74"/>
+      <c r="V11" s="74"/>
+      <c r="W11" s="75"/>
       <c r="X11" s="8"/>
       <c r="Y11" s="9"/>
       <c r="Z11" s="9"/>
@@ -2435,28 +2437,30 @@
       <c r="AK11" s="9"/>
       <c r="AL11" s="9"/>
       <c r="AM11" s="10"/>
-      <c r="AN11" s="113"/>
-      <c r="AO11" s="105"/>
-      <c r="AP11" s="105"/>
-      <c r="AQ11" s="104"/>
+      <c r="AN11" s="73"/>
+      <c r="AO11" s="74"/>
+      <c r="AP11" s="74"/>
+      <c r="AQ11" s="75"/>
       <c r="AR11" s="8"/>
       <c r="AS11" s="9"/>
       <c r="AT11" s="9"/>
       <c r="AU11" s="10"/>
       <c r="AV11" s="8"/>
       <c r="AW11" s="9"/>
-      <c r="AX11" s="103"/>
-      <c r="AY11" s="104"/>
-      <c r="AZ11" s="122"/>
+      <c r="AX11" s="104"/>
+      <c r="AY11" s="75"/>
+      <c r="AZ11" s="87"/>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A12" s="92" t="s">
+      <c r="A12" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="94">
+      <c r="B12" s="81">
         <v>1.5</v>
       </c>
-      <c r="C12" s="96"/>
+      <c r="C12" s="83">
+        <v>1</v>
+      </c>
       <c r="D12" s="18"/>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
@@ -2473,10 +2477,10 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
       <c r="S12" s="17"/>
-      <c r="T12" s="113"/>
-      <c r="U12" s="105"/>
-      <c r="V12" s="105"/>
-      <c r="W12" s="104"/>
+      <c r="T12" s="73"/>
+      <c r="U12" s="74"/>
+      <c r="V12" s="74"/>
+      <c r="W12" s="75"/>
       <c r="X12" s="15"/>
       <c r="Y12" s="16"/>
       <c r="Z12" s="16"/>
@@ -2493,26 +2497,26 @@
       <c r="AK12" s="16"/>
       <c r="AL12" s="16"/>
       <c r="AM12" s="17"/>
-      <c r="AN12" s="113"/>
-      <c r="AO12" s="105"/>
-      <c r="AP12" s="105"/>
-      <c r="AQ12" s="104"/>
+      <c r="AN12" s="73"/>
+      <c r="AO12" s="74"/>
+      <c r="AP12" s="74"/>
+      <c r="AQ12" s="75"/>
       <c r="AR12" s="15"/>
       <c r="AS12" s="16"/>
       <c r="AT12" s="16"/>
       <c r="AU12" s="17"/>
       <c r="AV12" s="15"/>
       <c r="AW12" s="16"/>
-      <c r="AX12" s="103"/>
-      <c r="AY12" s="104"/>
-      <c r="AZ12" s="98" t="s">
+      <c r="AX12" s="104"/>
+      <c r="AY12" s="75"/>
+      <c r="AZ12" s="88" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A13" s="93"/>
-      <c r="B13" s="95"/>
-      <c r="C13" s="97"/>
+      <c r="A13" s="91"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="93"/>
       <c r="D13" s="42"/>
       <c r="E13" s="41"/>
       <c r="F13" s="43"/>
@@ -2529,10 +2533,10 @@
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="12"/>
-      <c r="T13" s="113"/>
-      <c r="U13" s="105"/>
-      <c r="V13" s="105"/>
-      <c r="W13" s="104"/>
+      <c r="T13" s="73"/>
+      <c r="U13" s="74"/>
+      <c r="V13" s="74"/>
+      <c r="W13" s="75"/>
       <c r="X13" s="11"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
@@ -2549,28 +2553,30 @@
       <c r="AK13" s="32"/>
       <c r="AL13" s="32"/>
       <c r="AM13" s="31"/>
-      <c r="AN13" s="113"/>
-      <c r="AO13" s="105"/>
-      <c r="AP13" s="105"/>
-      <c r="AQ13" s="104"/>
+      <c r="AN13" s="73"/>
+      <c r="AO13" s="74"/>
+      <c r="AP13" s="74"/>
+      <c r="AQ13" s="75"/>
       <c r="AR13" s="33"/>
       <c r="AS13" s="32"/>
       <c r="AT13" s="32"/>
       <c r="AU13" s="31"/>
       <c r="AV13" s="33"/>
       <c r="AW13" s="32"/>
-      <c r="AX13" s="103"/>
-      <c r="AY13" s="104"/>
-      <c r="AZ13" s="99"/>
+      <c r="AX13" s="104"/>
+      <c r="AY13" s="75"/>
+      <c r="AZ13" s="89"/>
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A14" s="86" t="s">
+      <c r="A14" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="88">
+      <c r="B14" s="95">
         <v>1.5</v>
       </c>
-      <c r="C14" s="120"/>
+      <c r="C14" s="96">
+        <v>1</v>
+      </c>
       <c r="D14" s="28"/>
       <c r="E14" s="5"/>
       <c r="F14" s="30"/>
@@ -2587,10 +2593,10 @@
       <c r="Q14" s="30"/>
       <c r="R14" s="30"/>
       <c r="S14" s="29"/>
-      <c r="T14" s="113"/>
-      <c r="U14" s="105"/>
-      <c r="V14" s="105"/>
-      <c r="W14" s="104"/>
+      <c r="T14" s="73"/>
+      <c r="U14" s="74"/>
+      <c r="V14" s="74"/>
+      <c r="W14" s="75"/>
       <c r="X14" s="28"/>
       <c r="Y14" s="30"/>
       <c r="Z14" s="30"/>
@@ -2607,24 +2613,24 @@
       <c r="AK14" s="5"/>
       <c r="AL14" s="5"/>
       <c r="AM14" s="7"/>
-      <c r="AN14" s="113"/>
-      <c r="AO14" s="105"/>
-      <c r="AP14" s="105"/>
-      <c r="AQ14" s="104"/>
+      <c r="AN14" s="73"/>
+      <c r="AO14" s="74"/>
+      <c r="AP14" s="74"/>
+      <c r="AQ14" s="75"/>
       <c r="AR14" s="6"/>
       <c r="AS14" s="5"/>
       <c r="AT14" s="5"/>
       <c r="AU14" s="7"/>
       <c r="AV14" s="6"/>
       <c r="AW14" s="5"/>
-      <c r="AX14" s="103"/>
-      <c r="AY14" s="104"/>
-      <c r="AZ14" s="99"/>
+      <c r="AX14" s="104"/>
+      <c r="AY14" s="75"/>
+      <c r="AZ14" s="89"/>
     </row>
     <row r="15" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="87"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="91"/>
+      <c r="A15" s="80"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="84"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -2641,10 +2647,10 @@
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="113"/>
-      <c r="U15" s="105"/>
-      <c r="V15" s="105"/>
-      <c r="W15" s="104"/>
+      <c r="T15" s="73"/>
+      <c r="U15" s="74"/>
+      <c r="V15" s="74"/>
+      <c r="W15" s="75"/>
       <c r="X15" s="8"/>
       <c r="Y15" s="9"/>
       <c r="Z15" s="9"/>
@@ -2661,28 +2667,30 @@
       <c r="AK15" s="9"/>
       <c r="AL15" s="9"/>
       <c r="AM15" s="10"/>
-      <c r="AN15" s="113"/>
-      <c r="AO15" s="105"/>
-      <c r="AP15" s="105"/>
-      <c r="AQ15" s="104"/>
+      <c r="AN15" s="73"/>
+      <c r="AO15" s="74"/>
+      <c r="AP15" s="74"/>
+      <c r="AQ15" s="75"/>
       <c r="AR15" s="8"/>
       <c r="AS15" s="9"/>
       <c r="AT15" s="9"/>
       <c r="AU15" s="10"/>
       <c r="AV15" s="8"/>
       <c r="AW15" s="9"/>
-      <c r="AX15" s="103"/>
-      <c r="AY15" s="104"/>
-      <c r="AZ15" s="100"/>
+      <c r="AX15" s="104"/>
+      <c r="AY15" s="75"/>
+      <c r="AZ15" s="90"/>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A16" s="92" t="s">
+      <c r="A16" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="94">
+      <c r="B16" s="81">
         <v>1</v>
       </c>
-      <c r="C16" s="96"/>
+      <c r="C16" s="83">
+        <v>1.5</v>
+      </c>
       <c r="D16" s="15"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
@@ -2699,10 +2707,10 @@
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
       <c r="S16" s="17"/>
-      <c r="T16" s="113"/>
-      <c r="U16" s="105"/>
-      <c r="V16" s="105"/>
-      <c r="W16" s="104"/>
+      <c r="T16" s="73"/>
+      <c r="U16" s="74"/>
+      <c r="V16" s="74"/>
+      <c r="W16" s="75"/>
       <c r="X16" s="15"/>
       <c r="Y16" s="16"/>
       <c r="Z16" s="16"/>
@@ -2719,26 +2727,26 @@
       <c r="AK16" s="16"/>
       <c r="AL16" s="16"/>
       <c r="AM16" s="17"/>
-      <c r="AN16" s="113"/>
-      <c r="AO16" s="105"/>
-      <c r="AP16" s="105"/>
-      <c r="AQ16" s="104"/>
+      <c r="AN16" s="73"/>
+      <c r="AO16" s="74"/>
+      <c r="AP16" s="74"/>
+      <c r="AQ16" s="75"/>
       <c r="AR16" s="15"/>
       <c r="AS16" s="16"/>
       <c r="AT16" s="16"/>
       <c r="AU16" s="17"/>
       <c r="AV16" s="15"/>
       <c r="AW16" s="16"/>
-      <c r="AX16" s="103"/>
-      <c r="AY16" s="104"/>
-      <c r="AZ16" s="98" t="s">
+      <c r="AX16" s="104"/>
+      <c r="AY16" s="75"/>
+      <c r="AZ16" s="88" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A17" s="116"/>
-      <c r="B17" s="95"/>
-      <c r="C17" s="97"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="93"/>
       <c r="D17" s="11"/>
       <c r="E17" s="3"/>
       <c r="F17" s="32"/>
@@ -2755,10 +2763,10 @@
       <c r="Q17" s="3"/>
       <c r="R17" s="32"/>
       <c r="S17" s="12"/>
-      <c r="T17" s="113"/>
-      <c r="U17" s="105"/>
-      <c r="V17" s="105"/>
-      <c r="W17" s="104"/>
+      <c r="T17" s="73"/>
+      <c r="U17" s="74"/>
+      <c r="V17" s="74"/>
+      <c r="W17" s="75"/>
       <c r="X17" s="33"/>
       <c r="Y17" s="32"/>
       <c r="Z17" s="32"/>
@@ -2775,28 +2783,30 @@
       <c r="AK17" s="32"/>
       <c r="AL17" s="32"/>
       <c r="AM17" s="31"/>
-      <c r="AN17" s="113"/>
-      <c r="AO17" s="105"/>
-      <c r="AP17" s="105"/>
-      <c r="AQ17" s="104"/>
+      <c r="AN17" s="73"/>
+      <c r="AO17" s="74"/>
+      <c r="AP17" s="74"/>
+      <c r="AQ17" s="75"/>
       <c r="AR17" s="33"/>
       <c r="AS17" s="32"/>
       <c r="AT17" s="32"/>
       <c r="AU17" s="31"/>
       <c r="AV17" s="33"/>
       <c r="AW17" s="3"/>
-      <c r="AX17" s="103"/>
-      <c r="AY17" s="104"/>
-      <c r="AZ17" s="99"/>
+      <c r="AX17" s="104"/>
+      <c r="AY17" s="75"/>
+      <c r="AZ17" s="89"/>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A18" s="119" t="s">
+      <c r="A18" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="88">
+      <c r="B18" s="95">
         <v>2</v>
       </c>
-      <c r="C18" s="120"/>
+      <c r="C18" s="96">
+        <v>2</v>
+      </c>
       <c r="D18" s="28"/>
       <c r="E18" s="30"/>
       <c r="F18" s="5"/>
@@ -2813,10 +2823,10 @@
       <c r="Q18" s="30"/>
       <c r="R18" s="5"/>
       <c r="S18" s="29"/>
-      <c r="T18" s="113"/>
-      <c r="U18" s="105"/>
-      <c r="V18" s="105"/>
-      <c r="W18" s="104"/>
+      <c r="T18" s="73"/>
+      <c r="U18" s="74"/>
+      <c r="V18" s="74"/>
+      <c r="W18" s="75"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
@@ -2833,24 +2843,24 @@
       <c r="AK18" s="5"/>
       <c r="AL18" s="5"/>
       <c r="AM18" s="7"/>
-      <c r="AN18" s="113"/>
-      <c r="AO18" s="105"/>
-      <c r="AP18" s="105"/>
-      <c r="AQ18" s="104"/>
+      <c r="AN18" s="73"/>
+      <c r="AO18" s="74"/>
+      <c r="AP18" s="74"/>
+      <c r="AQ18" s="75"/>
       <c r="AR18" s="6"/>
       <c r="AS18" s="5"/>
       <c r="AT18" s="5"/>
       <c r="AU18" s="7"/>
       <c r="AV18" s="6"/>
       <c r="AW18" s="30"/>
-      <c r="AX18" s="103"/>
-      <c r="AY18" s="104"/>
-      <c r="AZ18" s="99"/>
+      <c r="AX18" s="104"/>
+      <c r="AY18" s="75"/>
+      <c r="AZ18" s="89"/>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A19" s="93"/>
-      <c r="B19" s="95"/>
-      <c r="C19" s="97"/>
+      <c r="A19" s="91"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="93"/>
       <c r="D19" s="11"/>
       <c r="E19" s="3"/>
       <c r="F19" s="32"/>
@@ -2867,10 +2877,10 @@
       <c r="Q19" s="32"/>
       <c r="R19" s="3"/>
       <c r="S19" s="31"/>
-      <c r="T19" s="113"/>
-      <c r="U19" s="105"/>
-      <c r="V19" s="105"/>
-      <c r="W19" s="104"/>
+      <c r="T19" s="73"/>
+      <c r="U19" s="74"/>
+      <c r="V19" s="74"/>
+      <c r="W19" s="75"/>
       <c r="X19" s="33"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
@@ -2887,28 +2897,30 @@
       <c r="AK19" s="32"/>
       <c r="AL19" s="32"/>
       <c r="AM19" s="31"/>
-      <c r="AN19" s="113"/>
-      <c r="AO19" s="105"/>
-      <c r="AP19" s="105"/>
-      <c r="AQ19" s="104"/>
+      <c r="AN19" s="73"/>
+      <c r="AO19" s="74"/>
+      <c r="AP19" s="74"/>
+      <c r="AQ19" s="75"/>
       <c r="AR19" s="33"/>
       <c r="AS19" s="3"/>
       <c r="AT19" s="32"/>
       <c r="AU19" s="31"/>
       <c r="AV19" s="33"/>
       <c r="AW19" s="32"/>
-      <c r="AX19" s="103"/>
-      <c r="AY19" s="104"/>
-      <c r="AZ19" s="99"/>
+      <c r="AX19" s="104"/>
+      <c r="AY19" s="75"/>
+      <c r="AZ19" s="89"/>
     </row>
     <row r="20" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A20" s="119" t="s">
+      <c r="A20" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="88">
+      <c r="B20" s="95">
         <v>0.5</v>
       </c>
-      <c r="C20" s="120"/>
+      <c r="C20" s="96">
+        <v>0.5</v>
+      </c>
       <c r="D20" s="28"/>
       <c r="E20" s="30"/>
       <c r="F20" s="5"/>
@@ -2925,10 +2937,10 @@
       <c r="Q20" s="5"/>
       <c r="R20" s="30"/>
       <c r="S20" s="7"/>
-      <c r="T20" s="113"/>
-      <c r="U20" s="105"/>
-      <c r="V20" s="105"/>
-      <c r="W20" s="104"/>
+      <c r="T20" s="73"/>
+      <c r="U20" s="74"/>
+      <c r="V20" s="74"/>
+      <c r="W20" s="75"/>
       <c r="X20" s="6"/>
       <c r="Y20" s="30"/>
       <c r="Z20" s="30"/>
@@ -2945,24 +2957,24 @@
       <c r="AK20" s="5"/>
       <c r="AL20" s="5"/>
       <c r="AM20" s="7"/>
-      <c r="AN20" s="113"/>
-      <c r="AO20" s="105"/>
-      <c r="AP20" s="105"/>
-      <c r="AQ20" s="104"/>
+      <c r="AN20" s="73"/>
+      <c r="AO20" s="74"/>
+      <c r="AP20" s="74"/>
+      <c r="AQ20" s="75"/>
       <c r="AR20" s="6"/>
       <c r="AS20" s="30"/>
       <c r="AT20" s="5"/>
       <c r="AU20" s="7"/>
       <c r="AV20" s="6"/>
       <c r="AW20" s="5"/>
-      <c r="AX20" s="103"/>
-      <c r="AY20" s="104"/>
-      <c r="AZ20" s="99"/>
+      <c r="AX20" s="104"/>
+      <c r="AY20" s="75"/>
+      <c r="AZ20" s="89"/>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A21" s="93"/>
-      <c r="B21" s="95"/>
-      <c r="C21" s="97"/>
+      <c r="A21" s="91"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="93"/>
       <c r="D21" s="33"/>
       <c r="E21" s="32"/>
       <c r="F21" s="32"/>
@@ -2979,10 +2991,10 @@
       <c r="Q21" s="32"/>
       <c r="R21" s="32"/>
       <c r="S21" s="31"/>
-      <c r="T21" s="113"/>
-      <c r="U21" s="105"/>
-      <c r="V21" s="105"/>
-      <c r="W21" s="104"/>
+      <c r="T21" s="73"/>
+      <c r="U21" s="74"/>
+      <c r="V21" s="74"/>
+      <c r="W21" s="75"/>
       <c r="X21" s="33"/>
       <c r="Y21" s="32"/>
       <c r="Z21" s="32"/>
@@ -2999,28 +3011,30 @@
       <c r="AK21" s="32"/>
       <c r="AL21" s="32"/>
       <c r="AM21" s="31"/>
-      <c r="AN21" s="113"/>
-      <c r="AO21" s="105"/>
-      <c r="AP21" s="105"/>
-      <c r="AQ21" s="104"/>
+      <c r="AN21" s="73"/>
+      <c r="AO21" s="74"/>
+      <c r="AP21" s="74"/>
+      <c r="AQ21" s="75"/>
       <c r="AR21" s="33"/>
       <c r="AS21" s="32"/>
       <c r="AT21" s="32"/>
       <c r="AU21" s="31"/>
       <c r="AV21" s="33"/>
       <c r="AW21" s="32"/>
-      <c r="AX21" s="103"/>
-      <c r="AY21" s="104"/>
-      <c r="AZ21" s="99"/>
+      <c r="AX21" s="104"/>
+      <c r="AY21" s="75"/>
+      <c r="AZ21" s="89"/>
     </row>
     <row r="22" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A22" s="119" t="s">
+      <c r="A22" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="88">
+      <c r="B22" s="95">
         <v>1</v>
       </c>
-      <c r="C22" s="120"/>
+      <c r="C22" s="96">
+        <v>1</v>
+      </c>
       <c r="D22" s="6"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -3037,10 +3051,10 @@
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
       <c r="S22" s="7"/>
-      <c r="T22" s="113"/>
-      <c r="U22" s="105"/>
-      <c r="V22" s="105"/>
-      <c r="W22" s="104"/>
+      <c r="T22" s="73"/>
+      <c r="U22" s="74"/>
+      <c r="V22" s="74"/>
+      <c r="W22" s="75"/>
       <c r="X22" s="6"/>
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
@@ -3057,24 +3071,24 @@
       <c r="AK22" s="5"/>
       <c r="AL22" s="5"/>
       <c r="AM22" s="7"/>
-      <c r="AN22" s="113"/>
-      <c r="AO22" s="105"/>
-      <c r="AP22" s="105"/>
-      <c r="AQ22" s="104"/>
+      <c r="AN22" s="73"/>
+      <c r="AO22" s="74"/>
+      <c r="AP22" s="74"/>
+      <c r="AQ22" s="75"/>
       <c r="AR22" s="6"/>
       <c r="AS22" s="5"/>
       <c r="AT22" s="5"/>
       <c r="AU22" s="7"/>
       <c r="AV22" s="6"/>
       <c r="AW22" s="5"/>
-      <c r="AX22" s="103"/>
-      <c r="AY22" s="104"/>
-      <c r="AZ22" s="99"/>
+      <c r="AX22" s="104"/>
+      <c r="AY22" s="75"/>
+      <c r="AZ22" s="89"/>
     </row>
     <row r="23" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A23" s="93"/>
-      <c r="B23" s="95"/>
-      <c r="C23" s="97"/>
+      <c r="A23" s="91"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="93"/>
       <c r="D23" s="11"/>
       <c r="E23" s="3"/>
       <c r="F23" s="32"/>
@@ -3091,10 +3105,10 @@
       <c r="Q23" s="32"/>
       <c r="R23" s="32"/>
       <c r="S23" s="31"/>
-      <c r="T23" s="113"/>
-      <c r="U23" s="105"/>
-      <c r="V23" s="105"/>
-      <c r="W23" s="104"/>
+      <c r="T23" s="73"/>
+      <c r="U23" s="74"/>
+      <c r="V23" s="74"/>
+      <c r="W23" s="75"/>
       <c r="X23" s="33"/>
       <c r="Y23" s="32"/>
       <c r="Z23" s="32"/>
@@ -3111,28 +3125,30 @@
       <c r="AK23" s="3"/>
       <c r="AL23" s="3"/>
       <c r="AM23" s="12"/>
-      <c r="AN23" s="113"/>
-      <c r="AO23" s="105"/>
-      <c r="AP23" s="105"/>
-      <c r="AQ23" s="104"/>
+      <c r="AN23" s="73"/>
+      <c r="AO23" s="74"/>
+      <c r="AP23" s="74"/>
+      <c r="AQ23" s="75"/>
       <c r="AR23" s="11"/>
       <c r="AS23" s="3"/>
       <c r="AT23" s="32"/>
       <c r="AU23" s="31"/>
       <c r="AV23" s="33"/>
       <c r="AW23" s="3"/>
-      <c r="AX23" s="103"/>
-      <c r="AY23" s="104"/>
-      <c r="AZ23" s="99"/>
+      <c r="AX23" s="104"/>
+      <c r="AY23" s="75"/>
+      <c r="AZ23" s="89"/>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A24" s="119" t="s">
+      <c r="A24" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="88">
+      <c r="B24" s="95">
         <v>1</v>
       </c>
-      <c r="C24" s="120"/>
+      <c r="C24" s="96">
+        <v>2</v>
+      </c>
       <c r="D24" s="28"/>
       <c r="E24" s="30"/>
       <c r="F24" s="5"/>
@@ -3149,10 +3165,10 @@
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
       <c r="S24" s="7"/>
-      <c r="T24" s="113"/>
-      <c r="U24" s="105"/>
-      <c r="V24" s="105"/>
-      <c r="W24" s="104"/>
+      <c r="T24" s="73"/>
+      <c r="U24" s="74"/>
+      <c r="V24" s="74"/>
+      <c r="W24" s="75"/>
       <c r="X24" s="6"/>
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
@@ -3169,24 +3185,24 @@
       <c r="AK24" s="30"/>
       <c r="AL24" s="30"/>
       <c r="AM24" s="29"/>
-      <c r="AN24" s="113"/>
-      <c r="AO24" s="105"/>
-      <c r="AP24" s="105"/>
-      <c r="AQ24" s="104"/>
+      <c r="AN24" s="73"/>
+      <c r="AO24" s="74"/>
+      <c r="AP24" s="74"/>
+      <c r="AQ24" s="75"/>
       <c r="AR24" s="28"/>
       <c r="AS24" s="30"/>
       <c r="AT24" s="5"/>
       <c r="AU24" s="7"/>
       <c r="AV24" s="6"/>
       <c r="AW24" s="30"/>
-      <c r="AX24" s="103"/>
-      <c r="AY24" s="104"/>
-      <c r="AZ24" s="99"/>
+      <c r="AX24" s="104"/>
+      <c r="AY24" s="75"/>
+      <c r="AZ24" s="89"/>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A25" s="93"/>
-      <c r="B25" s="117"/>
-      <c r="C25" s="118"/>
+      <c r="A25" s="91"/>
+      <c r="B25" s="100"/>
+      <c r="C25" s="101"/>
       <c r="D25" s="33"/>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
@@ -3203,10 +3219,10 @@
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="31"/>
-      <c r="T25" s="113"/>
-      <c r="U25" s="105"/>
-      <c r="V25" s="105"/>
-      <c r="W25" s="104"/>
+      <c r="T25" s="73"/>
+      <c r="U25" s="74"/>
+      <c r="V25" s="74"/>
+      <c r="W25" s="75"/>
       <c r="X25" s="33"/>
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
@@ -3223,28 +3239,30 @@
       <c r="AK25" s="3"/>
       <c r="AL25" s="3"/>
       <c r="AM25" s="12"/>
-      <c r="AN25" s="113"/>
-      <c r="AO25" s="105"/>
-      <c r="AP25" s="105"/>
-      <c r="AQ25" s="104"/>
+      <c r="AN25" s="73"/>
+      <c r="AO25" s="74"/>
+      <c r="AP25" s="74"/>
+      <c r="AQ25" s="75"/>
       <c r="AR25" s="11"/>
       <c r="AS25" s="3"/>
       <c r="AT25" s="3"/>
       <c r="AU25" s="12"/>
       <c r="AV25" s="11"/>
       <c r="AW25" s="3"/>
-      <c r="AX25" s="103"/>
-      <c r="AY25" s="104"/>
-      <c r="AZ25" s="99"/>
+      <c r="AX25" s="104"/>
+      <c r="AY25" s="75"/>
+      <c r="AZ25" s="89"/>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A26" s="86" t="s">
+      <c r="A26" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="121">
+      <c r="B26" s="98">
         <v>2</v>
       </c>
-      <c r="C26" s="90"/>
+      <c r="C26" s="102">
+        <v>2</v>
+      </c>
       <c r="D26" s="6"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -3261,10 +3279,10 @@
       <c r="Q26" s="30"/>
       <c r="R26" s="30"/>
       <c r="S26" s="7"/>
-      <c r="T26" s="113"/>
-      <c r="U26" s="105"/>
-      <c r="V26" s="105"/>
-      <c r="W26" s="104"/>
+      <c r="T26" s="73"/>
+      <c r="U26" s="74"/>
+      <c r="V26" s="74"/>
+      <c r="W26" s="75"/>
       <c r="X26" s="6"/>
       <c r="Y26" s="30"/>
       <c r="Z26" s="30"/>
@@ -3281,24 +3299,24 @@
       <c r="AK26" s="30"/>
       <c r="AL26" s="30"/>
       <c r="AM26" s="29"/>
-      <c r="AN26" s="113"/>
-      <c r="AO26" s="105"/>
-      <c r="AP26" s="105"/>
-      <c r="AQ26" s="104"/>
+      <c r="AN26" s="73"/>
+      <c r="AO26" s="74"/>
+      <c r="AP26" s="74"/>
+      <c r="AQ26" s="75"/>
       <c r="AR26" s="28"/>
       <c r="AS26" s="30"/>
       <c r="AT26" s="30"/>
       <c r="AU26" s="29"/>
       <c r="AV26" s="28"/>
       <c r="AW26" s="30"/>
-      <c r="AX26" s="103"/>
-      <c r="AY26" s="104"/>
-      <c r="AZ26" s="99"/>
+      <c r="AX26" s="104"/>
+      <c r="AY26" s="75"/>
+      <c r="AZ26" s="89"/>
     </row>
     <row r="27" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="87"/>
-      <c r="B27" s="89"/>
-      <c r="C27" s="91"/>
+      <c r="A27" s="80"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="84"/>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
@@ -3315,10 +3333,10 @@
       <c r="Q27" s="9"/>
       <c r="R27" s="9"/>
       <c r="S27" s="10"/>
-      <c r="T27" s="113"/>
-      <c r="U27" s="105"/>
-      <c r="V27" s="105"/>
-      <c r="W27" s="104"/>
+      <c r="T27" s="73"/>
+      <c r="U27" s="74"/>
+      <c r="V27" s="74"/>
+      <c r="W27" s="75"/>
       <c r="X27" s="8"/>
       <c r="Y27" s="9"/>
       <c r="Z27" s="9"/>
@@ -3335,28 +3353,30 @@
       <c r="AK27" s="9"/>
       <c r="AL27" s="9"/>
       <c r="AM27" s="10"/>
-      <c r="AN27" s="113"/>
-      <c r="AO27" s="105"/>
-      <c r="AP27" s="105"/>
-      <c r="AQ27" s="104"/>
+      <c r="AN27" s="73"/>
+      <c r="AO27" s="74"/>
+      <c r="AP27" s="74"/>
+      <c r="AQ27" s="75"/>
       <c r="AR27" s="8"/>
       <c r="AS27" s="9"/>
       <c r="AT27" s="9"/>
       <c r="AU27" s="10"/>
       <c r="AV27" s="8"/>
       <c r="AW27" s="9"/>
-      <c r="AX27" s="103"/>
-      <c r="AY27" s="104"/>
-      <c r="AZ27" s="100"/>
+      <c r="AX27" s="104"/>
+      <c r="AY27" s="75"/>
+      <c r="AZ27" s="90"/>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A28" s="92" t="s">
+      <c r="A28" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="94">
+      <c r="B28" s="81">
         <v>0.5</v>
       </c>
-      <c r="C28" s="96"/>
+      <c r="C28" s="83">
+        <v>0.5</v>
+      </c>
       <c r="D28" s="15"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
@@ -3373,10 +3393,10 @@
       <c r="Q28" s="16"/>
       <c r="R28" s="16"/>
       <c r="S28" s="17"/>
-      <c r="T28" s="113"/>
-      <c r="U28" s="105"/>
-      <c r="V28" s="105"/>
-      <c r="W28" s="104"/>
+      <c r="T28" s="73"/>
+      <c r="U28" s="74"/>
+      <c r="V28" s="74"/>
+      <c r="W28" s="75"/>
       <c r="X28" s="15"/>
       <c r="Y28" s="16"/>
       <c r="Z28" s="16"/>
@@ -3393,26 +3413,26 @@
       <c r="AK28" s="16"/>
       <c r="AL28" s="16"/>
       <c r="AM28" s="17"/>
-      <c r="AN28" s="113"/>
-      <c r="AO28" s="105"/>
-      <c r="AP28" s="105"/>
-      <c r="AQ28" s="104"/>
+      <c r="AN28" s="73"/>
+      <c r="AO28" s="74"/>
+      <c r="AP28" s="74"/>
+      <c r="AQ28" s="75"/>
       <c r="AR28" s="15"/>
       <c r="AS28" s="16"/>
       <c r="AT28" s="16"/>
       <c r="AU28" s="17"/>
       <c r="AV28" s="15"/>
       <c r="AW28" s="17"/>
-      <c r="AX28" s="105"/>
-      <c r="AY28" s="104"/>
-      <c r="AZ28" s="83" t="s">
+      <c r="AX28" s="74"/>
+      <c r="AY28" s="75"/>
+      <c r="AZ28" s="120" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="87"/>
-      <c r="B29" s="89"/>
-      <c r="C29" s="91"/>
+      <c r="A29" s="80"/>
+      <c r="B29" s="82"/>
+      <c r="C29" s="84"/>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
@@ -3429,10 +3449,10 @@
       <c r="Q29" s="9"/>
       <c r="R29" s="9"/>
       <c r="S29" s="10"/>
-      <c r="T29" s="113"/>
-      <c r="U29" s="105"/>
-      <c r="V29" s="105"/>
-      <c r="W29" s="104"/>
+      <c r="T29" s="73"/>
+      <c r="U29" s="74"/>
+      <c r="V29" s="74"/>
+      <c r="W29" s="75"/>
       <c r="X29" s="8"/>
       <c r="Y29" s="9"/>
       <c r="Z29" s="9"/>
@@ -3449,28 +3469,30 @@
       <c r="AK29" s="9"/>
       <c r="AL29" s="9"/>
       <c r="AM29" s="10"/>
-      <c r="AN29" s="113"/>
-      <c r="AO29" s="105"/>
-      <c r="AP29" s="105"/>
-      <c r="AQ29" s="104"/>
+      <c r="AN29" s="73"/>
+      <c r="AO29" s="74"/>
+      <c r="AP29" s="74"/>
+      <c r="AQ29" s="75"/>
       <c r="AR29" s="8"/>
       <c r="AS29" s="9"/>
       <c r="AT29" s="9"/>
       <c r="AU29" s="10"/>
       <c r="AV29" s="8"/>
       <c r="AW29" s="10"/>
-      <c r="AX29" s="105"/>
-      <c r="AY29" s="104"/>
-      <c r="AZ29" s="84"/>
+      <c r="AX29" s="74"/>
+      <c r="AY29" s="75"/>
+      <c r="AZ29" s="121"/>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A30" s="86" t="s">
+      <c r="A30" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="121">
+      <c r="B30" s="98">
         <v>0.5</v>
       </c>
-      <c r="C30" s="90"/>
+      <c r="C30" s="102">
+        <v>0.5</v>
+      </c>
       <c r="D30" s="6"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -3487,10 +3509,10 @@
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
       <c r="S30" s="7"/>
-      <c r="T30" s="113"/>
-      <c r="U30" s="105"/>
-      <c r="V30" s="105"/>
-      <c r="W30" s="104"/>
+      <c r="T30" s="73"/>
+      <c r="U30" s="74"/>
+      <c r="V30" s="74"/>
+      <c r="W30" s="75"/>
       <c r="X30" s="6"/>
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
@@ -3507,26 +3529,26 @@
       <c r="AK30" s="5"/>
       <c r="AL30" s="5"/>
       <c r="AM30" s="7"/>
-      <c r="AN30" s="113"/>
-      <c r="AO30" s="105"/>
-      <c r="AP30" s="105"/>
-      <c r="AQ30" s="104"/>
+      <c r="AN30" s="73"/>
+      <c r="AO30" s="74"/>
+      <c r="AP30" s="74"/>
+      <c r="AQ30" s="75"/>
       <c r="AR30" s="6"/>
       <c r="AS30" s="5"/>
       <c r="AT30" s="5"/>
       <c r="AU30" s="7"/>
       <c r="AV30" s="6"/>
       <c r="AW30" s="5"/>
-      <c r="AX30" s="103"/>
-      <c r="AY30" s="104"/>
-      <c r="AZ30" s="83" t="s">
+      <c r="AX30" s="104"/>
+      <c r="AY30" s="75"/>
+      <c r="AZ30" s="120" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A31" s="93"/>
-      <c r="B31" s="95"/>
-      <c r="C31" s="97"/>
+      <c r="A31" s="91"/>
+      <c r="B31" s="92"/>
+      <c r="C31" s="93"/>
       <c r="D31" s="11"/>
       <c r="E31" s="32"/>
       <c r="F31" s="3"/>
@@ -3543,10 +3565,10 @@
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
       <c r="S31" s="31"/>
-      <c r="T31" s="113"/>
-      <c r="U31" s="105"/>
-      <c r="V31" s="105"/>
-      <c r="W31" s="104"/>
+      <c r="T31" s="73"/>
+      <c r="U31" s="74"/>
+      <c r="V31" s="74"/>
+      <c r="W31" s="75"/>
       <c r="X31" s="33"/>
       <c r="Y31" s="32"/>
       <c r="Z31" s="32"/>
@@ -3563,28 +3585,30 @@
       <c r="AK31" s="32"/>
       <c r="AL31" s="32"/>
       <c r="AM31" s="31"/>
-      <c r="AN31" s="113"/>
-      <c r="AO31" s="105"/>
-      <c r="AP31" s="105"/>
-      <c r="AQ31" s="104"/>
+      <c r="AN31" s="73"/>
+      <c r="AO31" s="74"/>
+      <c r="AP31" s="74"/>
+      <c r="AQ31" s="75"/>
       <c r="AR31" s="33"/>
       <c r="AS31" s="32"/>
       <c r="AT31" s="32"/>
       <c r="AU31" s="31"/>
       <c r="AV31" s="33"/>
       <c r="AW31" s="32"/>
-      <c r="AX31" s="103"/>
-      <c r="AY31" s="104"/>
-      <c r="AZ31" s="85"/>
+      <c r="AX31" s="104"/>
+      <c r="AY31" s="75"/>
+      <c r="AZ31" s="122"/>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A32" s="119" t="s">
+      <c r="A32" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="88">
+      <c r="B32" s="95">
         <v>1</v>
       </c>
-      <c r="C32" s="120"/>
+      <c r="C32" s="96">
+        <v>1</v>
+      </c>
       <c r="D32" s="28"/>
       <c r="E32" s="5"/>
       <c r="F32" s="30"/>
@@ -3601,10 +3625,10 @@
       <c r="Q32" s="34"/>
       <c r="R32" s="30"/>
       <c r="S32" s="7"/>
-      <c r="T32" s="113"/>
-      <c r="U32" s="105"/>
-      <c r="V32" s="105"/>
-      <c r="W32" s="104"/>
+      <c r="T32" s="73"/>
+      <c r="U32" s="74"/>
+      <c r="V32" s="74"/>
+      <c r="W32" s="75"/>
       <c r="X32" s="6"/>
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
@@ -3621,24 +3645,24 @@
       <c r="AK32" s="5"/>
       <c r="AL32" s="5"/>
       <c r="AM32" s="7"/>
-      <c r="AN32" s="113"/>
-      <c r="AO32" s="105"/>
-      <c r="AP32" s="105"/>
-      <c r="AQ32" s="104"/>
+      <c r="AN32" s="73"/>
+      <c r="AO32" s="74"/>
+      <c r="AP32" s="74"/>
+      <c r="AQ32" s="75"/>
       <c r="AR32" s="6"/>
       <c r="AS32" s="5"/>
       <c r="AT32" s="5"/>
       <c r="AU32" s="7"/>
       <c r="AV32" s="6"/>
       <c r="AW32" s="5"/>
-      <c r="AX32" s="103"/>
-      <c r="AY32" s="104"/>
-      <c r="AZ32" s="85"/>
+      <c r="AX32" s="104"/>
+      <c r="AY32" s="75"/>
+      <c r="AZ32" s="122"/>
     </row>
     <row r="33" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A33" s="93"/>
-      <c r="B33" s="117"/>
-      <c r="C33" s="118"/>
+      <c r="A33" s="91"/>
+      <c r="B33" s="100"/>
+      <c r="C33" s="101"/>
       <c r="D33" s="33"/>
       <c r="E33" s="32"/>
       <c r="F33" s="3"/>
@@ -3655,10 +3679,10 @@
       <c r="Q33" s="54"/>
       <c r="R33" s="32"/>
       <c r="S33" s="31"/>
-      <c r="T33" s="113"/>
-      <c r="U33" s="105"/>
-      <c r="V33" s="105"/>
-      <c r="W33" s="104"/>
+      <c r="T33" s="73"/>
+      <c r="U33" s="74"/>
+      <c r="V33" s="74"/>
+      <c r="W33" s="75"/>
       <c r="X33" s="33"/>
       <c r="Y33" s="3"/>
       <c r="Z33" s="32"/>
@@ -3675,28 +3699,30 @@
       <c r="AK33" s="32"/>
       <c r="AL33" s="32"/>
       <c r="AM33" s="31"/>
-      <c r="AN33" s="113"/>
-      <c r="AO33" s="105"/>
-      <c r="AP33" s="105"/>
-      <c r="AQ33" s="104"/>
+      <c r="AN33" s="73"/>
+      <c r="AO33" s="74"/>
+      <c r="AP33" s="74"/>
+      <c r="AQ33" s="75"/>
       <c r="AR33" s="33"/>
       <c r="AS33" s="3"/>
       <c r="AT33" s="3"/>
       <c r="AU33" s="12"/>
       <c r="AV33" s="11"/>
       <c r="AW33" s="32"/>
-      <c r="AX33" s="103"/>
-      <c r="AY33" s="104"/>
-      <c r="AZ33" s="85"/>
+      <c r="AX33" s="104"/>
+      <c r="AY33" s="75"/>
+      <c r="AZ33" s="122"/>
     </row>
     <row r="34" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A34" s="119" t="s">
+      <c r="A34" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="88">
+      <c r="B34" s="95">
         <v>1</v>
       </c>
-      <c r="C34" s="90"/>
+      <c r="C34" s="102">
+        <v>1</v>
+      </c>
       <c r="D34" s="6"/>
       <c r="E34" s="5"/>
       <c r="F34" s="30"/>
@@ -3713,10 +3739,10 @@
       <c r="Q34" s="55"/>
       <c r="R34" s="24"/>
       <c r="S34" s="7"/>
-      <c r="T34" s="113"/>
-      <c r="U34" s="105"/>
-      <c r="V34" s="105"/>
-      <c r="W34" s="104"/>
+      <c r="T34" s="73"/>
+      <c r="U34" s="74"/>
+      <c r="V34" s="74"/>
+      <c r="W34" s="75"/>
       <c r="X34" s="6"/>
       <c r="Y34" s="30"/>
       <c r="Z34" s="5"/>
@@ -3733,24 +3759,24 @@
       <c r="AK34" s="5"/>
       <c r="AL34" s="5"/>
       <c r="AM34" s="7"/>
-      <c r="AN34" s="113"/>
-      <c r="AO34" s="105"/>
-      <c r="AP34" s="105"/>
-      <c r="AQ34" s="104"/>
+      <c r="AN34" s="73"/>
+      <c r="AO34" s="74"/>
+      <c r="AP34" s="74"/>
+      <c r="AQ34" s="75"/>
       <c r="AR34" s="6"/>
       <c r="AS34" s="30"/>
       <c r="AT34" s="30"/>
       <c r="AU34" s="29"/>
       <c r="AV34" s="28"/>
       <c r="AW34" s="5"/>
-      <c r="AX34" s="103"/>
-      <c r="AY34" s="104"/>
-      <c r="AZ34" s="85"/>
+      <c r="AX34" s="104"/>
+      <c r="AY34" s="75"/>
+      <c r="AZ34" s="122"/>
     </row>
     <row r="35" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A35" s="93"/>
-      <c r="B35" s="117"/>
-      <c r="C35" s="97"/>
+      <c r="A35" s="91"/>
+      <c r="B35" s="100"/>
+      <c r="C35" s="93"/>
       <c r="D35" s="33"/>
       <c r="E35" s="32"/>
       <c r="F35" s="32"/>
@@ -3767,10 +3793,10 @@
       <c r="Q35" s="54"/>
       <c r="R35" s="40"/>
       <c r="S35" s="12"/>
-      <c r="T35" s="113"/>
-      <c r="U35" s="105"/>
-      <c r="V35" s="105"/>
-      <c r="W35" s="104"/>
+      <c r="T35" s="73"/>
+      <c r="U35" s="74"/>
+      <c r="V35" s="74"/>
+      <c r="W35" s="75"/>
       <c r="X35" s="11"/>
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
@@ -3787,28 +3813,30 @@
       <c r="AK35" s="3"/>
       <c r="AL35" s="3"/>
       <c r="AM35" s="12"/>
-      <c r="AN35" s="113"/>
-      <c r="AO35" s="105"/>
-      <c r="AP35" s="105"/>
-      <c r="AQ35" s="104"/>
+      <c r="AN35" s="73"/>
+      <c r="AO35" s="74"/>
+      <c r="AP35" s="74"/>
+      <c r="AQ35" s="75"/>
       <c r="AR35" s="33"/>
       <c r="AS35" s="3"/>
       <c r="AT35" s="32"/>
       <c r="AU35" s="31"/>
       <c r="AV35" s="33"/>
       <c r="AW35" s="3"/>
-      <c r="AX35" s="103"/>
-      <c r="AY35" s="104"/>
-      <c r="AZ35" s="85"/>
+      <c r="AX35" s="104"/>
+      <c r="AY35" s="75"/>
+      <c r="AZ35" s="122"/>
     </row>
     <row r="36" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A36" s="119" t="s">
+      <c r="A36" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="88">
+      <c r="B36" s="95">
         <v>1</v>
       </c>
-      <c r="C36" s="120"/>
+      <c r="C36" s="96">
+        <v>1</v>
+      </c>
       <c r="D36" s="6"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -3825,10 +3853,10 @@
       <c r="Q36" s="5"/>
       <c r="R36" s="30"/>
       <c r="S36" s="49"/>
-      <c r="T36" s="113"/>
-      <c r="U36" s="105"/>
-      <c r="V36" s="105"/>
-      <c r="W36" s="104"/>
+      <c r="T36" s="73"/>
+      <c r="U36" s="74"/>
+      <c r="V36" s="74"/>
+      <c r="W36" s="75"/>
       <c r="X36" s="28"/>
       <c r="Y36" s="30"/>
       <c r="Z36" s="30"/>
@@ -3845,24 +3873,24 @@
       <c r="AK36" s="30"/>
       <c r="AL36" s="30"/>
       <c r="AM36" s="29"/>
-      <c r="AN36" s="113"/>
-      <c r="AO36" s="105"/>
-      <c r="AP36" s="105"/>
-      <c r="AQ36" s="104"/>
+      <c r="AN36" s="73"/>
+      <c r="AO36" s="74"/>
+      <c r="AP36" s="74"/>
+      <c r="AQ36" s="75"/>
       <c r="AR36" s="6"/>
       <c r="AS36" s="30"/>
       <c r="AT36" s="5"/>
       <c r="AU36" s="7"/>
       <c r="AV36" s="6"/>
       <c r="AW36" s="30"/>
-      <c r="AX36" s="103"/>
-      <c r="AY36" s="104"/>
-      <c r="AZ36" s="85"/>
+      <c r="AX36" s="104"/>
+      <c r="AY36" s="75"/>
+      <c r="AZ36" s="122"/>
     </row>
     <row r="37" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A37" s="93"/>
-      <c r="B37" s="117"/>
-      <c r="C37" s="118"/>
+      <c r="A37" s="91"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="101"/>
       <c r="D37" s="33"/>
       <c r="E37" s="32"/>
       <c r="F37" s="3"/>
@@ -3879,10 +3907,10 @@
       <c r="Q37" s="32"/>
       <c r="R37" s="3"/>
       <c r="S37" s="66"/>
-      <c r="T37" s="113"/>
-      <c r="U37" s="105"/>
-      <c r="V37" s="105"/>
-      <c r="W37" s="104"/>
+      <c r="T37" s="73"/>
+      <c r="U37" s="74"/>
+      <c r="V37" s="74"/>
+      <c r="W37" s="75"/>
       <c r="X37" s="33"/>
       <c r="Y37" s="32"/>
       <c r="Z37" s="32"/>
@@ -3899,28 +3927,30 @@
       <c r="AK37" s="32"/>
       <c r="AL37" s="32"/>
       <c r="AM37" s="12"/>
-      <c r="AN37" s="113"/>
-      <c r="AO37" s="105"/>
-      <c r="AP37" s="105"/>
-      <c r="AQ37" s="104"/>
+      <c r="AN37" s="73"/>
+      <c r="AO37" s="74"/>
+      <c r="AP37" s="74"/>
+      <c r="AQ37" s="75"/>
       <c r="AR37" s="11"/>
       <c r="AS37" s="3"/>
       <c r="AT37" s="32"/>
       <c r="AU37" s="12"/>
       <c r="AV37" s="11"/>
       <c r="AW37" s="3"/>
-      <c r="AX37" s="103"/>
-      <c r="AY37" s="104"/>
-      <c r="AZ37" s="85"/>
+      <c r="AX37" s="104"/>
+      <c r="AY37" s="75"/>
+      <c r="AZ37" s="122"/>
     </row>
     <row r="38" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A38" s="86" t="s">
+      <c r="A38" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="88">
+      <c r="B38" s="95">
         <v>1</v>
       </c>
-      <c r="C38" s="120"/>
+      <c r="C38" s="96">
+        <v>1</v>
+      </c>
       <c r="D38" s="6"/>
       <c r="E38" s="5"/>
       <c r="F38" s="30"/>
@@ -3937,10 +3967,10 @@
       <c r="Q38" s="5"/>
       <c r="R38" s="30"/>
       <c r="S38" s="25"/>
-      <c r="T38" s="113"/>
-      <c r="U38" s="105"/>
-      <c r="V38" s="105"/>
-      <c r="W38" s="104"/>
+      <c r="T38" s="73"/>
+      <c r="U38" s="74"/>
+      <c r="V38" s="74"/>
+      <c r="W38" s="75"/>
       <c r="X38" s="6"/>
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
@@ -3957,24 +3987,24 @@
       <c r="AK38" s="5"/>
       <c r="AL38" s="5"/>
       <c r="AM38" s="29"/>
-      <c r="AN38" s="113"/>
-      <c r="AO38" s="105"/>
-      <c r="AP38" s="105"/>
-      <c r="AQ38" s="104"/>
+      <c r="AN38" s="73"/>
+      <c r="AO38" s="74"/>
+      <c r="AP38" s="74"/>
+      <c r="AQ38" s="75"/>
       <c r="AR38" s="28"/>
       <c r="AS38" s="30"/>
       <c r="AT38" s="5"/>
       <c r="AU38" s="29"/>
       <c r="AV38" s="28"/>
       <c r="AW38" s="30"/>
-      <c r="AX38" s="103"/>
-      <c r="AY38" s="104"/>
-      <c r="AZ38" s="85"/>
+      <c r="AX38" s="104"/>
+      <c r="AY38" s="75"/>
+      <c r="AZ38" s="122"/>
     </row>
     <row r="39" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A39" s="116"/>
-      <c r="B39" s="117"/>
-      <c r="C39" s="118"/>
+      <c r="A39" s="99"/>
+      <c r="B39" s="100"/>
+      <c r="C39" s="101"/>
       <c r="D39" s="11"/>
       <c r="E39" s="3"/>
       <c r="F39" s="32"/>
@@ -3991,10 +4021,10 @@
       <c r="Q39" s="32"/>
       <c r="R39" s="3"/>
       <c r="S39" s="12"/>
-      <c r="T39" s="113"/>
-      <c r="U39" s="105"/>
-      <c r="V39" s="105"/>
-      <c r="W39" s="104"/>
+      <c r="T39" s="73"/>
+      <c r="U39" s="74"/>
+      <c r="V39" s="74"/>
+      <c r="W39" s="75"/>
       <c r="X39" s="39"/>
       <c r="Y39" s="54"/>
       <c r="Z39" s="32"/>
@@ -4011,28 +4041,30 @@
       <c r="AK39" s="32"/>
       <c r="AL39" s="32"/>
       <c r="AM39" s="31"/>
-      <c r="AN39" s="113"/>
-      <c r="AO39" s="105"/>
-      <c r="AP39" s="105"/>
-      <c r="AQ39" s="104"/>
+      <c r="AN39" s="73"/>
+      <c r="AO39" s="74"/>
+      <c r="AP39" s="74"/>
+      <c r="AQ39" s="75"/>
       <c r="AR39" s="33"/>
       <c r="AS39" s="32"/>
       <c r="AT39" s="3"/>
       <c r="AU39" s="31"/>
       <c r="AV39" s="11"/>
       <c r="AW39" s="3"/>
-      <c r="AX39" s="103"/>
-      <c r="AY39" s="104"/>
-      <c r="AZ39" s="85"/>
+      <c r="AX39" s="104"/>
+      <c r="AY39" s="75"/>
+      <c r="AZ39" s="122"/>
     </row>
     <row r="40" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A40" s="119" t="s">
+      <c r="A40" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="88">
+      <c r="B40" s="95">
         <v>1</v>
       </c>
-      <c r="C40" s="120"/>
+      <c r="C40" s="96">
+        <v>0.5</v>
+      </c>
       <c r="D40" s="28"/>
       <c r="E40" s="30"/>
       <c r="F40" s="5"/>
@@ -4049,10 +4081,10 @@
       <c r="Q40" s="5"/>
       <c r="R40" s="30"/>
       <c r="S40" s="29"/>
-      <c r="T40" s="113"/>
-      <c r="U40" s="105"/>
-      <c r="V40" s="105"/>
-      <c r="W40" s="104"/>
+      <c r="T40" s="73"/>
+      <c r="U40" s="74"/>
+      <c r="V40" s="74"/>
+      <c r="W40" s="75"/>
       <c r="X40" s="38"/>
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
@@ -4069,24 +4101,24 @@
       <c r="AK40" s="5"/>
       <c r="AL40" s="5"/>
       <c r="AM40" s="7"/>
-      <c r="AN40" s="113"/>
-      <c r="AO40" s="105"/>
-      <c r="AP40" s="105"/>
-      <c r="AQ40" s="104"/>
+      <c r="AN40" s="73"/>
+      <c r="AO40" s="74"/>
+      <c r="AP40" s="74"/>
+      <c r="AQ40" s="75"/>
       <c r="AR40" s="6"/>
       <c r="AS40" s="5"/>
       <c r="AT40" s="30"/>
       <c r="AU40" s="7"/>
       <c r="AV40" s="28"/>
       <c r="AW40" s="30"/>
-      <c r="AX40" s="103"/>
-      <c r="AY40" s="104"/>
-      <c r="AZ40" s="85"/>
+      <c r="AX40" s="104"/>
+      <c r="AY40" s="75"/>
+      <c r="AZ40" s="122"/>
     </row>
     <row r="41" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A41" s="116"/>
-      <c r="B41" s="117"/>
-      <c r="C41" s="118"/>
+      <c r="A41" s="99"/>
+      <c r="B41" s="100"/>
+      <c r="C41" s="101"/>
       <c r="D41" s="33"/>
       <c r="E41" s="32"/>
       <c r="F41" s="32"/>
@@ -4103,10 +4135,10 @@
       <c r="Q41" s="32"/>
       <c r="R41" s="3"/>
       <c r="S41" s="12"/>
-      <c r="T41" s="113"/>
-      <c r="U41" s="105"/>
-      <c r="V41" s="105"/>
-      <c r="W41" s="104"/>
+      <c r="T41" s="73"/>
+      <c r="U41" s="74"/>
+      <c r="V41" s="74"/>
+      <c r="W41" s="75"/>
       <c r="X41" s="39"/>
       <c r="Y41" s="40"/>
       <c r="Z41" s="3"/>
@@ -4123,28 +4155,30 @@
       <c r="AK41" s="3"/>
       <c r="AL41" s="32"/>
       <c r="AM41" s="12"/>
-      <c r="AN41" s="113"/>
-      <c r="AO41" s="105"/>
-      <c r="AP41" s="105"/>
-      <c r="AQ41" s="104"/>
+      <c r="AN41" s="73"/>
+      <c r="AO41" s="74"/>
+      <c r="AP41" s="74"/>
+      <c r="AQ41" s="75"/>
       <c r="AR41" s="11"/>
       <c r="AS41" s="3"/>
       <c r="AT41" s="3"/>
       <c r="AU41" s="12"/>
       <c r="AV41" s="11"/>
       <c r="AW41" s="32"/>
-      <c r="AX41" s="103"/>
-      <c r="AY41" s="104"/>
-      <c r="AZ41" s="85"/>
+      <c r="AX41" s="104"/>
+      <c r="AY41" s="75"/>
+      <c r="AZ41" s="122"/>
     </row>
     <row r="42" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A42" s="119" t="s">
+      <c r="A42" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="88">
+      <c r="B42" s="95">
         <v>2</v>
       </c>
-      <c r="C42" s="120"/>
+      <c r="C42" s="96">
+        <v>1</v>
+      </c>
       <c r="D42" s="6"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -4161,10 +4195,10 @@
       <c r="Q42" s="5"/>
       <c r="R42" s="30"/>
       <c r="S42" s="29"/>
-      <c r="T42" s="113"/>
-      <c r="U42" s="105"/>
-      <c r="V42" s="105"/>
-      <c r="W42" s="104"/>
+      <c r="T42" s="73"/>
+      <c r="U42" s="74"/>
+      <c r="V42" s="74"/>
+      <c r="W42" s="75"/>
       <c r="X42" s="28"/>
       <c r="Y42" s="34"/>
       <c r="Z42" s="34"/>
@@ -4181,24 +4215,24 @@
       <c r="AK42" s="30"/>
       <c r="AL42" s="5"/>
       <c r="AM42" s="29"/>
-      <c r="AN42" s="113"/>
-      <c r="AO42" s="105"/>
-      <c r="AP42" s="105"/>
-      <c r="AQ42" s="104"/>
+      <c r="AN42" s="73"/>
+      <c r="AO42" s="74"/>
+      <c r="AP42" s="74"/>
+      <c r="AQ42" s="75"/>
       <c r="AR42" s="28"/>
       <c r="AS42" s="30"/>
       <c r="AT42" s="30"/>
       <c r="AU42" s="29"/>
       <c r="AV42" s="28"/>
       <c r="AW42" s="5"/>
-      <c r="AX42" s="103"/>
-      <c r="AY42" s="104"/>
-      <c r="AZ42" s="85"/>
+      <c r="AX42" s="104"/>
+      <c r="AY42" s="75"/>
+      <c r="AZ42" s="122"/>
     </row>
     <row r="43" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A43" s="93"/>
-      <c r="B43" s="117"/>
-      <c r="C43" s="118"/>
+      <c r="A43" s="91"/>
+      <c r="B43" s="100"/>
+      <c r="C43" s="101"/>
       <c r="D43" s="11"/>
       <c r="E43" s="32"/>
       <c r="F43" s="3"/>
@@ -4215,10 +4249,10 @@
       <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
       <c r="S43" s="66"/>
-      <c r="T43" s="113"/>
-      <c r="U43" s="105"/>
-      <c r="V43" s="105"/>
-      <c r="W43" s="104"/>
+      <c r="T43" s="73"/>
+      <c r="U43" s="74"/>
+      <c r="V43" s="74"/>
+      <c r="W43" s="75"/>
       <c r="X43" s="11"/>
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
@@ -4235,28 +4269,30 @@
       <c r="AK43" s="32"/>
       <c r="AL43" s="3"/>
       <c r="AM43" s="12"/>
-      <c r="AN43" s="113"/>
-      <c r="AO43" s="105"/>
-      <c r="AP43" s="105"/>
-      <c r="AQ43" s="104"/>
+      <c r="AN43" s="73"/>
+      <c r="AO43" s="74"/>
+      <c r="AP43" s="74"/>
+      <c r="AQ43" s="75"/>
       <c r="AR43" s="11"/>
       <c r="AS43" s="3"/>
       <c r="AT43" s="3"/>
       <c r="AU43" s="12"/>
       <c r="AV43" s="11"/>
       <c r="AW43" s="3"/>
-      <c r="AX43" s="103"/>
-      <c r="AY43" s="104"/>
-      <c r="AZ43" s="85"/>
+      <c r="AX43" s="104"/>
+      <c r="AY43" s="75"/>
+      <c r="AZ43" s="122"/>
     </row>
     <row r="44" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A44" s="119" t="s">
+      <c r="A44" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="121">
+      <c r="B44" s="98">
         <v>2.5</v>
       </c>
-      <c r="C44" s="120"/>
+      <c r="C44" s="96">
+        <v>3</v>
+      </c>
       <c r="D44" s="28"/>
       <c r="E44" s="5"/>
       <c r="F44" s="30"/>
@@ -4273,10 +4309,10 @@
       <c r="Q44" s="30"/>
       <c r="R44" s="30"/>
       <c r="S44" s="7"/>
-      <c r="T44" s="113"/>
-      <c r="U44" s="105"/>
-      <c r="V44" s="105"/>
-      <c r="W44" s="104"/>
+      <c r="T44" s="73"/>
+      <c r="U44" s="74"/>
+      <c r="V44" s="74"/>
+      <c r="W44" s="75"/>
       <c r="X44" s="28"/>
       <c r="Y44" s="30"/>
       <c r="Z44" s="34"/>
@@ -4293,24 +4329,24 @@
       <c r="AK44" s="5"/>
       <c r="AL44" s="30"/>
       <c r="AM44" s="29"/>
-      <c r="AN44" s="113"/>
-      <c r="AO44" s="105"/>
-      <c r="AP44" s="105"/>
-      <c r="AQ44" s="104"/>
+      <c r="AN44" s="73"/>
+      <c r="AO44" s="74"/>
+      <c r="AP44" s="74"/>
+      <c r="AQ44" s="75"/>
       <c r="AR44" s="28"/>
       <c r="AS44" s="30"/>
       <c r="AT44" s="30"/>
       <c r="AU44" s="29"/>
       <c r="AV44" s="28"/>
       <c r="AW44" s="30"/>
-      <c r="AX44" s="103"/>
-      <c r="AY44" s="104"/>
-      <c r="AZ44" s="85"/>
+      <c r="AX44" s="104"/>
+      <c r="AY44" s="75"/>
+      <c r="AZ44" s="122"/>
     </row>
     <row r="45" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A45" s="93"/>
-      <c r="B45" s="95"/>
-      <c r="C45" s="118"/>
+      <c r="A45" s="91"/>
+      <c r="B45" s="92"/>
+      <c r="C45" s="101"/>
       <c r="D45" s="11"/>
       <c r="E45" s="3"/>
       <c r="F45" s="32"/>
@@ -4327,10 +4363,10 @@
       <c r="Q45" s="3"/>
       <c r="R45" s="3"/>
       <c r="S45" s="65"/>
-      <c r="T45" s="113"/>
-      <c r="U45" s="105"/>
-      <c r="V45" s="105"/>
-      <c r="W45" s="104"/>
+      <c r="T45" s="73"/>
+      <c r="U45" s="74"/>
+      <c r="V45" s="74"/>
+      <c r="W45" s="75"/>
       <c r="X45" s="11"/>
       <c r="Y45" s="32"/>
       <c r="Z45" s="3"/>
@@ -4347,28 +4383,30 @@
       <c r="AK45" s="3"/>
       <c r="AL45" s="3"/>
       <c r="AM45" s="12"/>
-      <c r="AN45" s="113"/>
-      <c r="AO45" s="105"/>
-      <c r="AP45" s="105"/>
-      <c r="AQ45" s="104"/>
+      <c r="AN45" s="73"/>
+      <c r="AO45" s="74"/>
+      <c r="AP45" s="74"/>
+      <c r="AQ45" s="75"/>
       <c r="AR45" s="11"/>
       <c r="AS45" s="3"/>
       <c r="AT45" s="3"/>
       <c r="AU45" s="12"/>
       <c r="AV45" s="11"/>
       <c r="AW45" s="3"/>
-      <c r="AX45" s="103"/>
-      <c r="AY45" s="104"/>
-      <c r="AZ45" s="85"/>
+      <c r="AX45" s="104"/>
+      <c r="AY45" s="75"/>
+      <c r="AZ45" s="122"/>
     </row>
     <row r="46" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A46" s="86" t="s">
+      <c r="A46" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="88">
+      <c r="B46" s="95">
         <v>2</v>
       </c>
-      <c r="C46" s="90"/>
+      <c r="C46" s="102">
+        <v>2</v>
+      </c>
       <c r="D46" s="28"/>
       <c r="E46" s="30"/>
       <c r="F46" s="5"/>
@@ -4385,10 +4423,10 @@
       <c r="Q46" s="30"/>
       <c r="R46" s="30"/>
       <c r="S46" s="29"/>
-      <c r="T46" s="113"/>
-      <c r="U46" s="105"/>
-      <c r="V46" s="105"/>
-      <c r="W46" s="104"/>
+      <c r="T46" s="73"/>
+      <c r="U46" s="74"/>
+      <c r="V46" s="74"/>
+      <c r="W46" s="75"/>
       <c r="X46" s="28"/>
       <c r="Y46" s="5"/>
       <c r="Z46" s="30"/>
@@ -4405,24 +4443,24 @@
       <c r="AK46" s="30"/>
       <c r="AL46" s="30"/>
       <c r="AM46" s="29"/>
-      <c r="AN46" s="113"/>
-      <c r="AO46" s="105"/>
-      <c r="AP46" s="105"/>
-      <c r="AQ46" s="104"/>
+      <c r="AN46" s="73"/>
+      <c r="AO46" s="74"/>
+      <c r="AP46" s="74"/>
+      <c r="AQ46" s="75"/>
       <c r="AR46" s="28"/>
       <c r="AS46" s="30"/>
       <c r="AT46" s="30"/>
       <c r="AU46" s="29"/>
       <c r="AV46" s="28"/>
       <c r="AW46" s="30"/>
-      <c r="AX46" s="103"/>
-      <c r="AY46" s="104"/>
-      <c r="AZ46" s="85"/>
+      <c r="AX46" s="104"/>
+      <c r="AY46" s="75"/>
+      <c r="AZ46" s="122"/>
     </row>
     <row r="47" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A47" s="116"/>
-      <c r="B47" s="117"/>
-      <c r="C47" s="97"/>
+      <c r="A47" s="99"/>
+      <c r="B47" s="100"/>
+      <c r="C47" s="93"/>
       <c r="D47" s="11"/>
       <c r="E47" s="32"/>
       <c r="F47" s="3"/>
@@ -4439,10 +4477,10 @@
       <c r="Q47" s="3"/>
       <c r="R47" s="32"/>
       <c r="S47" s="12"/>
-      <c r="T47" s="113"/>
-      <c r="U47" s="105"/>
-      <c r="V47" s="105"/>
-      <c r="W47" s="104"/>
+      <c r="T47" s="73"/>
+      <c r="U47" s="74"/>
+      <c r="V47" s="74"/>
+      <c r="W47" s="75"/>
       <c r="X47" s="11"/>
       <c r="Y47" s="3"/>
       <c r="Z47" s="3"/>
@@ -4459,28 +4497,30 @@
       <c r="AK47" s="32"/>
       <c r="AL47" s="3"/>
       <c r="AM47" s="31"/>
-      <c r="AN47" s="113"/>
-      <c r="AO47" s="105"/>
-      <c r="AP47" s="105"/>
-      <c r="AQ47" s="104"/>
+      <c r="AN47" s="73"/>
+      <c r="AO47" s="74"/>
+      <c r="AP47" s="74"/>
+      <c r="AQ47" s="75"/>
       <c r="AR47" s="33"/>
       <c r="AS47" s="32"/>
       <c r="AT47" s="32"/>
       <c r="AU47" s="31"/>
       <c r="AV47" s="33"/>
       <c r="AW47" s="32"/>
-      <c r="AX47" s="103"/>
-      <c r="AY47" s="104"/>
-      <c r="AZ47" s="85"/>
+      <c r="AX47" s="104"/>
+      <c r="AY47" s="75"/>
+      <c r="AZ47" s="122"/>
     </row>
     <row r="48" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A48" s="119" t="s">
+      <c r="A48" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="121">
+      <c r="B48" s="98">
         <v>0.5</v>
       </c>
-      <c r="C48" s="120"/>
+      <c r="C48" s="96">
+        <v>0.5</v>
+      </c>
       <c r="D48" s="28"/>
       <c r="E48" s="5"/>
       <c r="F48" s="30"/>
@@ -4497,10 +4537,10 @@
       <c r="Q48" s="30"/>
       <c r="R48" s="5"/>
       <c r="S48" s="29"/>
-      <c r="T48" s="113"/>
-      <c r="U48" s="105"/>
-      <c r="V48" s="105"/>
-      <c r="W48" s="104"/>
+      <c r="T48" s="73"/>
+      <c r="U48" s="74"/>
+      <c r="V48" s="74"/>
+      <c r="W48" s="75"/>
       <c r="X48" s="28"/>
       <c r="Y48" s="30"/>
       <c r="Z48" s="30"/>
@@ -4517,24 +4557,24 @@
       <c r="AK48" s="5"/>
       <c r="AL48" s="30"/>
       <c r="AM48" s="7"/>
-      <c r="AN48" s="113"/>
-      <c r="AO48" s="105"/>
-      <c r="AP48" s="105"/>
-      <c r="AQ48" s="104"/>
+      <c r="AN48" s="73"/>
+      <c r="AO48" s="74"/>
+      <c r="AP48" s="74"/>
+      <c r="AQ48" s="75"/>
       <c r="AR48" s="6"/>
       <c r="AS48" s="5"/>
       <c r="AT48" s="5"/>
       <c r="AU48" s="7"/>
       <c r="AV48" s="6"/>
       <c r="AW48" s="5"/>
-      <c r="AX48" s="103"/>
-      <c r="AY48" s="104"/>
-      <c r="AZ48" s="85"/>
+      <c r="AX48" s="104"/>
+      <c r="AY48" s="75"/>
+      <c r="AZ48" s="122"/>
     </row>
     <row r="49" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A49" s="116"/>
-      <c r="B49" s="95"/>
-      <c r="C49" s="118"/>
+      <c r="A49" s="99"/>
+      <c r="B49" s="92"/>
+      <c r="C49" s="101"/>
       <c r="D49" s="33"/>
       <c r="E49" s="32"/>
       <c r="F49" s="32"/>
@@ -4551,10 +4591,10 @@
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
       <c r="S49" s="12"/>
-      <c r="T49" s="113"/>
-      <c r="U49" s="105"/>
-      <c r="V49" s="105"/>
-      <c r="W49" s="104"/>
+      <c r="T49" s="73"/>
+      <c r="U49" s="74"/>
+      <c r="V49" s="74"/>
+      <c r="W49" s="75"/>
       <c r="X49" s="11"/>
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
@@ -4571,28 +4611,30 @@
       <c r="AK49" s="3"/>
       <c r="AL49" s="3"/>
       <c r="AM49" s="12"/>
-      <c r="AN49" s="113"/>
-      <c r="AO49" s="105"/>
-      <c r="AP49" s="105"/>
-      <c r="AQ49" s="104"/>
+      <c r="AN49" s="73"/>
+      <c r="AO49" s="74"/>
+      <c r="AP49" s="74"/>
+      <c r="AQ49" s="75"/>
       <c r="AR49" s="33"/>
       <c r="AS49" s="3"/>
       <c r="AT49" s="32"/>
       <c r="AU49" s="31"/>
       <c r="AV49" s="11"/>
       <c r="AW49" s="3"/>
-      <c r="AX49" s="103"/>
-      <c r="AY49" s="104"/>
-      <c r="AZ49" s="85"/>
+      <c r="AX49" s="104"/>
+      <c r="AY49" s="75"/>
+      <c r="AZ49" s="122"/>
     </row>
     <row r="50" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A50" s="119" t="s">
+      <c r="A50" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="B50" s="88">
+      <c r="B50" s="95">
         <v>2.5</v>
       </c>
-      <c r="C50" s="120"/>
+      <c r="C50" s="96">
+        <v>2</v>
+      </c>
       <c r="D50" s="6"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -4609,10 +4651,10 @@
       <c r="Q50" s="30"/>
       <c r="R50" s="30"/>
       <c r="S50" s="29"/>
-      <c r="T50" s="113"/>
-      <c r="U50" s="105"/>
-      <c r="V50" s="105"/>
-      <c r="W50" s="104"/>
+      <c r="T50" s="73"/>
+      <c r="U50" s="74"/>
+      <c r="V50" s="74"/>
+      <c r="W50" s="75"/>
       <c r="X50" s="28"/>
       <c r="Y50" s="30"/>
       <c r="Z50" s="30"/>
@@ -4629,24 +4671,24 @@
       <c r="AK50" s="30"/>
       <c r="AL50" s="30"/>
       <c r="AM50" s="29"/>
-      <c r="AN50" s="113"/>
-      <c r="AO50" s="105"/>
-      <c r="AP50" s="105"/>
-      <c r="AQ50" s="104"/>
+      <c r="AN50" s="73"/>
+      <c r="AO50" s="74"/>
+      <c r="AP50" s="74"/>
+      <c r="AQ50" s="75"/>
       <c r="AR50" s="6"/>
       <c r="AS50" s="30"/>
       <c r="AT50" s="5"/>
       <c r="AU50" s="7"/>
       <c r="AV50" s="28"/>
       <c r="AW50" s="30"/>
-      <c r="AX50" s="103"/>
-      <c r="AY50" s="104"/>
-      <c r="AZ50" s="85"/>
+      <c r="AX50" s="104"/>
+      <c r="AY50" s="75"/>
+      <c r="AZ50" s="122"/>
     </row>
     <row r="51" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A51" s="93"/>
-      <c r="B51" s="117"/>
-      <c r="C51" s="118"/>
+      <c r="A51" s="91"/>
+      <c r="B51" s="100"/>
+      <c r="C51" s="101"/>
       <c r="D51" s="11"/>
       <c r="E51" s="32"/>
       <c r="F51" s="3"/>
@@ -4663,10 +4705,10 @@
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
       <c r="S51" s="12"/>
-      <c r="T51" s="113"/>
-      <c r="U51" s="105"/>
-      <c r="V51" s="105"/>
-      <c r="W51" s="104"/>
+      <c r="T51" s="73"/>
+      <c r="U51" s="74"/>
+      <c r="V51" s="74"/>
+      <c r="W51" s="75"/>
       <c r="X51" s="33"/>
       <c r="Y51" s="32"/>
       <c r="Z51" s="3"/>
@@ -4683,28 +4725,30 @@
       <c r="AK51" s="32"/>
       <c r="AL51" s="3"/>
       <c r="AM51" s="12"/>
-      <c r="AN51" s="113"/>
-      <c r="AO51" s="105"/>
-      <c r="AP51" s="105"/>
-      <c r="AQ51" s="104"/>
+      <c r="AN51" s="73"/>
+      <c r="AO51" s="74"/>
+      <c r="AP51" s="74"/>
+      <c r="AQ51" s="75"/>
       <c r="AR51" s="11"/>
       <c r="AS51" s="3"/>
       <c r="AT51" s="3"/>
       <c r="AU51" s="12"/>
       <c r="AV51" s="11"/>
       <c r="AW51" s="3"/>
-      <c r="AX51" s="103"/>
-      <c r="AY51" s="104"/>
-      <c r="AZ51" s="85"/>
+      <c r="AX51" s="104"/>
+      <c r="AY51" s="75"/>
+      <c r="AZ51" s="122"/>
     </row>
     <row r="52" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A52" s="86" t="s">
+      <c r="A52" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="88">
+      <c r="B52" s="95">
         <v>1.5</v>
       </c>
-      <c r="C52" s="120"/>
+      <c r="C52" s="96">
+        <v>2</v>
+      </c>
       <c r="D52" s="28"/>
       <c r="E52" s="5"/>
       <c r="F52" s="30"/>
@@ -4721,10 +4765,10 @@
       <c r="Q52" s="30"/>
       <c r="R52" s="30"/>
       <c r="S52" s="29"/>
-      <c r="T52" s="113"/>
-      <c r="U52" s="105"/>
-      <c r="V52" s="105"/>
-      <c r="W52" s="104"/>
+      <c r="T52" s="73"/>
+      <c r="U52" s="74"/>
+      <c r="V52" s="74"/>
+      <c r="W52" s="75"/>
       <c r="X52" s="6"/>
       <c r="Y52" s="5"/>
       <c r="Z52" s="30"/>
@@ -4741,24 +4785,24 @@
       <c r="AK52" s="5"/>
       <c r="AL52" s="30"/>
       <c r="AM52" s="29"/>
-      <c r="AN52" s="113"/>
-      <c r="AO52" s="105"/>
-      <c r="AP52" s="105"/>
-      <c r="AQ52" s="104"/>
+      <c r="AN52" s="73"/>
+      <c r="AO52" s="74"/>
+      <c r="AP52" s="74"/>
+      <c r="AQ52" s="75"/>
       <c r="AR52" s="28"/>
       <c r="AS52" s="30"/>
       <c r="AT52" s="30"/>
       <c r="AU52" s="29"/>
       <c r="AV52" s="28"/>
       <c r="AW52" s="30"/>
-      <c r="AX52" s="103"/>
-      <c r="AY52" s="104"/>
-      <c r="AZ52" s="85"/>
+      <c r="AX52" s="104"/>
+      <c r="AY52" s="75"/>
+      <c r="AZ52" s="122"/>
     </row>
     <row r="53" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A53" s="116"/>
-      <c r="B53" s="117"/>
-      <c r="C53" s="118"/>
+      <c r="A53" s="99"/>
+      <c r="B53" s="100"/>
+      <c r="C53" s="101"/>
       <c r="D53" s="33"/>
       <c r="E53" s="32"/>
       <c r="F53" s="32"/>
@@ -4775,10 +4819,10 @@
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
       <c r="S53" s="12"/>
-      <c r="T53" s="113"/>
-      <c r="U53" s="105"/>
-      <c r="V53" s="105"/>
-      <c r="W53" s="104"/>
+      <c r="T53" s="73"/>
+      <c r="U53" s="74"/>
+      <c r="V53" s="74"/>
+      <c r="W53" s="75"/>
       <c r="X53" s="11"/>
       <c r="Y53" s="32"/>
       <c r="Z53" s="3"/>
@@ -4795,28 +4839,30 @@
       <c r="AK53" s="3"/>
       <c r="AL53" s="3"/>
       <c r="AM53" s="12"/>
-      <c r="AN53" s="113"/>
-      <c r="AO53" s="105"/>
-      <c r="AP53" s="105"/>
-      <c r="AQ53" s="104"/>
+      <c r="AN53" s="73"/>
+      <c r="AO53" s="74"/>
+      <c r="AP53" s="74"/>
+      <c r="AQ53" s="75"/>
       <c r="AR53" s="11"/>
       <c r="AS53" s="3"/>
       <c r="AT53" s="3"/>
       <c r="AU53" s="12"/>
       <c r="AV53" s="11"/>
       <c r="AW53" s="3"/>
-      <c r="AX53" s="103"/>
-      <c r="AY53" s="104"/>
-      <c r="AZ53" s="85"/>
+      <c r="AX53" s="104"/>
+      <c r="AY53" s="75"/>
+      <c r="AZ53" s="122"/>
     </row>
     <row r="54" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A54" s="119" t="s">
+      <c r="A54" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="88">
+      <c r="B54" s="95">
         <v>1.5</v>
       </c>
-      <c r="C54" s="90"/>
+      <c r="C54" s="102">
+        <v>1.5</v>
+      </c>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
@@ -4833,10 +4879,10 @@
       <c r="Q54" s="30"/>
       <c r="R54" s="30"/>
       <c r="S54" s="29"/>
-      <c r="T54" s="113"/>
-      <c r="U54" s="105"/>
-      <c r="V54" s="105"/>
-      <c r="W54" s="104"/>
+      <c r="T54" s="73"/>
+      <c r="U54" s="74"/>
+      <c r="V54" s="74"/>
+      <c r="W54" s="75"/>
       <c r="X54" s="28"/>
       <c r="Y54" s="5"/>
       <c r="Z54" s="30"/>
@@ -4853,24 +4899,24 @@
       <c r="AK54" s="30"/>
       <c r="AL54" s="30"/>
       <c r="AM54" s="29"/>
-      <c r="AN54" s="113"/>
-      <c r="AO54" s="105"/>
-      <c r="AP54" s="105"/>
-      <c r="AQ54" s="104"/>
+      <c r="AN54" s="73"/>
+      <c r="AO54" s="74"/>
+      <c r="AP54" s="74"/>
+      <c r="AQ54" s="75"/>
       <c r="AR54" s="28"/>
       <c r="AS54" s="30"/>
       <c r="AT54" s="30"/>
       <c r="AU54" s="29"/>
       <c r="AV54" s="28"/>
       <c r="AW54" s="30"/>
-      <c r="AX54" s="103"/>
-      <c r="AY54" s="104"/>
-      <c r="AZ54" s="85"/>
+      <c r="AX54" s="104"/>
+      <c r="AY54" s="75"/>
+      <c r="AZ54" s="122"/>
     </row>
     <row r="55" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A55" s="93"/>
-      <c r="B55" s="117"/>
-      <c r="C55" s="97"/>
+      <c r="A55" s="91"/>
+      <c r="B55" s="100"/>
+      <c r="C55" s="93"/>
       <c r="D55" s="11"/>
       <c r="E55" s="32"/>
       <c r="F55" s="3"/>
@@ -4887,10 +4933,10 @@
       <c r="Q55" s="32"/>
       <c r="R55" s="3"/>
       <c r="S55" s="31"/>
-      <c r="T55" s="113"/>
-      <c r="U55" s="105"/>
-      <c r="V55" s="105"/>
-      <c r="W55" s="104"/>
+      <c r="T55" s="73"/>
+      <c r="U55" s="74"/>
+      <c r="V55" s="74"/>
+      <c r="W55" s="75"/>
       <c r="X55" s="11"/>
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
@@ -4907,28 +4953,30 @@
       <c r="AK55" s="32"/>
       <c r="AL55" s="32"/>
       <c r="AM55" s="31"/>
-      <c r="AN55" s="113"/>
-      <c r="AO55" s="105"/>
-      <c r="AP55" s="105"/>
-      <c r="AQ55" s="104"/>
+      <c r="AN55" s="73"/>
+      <c r="AO55" s="74"/>
+      <c r="AP55" s="74"/>
+      <c r="AQ55" s="75"/>
       <c r="AR55" s="33"/>
       <c r="AS55" s="32"/>
       <c r="AT55" s="32"/>
       <c r="AU55" s="12"/>
       <c r="AV55" s="11"/>
       <c r="AW55" s="3"/>
-      <c r="AX55" s="103"/>
-      <c r="AY55" s="104"/>
-      <c r="AZ55" s="85"/>
+      <c r="AX55" s="104"/>
+      <c r="AY55" s="75"/>
+      <c r="AZ55" s="122"/>
     </row>
     <row r="56" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A56" s="119" t="s">
+      <c r="A56" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="121">
+      <c r="B56" s="98">
         <v>2</v>
       </c>
-      <c r="C56" s="120"/>
+      <c r="C56" s="96">
+        <v>2</v>
+      </c>
       <c r="D56" s="28"/>
       <c r="E56" s="5"/>
       <c r="F56" s="30"/>
@@ -4945,10 +4993,10 @@
       <c r="Q56" s="5"/>
       <c r="R56" s="30"/>
       <c r="S56" s="7"/>
-      <c r="T56" s="113"/>
-      <c r="U56" s="105"/>
-      <c r="V56" s="105"/>
-      <c r="W56" s="104"/>
+      <c r="T56" s="73"/>
+      <c r="U56" s="74"/>
+      <c r="V56" s="74"/>
+      <c r="W56" s="75"/>
       <c r="X56" s="28"/>
       <c r="Y56" s="30"/>
       <c r="Z56" s="30"/>
@@ -4965,24 +5013,24 @@
       <c r="AK56" s="24"/>
       <c r="AL56" s="5"/>
       <c r="AM56" s="7"/>
-      <c r="AN56" s="113"/>
-      <c r="AO56" s="105"/>
-      <c r="AP56" s="105"/>
-      <c r="AQ56" s="104"/>
+      <c r="AN56" s="73"/>
+      <c r="AO56" s="74"/>
+      <c r="AP56" s="74"/>
+      <c r="AQ56" s="75"/>
       <c r="AR56" s="6"/>
       <c r="AS56" s="5"/>
       <c r="AT56" s="5"/>
       <c r="AU56" s="29"/>
       <c r="AV56" s="28"/>
       <c r="AW56" s="30"/>
-      <c r="AX56" s="103"/>
-      <c r="AY56" s="104"/>
-      <c r="AZ56" s="85"/>
+      <c r="AX56" s="104"/>
+      <c r="AY56" s="75"/>
+      <c r="AZ56" s="122"/>
     </row>
     <row r="57" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A57" s="93"/>
-      <c r="B57" s="95"/>
-      <c r="C57" s="97"/>
+      <c r="A57" s="91"/>
+      <c r="B57" s="92"/>
+      <c r="C57" s="93"/>
       <c r="D57" s="11"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -4999,10 +5047,10 @@
       <c r="Q57" s="3"/>
       <c r="R57" s="3"/>
       <c r="S57" s="12"/>
-      <c r="T57" s="113"/>
-      <c r="U57" s="105"/>
-      <c r="V57" s="105"/>
-      <c r="W57" s="104"/>
+      <c r="T57" s="73"/>
+      <c r="U57" s="74"/>
+      <c r="V57" s="74"/>
+      <c r="W57" s="75"/>
       <c r="X57" s="33"/>
       <c r="Y57" s="3"/>
       <c r="Z57" s="32"/>
@@ -5015,32 +5063,32 @@
       <c r="AG57" s="3"/>
       <c r="AH57" s="3"/>
       <c r="AI57" s="12"/>
-      <c r="AJ57" s="11"/>
-      <c r="AK57" s="32"/>
+      <c r="AJ57" s="39"/>
+      <c r="AK57" s="54"/>
       <c r="AL57" s="3"/>
       <c r="AM57" s="12"/>
-      <c r="AN57" s="113"/>
-      <c r="AO57" s="105"/>
-      <c r="AP57" s="105"/>
-      <c r="AQ57" s="104"/>
+      <c r="AN57" s="73"/>
+      <c r="AO57" s="74"/>
+      <c r="AP57" s="74"/>
+      <c r="AQ57" s="75"/>
       <c r="AR57" s="11"/>
       <c r="AS57" s="3"/>
       <c r="AT57" s="3"/>
       <c r="AU57" s="31"/>
       <c r="AV57" s="33"/>
       <c r="AW57" s="3"/>
-      <c r="AX57" s="103"/>
-      <c r="AY57" s="104"/>
-      <c r="AZ57" s="85"/>
+      <c r="AX57" s="104"/>
+      <c r="AY57" s="75"/>
+      <c r="AZ57" s="122"/>
     </row>
     <row r="58" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A58" s="86" t="s">
+      <c r="A58" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="88">
+      <c r="B58" s="95">
         <v>2</v>
       </c>
-      <c r="C58" s="120"/>
+      <c r="C58" s="96"/>
       <c r="D58" s="28"/>
       <c r="E58" s="30"/>
       <c r="F58" s="30"/>
@@ -5057,10 +5105,10 @@
       <c r="Q58" s="30"/>
       <c r="R58" s="30"/>
       <c r="S58" s="29"/>
-      <c r="T58" s="113"/>
-      <c r="U58" s="105"/>
-      <c r="V58" s="105"/>
-      <c r="W58" s="104"/>
+      <c r="T58" s="73"/>
+      <c r="U58" s="74"/>
+      <c r="V58" s="74"/>
+      <c r="W58" s="75"/>
       <c r="X58" s="6"/>
       <c r="Y58" s="30"/>
       <c r="Z58" s="5"/>
@@ -5077,24 +5125,24 @@
       <c r="AK58" s="5"/>
       <c r="AL58" s="34"/>
       <c r="AM58" s="59"/>
-      <c r="AN58" s="113"/>
-      <c r="AO58" s="105"/>
-      <c r="AP58" s="105"/>
-      <c r="AQ58" s="104"/>
+      <c r="AN58" s="73"/>
+      <c r="AO58" s="74"/>
+      <c r="AP58" s="74"/>
+      <c r="AQ58" s="75"/>
       <c r="AR58" s="28"/>
       <c r="AS58" s="30"/>
       <c r="AT58" s="30"/>
       <c r="AU58" s="7"/>
       <c r="AV58" s="6"/>
       <c r="AW58" s="30"/>
-      <c r="AX58" s="103"/>
-      <c r="AY58" s="104"/>
-      <c r="AZ58" s="85"/>
+      <c r="AX58" s="104"/>
+      <c r="AY58" s="75"/>
+      <c r="AZ58" s="122"/>
     </row>
     <row r="59" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="87"/>
-      <c r="B59" s="89"/>
-      <c r="C59" s="91"/>
+      <c r="A59" s="80"/>
+      <c r="B59" s="82"/>
+      <c r="C59" s="84"/>
       <c r="D59" s="8"/>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
@@ -5111,10 +5159,10 @@
       <c r="Q59" s="9"/>
       <c r="R59" s="9"/>
       <c r="S59" s="10"/>
-      <c r="T59" s="113"/>
-      <c r="U59" s="105"/>
-      <c r="V59" s="105"/>
-      <c r="W59" s="104"/>
+      <c r="T59" s="73"/>
+      <c r="U59" s="74"/>
+      <c r="V59" s="74"/>
+      <c r="W59" s="75"/>
       <c r="X59" s="8"/>
       <c r="Y59" s="9"/>
       <c r="Z59" s="9"/>
@@ -5131,28 +5179,28 @@
       <c r="AK59" s="9"/>
       <c r="AL59" s="9"/>
       <c r="AM59" s="10"/>
-      <c r="AN59" s="113"/>
-      <c r="AO59" s="105"/>
-      <c r="AP59" s="105"/>
-      <c r="AQ59" s="104"/>
+      <c r="AN59" s="73"/>
+      <c r="AO59" s="74"/>
+      <c r="AP59" s="74"/>
+      <c r="AQ59" s="75"/>
       <c r="AR59" s="8"/>
       <c r="AS59" s="9"/>
       <c r="AT59" s="9"/>
       <c r="AU59" s="10"/>
       <c r="AV59" s="8"/>
       <c r="AW59" s="9"/>
-      <c r="AX59" s="103"/>
-      <c r="AY59" s="104"/>
-      <c r="AZ59" s="84"/>
+      <c r="AX59" s="104"/>
+      <c r="AY59" s="75"/>
+      <c r="AZ59" s="121"/>
     </row>
     <row r="60" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A60" s="92" t="s">
+      <c r="A60" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="B60" s="94">
+      <c r="B60" s="81">
         <v>0.5</v>
       </c>
-      <c r="C60" s="96"/>
+      <c r="C60" s="83"/>
       <c r="D60" s="15"/>
       <c r="E60" s="16"/>
       <c r="F60" s="16"/>
@@ -5169,10 +5217,10 @@
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
       <c r="S60" s="17"/>
-      <c r="T60" s="113"/>
-      <c r="U60" s="105"/>
-      <c r="V60" s="105"/>
-      <c r="W60" s="104"/>
+      <c r="T60" s="73"/>
+      <c r="U60" s="74"/>
+      <c r="V60" s="74"/>
+      <c r="W60" s="75"/>
       <c r="X60" s="15"/>
       <c r="Y60" s="16"/>
       <c r="Z60" s="16"/>
@@ -5189,26 +5237,26 @@
       <c r="AK60" s="16"/>
       <c r="AL60" s="16"/>
       <c r="AM60" s="17"/>
-      <c r="AN60" s="113"/>
-      <c r="AO60" s="105"/>
-      <c r="AP60" s="105"/>
-      <c r="AQ60" s="104"/>
+      <c r="AN60" s="73"/>
+      <c r="AO60" s="74"/>
+      <c r="AP60" s="74"/>
+      <c r="AQ60" s="75"/>
       <c r="AR60" s="23"/>
       <c r="AS60" s="16"/>
       <c r="AT60" s="16"/>
       <c r="AU60" s="17"/>
       <c r="AV60" s="15"/>
       <c r="AW60" s="16"/>
-      <c r="AX60" s="103"/>
-      <c r="AY60" s="104"/>
-      <c r="AZ60" s="98" t="s">
+      <c r="AX60" s="104"/>
+      <c r="AY60" s="75"/>
+      <c r="AZ60" s="88" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A61" s="93"/>
-      <c r="B61" s="95"/>
-      <c r="C61" s="97"/>
+      <c r="A61" s="91"/>
+      <c r="B61" s="92"/>
+      <c r="C61" s="93"/>
       <c r="D61" s="11"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -5225,10 +5273,10 @@
       <c r="Q61" s="3"/>
       <c r="R61" s="3"/>
       <c r="S61" s="12"/>
-      <c r="T61" s="113"/>
-      <c r="U61" s="105"/>
-      <c r="V61" s="105"/>
-      <c r="W61" s="104"/>
+      <c r="T61" s="73"/>
+      <c r="U61" s="74"/>
+      <c r="V61" s="74"/>
+      <c r="W61" s="75"/>
       <c r="X61" s="11"/>
       <c r="Y61" s="3"/>
       <c r="Z61" s="3"/>
@@ -5245,28 +5293,28 @@
       <c r="AK61" s="32"/>
       <c r="AL61" s="3"/>
       <c r="AM61" s="12"/>
-      <c r="AN61" s="113"/>
-      <c r="AO61" s="105"/>
-      <c r="AP61" s="105"/>
-      <c r="AQ61" s="104"/>
+      <c r="AN61" s="73"/>
+      <c r="AO61" s="74"/>
+      <c r="AP61" s="74"/>
+      <c r="AQ61" s="75"/>
       <c r="AR61" s="11"/>
       <c r="AS61" s="3"/>
       <c r="AT61" s="3"/>
       <c r="AU61" s="12"/>
       <c r="AV61" s="33"/>
       <c r="AW61" s="3"/>
-      <c r="AX61" s="103"/>
-      <c r="AY61" s="104"/>
-      <c r="AZ61" s="99"/>
+      <c r="AX61" s="104"/>
+      <c r="AY61" s="75"/>
+      <c r="AZ61" s="89"/>
     </row>
     <row r="62" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A62" s="86" t="s">
+      <c r="A62" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="B62" s="88">
+      <c r="B62" s="95">
         <v>2</v>
       </c>
-      <c r="C62" s="120"/>
+      <c r="C62" s="96"/>
       <c r="D62" s="28"/>
       <c r="E62" s="30"/>
       <c r="F62" s="30"/>
@@ -5283,10 +5331,10 @@
       <c r="Q62" s="30"/>
       <c r="R62" s="30"/>
       <c r="S62" s="29"/>
-      <c r="T62" s="113"/>
-      <c r="U62" s="105"/>
-      <c r="V62" s="105"/>
-      <c r="W62" s="104"/>
+      <c r="T62" s="73"/>
+      <c r="U62" s="74"/>
+      <c r="V62" s="74"/>
+      <c r="W62" s="75"/>
       <c r="X62" s="28"/>
       <c r="Y62" s="30"/>
       <c r="Z62" s="30"/>
@@ -5303,24 +5351,24 @@
       <c r="AK62" s="5"/>
       <c r="AL62" s="30"/>
       <c r="AM62" s="29"/>
-      <c r="AN62" s="113"/>
-      <c r="AO62" s="105"/>
-      <c r="AP62" s="105"/>
-      <c r="AQ62" s="104"/>
+      <c r="AN62" s="73"/>
+      <c r="AO62" s="74"/>
+      <c r="AP62" s="74"/>
+      <c r="AQ62" s="75"/>
       <c r="AR62" s="38"/>
       <c r="AS62" s="34"/>
       <c r="AT62" s="30"/>
       <c r="AU62" s="29"/>
       <c r="AV62" s="6"/>
       <c r="AW62" s="30"/>
-      <c r="AX62" s="103"/>
-      <c r="AY62" s="104"/>
-      <c r="AZ62" s="99"/>
+      <c r="AX62" s="104"/>
+      <c r="AY62" s="75"/>
+      <c r="AZ62" s="89"/>
     </row>
     <row r="63" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="87"/>
-      <c r="B63" s="89"/>
-      <c r="C63" s="91"/>
+      <c r="A63" s="80"/>
+      <c r="B63" s="82"/>
+      <c r="C63" s="84"/>
       <c r="D63" s="8"/>
       <c r="E63" s="9"/>
       <c r="F63" s="9"/>
@@ -5337,10 +5385,10 @@
       <c r="Q63" s="9"/>
       <c r="R63" s="9"/>
       <c r="S63" s="10"/>
-      <c r="T63" s="113"/>
-      <c r="U63" s="105"/>
-      <c r="V63" s="105"/>
-      <c r="W63" s="104"/>
+      <c r="T63" s="73"/>
+      <c r="U63" s="74"/>
+      <c r="V63" s="74"/>
+      <c r="W63" s="75"/>
       <c r="X63" s="8"/>
       <c r="Y63" s="9"/>
       <c r="Z63" s="9"/>
@@ -5357,28 +5405,28 @@
       <c r="AK63" s="9"/>
       <c r="AL63" s="9"/>
       <c r="AM63" s="10"/>
-      <c r="AN63" s="113"/>
-      <c r="AO63" s="105"/>
-      <c r="AP63" s="105"/>
-      <c r="AQ63" s="104"/>
+      <c r="AN63" s="73"/>
+      <c r="AO63" s="74"/>
+      <c r="AP63" s="74"/>
+      <c r="AQ63" s="75"/>
       <c r="AR63" s="8"/>
       <c r="AS63" s="9"/>
       <c r="AT63" s="9"/>
       <c r="AU63" s="10"/>
       <c r="AV63" s="8"/>
       <c r="AW63" s="9"/>
-      <c r="AX63" s="103"/>
-      <c r="AY63" s="104"/>
-      <c r="AZ63" s="100"/>
+      <c r="AX63" s="104"/>
+      <c r="AY63" s="75"/>
+      <c r="AZ63" s="90"/>
     </row>
     <row r="64" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A64" s="92" t="s">
+      <c r="A64" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="B64" s="94">
+      <c r="B64" s="81">
         <v>2.5</v>
       </c>
-      <c r="C64" s="96"/>
+      <c r="C64" s="83"/>
       <c r="D64" s="15"/>
       <c r="E64" s="16"/>
       <c r="F64" s="16"/>
@@ -5395,10 +5443,10 @@
       <c r="Q64" s="16"/>
       <c r="R64" s="16"/>
       <c r="S64" s="17"/>
-      <c r="T64" s="113"/>
-      <c r="U64" s="105"/>
-      <c r="V64" s="105"/>
-      <c r="W64" s="104"/>
+      <c r="T64" s="73"/>
+      <c r="U64" s="74"/>
+      <c r="V64" s="74"/>
+      <c r="W64" s="75"/>
       <c r="X64" s="15"/>
       <c r="Y64" s="16"/>
       <c r="Z64" s="16"/>
@@ -5415,26 +5463,26 @@
       <c r="AK64" s="16"/>
       <c r="AL64" s="16"/>
       <c r="AM64" s="17"/>
-      <c r="AN64" s="113"/>
-      <c r="AO64" s="105"/>
-      <c r="AP64" s="105"/>
-      <c r="AQ64" s="104"/>
+      <c r="AN64" s="73"/>
+      <c r="AO64" s="74"/>
+      <c r="AP64" s="74"/>
+      <c r="AQ64" s="75"/>
       <c r="AR64" s="15"/>
       <c r="AS64" s="16"/>
       <c r="AT64" s="27"/>
       <c r="AU64" s="58"/>
       <c r="AV64" s="15"/>
       <c r="AW64" s="16"/>
-      <c r="AX64" s="103"/>
-      <c r="AY64" s="104"/>
-      <c r="AZ64" s="98" t="s">
+      <c r="AX64" s="104"/>
+      <c r="AY64" s="75"/>
+      <c r="AZ64" s="88" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="87"/>
-      <c r="B65" s="89"/>
-      <c r="C65" s="91"/>
+      <c r="A65" s="80"/>
+      <c r="B65" s="82"/>
+      <c r="C65" s="84"/>
       <c r="D65" s="8"/>
       <c r="E65" s="9"/>
       <c r="F65" s="9"/>
@@ -5451,10 +5499,10 @@
       <c r="Q65" s="9"/>
       <c r="R65" s="9"/>
       <c r="S65" s="10"/>
-      <c r="T65" s="114"/>
-      <c r="U65" s="115"/>
-      <c r="V65" s="115"/>
-      <c r="W65" s="107"/>
+      <c r="T65" s="76"/>
+      <c r="U65" s="77"/>
+      <c r="V65" s="77"/>
+      <c r="W65" s="78"/>
       <c r="X65" s="8"/>
       <c r="Y65" s="9"/>
       <c r="Z65" s="9"/>
@@ -5471,19 +5519,19 @@
       <c r="AK65" s="9"/>
       <c r="AL65" s="9"/>
       <c r="AM65" s="10"/>
-      <c r="AN65" s="114"/>
-      <c r="AO65" s="115"/>
-      <c r="AP65" s="115"/>
-      <c r="AQ65" s="107"/>
+      <c r="AN65" s="76"/>
+      <c r="AO65" s="77"/>
+      <c r="AP65" s="77"/>
+      <c r="AQ65" s="78"/>
       <c r="AR65" s="8"/>
       <c r="AS65" s="9"/>
       <c r="AT65" s="9"/>
       <c r="AU65" s="10"/>
       <c r="AV65" s="8"/>
       <c r="AW65" s="9"/>
-      <c r="AX65" s="106"/>
-      <c r="AY65" s="107"/>
-      <c r="AZ65" s="100"/>
+      <c r="AX65" s="105"/>
+      <c r="AY65" s="78"/>
+      <c r="AZ65" s="90"/>
     </row>
     <row r="66" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="14" t="s">
@@ -5495,7 +5543,7 @@
       </c>
       <c r="C66" s="56">
         <f>SUM(C5:C65)</f>
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -5549,6 +5597,112 @@
     </row>
   </sheetData>
   <mergeCells count="130">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="AZ28:AZ29"/>
+    <mergeCell ref="AZ30:AZ59"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="X1:AA1"/>
+    <mergeCell ref="X2:AA2"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="AZ60:AZ63"/>
+    <mergeCell ref="AZ64:AZ65"/>
+    <mergeCell ref="AX4:AY65"/>
+    <mergeCell ref="AR1:AU1"/>
+    <mergeCell ref="AR2:AU2"/>
+    <mergeCell ref="AV1:AY1"/>
+    <mergeCell ref="AV2:AY2"/>
+    <mergeCell ref="AZ1:AZ3"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AF2:AI2"/>
+    <mergeCell ref="AJ1:AM1"/>
+    <mergeCell ref="AJ2:AM2"/>
+    <mergeCell ref="AN1:AQ1"/>
+    <mergeCell ref="AN2:AQ2"/>
+    <mergeCell ref="AN4:AQ65"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C46:C47"/>
     <mergeCell ref="T4:W65"/>
     <mergeCell ref="A64:A65"/>
     <mergeCell ref="B64:B65"/>
@@ -5573,112 +5727,6 @@
     <mergeCell ref="C52:C53"/>
     <mergeCell ref="A54:A55"/>
     <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="AZ60:AZ63"/>
-    <mergeCell ref="AZ64:AZ65"/>
-    <mergeCell ref="AX4:AY65"/>
-    <mergeCell ref="AR1:AU1"/>
-    <mergeCell ref="AR2:AU2"/>
-    <mergeCell ref="AV1:AY1"/>
-    <mergeCell ref="AV2:AY2"/>
-    <mergeCell ref="AZ1:AZ3"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AF2:AI2"/>
-    <mergeCell ref="AJ1:AM1"/>
-    <mergeCell ref="AJ2:AM2"/>
-    <mergeCell ref="AN1:AQ1"/>
-    <mergeCell ref="AN2:AQ2"/>
-    <mergeCell ref="AN4:AQ65"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="AZ28:AZ29"/>
-    <mergeCell ref="AZ30:AZ59"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="T2:W2"/>
-    <mergeCell ref="X1:AA1"/>
-    <mergeCell ref="X2:AA2"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="47" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
kurzer push um auf einem grösseren bildschirm einen screenshot zu machen hatte gerade wieder das selbe Problem mit git aber nach neu klonen geht es wieder
</commit_message>
<xml_diff>
--- a/Doku/Shannon_Neil_Schuerch_Zeitplan_IPA_2022.xlsx
+++ b/Doku/Shannon_Neil_Schuerch_Zeitplan_IPA_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Dashboardd\Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498C9E64-8935-4376-ACF8-501047E5DB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7384D140-9829-4F57-8386-F5049F513E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14625" xr2:uid="{B08A1154-B080-432D-B17F-9B53C1DBF0AA}"/>
   </bookViews>
@@ -1596,8 +1596,8 @@
   </sheetPr>
   <dimension ref="A1:BC66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BD28" sqref="BD28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AR7" sqref="AR7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,13 +2199,13 @@
       <c r="AI7" s="65"/>
       <c r="AJ7" s="39"/>
       <c r="AK7" s="40"/>
-      <c r="AL7" s="3"/>
-      <c r="AM7" s="12"/>
+      <c r="AL7" s="40"/>
+      <c r="AM7" s="65"/>
       <c r="AN7" s="73"/>
       <c r="AO7" s="74"/>
       <c r="AP7" s="74"/>
       <c r="AQ7" s="75"/>
-      <c r="AR7" s="11"/>
+      <c r="AR7" s="39"/>
       <c r="AS7" s="3"/>
       <c r="AT7" s="3"/>
       <c r="AU7" s="12"/>
@@ -2435,7 +2435,7 @@
       <c r="AI11" s="10"/>
       <c r="AJ11" s="8"/>
       <c r="AK11" s="9"/>
-      <c r="AL11" s="9"/>
+      <c r="AL11" s="53"/>
       <c r="AM11" s="10"/>
       <c r="AN11" s="73"/>
       <c r="AO11" s="74"/>
@@ -5177,8 +5177,8 @@
       <c r="AI59" s="10"/>
       <c r="AJ59" s="8"/>
       <c r="AK59" s="9"/>
-      <c r="AL59" s="9"/>
-      <c r="AM59" s="10"/>
+      <c r="AL59" s="53"/>
+      <c r="AM59" s="67"/>
       <c r="AN59" s="73"/>
       <c r="AO59" s="74"/>
       <c r="AP59" s="74"/>
@@ -5297,7 +5297,7 @@
       <c r="AO61" s="74"/>
       <c r="AP61" s="74"/>
       <c r="AQ61" s="75"/>
-      <c r="AR61" s="11"/>
+      <c r="AR61" s="39"/>
       <c r="AS61" s="3"/>
       <c r="AT61" s="3"/>
       <c r="AU61" s="12"/>
@@ -5409,7 +5409,7 @@
       <c r="AO63" s="74"/>
       <c r="AP63" s="74"/>
       <c r="AQ63" s="75"/>
-      <c r="AR63" s="8"/>
+      <c r="AR63" s="69"/>
       <c r="AS63" s="9"/>
       <c r="AT63" s="9"/>
       <c r="AU63" s="10"/>

</xml_diff>